<commit_message>
Paystubs and Verification Of Employemnet Business rules added Short Forms of Document Types added
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.malyala\Documents\UiPath\AZ-Application Review Process_Performer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.malyala\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E09ED113-815E-49D7-9934-940C7510BC26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21E9593-217E-4926-B391-843CD995FC8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="303">
   <si>
     <t>Name</t>
   </si>
@@ -202,9 +202,6 @@
     <t>FailureEmailBody</t>
   </si>
   <si>
-    <t>Hello,&lt;br&gt;AZ-Application Review Process_Performer failed to process. Reason:&lt;br&gt;&lt;Reason&gt;&lt;br&gt;&lt;br&gt;Thanks,Bot</t>
-  </si>
-  <si>
     <t>TempFolder</t>
   </si>
   <si>
@@ -818,6 +815,126 @@
   </si>
   <si>
     <t>Emergency Contact Form</t>
+  </si>
+  <si>
+    <t>InputFilesStorageBucketName</t>
+  </si>
+  <si>
+    <t>The {0} process has encountered a System Error.\n\nMachine Name: {1} \n\nLAN ID: {2} \n\nException Timestamp: {3} \n\nTransaction Reference: {4} \n\nException Message: {5} \n\nException Source: {6}</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>Pay Stub</t>
+  </si>
+  <si>
+    <t>PS_CompanyNameCheck</t>
+  </si>
+  <si>
+    <t>Company Name does not match across the Paystub, Exact Day Calculator, and ICW.</t>
+  </si>
+  <si>
+    <t>PS_MemNameCheck</t>
+  </si>
+  <si>
+    <t>Member listed does not match across the Paystub, Exact Day Calculator, and ICW.</t>
+  </si>
+  <si>
+    <t>Frequency of pay does not match across the Paystub, Exact Day Calculator, and ICW.</t>
+  </si>
+  <si>
+    <t>The date on the check stub is greater than 120 days old.</t>
+  </si>
+  <si>
+    <t>PS_CheckDateCheck</t>
+  </si>
+  <si>
+    <t>The application is for The Safford property but the Year to Date Income is not complete in the Exact Day Calculator.</t>
+  </si>
+  <si>
+    <t>PS_YearTodateIncome</t>
+  </si>
+  <si>
+    <t>PS_PeriodBeginCheck</t>
+  </si>
+  <si>
+    <t>PS_PeriodEndCheck</t>
+  </si>
+  <si>
+    <t>Period Begin does not match on the Paystub and Exact Day Calculator.</t>
+  </si>
+  <si>
+    <t>Period End does not match on the Paystub and Exact Day Calculator.</t>
+  </si>
+  <si>
+    <t>Gross Pay listed on the Paystub does not match the Exact Day Calculator.</t>
+  </si>
+  <si>
+    <t>PS_GrossPay</t>
+  </si>
+  <si>
+    <t>Highest Calculated Income on the Exact Day Calculator does not match Verified Income on the ICW.</t>
+  </si>
+  <si>
+    <t>PS_HighestCalValue</t>
+  </si>
+  <si>
+    <t>Pay Frequency calculated form the paystub does not match that listed on the Exact Day Calculator.</t>
+  </si>
+  <si>
+    <t>PS_FrequencyCheck</t>
+  </si>
+  <si>
+    <t>PS_PayFrequencyCalcCheck</t>
+  </si>
+  <si>
+    <t>VOE_CompanyNameCheck</t>
+  </si>
+  <si>
+    <t>VOE_EmployeeNameCheck</t>
+  </si>
+  <si>
+    <t>VOE_FrequencyCheck</t>
+  </si>
+  <si>
+    <t>Company Name across the Verification of Employment, Exact Day Calculator, and ICW do not match.</t>
+  </si>
+  <si>
+    <t>Employee Name across the Verification of Employment, Exact Day Calculator, and ICW do not match.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presently Employed has been listed as No on the Verification of Employment. Needs additional review. </t>
+  </si>
+  <si>
+    <t>VOE_PresentlyEmployedCheck</t>
+  </si>
+  <si>
+    <t>VOE_PresentlyEmployedDocumented</t>
+  </si>
+  <si>
+    <t>Presently Employed was documented as Yes on the Verification of Employment but no Date first employed was provided.</t>
+  </si>
+  <si>
+    <t>Date on the Verification of Employment is over 120 days in the past.</t>
+  </si>
+  <si>
+    <t>VOE_DateCheck</t>
+  </si>
+  <si>
+    <t>Pay Frequency on the Verification of Employment, Exact Day Calculator, and ICW do not match.</t>
+  </si>
+  <si>
+    <t>VOE_RegularRateMatch</t>
+  </si>
+  <si>
+    <t>Amount listed on Verification of Employment and Exact Day Calculator do not match.</t>
+  </si>
+  <si>
+    <t>VOE_SignatureCheck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verification of Employment has not been signed. </t>
   </si>
 </sst>
 </file>
@@ -1195,8 +1312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1276,138 +1393,145 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B14" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B16" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B19" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B21" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B22" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>265</v>
+      </c>
+      <c r="B23" t="s">
+        <v>266</v>
+      </c>
+    </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2393,8 +2517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2589,7 +2713,7 @@
         <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2603,58 +2727,58 @@
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" t="s">
         <v>68</v>
-      </c>
-      <c r="B26" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" t="s">
         <v>74</v>
-      </c>
-      <c r="B27" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" t="s">
         <v>65</v>
-      </c>
-      <c r="B28" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" t="s">
         <v>71</v>
-      </c>
-      <c r="B29" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3631,7 +3755,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3752,37 +3876,44 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
         <v>59</v>
-      </c>
-      <c r="B12" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B14" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
@@ -4777,10 +4908,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
-  <dimension ref="A1:C89"/>
+  <dimension ref="A1:C109"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4800,613 +4931,757 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3" t="s">
         <v>212</v>
-      </c>
-      <c r="B3" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B5" t="s">
         <v>196</v>
-      </c>
-      <c r="B5" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
+        <v>224</v>
+      </c>
+      <c r="B9" t="s">
         <v>225</v>
-      </c>
-      <c r="B9" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
+        <v>197</v>
+      </c>
+      <c r="B11" t="s">
         <v>198</v>
-      </c>
-      <c r="B11" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" t="s">
         <v>84</v>
-      </c>
-      <c r="B14" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
+        <v>213</v>
+      </c>
+      <c r="B15" t="s">
         <v>214</v>
-      </c>
-      <c r="B15" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
+        <v>215</v>
+      </c>
+      <c r="B16" t="s">
         <v>216</v>
-      </c>
-      <c r="B16" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" t="s">
         <v>86</v>
-      </c>
-      <c r="B17" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" t="s">
         <v>88</v>
-      </c>
-      <c r="B18" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" t="s">
         <v>91</v>
-      </c>
-      <c r="B20" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" t="s">
         <v>93</v>
-      </c>
-      <c r="B23" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" t="s">
         <v>95</v>
-      </c>
-      <c r="B24" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
+        <v>108</v>
+      </c>
+      <c r="B33" t="s">
         <v>109</v>
-      </c>
-      <c r="B33" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
+        <v>120</v>
+      </c>
+      <c r="B35" t="s">
         <v>121</v>
-      </c>
-      <c r="B35" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
+        <v>122</v>
+      </c>
+      <c r="B36" t="s">
         <v>123</v>
-      </c>
-      <c r="B36" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B37" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B39" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B40" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
+        <v>221</v>
+      </c>
+      <c r="B41" t="s">
         <v>222</v>
-      </c>
-      <c r="B41" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B44" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
+        <v>125</v>
+      </c>
+      <c r="B45" t="s">
         <v>126</v>
-      </c>
-      <c r="B45" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B46" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
+        <v>203</v>
+      </c>
+      <c r="B48" t="s">
         <v>204</v>
-      </c>
-      <c r="B48" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B49" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B50" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B51" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B52" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B53" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B54" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B55" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B56" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B57" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B59" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B60" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B61" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B62" t="s">
+        <v>133</v>
+      </c>
+      <c r="C62" t="s">
         <v>134</v>
-      </c>
-      <c r="C62" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B63" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B64" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B65" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
+        <v>205</v>
+      </c>
+      <c r="B67" t="s">
         <v>206</v>
-      </c>
-      <c r="B67" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B68" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B69" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B70" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B71" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B72" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B74" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B75" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B76" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B77" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
+        <v>209</v>
+      </c>
+      <c r="B79" t="s">
         <v>210</v>
-      </c>
-      <c r="B79" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B80" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B81" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
+        <v>207</v>
+      </c>
+      <c r="B83" t="s">
         <v>208</v>
-      </c>
-      <c r="B83" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B84" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B85" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B86" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B87" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
+        <v>217</v>
+      </c>
+      <c r="B88" t="s">
         <v>218</v>
-      </c>
-      <c r="B88" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
+        <v>191</v>
+      </c>
+      <c r="B89" t="s">
         <v>192</v>
       </c>
-      <c r="B89" t="s">
-        <v>193</v>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>267</v>
+      </c>
+      <c r="B91" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>269</v>
+      </c>
+      <c r="B92" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>285</v>
+      </c>
+      <c r="B93" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>273</v>
+      </c>
+      <c r="B94" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>275</v>
+      </c>
+      <c r="B95" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>276</v>
+      </c>
+      <c r="B96" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>277</v>
+      </c>
+      <c r="B97" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>281</v>
+      </c>
+      <c r="B98" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>286</v>
+      </c>
+      <c r="B99" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>283</v>
+      </c>
+      <c r="B100" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>287</v>
+      </c>
+      <c r="B102" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>289</v>
+      </c>
+      <c r="B103" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>288</v>
+      </c>
+      <c r="B104" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>293</v>
+      </c>
+      <c r="B105" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>294</v>
+      </c>
+      <c r="B106" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>297</v>
+      </c>
+      <c r="B107" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>299</v>
+      </c>
+      <c r="B108" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>301</v>
+      </c>
+      <c r="B109" t="s">
+        <v>302</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Business Rules for VOE and Offer Letter
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.malyala\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21E9593-217E-4926-B391-843CD995FC8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5537F5A-8271-4CDB-ACC5-3CECD041E3C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="329">
   <si>
     <t>Name</t>
   </si>
@@ -205,9 +205,6 @@
     <t>TempFolder</t>
   </si>
   <si>
-    <t>TempFolderForPDFs</t>
-  </si>
-  <si>
     <t>BE_002</t>
   </si>
   <si>
@@ -935,6 +932,87 @@
   </si>
   <si>
     <t xml:space="preserve">Verification of Employment has not been signed. </t>
+  </si>
+  <si>
+    <t>LocalPDFsFolder</t>
+  </si>
+  <si>
+    <t>YardiFindingType</t>
+  </si>
+  <si>
+    <t>YardiFinding</t>
+  </si>
+  <si>
+    <t>VOE_RTTotalPerYearMatch</t>
+  </si>
+  <si>
+    <t>VOE_OTAmountMatch</t>
+  </si>
+  <si>
+    <t>VOE_OTTotalPerYearMatch</t>
+  </si>
+  <si>
+    <t>VOE_SPAmountMatch</t>
+  </si>
+  <si>
+    <t>VOE_SPTotalPerYearMatch</t>
+  </si>
+  <si>
+    <t>VOE_TotalGrossPay</t>
+  </si>
+  <si>
+    <t>Total listed on the Exact Day Calculator does not match the Verified Income on the ICW.</t>
+  </si>
+  <si>
+    <t>The calculated Shift Differential Wage Per Year based on the Verification of Employment does not match the Shift differential Total Per Year on the Exact Day Calculator.</t>
+  </si>
+  <si>
+    <t>Sift Differential Rate listed on Verification of Employment and Exact Day Calculator do not match.</t>
+  </si>
+  <si>
+    <t>The calculated Overtime Wage Per Year based on the Verification of Employment does not match the OT Rate Total Per Year on the Exact Day Calculator.</t>
+  </si>
+  <si>
+    <t>Overtime Rate listed on Verification of Employment and Exact Day Calculator do not match.</t>
+  </si>
+  <si>
+    <t>The calculated Gross Wage Per Year based on the Verification of Employment does not match the Regular Rate Total Per Year on the Exact Day Calculator.</t>
+  </si>
+  <si>
+    <t>VOE</t>
+  </si>
+  <si>
+    <t>OL</t>
+  </si>
+  <si>
+    <t>Verification of Employment</t>
+  </si>
+  <si>
+    <t>Offer Letter</t>
+  </si>
+  <si>
+    <t>OL_DateCheck</t>
+  </si>
+  <si>
+    <t>OL_EmployerCheck</t>
+  </si>
+  <si>
+    <t>OL_EmployeeCheck</t>
+  </si>
+  <si>
+    <t>OL_PayCycleCheck</t>
+  </si>
+  <si>
+    <t>Date on the Offer Letter is greater than 120 days in the past.</t>
+  </si>
+  <si>
+    <t>Employer listed on the Offer Letter, Exact Day Calculator, and ICW do not match.</t>
+  </si>
+  <si>
+    <t>Employee Name listed on the Offer Letter, Exact Day Calculator, and ICW do not match.</t>
+  </si>
+  <si>
+    <t>Pay Frequency listed on the Offer Letter, Exact Day Calculator, and ICW do not match.</t>
   </si>
 </sst>
 </file>
@@ -1310,10 +1388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1393,132 +1471,132 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" t="s">
-        <v>228</v>
+      <c r="A8" s="2" t="s">
+        <v>302</v>
       </c>
       <c r="B8" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>227</v>
+      </c>
+      <c r="B9" t="s">
         <v>229</v>
       </c>
-      <c r="B9" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A11" t="s">
-        <v>235</v>
-      </c>
-      <c r="B11" t="s">
-        <v>257</v>
-      </c>
-    </row>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>228</v>
+      </c>
+      <c r="B10" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B12" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B13" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B14" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B15" t="s">
-        <v>255</v>
-      </c>
-      <c r="C15" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B16" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C16" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B17" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="C17" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B18" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="C18" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B19" t="s">
-        <v>248</v>
+        <v>255</v>
+      </c>
+      <c r="C19" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B20" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B21" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B22" t="s">
         <v>253</v>
@@ -1526,15 +1604,36 @@
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
+        <v>245</v>
+      </c>
+      <c r="B23" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>264</v>
+      </c>
+      <c r="B24" t="s">
         <v>265</v>
       </c>
-      <c r="B23" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>317</v>
+      </c>
+      <c r="B25" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>318</v>
+      </c>
+      <c r="B26" t="s">
+        <v>320</v>
+      </c>
+    </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2506,6 +2605,7 @@
     <row r="995" ht="14.25" customHeight="1"/>
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
+    <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2517,8 +2617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2713,7 +2813,7 @@
         <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2727,58 +2827,58 @@
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" t="s">
         <v>67</v>
-      </c>
-      <c r="B26" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" t="s">
         <v>73</v>
-      </c>
-      <c r="B27" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" t="s">
         <v>64</v>
-      </c>
-      <c r="B28" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" t="s">
         <v>70</v>
-      </c>
-      <c r="B29" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
@@ -3755,7 +3855,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3876,10 +3976,10 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -3887,50 +3987,64 @@
         <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+        <v>262</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>304</v>
+      </c>
+      <c r="B17" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -4908,10 +5022,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
-  <dimension ref="A1:C109"/>
+  <dimension ref="A1:C120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="B109" sqref="B109"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4931,757 +5045,837 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B3" t="s">
         <v>211</v>
-      </c>
-      <c r="B3" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B5" t="s">
         <v>195</v>
-      </c>
-      <c r="B5" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9" t="s">
         <v>224</v>
-      </c>
-      <c r="B9" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
+        <v>196</v>
+      </c>
+      <c r="B11" t="s">
         <v>197</v>
-      </c>
-      <c r="B11" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" t="s">
         <v>83</v>
-      </c>
-      <c r="B14" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
+        <v>212</v>
+      </c>
+      <c r="B15" t="s">
         <v>213</v>
-      </c>
-      <c r="B15" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
+        <v>214</v>
+      </c>
+      <c r="B16" t="s">
         <v>215</v>
-      </c>
-      <c r="B16" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" t="s">
         <v>85</v>
-      </c>
-      <c r="B17" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" t="s">
         <v>87</v>
-      </c>
-      <c r="B18" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" t="s">
         <v>90</v>
-      </c>
-      <c r="B20" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B22" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" t="s">
         <v>92</v>
-      </c>
-      <c r="B23" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" t="s">
         <v>94</v>
-      </c>
-      <c r="B24" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B28" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B30" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B32" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
+        <v>107</v>
+      </c>
+      <c r="B33" t="s">
         <v>108</v>
-      </c>
-      <c r="B33" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B34" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
+        <v>119</v>
+      </c>
+      <c r="B35" t="s">
         <v>120</v>
-      </c>
-      <c r="B35" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
+        <v>121</v>
+      </c>
+      <c r="B36" t="s">
         <v>122</v>
-      </c>
-      <c r="B36" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B37" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B39" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B40" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
+        <v>220</v>
+      </c>
+      <c r="B41" t="s">
         <v>221</v>
-      </c>
-      <c r="B41" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B44" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
+        <v>124</v>
+      </c>
+      <c r="B45" t="s">
         <v>125</v>
-      </c>
-      <c r="B45" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B46" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
+        <v>202</v>
+      </c>
+      <c r="B48" t="s">
         <v>203</v>
-      </c>
-      <c r="B48" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B49" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B50" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B51" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B52" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B53" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B54" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B55" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B56" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B57" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B59" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B60" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B61" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B62" t="s">
+        <v>132</v>
+      </c>
+      <c r="C62" t="s">
         <v>133</v>
-      </c>
-      <c r="C62" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B63" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B64" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B65" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
+        <v>204</v>
+      </c>
+      <c r="B67" t="s">
         <v>205</v>
-      </c>
-      <c r="B67" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B68" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="69" spans="1:2">
       <c r="A69" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B69" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="70" spans="1:2">
       <c r="A70" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B70" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="71" spans="1:2">
       <c r="A71" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B71" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="72" spans="1:2">
       <c r="A72" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B72" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B74" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B75" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B76" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B77" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
+        <v>208</v>
+      </c>
+      <c r="B79" t="s">
         <v>209</v>
-      </c>
-      <c r="B79" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B80" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B81" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
+        <v>206</v>
+      </c>
+      <c r="B83" t="s">
         <v>207</v>
-      </c>
-      <c r="B83" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B84" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B85" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B86" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B87" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
+        <v>216</v>
+      </c>
+      <c r="B88" t="s">
         <v>217</v>
-      </c>
-      <c r="B88" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
+        <v>190</v>
+      </c>
+      <c r="B89" t="s">
         <v>191</v>
-      </c>
-      <c r="B89" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
+        <v>266</v>
+      </c>
+      <c r="B91" t="s">
         <v>267</v>
-      </c>
-      <c r="B91" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
+        <v>268</v>
+      </c>
+      <c r="B92" t="s">
         <v>269</v>
-      </c>
-      <c r="B92" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B93" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B94" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B95" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B96" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B97" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B98" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B99" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B100" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B102" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B103" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B104" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B105" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
+        <v>293</v>
+      </c>
+      <c r="B106" t="s">
         <v>294</v>
-      </c>
-      <c r="B106" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B107" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
+        <v>298</v>
+      </c>
+      <c r="B108" t="s">
         <v>299</v>
-      </c>
-      <c r="B108" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
+        <v>300</v>
+      </c>
+      <c r="B109" t="s">
         <v>301</v>
       </c>
-      <c r="B109" t="s">
-        <v>302</v>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>305</v>
+      </c>
+      <c r="B110" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
+        <v>306</v>
+      </c>
+      <c r="B111" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
+        <v>307</v>
+      </c>
+      <c r="B112" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>308</v>
+      </c>
+      <c r="B113" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>309</v>
+      </c>
+      <c r="B114" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
+        <v>310</v>
+      </c>
+      <c r="B115" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>321</v>
+      </c>
+      <c r="B117" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
+        <v>322</v>
+      </c>
+      <c r="B118" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
+        <v>323</v>
+      </c>
+      <c r="B119" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
+        <v>324</v>
+      </c>
+      <c r="B120" t="s">
+        <v>328</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
businessRules added for Verification of Employment, Offe Letter, Work Number
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.malyala\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5537F5A-8271-4CDB-ACC5-3CECD041E3C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72E678D-DF61-4AB7-9F66-1D5789D1D9B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="356">
   <si>
     <t>Name</t>
   </si>
@@ -1013,6 +1013,87 @@
   </si>
   <si>
     <t>Pay Frequency listed on the Offer Letter, Exact Day Calculator, and ICW do not match.</t>
+  </si>
+  <si>
+    <t>VOE_BlankFieldsCheck</t>
+  </si>
+  <si>
+    <t>Not all fields have been documented appropriately on the Verification of Employment.</t>
+  </si>
+  <si>
+    <t>VOE_PerYearEarningsCheck</t>
+  </si>
+  <si>
+    <t>PS_PerYearEarningsCheck</t>
+  </si>
+  <si>
+    <t>OL_PerYearEarningsCheck</t>
+  </si>
+  <si>
+    <t>VOE_CommissionsBonusTipsPopulated</t>
+  </si>
+  <si>
+    <t>Commission, bonuses, tips, other amount has been populated. Needs additional review.</t>
+  </si>
+  <si>
+    <t>OL_HourlyPayRateCheck</t>
+  </si>
+  <si>
+    <t>OL_SalariedPayRateCheck</t>
+  </si>
+  <si>
+    <t>Pay Amount listed on the Offer Letter and Exact Day Calculator do not match.</t>
+  </si>
+  <si>
+    <t>OL_WeeklyHoursCheck</t>
+  </si>
+  <si>
+    <t>Weekly Hours listed on the Offer Letter and Exact Day Calculator do not match.</t>
+  </si>
+  <si>
+    <t>OL_NoOfPayPeriodsNot1</t>
+  </si>
+  <si>
+    <t>Number of pay periods for a salaried employee is not listed as 1 on the Exact Day Calculator.</t>
+  </si>
+  <si>
+    <t>WN</t>
+  </si>
+  <si>
+    <t>Work Number</t>
+  </si>
+  <si>
+    <t>WN_Datecheck</t>
+  </si>
+  <si>
+    <t>WN_EmployerCheck</t>
+  </si>
+  <si>
+    <t>WN_EmployeeCheck</t>
+  </si>
+  <si>
+    <t>WN_StatusCheck</t>
+  </si>
+  <si>
+    <t>WN_PayCycleCheck</t>
+  </si>
+  <si>
+    <t>WN_PerYearEarningsCheck</t>
+  </si>
+  <si>
+    <t>Date on the Work Number is greater than 120 days in the past.</t>
+  </si>
+  <si>
+    <t>Employer Name listed on the Work Number, Exact Day Calculator, and ICW do not match.</t>
+  </si>
+  <si>
+    <t>Employee Name listed on the Work Number, Exact Day Calculator, and ICW do not match.</t>
+  </si>
+  <si>
+    <t>Work Number status is not listed as active.</t>
+  </si>
+  <si>
+    <t>Pay Frequency listed on the Work Number, Exact Day Calculator, and ICW do not match.</t>
   </si>
 </sst>
 </file>
@@ -1391,7 +1472,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1634,7 +1715,14 @@
         <v>320</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" t="s">
+        <v>343</v>
+      </c>
+      <c r="B27" t="s">
+        <v>344</v>
+      </c>
+    </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
@@ -5022,10 +5110,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
-  <dimension ref="A1:C120"/>
+  <dimension ref="A1:C136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="A110" sqref="A110"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="B128" sqref="B128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5734,148 +5822,268 @@
         <v>281</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
-      <c r="A102" t="s">
-        <v>286</v>
-      </c>
-      <c r="B102" t="s">
-        <v>289</v>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>332</v>
+      </c>
+      <c r="B101" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="103" spans="1:2">
       <c r="A103" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B103" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B104" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B105" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B106" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B107" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B108" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B109" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B110" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B111" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B112" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B113" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B114" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
+        <v>309</v>
+      </c>
+      <c r="B115" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
         <v>310</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B116" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>321</v>
+        <v>329</v>
       </c>
       <c r="B117" t="s">
-        <v>325</v>
+        <v>330</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
       <c r="B118" t="s">
-        <v>326</v>
+        <v>273</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
+        <v>334</v>
+      </c>
+      <c r="B119" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>321</v>
+      </c>
+      <c r="B121" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" t="s">
+        <v>322</v>
+      </c>
+      <c r="B122" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" t="s">
         <v>323</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B123" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
-      <c r="A120" t="s">
+    <row r="124" spans="1:2">
+      <c r="A124" t="s">
         <v>324</v>
       </c>
-      <c r="B120" t="s">
+      <c r="B124" t="s">
         <v>328</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2">
+      <c r="A125" t="s">
+        <v>333</v>
+      </c>
+      <c r="B125" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2">
+      <c r="A126" t="s">
+        <v>339</v>
+      </c>
+      <c r="B126" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2">
+      <c r="A127" t="s">
+        <v>336</v>
+      </c>
+      <c r="B127" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2">
+      <c r="A128" t="s">
+        <v>337</v>
+      </c>
+      <c r="B128" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2">
+      <c r="A129" t="s">
+        <v>341</v>
+      </c>
+      <c r="B129" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" t="s">
+        <v>345</v>
+      </c>
+      <c r="B131" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2">
+      <c r="A132" t="s">
+        <v>346</v>
+      </c>
+      <c r="B132" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2">
+      <c r="A133" t="s">
+        <v>347</v>
+      </c>
+      <c r="B133" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
+      <c r="A134" t="s">
+        <v>348</v>
+      </c>
+      <c r="B134" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2">
+      <c r="A135" t="s">
+        <v>349</v>
+      </c>
+      <c r="B135" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2">
+      <c r="A136" t="s">
+        <v>350</v>
+      </c>
+      <c r="B136" t="s">
+        <v>273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added business rules for Child Spoort Payment History and SSBL
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.malyala\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F13FDF8-4B06-41BA-AE27-18C0FDB82D95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83151E04-A2B3-4A75-881A-511D7E0479BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="469">
   <si>
     <t>Name</t>
   </si>
@@ -1299,6 +1299,153 @@
   </si>
   <si>
     <t>Profit/Loss Statement</t>
+  </si>
+  <si>
+    <t>CSPH_ParentNameMatch</t>
+  </si>
+  <si>
+    <t>CSPH_FrequencyCheck</t>
+  </si>
+  <si>
+    <t>CSPH_DateCheck</t>
+  </si>
+  <si>
+    <t>CSPH_PaymentAmountCheck</t>
+  </si>
+  <si>
+    <t>CSPH_TotalPerYearCheck</t>
+  </si>
+  <si>
+    <t>CSPH_EndDateCheck</t>
+  </si>
+  <si>
+    <t>CSPH_StartDateCheck</t>
+  </si>
+  <si>
+    <t>CSPH_SumPaymentsCheck</t>
+  </si>
+  <si>
+    <t>CSPH_PerYearPaymentsInICW</t>
+  </si>
+  <si>
+    <t>Payment Amount listed on the Child Support Payment History and Child Support Calcs do not match.</t>
+  </si>
+  <si>
+    <t>Payments in a Year listed on the Child Support Payment History and Child Support Calcs do not match.</t>
+  </si>
+  <si>
+    <t>Total Child Support Payment in a Year listed on Child Support Calcs and the ICW do not match.</t>
+  </si>
+  <si>
+    <t>Start Date of Payments listed on the Child Support Payment History and Child Support Calcs do not match.</t>
+  </si>
+  <si>
+    <t>End Date of Payments listed on the Child Support Payment History and Child Support Calcs do not match.</t>
+  </si>
+  <si>
+    <t>Sum of Payments calculated from Child Support Payment History and listed on Child Support Calcs do not match.</t>
+  </si>
+  <si>
+    <t>Unable to determine frequency of payments from the Child Support Payment History.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date on the Child Support Payment History is over 120 days old. </t>
+  </si>
+  <si>
+    <t>Child's Name listed on the Child Support Payment History and Child Support Calcs do not match.</t>
+  </si>
+  <si>
+    <t>Receiving Parent listed on the Child Support Payment History, Child Support Calcs, and ICW do not match.</t>
+  </si>
+  <si>
+    <t>CSPH_ChildrenNamesCheck</t>
+  </si>
+  <si>
+    <t>CSPH_PaymentsInYearCheck</t>
+  </si>
+  <si>
+    <t>SSBL</t>
+  </si>
+  <si>
+    <t>Social Security Benefits Letter</t>
+  </si>
+  <si>
+    <t>CSPH</t>
+  </si>
+  <si>
+    <t>Child Support Payment History</t>
+  </si>
+  <si>
+    <t>CSC</t>
+  </si>
+  <si>
+    <t>Child Support Calcs</t>
+  </si>
+  <si>
+    <t>SSBL_EmployeeCheck</t>
+  </si>
+  <si>
+    <t>SSBL_DateCheck</t>
+  </si>
+  <si>
+    <t>SSBL_BNCNumberCheck</t>
+  </si>
+  <si>
+    <t>SSBL_MonthlyAmountCheck</t>
+  </si>
+  <si>
+    <t>SSBL_YearlyAmountCheck</t>
+  </si>
+  <si>
+    <t>SSBL_COLALetterCheck</t>
+  </si>
+  <si>
+    <t>SSBL_PressReleaseYearCheck</t>
+  </si>
+  <si>
+    <t>SSBL_ApplicantNameCheckCola</t>
+  </si>
+  <si>
+    <t>SSBL_MonthlyAmountCheckCola</t>
+  </si>
+  <si>
+    <t>SSBL_MIMonthCheck</t>
+  </si>
+  <si>
+    <t>SSBL_TotalPerYearMatchICW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Applicant Name listed on the Social Security Benefits Letter and ICW do not match. </t>
+  </si>
+  <si>
+    <t>Date of the Social Security Benefits Letter is over 120 days in the past.</t>
+  </si>
+  <si>
+    <t>BNC# listed on the Social Security Benefits Letter does not match on every page.</t>
+  </si>
+  <si>
+    <t>Monthly Amount listed on the Social Security Benefits Letter and the ICW do not match.</t>
+  </si>
+  <si>
+    <t>Yearly Amount calculated from the Social Security Benefits Letter does not math the ICW.</t>
+  </si>
+  <si>
+    <t>COLA Letter is missing from the application.</t>
+  </si>
+  <si>
+    <t>Press Release Year from the COLA Letter is not next year as expected.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Applicant Name listed on the Social Security Benefits Letter and COLA Calculator do not match. </t>
+  </si>
+  <si>
+    <t>Monthly Amount listed on the Social Security Benefits Letter and the COLA Calculator do not match.</t>
+  </si>
+  <si>
+    <t>Move In Month listed on the COLA Calculator does not match that as the next full months following the Move In Date on the Application Summary.</t>
+  </si>
+  <si>
+    <t>Total per year listed on the COLA Calculator and ICW do not match.</t>
   </si>
 </sst>
 </file>
@@ -1677,7 +1824,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1968,22 +2115,43 @@
         <v>419</v>
       </c>
     </row>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="33" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>445</v>
+      </c>
+      <c r="B33" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A34" t="s">
+        <v>443</v>
+      </c>
+      <c r="B34" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
+        <v>441</v>
+      </c>
+      <c r="B35" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -5357,10 +5525,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
-  <dimension ref="A1:C167"/>
+  <dimension ref="A1:C191"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
-      <selection activeCell="A166" sqref="A166"/>
+    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
+      <selection activeCell="B186" sqref="B186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6565,6 +6733,182 @@
         <v>399</v>
       </c>
     </row>
+    <row r="169" spans="1:2">
+      <c r="A169" t="s">
+        <v>420</v>
+      </c>
+      <c r="B169" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2">
+      <c r="A170" t="s">
+        <v>421</v>
+      </c>
+      <c r="B170" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2">
+      <c r="A171" t="s">
+        <v>422</v>
+      </c>
+      <c r="B171" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2">
+      <c r="A172" t="s">
+        <v>439</v>
+      </c>
+      <c r="B172" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2">
+      <c r="A173" t="s">
+        <v>423</v>
+      </c>
+      <c r="B173" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2">
+      <c r="A174" t="s">
+        <v>440</v>
+      </c>
+      <c r="B174" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2">
+      <c r="A175" t="s">
+        <v>424</v>
+      </c>
+      <c r="B175" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2">
+      <c r="A176" t="s">
+        <v>426</v>
+      </c>
+      <c r="B176" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2">
+      <c r="A177" t="s">
+        <v>425</v>
+      </c>
+      <c r="B177" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="A178" t="s">
+        <v>427</v>
+      </c>
+      <c r="B178" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
+      <c r="A179" t="s">
+        <v>428</v>
+      </c>
+      <c r="B179" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2">
+      <c r="A181" t="s">
+        <v>447</v>
+      </c>
+      <c r="B181" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2">
+      <c r="A182" t="s">
+        <v>448</v>
+      </c>
+      <c r="B182" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2">
+      <c r="A183" t="s">
+        <v>449</v>
+      </c>
+      <c r="B183" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2">
+      <c r="A184" t="s">
+        <v>450</v>
+      </c>
+      <c r="B184" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2">
+      <c r="A185" t="s">
+        <v>451</v>
+      </c>
+      <c r="B185" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2">
+      <c r="A186" t="s">
+        <v>452</v>
+      </c>
+      <c r="B186" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2">
+      <c r="A187" t="s">
+        <v>453</v>
+      </c>
+      <c r="B187" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2">
+      <c r="A188" t="s">
+        <v>454</v>
+      </c>
+      <c r="B188" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2">
+      <c r="A189" t="s">
+        <v>455</v>
+      </c>
+      <c r="B189" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2">
+      <c r="A190" t="s">
+        <v>456</v>
+      </c>
+      <c r="B190" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2">
+      <c r="A191" t="s">
+        <v>457</v>
+      </c>
+      <c r="B191" t="s">
+        <v>468</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
business Rules added for SSBL, VVRC
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.malyala\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83151E04-A2B3-4A75-881A-511D7E0479BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB99A3D-5195-4071-9BD7-3016DBE3CF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="481">
   <si>
     <t>Name</t>
   </si>
@@ -1446,6 +1446,42 @@
   </si>
   <si>
     <t>Total per year listed on the COLA Calculator and ICW do not match.</t>
+  </si>
+  <si>
+    <t>VRCC_ResidentNameCheck</t>
+  </si>
+  <si>
+    <t>VRCC_DateCheck</t>
+  </si>
+  <si>
+    <t>VRCC_AnticipatedAmount</t>
+  </si>
+  <si>
+    <t>VRCC_SignCheck</t>
+  </si>
+  <si>
+    <t>VRCC_DateSignedCheck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name listed on the Verification of Reoccurring Cash Contribution and ICW do not match. </t>
+  </si>
+  <si>
+    <t>Date listed on the Verification of Reoccurring Cash Contribution is over 120 days in the past.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount listed on the Verification of Reoccurring Cash Contribution and ICW do not match. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verification of Reoccurring Cash Contribution has not been signed. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verification of Reoccurring Cash Contribution has not been dated appropriately. </t>
+  </si>
+  <si>
+    <t>VRCC</t>
+  </si>
+  <si>
+    <t>Verification of Reoccurring Cash Contributions</t>
   </si>
 </sst>
 </file>
@@ -1824,7 +1860,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2139,7 +2175,14 @@
         <v>442</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A36" t="s">
+        <v>479</v>
+      </c>
+      <c r="B36" t="s">
+        <v>480</v>
+      </c>
+    </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
@@ -5525,10 +5568,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
-  <dimension ref="A1:C191"/>
+  <dimension ref="A1:C197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
-      <selection activeCell="B186" sqref="B186"/>
+    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
+      <selection activeCell="A166" sqref="A166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6909,6 +6952,46 @@
         <v>468</v>
       </c>
     </row>
+    <row r="193" spans="1:2">
+      <c r="A193" t="s">
+        <v>469</v>
+      </c>
+      <c r="B193" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2">
+      <c r="A194" t="s">
+        <v>470</v>
+      </c>
+      <c r="B194" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2">
+      <c r="A195" t="s">
+        <v>471</v>
+      </c>
+      <c r="B195" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2">
+      <c r="A196" t="s">
+        <v>472</v>
+      </c>
+      <c r="B196" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2">
+      <c r="A197" t="s">
+        <v>473</v>
+      </c>
+      <c r="B197" t="s">
+        <v>478</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Audit findings based on the issues and Array change
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.malyala\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DB99A3D-5195-4071-9BD7-3016DBE3CF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBAA80C-E034-46F5-B039-D0C1A842A0AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
-    <sheet name="Constants" sheetId="2" r:id="rId2"/>
-    <sheet name="Assets" sheetId="3" r:id="rId3"/>
-    <sheet name="Findings" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
+    <sheet name="Constants" sheetId="2" r:id="rId3"/>
+    <sheet name="Assets" sheetId="3" r:id="rId4"/>
+    <sheet name="Findings" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="532">
   <si>
     <t>Name</t>
   </si>
@@ -704,9 +705,6 @@
     <t>IAQ_AssetSourceListed</t>
   </si>
   <si>
-    <t>Asset soruces from the asset checklist do not match that listed on the ICW.</t>
-  </si>
-  <si>
     <t>IAQ_IncomeSourceListed</t>
   </si>
   <si>
@@ -782,18 +780,6 @@
     <t>Income &amp; Asset Questionnaire</t>
   </si>
   <si>
-    <t>Self Certification of Non-Employment Form</t>
-  </si>
-  <si>
-    <t>Asset Self Certification Form</t>
-  </si>
-  <si>
-    <t>Affidavit of Student Financial Assistance Form</t>
-  </si>
-  <si>
-    <t>Student Certification Form</t>
-  </si>
-  <si>
     <t>Certification of Zero Income</t>
   </si>
   <si>
@@ -806,9 +792,6 @@
     <t>AZ Income Limit Table</t>
   </si>
   <si>
-    <t>Member Information Document Form</t>
-  </si>
-  <si>
     <t>ICW (Income Calculation Worksheet)</t>
   </si>
   <si>
@@ -836,9 +819,6 @@
     <t>PS</t>
   </si>
   <si>
-    <t>Pay Stub</t>
-  </si>
-  <si>
     <t>PS_CompanyNameCheck</t>
   </si>
   <si>
@@ -1379,9 +1359,6 @@
     <t>CSC</t>
   </si>
   <si>
-    <t>Child Support Calcs</t>
-  </si>
-  <si>
     <t>SSBL_EmployeeCheck</t>
   </si>
   <si>
@@ -1482,6 +1459,183 @@
   </si>
   <si>
     <t>Verification of Reoccurring Cash Contributions</t>
+  </si>
+  <si>
+    <t>SSIB_EmployeeCheck</t>
+  </si>
+  <si>
+    <t>SSIB_DateCheck</t>
+  </si>
+  <si>
+    <t>SSIB_BNCNumberCheck</t>
+  </si>
+  <si>
+    <t>SSIB_MonthlyAmountCheck</t>
+  </si>
+  <si>
+    <t>SSIB_YearlyAmountCheck</t>
+  </si>
+  <si>
+    <t>SSIB_COLALetterCheck</t>
+  </si>
+  <si>
+    <t>SSIB_PressReleaseYearCheck</t>
+  </si>
+  <si>
+    <t>SSIB_ApplicantNameCheckCola</t>
+  </si>
+  <si>
+    <t>SSIB_MonthlyAmountCheckCola</t>
+  </si>
+  <si>
+    <t>SSIB_MIMonthCheck</t>
+  </si>
+  <si>
+    <t>SSIB_TotalPerYearMatchICW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Applicant Name listed on the Supplemental Security Income Letter and ICW do not match. </t>
+  </si>
+  <si>
+    <t>Date of the Supplemental Security Income Letter is over 120 days in the past.</t>
+  </si>
+  <si>
+    <t>BNC# listed on the Supplemental Security Income Letter does not match on every page.</t>
+  </si>
+  <si>
+    <t>Monthly Amount listed on the Supplemental Security Income Letter and the ICW do not match.</t>
+  </si>
+  <si>
+    <t>Yearly Amount calculated from the Supplemental Security Income Letter does not math the ICW.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Applicant Name listed on the Supplemental Security Income Letter and COLA Calculator do not match. </t>
+  </si>
+  <si>
+    <t>Monthly Amount listed on the Supplemental Security Income Letter and the COLA Calculator do not match.</t>
+  </si>
+  <si>
+    <t>EDC</t>
+  </si>
+  <si>
+    <t>COLALetter</t>
+  </si>
+  <si>
+    <t>COLA Letter</t>
+  </si>
+  <si>
+    <t>COLACalc</t>
+  </si>
+  <si>
+    <t>SSIB</t>
+  </si>
+  <si>
+    <t>Supplemental Security Income Benefits Letter</t>
+  </si>
+  <si>
+    <t>Income Calculation Worksheet</t>
+  </si>
+  <si>
+    <t>Asset Self-Certification</t>
+  </si>
+  <si>
+    <t>Arizona Income Limit Table</t>
+  </si>
+  <si>
+    <t>Member Information Document</t>
+  </si>
+  <si>
+    <t>Self-Certification of Non-Employment</t>
+  </si>
+  <si>
+    <t>Affidavit of Student Financial Assistance</t>
+  </si>
+  <si>
+    <t>Paystub</t>
+  </si>
+  <si>
+    <t>Profit Loss Statement</t>
+  </si>
+  <si>
+    <t>Child Support Cals</t>
+  </si>
+  <si>
+    <t>COLA Calculations</t>
+  </si>
+  <si>
+    <t>RequiredDocumentclassification</t>
+  </si>
+  <si>
+    <t>Bucket</t>
+  </si>
+  <si>
+    <t>Certifications</t>
+  </si>
+  <si>
+    <t>Applications</t>
+  </si>
+  <si>
+    <t>Assets</t>
+  </si>
+  <si>
+    <t>File Checklist</t>
+  </si>
+  <si>
+    <t>Property Management Documents</t>
+  </si>
+  <si>
+    <t>Student Certification</t>
+  </si>
+  <si>
+    <t>Student Status</t>
+  </si>
+  <si>
+    <t>Income</t>
+  </si>
+  <si>
+    <t>Child Support Self-Certification</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Affidavit of Paternity</t>
+  </si>
+  <si>
+    <t>Dominium Release of Information</t>
+  </si>
+  <si>
+    <t>Housing Disclosure</t>
+  </si>
+  <si>
+    <t>Anticipated Household Addition</t>
+  </si>
+  <si>
+    <t>Family Composition</t>
+  </si>
+  <si>
+    <t>Child Support</t>
+  </si>
+  <si>
+    <t>COLA Calculator</t>
+  </si>
+  <si>
+    <t>Verification of Reoccuring Cash Contributions</t>
+  </si>
+  <si>
+    <t>VAWA Acknowledgement</t>
+  </si>
+  <si>
+    <t>C:\Users\harika.malyala\Documents\AZApplicationReview\Prompts\</t>
+  </si>
+  <si>
+    <t>Replace_JArraayInJSON</t>
+  </si>
+  <si>
+    <t>Replace_JObjectInJSON</t>
+  </si>
+  <si>
+    <t>Asset sources from the asset checklist do not match that listed on the ICW.</t>
   </si>
 </sst>
 </file>
@@ -1857,10 +2011,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1940,253 +2094,284 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B7" t="s">
-        <v>233</v>
+        <v>528</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="B8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B12" t="s">
-        <v>256</v>
+        <v>497</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B13" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B14" t="s">
-        <v>248</v>
+        <v>498</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B15" t="s">
-        <v>249</v>
+        <v>502</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B16" t="s">
-        <v>254</v>
+        <v>499</v>
       </c>
       <c r="C16" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B17" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="C17" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B18" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C18" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B19" t="s">
+        <v>500</v>
+      </c>
+      <c r="C19" t="s">
         <v>255</v>
-      </c>
-      <c r="C19" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B20" t="s">
-        <v>247</v>
+        <v>501</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B21" t="s">
-        <v>250</v>
+        <v>514</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B22" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B23" t="s">
-        <v>252</v>
+        <v>527</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>264</v>
+        <v>491</v>
       </c>
       <c r="B24" t="s">
-        <v>265</v>
+        <v>253</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>317</v>
+        <v>258</v>
       </c>
       <c r="B25" t="s">
-        <v>319</v>
+        <v>503</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="B26" t="s">
-        <v>320</v>
+        <v>312</v>
+      </c>
+      <c r="C26" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>343</v>
+        <v>311</v>
       </c>
       <c r="B27" t="s">
-        <v>344</v>
+        <v>313</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>366</v>
+        <v>336</v>
       </c>
       <c r="B28" t="s">
-        <v>367</v>
+        <v>337</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>414</v>
+        <v>359</v>
       </c>
       <c r="B29" t="s">
-        <v>415</v>
+        <v>360</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A30">
+      <c r="A30" t="s">
+        <v>407</v>
+      </c>
+      <c r="B30" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31">
         <v>1040</v>
       </c>
-      <c r="B30">
+      <c r="B31">
         <v>1040</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A31" t="s">
-        <v>416</v>
-      </c>
-      <c r="B31" t="s">
-        <v>417</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="B32" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>445</v>
+        <v>411</v>
       </c>
       <c r="B33" t="s">
-        <v>446</v>
+        <v>504</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="B34" t="s">
-        <v>444</v>
+        <v>505</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="B35" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>479</v>
+        <v>492</v>
       </c>
       <c r="B36" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
+        <v>493</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A37" t="s">
+        <v>494</v>
+      </c>
+      <c r="B37" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A38" t="s">
+        <v>434</v>
+      </c>
+      <c r="B38" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A39" t="s">
+        <v>495</v>
+      </c>
+      <c r="B39" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A40" t="s">
+        <v>471</v>
+      </c>
+      <c r="B40" t="s">
+        <v>472</v>
+      </c>
+    </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3145,6 +3330,10 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
+    <row r="1002" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3153,11 +3342,349 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80DB68E2-2057-45AB-A45E-3EB9CF844C19}">
+  <dimension ref="A1:B40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="46.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>507</v>
+      </c>
+      <c r="B1" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>250</v>
+      </c>
+      <c r="B2" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>497</v>
+      </c>
+      <c r="B3" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B4" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>498</v>
+      </c>
+      <c r="B5" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>249</v>
+      </c>
+      <c r="B6" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>499</v>
+      </c>
+      <c r="B7" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>245</v>
+      </c>
+      <c r="B8" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>500</v>
+      </c>
+      <c r="B9" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>248</v>
+      </c>
+      <c r="B10" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>514</v>
+      </c>
+      <c r="B11" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>247</v>
+      </c>
+      <c r="B12" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>246</v>
+      </c>
+      <c r="B13" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>501</v>
+      </c>
+      <c r="B14" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>502</v>
+      </c>
+      <c r="B15" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>517</v>
+      </c>
+      <c r="B16" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>519</v>
+      </c>
+      <c r="B17" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>520</v>
+      </c>
+      <c r="B18" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>255</v>
+      </c>
+      <c r="B19" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>252</v>
+      </c>
+      <c r="B20" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>521</v>
+      </c>
+      <c r="B21" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>522</v>
+      </c>
+      <c r="B22" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>253</v>
+      </c>
+      <c r="B23" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>254</v>
+      </c>
+      <c r="B24" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>518</v>
+      </c>
+      <c r="B25" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>503</v>
+      </c>
+      <c r="B26" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>313</v>
+      </c>
+      <c r="B27" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>337</v>
+      </c>
+      <c r="B28" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>360</v>
+      </c>
+      <c r="B29" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>408</v>
+      </c>
+      <c r="B30" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31">
+        <v>1040</v>
+      </c>
+      <c r="B31" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>410</v>
+      </c>
+      <c r="B32" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>412</v>
+      </c>
+      <c r="B33" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>505</v>
+      </c>
+      <c r="B34" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>437</v>
+      </c>
+      <c r="B35" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>435</v>
+      </c>
+      <c r="B36" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>496</v>
+      </c>
+      <c r="B37" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>493</v>
+      </c>
+      <c r="B38" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>525</v>
+      </c>
+      <c r="B39" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>526</v>
+      </c>
+      <c r="B40" t="s">
+        <v>516</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z992"/>
+  <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3352,75 +3879,75 @@
         <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="22" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A22" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" t="s">
-        <v>49</v>
-      </c>
-    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B26" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B27" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
         <v>69</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
@@ -4383,18 +4910,19 @@
     <row r="990" ht="14.25" customHeight="1"/>
     <row r="991" ht="14.25" customHeight="1"/>
     <row r="992" ht="14.25" customHeight="1"/>
+    <row r="993" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4515,10 +5043,10 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -4531,54 +5059,68 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="B17" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="B18" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
+        <v>358</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>529</v>
+      </c>
+      <c r="B19" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A20" t="s">
+        <v>530</v>
+      </c>
+      <c r="B20" t="s">
+        <v>530</v>
+      </c>
+    </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
@@ -5566,12 +6108,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
-  <dimension ref="A1:C197"/>
+  <dimension ref="A1:C209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
-      <selection activeCell="A166" sqref="A166"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5631,10 +6173,10 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
+        <v>222</v>
+      </c>
+      <c r="B9" t="s">
         <v>223</v>
-      </c>
-      <c r="B9" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -5866,12 +6408,12 @@
         <v>220</v>
       </c>
       <c r="B41" t="s">
-        <v>221</v>
+        <v>531</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B42" t="s">
         <v>109</v>
@@ -6202,794 +6744,882 @@
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="B91" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="B92" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="B93" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="B94" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="B95" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="B96" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="B97" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="B98" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="B99" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="B100" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="B101" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="B102" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="B104" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="B105" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="B106" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="B107" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="B108" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="B109" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="B110" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="B111" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="B112" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="B113" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
+        <v>300</v>
+      </c>
+      <c r="B114" t="s">
         <v>307</v>
-      </c>
-      <c r="B114" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="B115" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="B116" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="B117" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="B118" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="B119" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="B120" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="B122" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="B123" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="B124" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="B125" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="B126" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="B127" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="B128" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="B129" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="B130" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="B132" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="B133" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="B134" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="B135" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="B136" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="B137" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="B138" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="B139" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="B140" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="B141" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="B142" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="B144" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="B145" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="B146" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="B147" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="B148" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="B149" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="B150" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="B151" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="B152" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="B154" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="B155" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="B156" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="B157" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="B158" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="B159" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="B160" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="B161" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="B162" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="B163" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="B164" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="B165" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="B166" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="B167" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="B169" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="B170" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="B171" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="B172" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="B173" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="B174" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" t="s">
+        <v>417</v>
+      </c>
+      <c r="B175" t="s">
         <v>424</v>
-      </c>
-      <c r="B175" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="B176" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="B177" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" t="s">
+        <v>420</v>
+      </c>
+      <c r="B178" t="s">
         <v>427</v>
-      </c>
-      <c r="B178" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="B179" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="B181" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="B182" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="B183" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="B184" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="B185" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="B186" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="B187" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="B188" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="B189" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="B190" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
       <c r="B191" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="B193" t="s">
-        <v>474</v>
+        <v>484</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
       <c r="B194" t="s">
-        <v>475</v>
+        <v>485</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
       <c r="B195" t="s">
-        <v>476</v>
+        <v>486</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
       <c r="B196" t="s">
-        <v>477</v>
+        <v>487</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
       <c r="B197" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2">
+      <c r="A198" t="s">
         <v>478</v>
+      </c>
+      <c r="B198" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2">
+      <c r="A199" t="s">
+        <v>479</v>
+      </c>
+      <c r="B199" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2">
+      <c r="A200" t="s">
+        <v>480</v>
+      </c>
+      <c r="B200" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2">
+      <c r="A201" t="s">
+        <v>481</v>
+      </c>
+      <c r="B201" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2">
+      <c r="A202" t="s">
+        <v>482</v>
+      </c>
+      <c r="B202" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2">
+      <c r="A203" t="s">
+        <v>483</v>
+      </c>
+      <c r="B203" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2">
+      <c r="A205" t="s">
+        <v>461</v>
+      </c>
+      <c r="B205" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2">
+      <c r="A206" t="s">
+        <v>462</v>
+      </c>
+      <c r="B206" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2">
+      <c r="A207" t="s">
+        <v>463</v>
+      </c>
+      <c r="B207" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2">
+      <c r="A208" t="s">
+        <v>464</v>
+      </c>
+      <c r="B208" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2">
+      <c r="A209" t="s">
+        <v>465</v>
+      </c>
+      <c r="B209" t="s">
+        <v>470</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates in Audit findings
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.malyala\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBAA80C-E034-46F5-B039-D0C1A842A0AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79805BC-8C86-4593-A2E8-A227FC057837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -507,15 +507,6 @@
     <t>ASC_SavingsAccountMatch</t>
   </si>
   <si>
-    <t>Tax credit provided does not match that listed on the ICW.</t>
-  </si>
-  <si>
-    <t>Checking account value diesn not match that listed on the ICW.</t>
-  </si>
-  <si>
-    <t>Saving account value listed does ot match that listed on the ICW.</t>
-  </si>
-  <si>
     <t>ASFA_AllQstnsYesHasAmount</t>
   </si>
   <si>
@@ -627,9 +618,6 @@
     <t>ICWExists</t>
   </si>
   <si>
-    <t>If ICW is missing, create a finding.</t>
-  </si>
-  <si>
     <t>ASExists</t>
   </si>
   <si>
@@ -813,9 +801,6 @@
     <t>InputFilesStorageBucketName</t>
   </si>
   <si>
-    <t>The {0} process has encountered a System Error.\n\nMachine Name: {1} \n\nLAN ID: {2} \n\nException Timestamp: {3} \n\nTransaction Reference: {4} \n\nException Message: {5} \n\nException Source: {6}</t>
-  </si>
-  <si>
     <t>PS</t>
   </si>
   <si>
@@ -1056,9 +1041,6 @@
     <t>Work Number</t>
   </si>
   <si>
-    <t>WN_Datecheck</t>
-  </si>
-  <si>
     <t>WN_EmployerCheck</t>
   </si>
   <si>
@@ -1125,9 +1107,6 @@
     <t>Verification Services</t>
   </si>
   <si>
-    <t>VS_Datecheck</t>
-  </si>
-  <si>
     <t>VS_EmployerCheck</t>
   </si>
   <si>
@@ -1146,9 +1125,6 @@
     <t>Pay Frequency listed on Verification Services, Exact Day Calculator, and ICW do not match.</t>
   </si>
   <si>
-    <t>VS_PayFrequency</t>
-  </si>
-  <si>
     <t>Two most recent Period Starts listed on the Verification Services and Exact Day Calculator do not match.</t>
   </si>
   <si>
@@ -1636,6 +1612,30 @@
   </si>
   <si>
     <t>Asset sources from the asset checklist do not match that listed on the ICW.</t>
+  </si>
+  <si>
+    <t>Tax Refund provided does not match that listed on the ICW.</t>
+  </si>
+  <si>
+    <t>The Income Calculation Worksheet is missing from the application.</t>
+  </si>
+  <si>
+    <t>Checking account value does not match that listed on the ICW.</t>
+  </si>
+  <si>
+    <t>Saving account value listed does not match that listed on the ICW.</t>
+  </si>
+  <si>
+    <t>WN_DateCheck</t>
+  </si>
+  <si>
+    <t>VS_PayCycleCheck</t>
+  </si>
+  <si>
+    <t>VS_DateCheck</t>
+  </si>
+  <si>
+    <t>The {0} process has encountered a System Error.\n\nMachine Name: {1} &lt;br&gt;&lt;br&gt;LAN ID: {2} \n\nException Timestamp: {3} &lt;br&gt;&lt;br&gt;Transaction Reference: {4} &lt;br&gt;&lt;br&gt;Exception Message: {5} &lt;br&gt;&lt;br&gt;Exception Source: {6}</t>
   </si>
 </sst>
 </file>
@@ -2013,7 +2013,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -2094,202 +2094,202 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B7" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="B8" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B9" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B10" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B12" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B13" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B14" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B15" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B16" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="C16" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B17" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C17" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B18" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C18" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B19" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="C19" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B20" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B21" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B22" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B23" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="B24" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B25" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="B26" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="C26" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B27" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="B28" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="B29" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="B30" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
@@ -2302,74 +2302,74 @@
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="B32" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="B33" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="B34" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="B35" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="B36" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="B37" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="B38" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="B39" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="B40" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3356,242 +3356,242 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
       <c r="B1" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B2" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="B3" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B4" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="B5" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B6" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="B7" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B8" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="B9" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B10" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="B11" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B12" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B13" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="B14" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="B15" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="B16" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="B17" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="B18" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B19" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B20" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="B21" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="B22" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B23" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="B24" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="B25" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="B26" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B27" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="B28" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="B29" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="B30" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -3599,79 +3599,79 @@
         <v>1040</v>
       </c>
       <c r="B31" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="B32" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="B33" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="B34" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="B35" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="B36" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="B37" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="B38" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="B39" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="B40" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
     </row>
   </sheetData>
@@ -3683,8 +3683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3879,7 +3879,7 @@
         <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>257</v>
+        <v>531</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
@@ -5043,10 +5043,10 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -5059,66 +5059,66 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B13" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B14" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="B17" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="B18" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="B19" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="B20" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
@@ -6112,8 +6112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
   <dimension ref="A1:C209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6133,18 +6133,18 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="B3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B5" t="s">
-        <v>195</v>
+        <v>525</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6157,10 +6157,10 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -6173,18 +6173,18 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B9" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B11" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -6213,18 +6213,18 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B15" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="B16" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -6261,10 +6261,10 @@
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B22" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -6333,10 +6333,10 @@
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B32" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -6405,15 +6405,15 @@
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B41" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B42" t="s">
         <v>109</v>
@@ -6421,7 +6421,7 @@
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B44" t="s">
         <v>123</v>
@@ -6445,10 +6445,10 @@
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B48" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -6504,7 +6504,7 @@
         <v>152</v>
       </c>
       <c r="B55" t="s">
-        <v>155</v>
+        <v>524</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -6512,7 +6512,7 @@
         <v>153</v>
       </c>
       <c r="B56" t="s">
-        <v>156</v>
+        <v>526</v>
       </c>
     </row>
     <row r="57" spans="1:3">
@@ -6520,36 +6520,36 @@
         <v>154</v>
       </c>
       <c r="B57" t="s">
-        <v>157</v>
+        <v>527</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
+        <v>157</v>
+      </c>
+      <c r="B59" t="s">
         <v>160</v>
-      </c>
-      <c r="B59" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
+        <v>158</v>
+      </c>
+      <c r="B60" t="s">
         <v>161</v>
-      </c>
-      <c r="B60" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
+        <v>159</v>
+      </c>
+      <c r="B61" t="s">
         <v>162</v>
-      </c>
-      <c r="B61" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B62" t="s">
         <v>132</v>
@@ -6560,7 +6560,7 @@
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B63" t="s">
         <v>134</v>
@@ -6584,10 +6584,10 @@
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B67" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -6595,7 +6595,7 @@
         <v>139</v>
       </c>
       <c r="B68" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -6603,7 +6603,7 @@
         <v>141</v>
       </c>
       <c r="B69" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -6611,7 +6611,7 @@
         <v>140</v>
       </c>
       <c r="B70" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -6619,7 +6619,7 @@
         <v>142</v>
       </c>
       <c r="B71" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -6627,999 +6627,999 @@
         <v>143</v>
       </c>
       <c r="B72" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="74" spans="1:2">
       <c r="A74" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B74" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="75" spans="1:2">
       <c r="A75" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B75" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="76" spans="1:2">
       <c r="A76" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B76" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="77" spans="1:2">
       <c r="A77" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B77" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="79" spans="1:2">
       <c r="A79" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B79" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="80" spans="1:2">
       <c r="A80" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B80" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B81" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B83" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B84" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
+        <v>181</v>
+      </c>
+      <c r="B85" t="s">
         <v>184</v>
-      </c>
-      <c r="B85" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
+        <v>182</v>
+      </c>
+      <c r="B86" t="s">
         <v>185</v>
-      </c>
-      <c r="B86" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B87" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B88" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B89" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B91" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B92" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B93" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B94" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B95" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B96" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B97" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="B98" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B99" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="B100" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="B101" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="B102" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B104" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="105" spans="1:2">
       <c r="A105" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="B105" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B106" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="B107" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B108" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B109" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B110" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="B111" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="B112" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="B113" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="B114" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
+        <v>296</v>
+      </c>
+      <c r="B115" t="s">
         <v>301</v>
-      </c>
-      <c r="B115" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="B116" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="B117" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="B118" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B119" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="B120" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B122" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="B123" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="B124" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B125" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="B126" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B127" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B128" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="B129" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="B130" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
+        <v>528</v>
+      </c>
+      <c r="B132" t="s">
         <v>338</v>
-      </c>
-      <c r="B132" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
+        <v>333</v>
+      </c>
+      <c r="B133" t="s">
         <v>339</v>
-      </c>
-      <c r="B133" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
+        <v>334</v>
+      </c>
+      <c r="B134" t="s">
         <v>340</v>
-      </c>
-      <c r="B134" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
+        <v>335</v>
+      </c>
+      <c r="B135" t="s">
         <v>341</v>
-      </c>
-      <c r="B135" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
+        <v>336</v>
+      </c>
+      <c r="B136" t="s">
         <v>342</v>
-      </c>
-      <c r="B136" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="B137" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="B138" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="B139" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="B140" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="B141" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
       <c r="B142" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>361</v>
+        <v>530</v>
       </c>
       <c r="B144" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="B145" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="B146" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>368</v>
+        <v>529</v>
       </c>
       <c r="B147" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="B148" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="B149" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="B150" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="B151" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="B152" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="B154" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="B155" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="B156" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="B157" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="B158" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="B159" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="B160" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="B161" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="B162" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="B163" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="B164" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="B165" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="B166" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="B167" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="B169" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="B170" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="B171" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="B172" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="B173" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="B174" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="B175" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="B176" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" t="s">
+        <v>410</v>
+      </c>
+      <c r="B177" t="s">
         <v>418</v>
-      </c>
-      <c r="B177" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="B178" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="B179" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="B181" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="B182" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="B183" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="B184" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="B185" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="B186" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="B187" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="B188" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="B189" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="B190" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="B191" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
       <c r="B193" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="B194" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="B195" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="B196" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
       <c r="B197" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="B198" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="B199" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="B200" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
     </row>
     <row r="201" spans="1:2">
       <c r="A201" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="B201" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="B202" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="B203" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="B205" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
       <c r="B206" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="B207" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="B208" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
       <c r="B209" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated code to fix the defects while running UAT
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.malyala\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79805BC-8C86-4593-A2E8-A227FC057837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5427DEE-2D6A-4718-A2BA-2DD9F90B84BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="608">
   <si>
     <t>Name</t>
   </si>
@@ -372,9 +372,6 @@
     <t>At least one field marked yes does not match the ICW.</t>
   </si>
   <si>
-    <t>IncomeQstnsAnsweredYes</t>
-  </si>
-  <si>
     <t>Field 16 on the asset checklist is left blank.</t>
   </si>
   <si>
@@ -855,15 +852,9 @@
     <t>PS_HighestCalValue</t>
   </si>
   <si>
-    <t>Pay Frequency calculated form the paystub does not match that listed on the Exact Day Calculator.</t>
-  </si>
-  <si>
     <t>PS_FrequencyCheck</t>
   </si>
   <si>
-    <t>PS_PayFrequencyCalcCheck</t>
-  </si>
-  <si>
     <t>VOE_CompanyNameCheck</t>
   </si>
   <si>
@@ -1636,6 +1627,243 @@
   </si>
   <si>
     <t>The {0} process has encountered a System Error.\n\nMachine Name: {1} &lt;br&gt;&lt;br&gt;LAN ID: {2} \n\nException Timestamp: {3} &lt;br&gt;&lt;br&gt;Transaction Reference: {4} &lt;br&gt;&lt;br&gt;Exception Message: {5} &lt;br&gt;&lt;br&gt;Exception Source: {6}</t>
+  </si>
+  <si>
+    <t>PS_CheckDateWithMoveIn</t>
+  </si>
+  <si>
+    <t>VOE_DateCheckWithMoveIn</t>
+  </si>
+  <si>
+    <t>OL_DateCheckWithMoveIn</t>
+  </si>
+  <si>
+    <t>WN_DateCheckWithMoveIn</t>
+  </si>
+  <si>
+    <t>VS_DateCheckWithMoveIn</t>
+  </si>
+  <si>
+    <t>SEC_CheckDateWithMoveIn</t>
+  </si>
+  <si>
+    <t>CSPH_DateCheckWithMoveIn</t>
+  </si>
+  <si>
+    <t>SSIB_DateCheckWithMoveIn</t>
+  </si>
+  <si>
+    <t>VRCC_DateCheckWithMoveIn</t>
+  </si>
+  <si>
+    <t>The date on the check stub is not with in 120 days of Move-In date.</t>
+  </si>
+  <si>
+    <t>PS_EDCCheck</t>
+  </si>
+  <si>
+    <t>Exact Day Calculator does not exist for Paystub findings</t>
+  </si>
+  <si>
+    <t>VOE_EDCCheck</t>
+  </si>
+  <si>
+    <t>Exact Day Calculator does not exist for Verification of employment findings</t>
+  </si>
+  <si>
+    <t>OL_EDCCheck</t>
+  </si>
+  <si>
+    <t>Exact Day Calculator does not exist for Offer Letter findings</t>
+  </si>
+  <si>
+    <t>WN_EDCCheck</t>
+  </si>
+  <si>
+    <t>Exact Day Calculator does not exist for Work Number findings</t>
+  </si>
+  <si>
+    <t>VS_EDCCheck</t>
+  </si>
+  <si>
+    <t>Exact Day Calculator does not exist for Verification services findings</t>
+  </si>
+  <si>
+    <t>SSBL_COLACalcCheck</t>
+  </si>
+  <si>
+    <t>COLA Calc is missing from the application</t>
+  </si>
+  <si>
+    <t>SSIB_COLACalcCheck</t>
+  </si>
+  <si>
+    <t>PS_FindingError</t>
+  </si>
+  <si>
+    <t>Errors in Validating findings for Paystub</t>
+  </si>
+  <si>
+    <t>SR_FindingError</t>
+  </si>
+  <si>
+    <t>Errors in Validating findings for Screening Document</t>
+  </si>
+  <si>
+    <t>VRCC_FindingError</t>
+  </si>
+  <si>
+    <t>SSIB_FindingError</t>
+  </si>
+  <si>
+    <t>Errors in Validating findings for Verification of Reoccurring Cash Contribution</t>
+  </si>
+  <si>
+    <t>SSBL_FindingError</t>
+  </si>
+  <si>
+    <t>Errors in Validating findings for Supplemental Security Income Letter</t>
+  </si>
+  <si>
+    <t>ICW_FindingError</t>
+  </si>
+  <si>
+    <t>CSPH_FindingError</t>
+  </si>
+  <si>
+    <t>SEC_FindingError</t>
+  </si>
+  <si>
+    <t>VS_FindingError</t>
+  </si>
+  <si>
+    <t>WN_FindingError</t>
+  </si>
+  <si>
+    <t>OL_FindingError</t>
+  </si>
+  <si>
+    <t>VOE_FindingError</t>
+  </si>
+  <si>
+    <t>VAWA_FindingError</t>
+  </si>
+  <si>
+    <t>CZI_FindingError</t>
+  </si>
+  <si>
+    <t>SC_FindingError</t>
+  </si>
+  <si>
+    <t>ASFA_FindingError</t>
+  </si>
+  <si>
+    <t>ASC_FindingError</t>
+  </si>
+  <si>
+    <t>SCNE_FindingError</t>
+  </si>
+  <si>
+    <t>IAQ_FindingError</t>
+  </si>
+  <si>
+    <t>MID_FindingError</t>
+  </si>
+  <si>
+    <t>AS_FindingError</t>
+  </si>
+  <si>
+    <t>IAQ_CertificationDateCheck</t>
+  </si>
+  <si>
+    <t>The effective dates on the ICW, Application Summary, and Income &amp; Asset Questionnaire do not match as expected.</t>
+  </si>
+  <si>
+    <t>Errors in Validating findings for ICW</t>
+  </si>
+  <si>
+    <t>Errors in Validating findings for Application Summary</t>
+  </si>
+  <si>
+    <t>Errors in Validating findings for Member Information Document</t>
+  </si>
+  <si>
+    <t>Errors in Validating findings for Income &amp; Assest Questionnaire</t>
+  </si>
+  <si>
+    <t>Errors in Validating findings for Self Certification of Non Employment.</t>
+  </si>
+  <si>
+    <t>Errors in Validating findings for Asset Self Certification &amp; Worksheet</t>
+  </si>
+  <si>
+    <t>Errors in Validating findings for Affidavit of Student Financial Assistance</t>
+  </si>
+  <si>
+    <t>Errors in Validating findings for Student Certification</t>
+  </si>
+  <si>
+    <t>Errors in Validating findings for Certificatio of Zero Income.</t>
+  </si>
+  <si>
+    <t>Errors in Validating findings for VAWA Acknowledgement</t>
+  </si>
+  <si>
+    <t>Errors in Validating findings for Verification of Employment</t>
+  </si>
+  <si>
+    <t>Errors in Validating findings for Offer Letter</t>
+  </si>
+  <si>
+    <t>Errors in Validating findings for Work Number</t>
+  </si>
+  <si>
+    <t>Errors in Validating findings for Verification Services</t>
+  </si>
+  <si>
+    <t>Errors in Validating findings for Self-Employment Certification</t>
+  </si>
+  <si>
+    <t>Errors in Validating findings for Child Support Payment History</t>
+  </si>
+  <si>
+    <t>ICW_AssetsOver51600</t>
+  </si>
+  <si>
+    <t>Assets over 51600 need to be verified</t>
+  </si>
+  <si>
+    <t>SEC_1040ScheduleExists</t>
+  </si>
+  <si>
+    <t>SEC_ProfitLossExists</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Profit Loss forms does not exist for Self-Employment Verification </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1040, Schedulec forms does not exist for Self-Employment Verification </t>
+  </si>
+  <si>
+    <t>IAQ_AssetsValueMatch</t>
+  </si>
+  <si>
+    <t>Assets value does not match that listed on the ICW.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not using it anymore </t>
+  </si>
+  <si>
+    <t>CZI_MinimalExpenseMarkedNA</t>
+  </si>
+  <si>
+    <t>The required minimal expenses on the Certification of Zero Income are marked N/A</t>
+  </si>
+  <si>
+    <t>MoveInDateEmpty</t>
+  </si>
+  <si>
+    <t>The move-in date is blank</t>
   </si>
 </sst>
 </file>
@@ -2013,7 +2241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -2094,202 +2322,202 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B7" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B8" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B12" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B14" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B15" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B16" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="C16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B18" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C18" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B19" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="C19" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B20" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B21" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B23" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="B24" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B25" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B26" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C26" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B27" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B28" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B29" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B30" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
@@ -2302,74 +2530,74 @@
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="B32" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B33" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B34" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B35" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="B36" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="B37" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B38" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="B39" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="B40" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3356,242 +3584,242 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="B1" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B2" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="B3" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B4" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="B5" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B6" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B7" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B8" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="B9" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B10" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B11" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B12" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B13" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B14" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="B15" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="B16" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="B17" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="B18" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B19" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B20" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="B21" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="B22" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B23" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B24" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="B25" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="B26" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B27" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B28" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="B29" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B30" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -3599,79 +3827,79 @@
         <v>1040</v>
       </c>
       <c r="B31" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="B32" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B33" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B34" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B35" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B36" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="B37" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B38" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="B39" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="B40" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
   </sheetData>
@@ -3683,8 +3911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3879,7 +4107,7 @@
         <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
@@ -5043,10 +5271,10 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
@@ -5059,66 +5287,66 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B17" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="B18" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="B19" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="B20" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
@@ -6110,10 +6338,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
-  <dimension ref="A1:C209"/>
+  <dimension ref="A1:C251"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6133,18 +6361,18 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B3" t="s">
         <v>206</v>
-      </c>
-      <c r="B3" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B5" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6157,10 +6385,10 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -6173,1453 +6401,1792 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
+        <v>217</v>
+      </c>
+      <c r="B9" t="s">
         <v>218</v>
       </c>
-      <c r="B9" t="s">
-        <v>219</v>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>595</v>
+      </c>
+      <c r="B10" t="s">
+        <v>596</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>192</v>
+        <v>561</v>
       </c>
       <c r="B11" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B12" t="s">
-        <v>75</v>
+        <v>579</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>191</v>
       </c>
       <c r="B13" t="s">
-        <v>76</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B14" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>208</v>
+        <v>606</v>
       </c>
       <c r="B15" t="s">
-        <v>209</v>
+        <v>607</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>210</v>
+        <v>80</v>
       </c>
       <c r="B16" t="s">
-        <v>211</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>207</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>208</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>81</v>
+        <v>209</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B20" t="s">
-        <v>90</v>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>194</v>
+        <v>81</v>
       </c>
       <c r="B22" t="s">
-        <v>196</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>93</v>
+        <v>576</v>
       </c>
       <c r="B24" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
-        <v>101</v>
-      </c>
-      <c r="B25" t="s">
-        <v>95</v>
+        <v>580</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>102</v>
+        <v>193</v>
       </c>
       <c r="B26" t="s">
-        <v>96</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B28" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B29" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B30" t="s">
-        <v>100</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>103</v>
+      </c>
+      <c r="B31" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>195</v>
+        <v>104</v>
       </c>
       <c r="B32" t="s">
-        <v>197</v>
+        <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B33" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B34" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>119</v>
+        <v>575</v>
       </c>
       <c r="B35" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" t="s">
-        <v>121</v>
-      </c>
-      <c r="B36" t="s">
-        <v>122</v>
+        <v>581</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>115</v>
+        <v>194</v>
       </c>
       <c r="B37" t="s">
-        <v>111</v>
+        <v>196</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B38" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B39" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B40" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>216</v>
+        <v>114</v>
       </c>
       <c r="B41" t="s">
-        <v>523</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>217</v>
+        <v>115</v>
       </c>
       <c r="B42" t="s">
-        <v>109</v>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>116</v>
+      </c>
+      <c r="B43" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>168</v>
+        <v>117</v>
       </c>
       <c r="B44" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>124</v>
+        <v>215</v>
       </c>
       <c r="B45" t="s">
-        <v>125</v>
+        <v>520</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>127</v>
+        <v>216</v>
       </c>
       <c r="B46" t="s">
-        <v>126</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>577</v>
+      </c>
+      <c r="B47" t="s">
+        <v>578</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>198</v>
+        <v>601</v>
       </c>
       <c r="B48" t="s">
-        <v>199</v>
+        <v>602</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>128</v>
+        <v>574</v>
       </c>
       <c r="B49" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" t="s">
-        <v>129</v>
-      </c>
-      <c r="B50" t="s">
-        <v>131</v>
+        <v>582</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>144</v>
+        <v>167</v>
       </c>
       <c r="B51" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="B52" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
       <c r="B53" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>147</v>
+        <v>573</v>
       </c>
       <c r="B54" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" t="s">
-        <v>152</v>
-      </c>
-      <c r="B55" t="s">
-        <v>524</v>
+        <v>583</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>153</v>
+        <v>197</v>
       </c>
       <c r="B56" t="s">
-        <v>526</v>
+        <v>198</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="B57" t="s">
-        <v>527</v>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>128</v>
+      </c>
+      <c r="B58" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="B59" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="B60" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="B61" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B62" t="s">
-        <v>132</v>
-      </c>
-      <c r="C62" t="s">
-        <v>133</v>
+        <v>150</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B63" t="s">
-        <v>134</v>
+        <v>521</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
+        <v>152</v>
+      </c>
+      <c r="B64" t="s">
+        <v>523</v>
+      </c>
+      <c r="C64" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>153</v>
+      </c>
+      <c r="B65" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>572</v>
+      </c>
+      <c r="B66" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>156</v>
+      </c>
+      <c r="B68" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>157</v>
+      </c>
+      <c r="B69" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>158</v>
+      </c>
+      <c r="B70" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>154</v>
+      </c>
+      <c r="B71" t="s">
+        <v>131</v>
+      </c>
+      <c r="C71" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>155</v>
+      </c>
+      <c r="B72" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>136</v>
+      </c>
+      <c r="B73" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
         <v>137</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B74" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
-      <c r="A65" t="s">
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>571</v>
+      </c>
+      <c r="B75" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>199</v>
+      </c>
+      <c r="B77" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
         <v>138</v>
       </c>
-      <c r="B65" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
-      <c r="A67" t="s">
-        <v>200</v>
-      </c>
-      <c r="B67" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
-      <c r="A68" t="s">
+      <c r="B78" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>140</v>
+      </c>
+      <c r="B79" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
         <v>139</v>
       </c>
-      <c r="B68" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
-      <c r="A69" t="s">
-        <v>141</v>
-      </c>
-      <c r="B69" t="s">
+      <c r="B80" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
-      <c r="A70" t="s">
-        <v>140</v>
-      </c>
-      <c r="B70" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
-      <c r="A71" t="s">
-        <v>142</v>
-      </c>
-      <c r="B71" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
-      <c r="A72" t="s">
-        <v>143</v>
-      </c>
-      <c r="B72" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
-      <c r="A74" t="s">
-        <v>169</v>
-      </c>
-      <c r="B74" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
-      <c r="A75" t="s">
-        <v>170</v>
-      </c>
-      <c r="B75" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
-      <c r="A76" t="s">
-        <v>171</v>
-      </c>
-      <c r="B76" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
-      <c r="A77" t="s">
-        <v>172</v>
-      </c>
-      <c r="B77" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
-      <c r="A79" t="s">
-        <v>204</v>
-      </c>
-      <c r="B79" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
-      <c r="A80" t="s">
-        <v>177</v>
-      </c>
-      <c r="B80" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>178</v>
+        <v>141</v>
       </c>
       <c r="B81" t="s">
-        <v>180</v>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>142</v>
+      </c>
+      <c r="B82" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>202</v>
+        <v>570</v>
       </c>
       <c r="B83" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" t="s">
-        <v>186</v>
-      </c>
-      <c r="B84" t="s">
-        <v>183</v>
+        <v>586</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="B85" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="B86" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>215</v>
+        <v>170</v>
       </c>
       <c r="B87" t="s">
-        <v>214</v>
+        <v>174</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>212</v>
+        <v>171</v>
       </c>
       <c r="B88" t="s">
-        <v>213</v>
+        <v>175</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>187</v>
+        <v>604</v>
       </c>
       <c r="B89" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" t="s">
-        <v>254</v>
-      </c>
-      <c r="B91" t="s">
-        <v>255</v>
+        <v>605</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>569</v>
+      </c>
+      <c r="B90" t="s">
+        <v>587</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>256</v>
+        <v>203</v>
       </c>
       <c r="B92" t="s">
-        <v>257</v>
+        <v>204</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>272</v>
+        <v>176</v>
       </c>
       <c r="B93" t="s">
-        <v>258</v>
+        <v>178</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>260</v>
+        <v>177</v>
       </c>
       <c r="B94" t="s">
-        <v>259</v>
+        <v>179</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>262</v>
+        <v>568</v>
       </c>
       <c r="B95" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
-      <c r="A96" t="s">
-        <v>263</v>
-      </c>
-      <c r="B96" t="s">
-        <v>265</v>
+        <v>588</v>
       </c>
     </row>
     <row r="97" spans="1:2">
       <c r="A97" t="s">
-        <v>264</v>
+        <v>201</v>
       </c>
       <c r="B97" t="s">
-        <v>266</v>
+        <v>202</v>
       </c>
     </row>
     <row r="98" spans="1:2">
       <c r="A98" t="s">
-        <v>268</v>
+        <v>185</v>
       </c>
       <c r="B98" t="s">
-        <v>267</v>
+        <v>182</v>
       </c>
     </row>
     <row r="99" spans="1:2">
       <c r="A99" t="s">
-        <v>273</v>
+        <v>180</v>
       </c>
       <c r="B99" t="s">
-        <v>271</v>
+        <v>183</v>
       </c>
     </row>
     <row r="100" spans="1:2">
       <c r="A100" t="s">
-        <v>270</v>
+        <v>181</v>
       </c>
       <c r="B100" t="s">
-        <v>269</v>
+        <v>184</v>
       </c>
     </row>
     <row r="101" spans="1:2">
       <c r="A101" t="s">
-        <v>320</v>
+        <v>214</v>
       </c>
       <c r="B101" t="s">
-        <v>261</v>
+        <v>213</v>
       </c>
     </row>
     <row r="102" spans="1:2">
       <c r="A102" t="s">
-        <v>369</v>
+        <v>211</v>
       </c>
       <c r="B102" t="s">
-        <v>370</v>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>186</v>
+      </c>
+      <c r="B103" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="104" spans="1:2">
       <c r="A104" t="s">
-        <v>274</v>
+        <v>554</v>
       </c>
       <c r="B104" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2">
-      <c r="A105" t="s">
-        <v>276</v>
-      </c>
-      <c r="B105" t="s">
-        <v>285</v>
+        <v>555</v>
       </c>
     </row>
     <row r="106" spans="1:2">
       <c r="A106" t="s">
-        <v>275</v>
+        <v>539</v>
       </c>
       <c r="B106" t="s">
-        <v>278</v>
+        <v>540</v>
       </c>
     </row>
     <row r="107" spans="1:2">
       <c r="A107" t="s">
-        <v>280</v>
+        <v>253</v>
       </c>
       <c r="B107" t="s">
-        <v>279</v>
+        <v>254</v>
       </c>
     </row>
     <row r="108" spans="1:2">
       <c r="A108" t="s">
-        <v>281</v>
+        <v>255</v>
       </c>
       <c r="B108" t="s">
-        <v>282</v>
+        <v>256</v>
       </c>
     </row>
     <row r="109" spans="1:2">
       <c r="A109" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="B109" t="s">
-        <v>283</v>
+        <v>257</v>
       </c>
     </row>
     <row r="110" spans="1:2">
       <c r="A110" t="s">
-        <v>286</v>
+        <v>259</v>
       </c>
       <c r="B110" t="s">
-        <v>287</v>
+        <v>258</v>
       </c>
     </row>
     <row r="111" spans="1:2">
       <c r="A111" t="s">
-        <v>288</v>
+        <v>529</v>
       </c>
       <c r="B111" t="s">
-        <v>289</v>
+        <v>538</v>
       </c>
     </row>
     <row r="112" spans="1:2">
       <c r="A112" t="s">
-        <v>293</v>
+        <v>261</v>
       </c>
       <c r="B112" t="s">
-        <v>304</v>
+        <v>260</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>294</v>
+        <v>262</v>
       </c>
       <c r="B113" t="s">
-        <v>303</v>
+        <v>264</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>295</v>
+        <v>263</v>
       </c>
       <c r="B114" t="s">
-        <v>302</v>
+        <v>265</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>296</v>
+        <v>267</v>
       </c>
       <c r="B115" t="s">
-        <v>301</v>
+        <v>266</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>297</v>
+        <v>269</v>
       </c>
       <c r="B116" t="s">
-        <v>300</v>
+        <v>268</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>298</v>
+        <v>317</v>
       </c>
       <c r="B117" t="s">
-        <v>299</v>
+        <v>260</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>317</v>
+        <v>366</v>
       </c>
       <c r="B118" t="s">
-        <v>318</v>
+        <v>367</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>319</v>
+        <v>552</v>
       </c>
       <c r="B119" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2">
-      <c r="A120" t="s">
-        <v>322</v>
-      </c>
-      <c r="B120" t="s">
-        <v>323</v>
+        <v>553</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>541</v>
+      </c>
+      <c r="B121" t="s">
+        <v>542</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>309</v>
+        <v>271</v>
       </c>
       <c r="B122" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" ht="13.5" customHeight="1">
       <c r="A123" t="s">
-        <v>310</v>
+        <v>273</v>
       </c>
       <c r="B123" t="s">
-        <v>314</v>
+        <v>282</v>
       </c>
     </row>
     <row r="124" spans="1:2">
       <c r="A124" t="s">
-        <v>311</v>
+        <v>272</v>
       </c>
       <c r="B124" t="s">
-        <v>315</v>
+        <v>275</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>312</v>
+        <v>277</v>
       </c>
       <c r="B125" t="s">
-        <v>316</v>
+        <v>276</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>321</v>
+        <v>278</v>
       </c>
       <c r="B126" t="s">
-        <v>261</v>
+        <v>279</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>327</v>
+        <v>281</v>
       </c>
       <c r="B127" t="s">
-        <v>328</v>
+        <v>280</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>324</v>
+        <v>530</v>
       </c>
       <c r="B128" t="s">
-        <v>326</v>
+        <v>280</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>325</v>
+        <v>283</v>
       </c>
       <c r="B129" t="s">
-        <v>326</v>
+        <v>284</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>329</v>
+        <v>285</v>
       </c>
       <c r="B130" t="s">
-        <v>330</v>
+        <v>286</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" t="s">
+        <v>290</v>
+      </c>
+      <c r="B131" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>528</v>
+        <v>291</v>
       </c>
       <c r="B132" t="s">
-        <v>338</v>
+        <v>300</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>333</v>
+        <v>292</v>
       </c>
       <c r="B133" t="s">
-        <v>339</v>
+        <v>299</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>334</v>
+        <v>293</v>
       </c>
       <c r="B134" t="s">
-        <v>340</v>
+        <v>298</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>335</v>
+        <v>294</v>
       </c>
       <c r="B135" t="s">
-        <v>341</v>
+        <v>297</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>336</v>
+        <v>295</v>
       </c>
       <c r="B136" t="s">
-        <v>342</v>
+        <v>296</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>337</v>
+        <v>314</v>
       </c>
       <c r="B137" t="s">
-        <v>261</v>
+        <v>315</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>343</v>
+        <v>316</v>
       </c>
       <c r="B138" t="s">
-        <v>344</v>
+        <v>260</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>345</v>
+        <v>319</v>
       </c>
       <c r="B139" t="s">
-        <v>346</v>
+        <v>320</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>348</v>
+        <v>567</v>
       </c>
       <c r="B140" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2">
-      <c r="A141" t="s">
-        <v>349</v>
-      </c>
-      <c r="B141" t="s">
-        <v>350</v>
+        <v>589</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>351</v>
+        <v>543</v>
       </c>
       <c r="B142" t="s">
-        <v>269</v>
+        <v>544</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" t="s">
+        <v>306</v>
+      </c>
+      <c r="B143" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B144" t="s">
-        <v>357</v>
+        <v>310</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>355</v>
+        <v>307</v>
       </c>
       <c r="B145" t="s">
-        <v>358</v>
+        <v>311</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>356</v>
+        <v>308</v>
       </c>
       <c r="B146" t="s">
-        <v>359</v>
+        <v>312</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>529</v>
+        <v>309</v>
       </c>
       <c r="B147" t="s">
-        <v>360</v>
+        <v>313</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>364</v>
+        <v>318</v>
       </c>
       <c r="B148" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>365</v>
+        <v>324</v>
       </c>
       <c r="B149" t="s">
-        <v>361</v>
+        <v>325</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>366</v>
+        <v>321</v>
       </c>
       <c r="B150" t="s">
-        <v>362</v>
+        <v>323</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>367</v>
+        <v>322</v>
       </c>
       <c r="B151" t="s">
-        <v>363</v>
+        <v>323</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>368</v>
+        <v>326</v>
       </c>
       <c r="B152" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="154" spans="1:2">
-      <c r="A154" t="s">
-        <v>385</v>
-      </c>
-      <c r="B154" t="s">
-        <v>371</v>
+        <v>327</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2">
+      <c r="A153" t="s">
+        <v>566</v>
+      </c>
+      <c r="B153" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>386</v>
+        <v>545</v>
       </c>
       <c r="B155" t="s">
-        <v>372</v>
+        <v>546</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>387</v>
+        <v>525</v>
       </c>
       <c r="B156" t="s">
-        <v>373</v>
+        <v>335</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>388</v>
+        <v>532</v>
       </c>
       <c r="B157" t="s">
-        <v>374</v>
+        <v>335</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>389</v>
+        <v>330</v>
       </c>
       <c r="B158" t="s">
-        <v>375</v>
+        <v>336</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>390</v>
+        <v>331</v>
       </c>
       <c r="B159" t="s">
-        <v>376</v>
+        <v>337</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>391</v>
+        <v>332</v>
       </c>
       <c r="B160" t="s">
-        <v>377</v>
+        <v>338</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>392</v>
+        <v>333</v>
       </c>
       <c r="B161" t="s">
-        <v>378</v>
+        <v>339</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>393</v>
+        <v>334</v>
       </c>
       <c r="B162" t="s">
-        <v>379</v>
+        <v>260</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>394</v>
+        <v>340</v>
       </c>
       <c r="B163" t="s">
-        <v>380</v>
+        <v>341</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>395</v>
+        <v>342</v>
       </c>
       <c r="B164" t="s">
-        <v>381</v>
+        <v>343</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>396</v>
+        <v>345</v>
       </c>
       <c r="B165" t="s">
-        <v>382</v>
+        <v>344</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>397</v>
+        <v>346</v>
       </c>
       <c r="B166" t="s">
-        <v>383</v>
+        <v>347</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>398</v>
+        <v>348</v>
       </c>
       <c r="B167" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2">
-      <c r="A169" t="s">
-        <v>405</v>
-      </c>
-      <c r="B169" t="s">
-        <v>423</v>
+        <v>268</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2">
+      <c r="A168" t="s">
+        <v>565</v>
+      </c>
+      <c r="B168" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>406</v>
+        <v>547</v>
       </c>
       <c r="B170" t="s">
-        <v>420</v>
+        <v>548</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>407</v>
+        <v>527</v>
       </c>
       <c r="B171" t="s">
-        <v>421</v>
+        <v>354</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>424</v>
+        <v>533</v>
       </c>
       <c r="B172" t="s">
-        <v>422</v>
+        <v>354</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" t="s">
-        <v>408</v>
+        <v>352</v>
       </c>
       <c r="B173" t="s">
-        <v>414</v>
+        <v>355</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" t="s">
-        <v>425</v>
+        <v>353</v>
       </c>
       <c r="B174" t="s">
-        <v>415</v>
+        <v>356</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" t="s">
-        <v>409</v>
+        <v>526</v>
       </c>
       <c r="B175" t="s">
-        <v>416</v>
+        <v>357</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" t="s">
-        <v>411</v>
+        <v>361</v>
       </c>
       <c r="B176" t="s">
-        <v>417</v>
+        <v>260</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" t="s">
-        <v>410</v>
+        <v>362</v>
       </c>
       <c r="B177" t="s">
-        <v>418</v>
+        <v>358</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" t="s">
-        <v>412</v>
+        <v>363</v>
       </c>
       <c r="B178" t="s">
-        <v>419</v>
+        <v>359</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" t="s">
-        <v>413</v>
+        <v>364</v>
       </c>
       <c r="B179" t="s">
-        <v>416</v>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2">
+      <c r="A180" t="s">
+        <v>365</v>
+      </c>
+      <c r="B180" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181" t="s">
-        <v>431</v>
+        <v>564</v>
       </c>
       <c r="B181" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="182" spans="1:2">
-      <c r="A182" t="s">
-        <v>432</v>
-      </c>
-      <c r="B182" t="s">
-        <v>443</v>
+        <v>592</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" t="s">
-        <v>433</v>
+        <v>597</v>
       </c>
       <c r="B183" t="s">
-        <v>444</v>
+        <v>600</v>
       </c>
     </row>
     <row r="184" spans="1:2">
       <c r="A184" t="s">
-        <v>434</v>
+        <v>598</v>
       </c>
       <c r="B184" t="s">
-        <v>445</v>
+        <v>599</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" t="s">
-        <v>435</v>
+        <v>382</v>
       </c>
       <c r="B185" t="s">
-        <v>446</v>
+        <v>368</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" t="s">
-        <v>436</v>
+        <v>383</v>
       </c>
       <c r="B186" t="s">
-        <v>447</v>
+        <v>369</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" t="s">
-        <v>437</v>
+        <v>534</v>
       </c>
       <c r="B187" t="s">
-        <v>448</v>
+        <v>369</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" t="s">
-        <v>438</v>
+        <v>384</v>
       </c>
       <c r="B188" t="s">
-        <v>449</v>
+        <v>370</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" t="s">
-        <v>439</v>
+        <v>385</v>
       </c>
       <c r="B189" t="s">
-        <v>450</v>
+        <v>371</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" t="s">
-        <v>440</v>
+        <v>386</v>
       </c>
       <c r="B190" t="s">
-        <v>451</v>
+        <v>372</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" t="s">
-        <v>441</v>
+        <v>387</v>
       </c>
       <c r="B191" t="s">
-        <v>452</v>
+        <v>373</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2">
+      <c r="A192" t="s">
+        <v>388</v>
+      </c>
+      <c r="B192" t="s">
+        <v>374</v>
       </c>
     </row>
     <row r="193" spans="1:2">
       <c r="A193" t="s">
-        <v>465</v>
+        <v>389</v>
       </c>
       <c r="B193" t="s">
-        <v>476</v>
+        <v>375</v>
       </c>
     </row>
     <row r="194" spans="1:2">
       <c r="A194" t="s">
-        <v>466</v>
+        <v>390</v>
       </c>
       <c r="B194" t="s">
-        <v>477</v>
+        <v>376</v>
       </c>
     </row>
     <row r="195" spans="1:2">
       <c r="A195" t="s">
-        <v>467</v>
+        <v>391</v>
       </c>
       <c r="B195" t="s">
-        <v>478</v>
+        <v>377</v>
       </c>
     </row>
     <row r="196" spans="1:2">
       <c r="A196" t="s">
-        <v>468</v>
+        <v>392</v>
       </c>
       <c r="B196" t="s">
-        <v>479</v>
+        <v>378</v>
       </c>
     </row>
     <row r="197" spans="1:2">
       <c r="A197" t="s">
-        <v>469</v>
+        <v>393</v>
       </c>
       <c r="B197" t="s">
-        <v>480</v>
+        <v>379</v>
       </c>
     </row>
     <row r="198" spans="1:2">
       <c r="A198" t="s">
-        <v>470</v>
+        <v>394</v>
       </c>
       <c r="B198" t="s">
-        <v>447</v>
+        <v>380</v>
       </c>
     </row>
     <row r="199" spans="1:2">
       <c r="A199" t="s">
-        <v>471</v>
+        <v>395</v>
       </c>
       <c r="B199" t="s">
-        <v>448</v>
+        <v>381</v>
       </c>
     </row>
     <row r="200" spans="1:2">
       <c r="A200" t="s">
-        <v>472</v>
+        <v>563</v>
       </c>
       <c r="B200" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="201" spans="1:2">
-      <c r="A201" t="s">
-        <v>473</v>
-      </c>
-      <c r="B201" t="s">
-        <v>482</v>
+        <v>593</v>
       </c>
     </row>
     <row r="202" spans="1:2">
       <c r="A202" t="s">
-        <v>474</v>
+        <v>402</v>
       </c>
       <c r="B202" t="s">
-        <v>451</v>
+        <v>420</v>
       </c>
     </row>
     <row r="203" spans="1:2">
       <c r="A203" t="s">
-        <v>475</v>
+        <v>403</v>
       </c>
       <c r="B203" t="s">
-        <v>452</v>
+        <v>417</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2">
+      <c r="A204" t="s">
+        <v>404</v>
+      </c>
+      <c r="B204" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="205" spans="1:2">
       <c r="A205" t="s">
-        <v>453</v>
+        <v>535</v>
       </c>
       <c r="B205" t="s">
-        <v>458</v>
+        <v>418</v>
       </c>
     </row>
     <row r="206" spans="1:2">
       <c r="A206" t="s">
-        <v>454</v>
+        <v>421</v>
       </c>
       <c r="B206" t="s">
-        <v>459</v>
+        <v>419</v>
       </c>
     </row>
     <row r="207" spans="1:2">
       <c r="A207" t="s">
-        <v>455</v>
+        <v>405</v>
       </c>
       <c r="B207" t="s">
-        <v>460</v>
+        <v>411</v>
       </c>
     </row>
     <row r="208" spans="1:2">
       <c r="A208" t="s">
-        <v>456</v>
+        <v>422</v>
       </c>
       <c r="B208" t="s">
-        <v>461</v>
+        <v>412</v>
       </c>
     </row>
     <row r="209" spans="1:2">
       <c r="A209" t="s">
+        <v>406</v>
+      </c>
+      <c r="B209" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2">
+      <c r="A210" t="s">
+        <v>408</v>
+      </c>
+      <c r="B210" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2">
+      <c r="A211" t="s">
+        <v>407</v>
+      </c>
+      <c r="B211" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2">
+      <c r="A212" t="s">
+        <v>409</v>
+      </c>
+      <c r="B212" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2">
+      <c r="A213" t="s">
+        <v>410</v>
+      </c>
+      <c r="B213" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2">
+      <c r="A214" t="s">
+        <v>562</v>
+      </c>
+      <c r="B214" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2">
+      <c r="A216" t="s">
+        <v>549</v>
+      </c>
+      <c r="B216" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2">
+      <c r="A217" t="s">
+        <v>428</v>
+      </c>
+      <c r="B217" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2">
+      <c r="A218" t="s">
+        <v>429</v>
+      </c>
+      <c r="B218" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2">
+      <c r="A219" t="s">
+        <v>430</v>
+      </c>
+      <c r="B219" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2">
+      <c r="A220" t="s">
+        <v>431</v>
+      </c>
+      <c r="B220" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2">
+      <c r="A221" t="s">
+        <v>432</v>
+      </c>
+      <c r="B221" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2">
+      <c r="A222" t="s">
+        <v>433</v>
+      </c>
+      <c r="B222" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2">
+      <c r="A223" t="s">
+        <v>434</v>
+      </c>
+      <c r="B223" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2">
+      <c r="A224" t="s">
+        <v>435</v>
+      </c>
+      <c r="B224" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2">
+      <c r="A225" t="s">
+        <v>436</v>
+      </c>
+      <c r="B225" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2">
+      <c r="A226" t="s">
+        <v>437</v>
+      </c>
+      <c r="B226" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2">
+      <c r="A227" t="s">
+        <v>438</v>
+      </c>
+      <c r="B227" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2">
+      <c r="A228" t="s">
+        <v>559</v>
+      </c>
+      <c r="B228" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2">
+      <c r="A230" t="s">
+        <v>551</v>
+      </c>
+      <c r="B230" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2">
+      <c r="A231" t="s">
+        <v>462</v>
+      </c>
+      <c r="B231" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2">
+      <c r="A232" t="s">
+        <v>463</v>
+      </c>
+      <c r="B232" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2">
+      <c r="A233" t="s">
+        <v>536</v>
+      </c>
+      <c r="B233" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2">
+      <c r="A234" t="s">
+        <v>464</v>
+      </c>
+      <c r="B234" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2">
+      <c r="A235" t="s">
+        <v>465</v>
+      </c>
+      <c r="B235" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2">
+      <c r="A236" t="s">
+        <v>466</v>
+      </c>
+      <c r="B236" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2">
+      <c r="A237" t="s">
+        <v>467</v>
+      </c>
+      <c r="B237" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2">
+      <c r="A238" t="s">
+        <v>468</v>
+      </c>
+      <c r="B238" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2">
+      <c r="A239" t="s">
+        <v>469</v>
+      </c>
+      <c r="B239" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2">
+      <c r="A240" t="s">
+        <v>470</v>
+      </c>
+      <c r="B240" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2">
+      <c r="A241" t="s">
+        <v>471</v>
+      </c>
+      <c r="B241" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2">
+      <c r="A242" t="s">
+        <v>472</v>
+      </c>
+      <c r="B242" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2">
+      <c r="A243" t="s">
+        <v>557</v>
+      </c>
+      <c r="B243" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2">
+      <c r="A245" t="s">
+        <v>450</v>
+      </c>
+      <c r="B245" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2">
+      <c r="A246" t="s">
+        <v>451</v>
+      </c>
+      <c r="B246" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2">
+      <c r="A247" t="s">
+        <v>537</v>
+      </c>
+      <c r="B247" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2">
+      <c r="A248" t="s">
+        <v>452</v>
+      </c>
+      <c r="B248" t="s">
         <v>457</v>
       </c>
-      <c r="B209" t="s">
-        <v>462</v>
+    </row>
+    <row r="249" spans="1:2">
+      <c r="A249" t="s">
+        <v>453</v>
+      </c>
+      <c r="B249" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2">
+      <c r="A250" t="s">
+        <v>454</v>
+      </c>
+      <c r="B250" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2">
+      <c r="A251" t="s">
+        <v>556</v>
+      </c>
+      <c r="B251" t="s">
+        <v>558</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Sharepoint Upload authentication fix, AssetSources fix
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.malyala\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC42D777-221E-4629-875A-FFFA9B9D696C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF5888C2-6444-4995-A932-71103C0D22AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2970" yWindow="3255" windowWidth="21510" windowHeight="9825" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="637">
   <si>
     <t>Name</t>
   </si>
@@ -411,9 +411,6 @@
     <t>SCNE_HasSignature</t>
   </si>
   <si>
-    <t>Signautre is missing from the Self Certification of Non Employment.</t>
-  </si>
-  <si>
     <t>Date is missing from the Self Certification of Non Employment.</t>
   </si>
   <si>
@@ -438,9 +435,6 @@
     <t>Not every field in Part 4 have been answered on the Affidavit of Student Financial Assistance.</t>
   </si>
   <si>
-    <t>Signautre is missing from the Affidavit of Student Financial Assistance.</t>
-  </si>
-  <si>
     <t>Date is missing from the Affidavit of Student Financial Assistance.</t>
   </si>
   <si>
@@ -477,18 +471,6 @@
     <t>ASC_part_4_is_not_null</t>
   </si>
   <si>
-    <t>Part 1 of the Asset Self Certifiation has not been completed.</t>
-  </si>
-  <si>
-    <t>Part 2 of the Asset Self Certifiation has not been completed.</t>
-  </si>
-  <si>
-    <t>Part 3 of the Asset Self Certifiation has not been completed.</t>
-  </si>
-  <si>
-    <t>Part 4 of the Asset Self Certifiation has not been completed.</t>
-  </si>
-  <si>
     <t>ASC_TaxCreditMatch</t>
   </si>
   <si>
@@ -561,9 +543,6 @@
     <t>Signature is left blank on the Certification of Zero Income.</t>
   </si>
   <si>
-    <t>Date is left blank on the Certificatio of Zero Income.</t>
-  </si>
-  <si>
     <t>VAWA_HasSignature</t>
   </si>
   <si>
@@ -624,9 +603,6 @@
     <t>At least one household member is missing the required Member Information Document Form.</t>
   </si>
   <si>
-    <t>Income &amp; Assest Questionnaire is missing from the application.</t>
-  </si>
-  <si>
     <t>ASCExists</t>
   </si>
   <si>
@@ -1761,9 +1737,6 @@
     <t>Errors in Validating findings for Member Information Document</t>
   </si>
   <si>
-    <t>Errors in Validating findings for Income &amp; Assest Questionnaire</t>
-  </si>
-  <si>
     <t>Errors in Validating findings for Self Certification of Non Employment.</t>
   </si>
   <si>
@@ -1776,9 +1749,6 @@
     <t>Errors in Validating findings for Student Certification</t>
   </si>
   <si>
-    <t>Errors in Validating findings for Certificatio of Zero Income.</t>
-  </si>
-  <si>
     <t>Errors in Validating findings for VAWA Acknowledgement</t>
   </si>
   <si>
@@ -1902,12 +1872,6 @@
     <t>IAQ_IncomeTypeListed</t>
   </si>
   <si>
-    <t>Income Types listed on Income &amp; Assest Questionnaire does not match the ICW</t>
-  </si>
-  <si>
-    <t>Income Sources listed on Income &amp; Assest Questionnaire does not match the ICW</t>
-  </si>
-  <si>
     <t>At least one field on the Affidavit of Student Financial Assistance has been marked yes. This requires manual review.</t>
   </si>
   <si>
@@ -1923,9 +1887,6 @@
     <t>Sharepoint_LLMSubfolder</t>
   </si>
   <si>
-    <t>Supporting documents do not exist for Self-Empoyment Verification</t>
-  </si>
-  <si>
     <t>SEC_SupportingDocumentsExist</t>
   </si>
   <si>
@@ -1942,6 +1903,54 @@
   </si>
   <si>
     <t>Yearly Amount calculated from the Supplemental Security Income Letter does not match the ICW.</t>
+  </si>
+  <si>
+    <t>Income &amp; Asset Questionnaire is missing from the application.</t>
+  </si>
+  <si>
+    <t>Income Sources listed on Income &amp; Asset Questionnaire does not match the ICW</t>
+  </si>
+  <si>
+    <t>Income Types listed on Income &amp; Asset Questionnaire does not match the ICW</t>
+  </si>
+  <si>
+    <t>Errors in Validating findings for Income &amp; Asset Questionnaire</t>
+  </si>
+  <si>
+    <t>Signature is missing from the Self Certification of Non Employment.</t>
+  </si>
+  <si>
+    <t>Part 1 of the Asset Self Certification has not been completed.</t>
+  </si>
+  <si>
+    <t>Part 2 of the Asset Self Certification has not been completed.</t>
+  </si>
+  <si>
+    <t>Part 3 of the Asset Self Certification has not been completed.</t>
+  </si>
+  <si>
+    <t>Part 4 of the Asset Self Certification has not been completed.</t>
+  </si>
+  <si>
+    <t>Signature is missing from the Affidavit of Student Financial Assistance.</t>
+  </si>
+  <si>
+    <t>Date is left blank on the Certification of Zero Income.</t>
+  </si>
+  <si>
+    <t>Errors in Validating findings for Certification of Zero Income.</t>
+  </si>
+  <si>
+    <t>Supporting documents do not exist for Self-Employment Verification</t>
+  </si>
+  <si>
+    <t>SharePoint_AppID</t>
+  </si>
+  <si>
+    <t>Sharepoint_TenantID</t>
+  </si>
+  <si>
+    <t>Sharepoint_SecretID</t>
   </si>
 </sst>
 </file>
@@ -2319,7 +2328,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -2400,202 +2409,202 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B7" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="B8" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B9" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="B10" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B12" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="B13" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="B14" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="B15" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="B16" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="C16" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
+        <v>223</v>
+      </c>
+      <c r="B17" t="s">
         <v>231</v>
       </c>
-      <c r="B17" t="s">
-        <v>239</v>
-      </c>
       <c r="C17" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="B18" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C18" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="B19" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="C19" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="B20" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="B21" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="B22" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="B23" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="B24" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="B25" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="B26" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="C26" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="B27" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="B28" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="B29" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="B30" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
@@ -2608,74 +2617,74 @@
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="B32" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="B33" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="B34" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="B35" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="B36" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="B37" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="B38" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="B39" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="B40" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3662,242 +3671,242 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="B1" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="B2" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
       <c r="B3" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="B4" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="B5" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="B6" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="B7" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="B8" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="B9" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="B10" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="B11" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="B12" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="B13" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="B14" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="B15" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="B16" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="B17" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="B18" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B19" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="B20" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="B21" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="B22" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="B23" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="B24" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="B25" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="B26" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="B27" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="B28" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="B29" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="B30" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -3905,79 +3914,79 @@
         <v>1040</v>
       </c>
       <c r="B31" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="B32" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="B33" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="B34" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="B35" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="B36" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="B37" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
       <c r="B38" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="B39" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
       <c r="B40" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
     </row>
   </sheetData>
@@ -3987,10 +3996,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z993"/>
+  <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4185,76 +4194,83 @@
         <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+        <v>511</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" t="s">
+        <v>636</v>
+      </c>
+      <c r="B21" t="s">
+        <v>636</v>
+      </c>
+    </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A23" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" t="s">
-        <v>49</v>
-      </c>
-    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B26" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B28" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B29" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
         <v>69</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
@@ -5217,6 +5233,7 @@
     <row r="991" ht="14.25" customHeight="1"/>
     <row r="992" ht="14.25" customHeight="1"/>
     <row r="993" ht="14.25" customHeight="1"/>
+    <row r="994" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5227,8 +5244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5349,42 +5366,42 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>605</v>
+        <v>595</v>
       </c>
       <c r="B12" t="s">
-        <v>605</v>
+        <v>595</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>606</v>
+        <v>596</v>
       </c>
       <c r="B13" t="s">
-        <v>606</v>
+        <v>596</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>607</v>
+        <v>597</v>
       </c>
       <c r="B14" t="s">
-        <v>607</v>
+        <v>597</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
       <c r="B15" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
@@ -5397,102 +5414,116 @@
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="B17" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="B18" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="B21" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="B22" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="B23" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="B24" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>623</v>
+        <v>611</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>623</v>
+        <v>611</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>625</v>
+        <v>613</v>
       </c>
       <c r="B26" t="s">
-        <v>625</v>
+        <v>613</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>624</v>
+        <v>612</v>
       </c>
       <c r="B27" t="s">
-        <v>624</v>
+        <v>612</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>626</v>
+        <v>614</v>
       </c>
       <c r="B28" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
+        <v>614</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>634</v>
+      </c>
+      <c r="B29" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A30" t="s">
+        <v>635</v>
+      </c>
+      <c r="B30" t="s">
+        <v>635</v>
+      </c>
+    </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" customFormat="1" ht="14.25" customHeight="1"/>
@@ -6479,8 +6510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
   <dimension ref="A1:C254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A231" workbookViewId="0">
-      <selection activeCell="B239" sqref="B239"/>
+    <sheetView topLeftCell="A171" workbookViewId="0">
+      <selection activeCell="B192" sqref="B192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6500,18 +6531,18 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="B5" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6524,10 +6555,10 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B7" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -6540,34 +6571,34 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="B9" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>586</v>
+        <v>576</v>
       </c>
       <c r="B10" t="s">
-        <v>587</v>
+        <v>577</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
       <c r="B11" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B13" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -6580,10 +6611,10 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>597</v>
+        <v>587</v>
       </c>
       <c r="B15" t="s">
-        <v>598</v>
+        <v>588</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -6604,18 +6635,18 @@
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B18" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="B19" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -6652,18 +6683,18 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="B24" t="s">
-        <v>571</v>
+        <v>563</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B26" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -6732,18 +6763,18 @@
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="B35" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="B37" t="s">
-        <v>194</v>
+        <v>621</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -6804,55 +6835,55 @@
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B45" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="B46" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>619</v>
+        <v>609</v>
       </c>
       <c r="B47" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
       <c r="B48" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>592</v>
+        <v>582</v>
       </c>
       <c r="B49" t="s">
-        <v>593</v>
+        <v>583</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
       <c r="B50" t="s">
-        <v>573</v>
+        <v>624</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="B52" t="s">
         <v>121</v>
@@ -6863,1517 +6894,1517 @@
         <v>122</v>
       </c>
       <c r="B53" t="s">
-        <v>123</v>
+        <v>625</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B54" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
       <c r="B55" t="s">
-        <v>574</v>
+        <v>565</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B57" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B58" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B59" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B60" t="s">
-        <v>145</v>
+        <v>626</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B61" t="s">
-        <v>146</v>
+        <v>627</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B62" t="s">
-        <v>147</v>
+        <v>628</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B63" t="s">
-        <v>148</v>
+        <v>629</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B64" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B65" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="C65" t="s">
-        <v>594</v>
+        <v>584</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B66" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
       <c r="B67" t="s">
-        <v>575</v>
+        <v>566</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B69" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="B70" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="B71" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B72" t="s">
-        <v>622</v>
+        <v>610</v>
       </c>
       <c r="C72" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B73" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B74" t="s">
-        <v>132</v>
+        <v>630</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B75" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
       <c r="B76" t="s">
-        <v>576</v>
+        <v>567</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B78" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B79" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B80" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B81" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B82" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B83" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
       <c r="B84" t="s">
-        <v>577</v>
+        <v>568</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="B86" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B87" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B88" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="B89" t="s">
-        <v>173</v>
+        <v>631</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>595</v>
+        <v>585</v>
       </c>
       <c r="B90" t="s">
-        <v>596</v>
+        <v>586</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
       <c r="B91" t="s">
-        <v>578</v>
+        <v>632</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B93" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="B94" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B95" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="B96" t="s">
-        <v>579</v>
+        <v>569</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B98" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B99" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C99" t="s">
-        <v>631</v>
+        <v>618</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="B100" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="C100" t="s">
-        <v>631</v>
+        <v>618</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="B101" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C101" t="s">
-        <v>631</v>
+        <v>618</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="B102" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="B103" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="B104" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="C104" t="s">
-        <v>631</v>
+        <v>618</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
       <c r="B105" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="B107" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="B108" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="B109" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="B110" t="s">
-        <v>599</v>
+        <v>589</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="B111" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="B112" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="B113" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="B114" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="B115" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="B116" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="B117" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B118" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="B119" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
       <c r="B120" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
     </row>
     <row r="122" spans="1:2">
       <c r="A122" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
       <c r="B122" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="B123" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="13.5" customHeight="1">
       <c r="A124" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="B124" t="s">
-        <v>600</v>
+        <v>590</v>
       </c>
     </row>
     <row r="125" spans="1:2">
       <c r="A125" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="B125" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="B126" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="B127" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="B128" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="B129" t="s">
-        <v>609</v>
+        <v>599</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="B130" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="B131" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="B132" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="B133" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="B134" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="B135" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="B136" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="B137" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="B138" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="B139" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="B140" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>558</v>
+        <v>550</v>
       </c>
       <c r="B141" t="s">
-        <v>580</v>
+        <v>570</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="B143" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="B144" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="B145" t="s">
-        <v>610</v>
+        <v>600</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="B146" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B147" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="B148" t="s">
-        <v>601</v>
+        <v>591</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="B149" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="B150" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="B151" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="B152" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="B153" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>557</v>
+        <v>549</v>
       </c>
       <c r="B154" t="s">
-        <v>581</v>
+        <v>571</v>
       </c>
     </row>
     <row r="156" spans="1:2">
       <c r="A156" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="B156" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="B157" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="B158" t="s">
-        <v>611</v>
+        <v>601</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="B159" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="B160" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="B161" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="B162" t="s">
-        <v>602</v>
+        <v>592</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="B163" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="B164" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="B165" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="B166" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="B167" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="B168" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
       <c r="B169" t="s">
-        <v>582</v>
+        <v>572</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="B171" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="B172" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="B173" t="s">
-        <v>612</v>
+        <v>602</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="B174" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="B175" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="B176" t="s">
-        <v>603</v>
+        <v>593</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="B177" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="B178" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="B179" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="B180" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="B181" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
       <c r="B182" t="s">
-        <v>583</v>
+        <v>573</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" t="s">
-        <v>588</v>
+        <v>578</v>
       </c>
       <c r="B184" t="s">
-        <v>591</v>
+        <v>581</v>
       </c>
       <c r="C184" t="s">
-        <v>629</v>
+        <v>616</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="s">
-        <v>589</v>
+        <v>579</v>
       </c>
       <c r="B185" t="s">
-        <v>590</v>
+        <v>580</v>
       </c>
       <c r="C185" t="s">
-        <v>630</v>
+        <v>617</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="s">
-        <v>628</v>
+        <v>615</v>
       </c>
       <c r="B186" t="s">
-        <v>627</v>
+        <v>633</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="B187" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="B188" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="B189" t="s">
-        <v>613</v>
+        <v>603</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="B190" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="B191" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="B192" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="B193" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="C193" t="s">
-        <v>631</v>
+        <v>618</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="B194" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="B195" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="B196" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="B197" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="B198" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="B199" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="B200" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="B201" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
       <c r="B202" t="s">
-        <v>584</v>
+        <v>574</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="B204" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="B205" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="B206" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="B207" t="s">
-        <v>614</v>
+        <v>604</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="B208" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="B209" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="B210" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="C210" t="s">
-        <v>604</v>
+        <v>594</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="B211" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="B212" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" t="s">
+        <v>392</v>
+      </c>
+      <c r="B213" t="s">
         <v>400</v>
-      </c>
-      <c r="B213" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="B214" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="B215" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
       <c r="B216" t="s">
-        <v>585</v>
+        <v>575</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
       <c r="B218" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="B219" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="B220" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" t="s">
-        <v>615</v>
+        <v>605</v>
       </c>
       <c r="B221" t="s">
-        <v>616</v>
+        <v>606</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="B222" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
     </row>
     <row r="223" spans="1:3">
       <c r="A223" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="B223" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="B224" t="s">
-        <v>632</v>
+        <v>619</v>
       </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="B225" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
     </row>
     <row r="226" spans="1:2">
       <c r="A226" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="B226" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
     </row>
     <row r="227" spans="1:2">
       <c r="A227" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="B227" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
     </row>
     <row r="228" spans="1:2">
       <c r="A228" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="B228" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
     </row>
     <row r="229" spans="1:2">
       <c r="A229" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="B229" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
     </row>
     <row r="230" spans="1:2">
       <c r="A230" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="B230" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
     </row>
     <row r="231" spans="1:2">
       <c r="A231" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
       <c r="B231" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
     </row>
     <row r="233" spans="1:2">
       <c r="A233" t="s">
-        <v>542</v>
+        <v>534</v>
       </c>
       <c r="B233" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
     </row>
     <row r="234" spans="1:2">
       <c r="A234" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
       <c r="B234" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
     </row>
     <row r="235" spans="1:2">
       <c r="A235" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
       <c r="B235" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
     </row>
     <row r="236" spans="1:2">
       <c r="A236" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="B236" t="s">
-        <v>618</v>
+        <v>608</v>
       </c>
     </row>
     <row r="237" spans="1:2">
       <c r="A237" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="B237" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
     </row>
     <row r="238" spans="1:2">
       <c r="A238" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
       <c r="B238" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
     </row>
     <row r="239" spans="1:2">
       <c r="A239" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="B239" t="s">
-        <v>633</v>
+        <v>620</v>
       </c>
     </row>
     <row r="240" spans="1:2">
       <c r="A240" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
       <c r="B240" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
     </row>
     <row r="241" spans="1:2">
       <c r="A241" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="B241" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
     </row>
     <row r="242" spans="1:2">
       <c r="A242" t="s">
+        <v>453</v>
+      </c>
+      <c r="B242" t="s">
         <v>461</v>
-      </c>
-      <c r="B242" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="243" spans="1:2">
       <c r="A243" t="s">
+        <v>454</v>
+      </c>
+      <c r="B243" t="s">
         <v>462</v>
-      </c>
-      <c r="B243" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="244" spans="1:2">
       <c r="A244" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="B244" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
     </row>
     <row r="245" spans="1:2">
       <c r="A245" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="B245" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
     </row>
     <row r="246" spans="1:2">
       <c r="A246" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="B246" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
     </row>
     <row r="248" spans="1:2">
       <c r="A248" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="B248" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
     </row>
     <row r="249" spans="1:2">
       <c r="A249" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="B249" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
     </row>
     <row r="250" spans="1:2">
       <c r="A250" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="B250" t="s">
-        <v>617</v>
+        <v>607</v>
       </c>
     </row>
     <row r="251" spans="1:2">
       <c r="A251" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="B251" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
     </row>
     <row r="252" spans="1:2">
       <c r="A252" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="B252" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
     </row>
     <row r="253" spans="1:2">
       <c r="A253" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="B253" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
     </row>
     <row r="254" spans="1:2">
       <c r="A254" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
       <c r="B254" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest version of code as of 12-11-25
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.malyala\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A34E93E-1990-42A1-AAFE-02D81E038CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1189A6EE-C5D3-412F-99E5-5B955288D299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="2265" windowWidth="21510" windowHeight="9825" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="656">
   <si>
     <t>Name</t>
   </si>
@@ -1356,27 +1356,9 @@
     <t>VRCC_DateSignedCheck</t>
   </si>
   <si>
-    <t xml:space="preserve">Name listed on the Verification of Reoccurring Cash Contribution and ICW do not match. </t>
-  </si>
-  <si>
-    <t>Date listed on the Verification of Reoccurring Cash Contribution is over 120 days in the past.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amount listed on the Verification of Reoccurring Cash Contribution and ICW do not match. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verification of Reoccurring Cash Contribution has not been signed. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verification of Reoccurring Cash Contribution has not been dated appropriately. </t>
-  </si>
-  <si>
     <t>VRCC</t>
   </si>
   <si>
-    <t>Verification of Reoccurring Cash Contributions</t>
-  </si>
-  <si>
     <t>SSIB_EmployeeCheck</t>
   </si>
   <si>
@@ -1662,9 +1644,6 @@
     <t>SSIB_FindingError</t>
   </si>
   <si>
-    <t>Errors in Validating findings for Verification of Reoccurring Cash Contribution</t>
-  </si>
-  <si>
     <t>SSBL_FindingError</t>
   </si>
   <si>
@@ -1788,9 +1767,6 @@
     <t>IAQ_AssetsValueMatch</t>
   </si>
   <si>
-    <t>Assets value does not match that listed on the ICW.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Not using it anymore </t>
   </si>
   <si>
@@ -1860,9 +1836,6 @@
     <t>Date of the Social Security Benefits Letter is not with in 120 days of Move-In date.</t>
   </si>
   <si>
-    <t>Date listed on the Verification of Reoccurring Cash Contribution is not with in 120 days of Move-In date.</t>
-  </si>
-  <si>
     <t>Date of the Supplemental Security Income Letter is not with in 120 days of Move-In date.</t>
   </si>
   <si>
@@ -1978,6 +1951,63 @@
   </si>
   <si>
     <t>Income Asset Questionnaire</t>
+  </si>
+  <si>
+    <t>SSBL_OverPayment</t>
+  </si>
+  <si>
+    <t>Manual review required, overpayment detected on SS/SSI benefit letter.</t>
+  </si>
+  <si>
+    <t>Asset Self Certification</t>
+  </si>
+  <si>
+    <t>Self Certification of Non Employment</t>
+  </si>
+  <si>
+    <t>Screening</t>
+  </si>
+  <si>
+    <t>Self Employment Certification</t>
+  </si>
+  <si>
+    <t>Verification of Recurring Cash Contributions</t>
+  </si>
+  <si>
+    <t>SSIB_OverPayment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name listed on the Verification of Reccurring Cash Contribution and ICW do not match. </t>
+  </si>
+  <si>
+    <t>Date listed on the Verification of Reccurring Cash Contribution is over 120 days in the past.</t>
+  </si>
+  <si>
+    <t>Date listed on the Verification of Reccurring Cash Contribution is not with in 120 days of Move-In date.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount listed on the Verification of Reccurring Cash Contribution and ICW do not match. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verification of Reccurring Cash Contribution has not been signed. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verification of Reccurring Cash Contribution has not been dated appropriately. </t>
+  </si>
+  <si>
+    <t>Errors in Validating findings for Verification of Reccurring Cash Contribution</t>
+  </si>
+  <si>
+    <t>LLM_ImageQuality</t>
+  </si>
+  <si>
+    <t>SC_AllFullTimeStudents</t>
+  </si>
+  <si>
+    <t>All household members have been or will be students for the next five months. Manual review required.</t>
+  </si>
+  <si>
+    <t>Assets Type and  value does not match that listed on the ICW.</t>
   </si>
 </sst>
 </file>
@@ -2355,8 +2385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2439,7 +2469,7 @@
         <v>210</v>
       </c>
       <c r="B7" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -2472,7 +2502,7 @@
         <v>218</v>
       </c>
       <c r="B12" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
@@ -2488,7 +2518,7 @@
         <v>220</v>
       </c>
       <c r="B14" t="s">
-        <v>469</v>
+        <v>639</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
@@ -2496,7 +2526,7 @@
         <v>221</v>
       </c>
       <c r="B15" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
@@ -2504,7 +2534,7 @@
         <v>222</v>
       </c>
       <c r="B16" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="C16" t="s">
         <v>237</v>
@@ -2526,7 +2556,7 @@
         <v>224</v>
       </c>
       <c r="B18" t="s">
-        <v>645</v>
+        <v>636</v>
       </c>
       <c r="C18" t="s">
         <v>239</v>
@@ -2537,7 +2567,7 @@
         <v>225</v>
       </c>
       <c r="B19" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="C19" t="s">
         <v>240</v>
@@ -2548,7 +2578,7 @@
         <v>226</v>
       </c>
       <c r="B20" t="s">
-        <v>472</v>
+        <v>640</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
@@ -2556,7 +2586,7 @@
         <v>227</v>
       </c>
       <c r="B21" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
@@ -2564,7 +2594,7 @@
         <v>228</v>
       </c>
       <c r="B22" t="s">
-        <v>233</v>
+        <v>641</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
@@ -2572,12 +2602,12 @@
         <v>229</v>
       </c>
       <c r="B23" t="s">
-        <v>498</v>
+        <v>492</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="B24" t="s">
         <v>238</v>
@@ -2588,7 +2618,7 @@
         <v>242</v>
       </c>
       <c r="B25" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
@@ -2631,7 +2661,7 @@
         <v>380</v>
       </c>
       <c r="B30" t="s">
-        <v>381</v>
+        <v>642</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
@@ -2655,7 +2685,7 @@
         <v>384</v>
       </c>
       <c r="B33" t="s">
-        <v>475</v>
+        <v>469</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
@@ -2663,7 +2693,7 @@
         <v>411</v>
       </c>
       <c r="B34" t="s">
-        <v>639</v>
+        <v>630</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
@@ -2676,18 +2706,18 @@
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="B36" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="B37" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1">
@@ -2700,18 +2730,18 @@
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="B39" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="B40" t="s">
-        <v>444</v>
+        <v>643</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3687,7 +3717,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80DB68E2-2057-45AB-A45E-3EB9CF844C19}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -3698,10 +3728,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="B1" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -3709,15 +3739,15 @@
         <v>235</v>
       </c>
       <c r="B2" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="B3" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3725,15 +3755,15 @@
         <v>236</v>
       </c>
       <c r="B4" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="B5" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -3741,15 +3771,15 @@
         <v>234</v>
       </c>
       <c r="B6" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="B7" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -3757,15 +3787,15 @@
         <v>230</v>
       </c>
       <c r="B8" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="B9" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -3773,15 +3803,15 @@
         <v>233</v>
       </c>
       <c r="B10" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="B11" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -3797,47 +3827,47 @@
         <v>231</v>
       </c>
       <c r="B13" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="B14" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>473</v>
+        <v>467</v>
       </c>
       <c r="B15" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>488</v>
+        <v>482</v>
       </c>
       <c r="B16" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>490</v>
+        <v>484</v>
       </c>
       <c r="B17" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="B18" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -3845,7 +3875,7 @@
         <v>240</v>
       </c>
       <c r="B19" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -3853,23 +3883,23 @@
         <v>237</v>
       </c>
       <c r="B20" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>492</v>
+        <v>486</v>
       </c>
       <c r="B21" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>493</v>
+        <v>487</v>
       </c>
       <c r="B22" t="s">
-        <v>494</v>
+        <v>488</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -3877,7 +3907,7 @@
         <v>238</v>
       </c>
       <c r="B23" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -3885,23 +3915,23 @@
         <v>239</v>
       </c>
       <c r="B24" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
       <c r="B25" t="s">
-        <v>489</v>
+        <v>483</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>474</v>
+        <v>468</v>
       </c>
       <c r="B26" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -3909,7 +3939,7 @@
         <v>292</v>
       </c>
       <c r="B27" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -3917,7 +3947,7 @@
         <v>315</v>
       </c>
       <c r="B28" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -3925,7 +3955,7 @@
         <v>336</v>
       </c>
       <c r="B29" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -3933,7 +3963,7 @@
         <v>381</v>
       </c>
       <c r="B30" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -3941,7 +3971,7 @@
         <v>1040</v>
       </c>
       <c r="B31" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -3949,7 +3979,7 @@
         <v>383</v>
       </c>
       <c r="B32" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -3957,15 +3987,15 @@
         <v>385</v>
       </c>
       <c r="B33" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="B34" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -3973,7 +4003,7 @@
         <v>410</v>
       </c>
       <c r="B35" t="s">
-        <v>495</v>
+        <v>489</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -3981,39 +4011,39 @@
         <v>408</v>
       </c>
       <c r="B36" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="B37" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
       <c r="B38" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>496</v>
+        <v>490</v>
       </c>
       <c r="B39" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>497</v>
+        <v>491</v>
       </c>
       <c r="B40" t="s">
-        <v>487</v>
+        <v>481</v>
       </c>
     </row>
   </sheetData>
@@ -4221,15 +4251,15 @@
         <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>635</v>
+        <v>626</v>
       </c>
       <c r="B21" t="s">
-        <v>635</v>
+        <v>626</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
@@ -5269,10 +5299,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1010"/>
+  <dimension ref="A1:Z1011"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5401,197 +5431,204 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="B12" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
       <c r="B13" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="B14" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
       <c r="B15" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>640</v>
+        <v>631</v>
       </c>
       <c r="B16" t="s">
-        <v>640</v>
+        <v>631</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>642</v>
+        <v>633</v>
       </c>
       <c r="B17" t="s">
-        <v>642</v>
+        <v>633</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>644</v>
+        <v>635</v>
       </c>
       <c r="B18" t="s">
-        <v>644</v>
+        <v>635</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>641</v>
+        <v>632</v>
       </c>
       <c r="B19" t="s">
-        <v>641</v>
+        <v>632</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>643</v>
+        <v>634</v>
       </c>
       <c r="B20" t="s">
-        <v>643</v>
+        <v>634</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>652</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>652</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1">
       <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
         <v>209</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>209</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A23" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="B23" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>241</v>
+        <v>215</v>
+      </c>
+      <c r="B24" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1">
       <c r="A25" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A26" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>276</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A26" t="s">
-        <v>277</v>
-      </c>
-      <c r="B26" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>334</v>
+        <v>277</v>
       </c>
       <c r="B27" t="s">
-        <v>334</v>
+        <v>277</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>500</v>
+        <v>334</v>
       </c>
       <c r="B28" t="s">
-        <v>500</v>
+        <v>334</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
       <c r="B29" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A30" s="2" t="s">
-        <v>610</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>610</v>
+      <c r="A30" t="s">
+        <v>495</v>
+      </c>
+      <c r="B30" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A31" t="s">
-        <v>612</v>
-      </c>
-      <c r="B31" t="s">
-        <v>612</v>
+      <c r="A31" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A32" s="2" t="s">
-        <v>611</v>
+      <c r="A32" t="s">
+        <v>603</v>
       </c>
       <c r="B32" t="s">
-        <v>611</v>
+        <v>603</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
-      <c r="A33" t="s">
-        <v>613</v>
+      <c r="A33" s="2" t="s">
+        <v>602</v>
       </c>
       <c r="B33" t="s">
-        <v>613</v>
+        <v>602</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>633</v>
+        <v>604</v>
       </c>
       <c r="B34" t="s">
-        <v>633</v>
+        <v>604</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>634</v>
+        <v>624</v>
       </c>
       <c r="B35" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
+        <v>624</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A36" t="s">
+        <v>625</v>
+      </c>
+      <c r="B36" t="s">
+        <v>625</v>
+      </c>
+    </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
@@ -6566,6 +6603,7 @@
     <row r="1008" ht="14.25" customHeight="1"/>
     <row r="1009" ht="14.25" customHeight="1"/>
     <row r="1010" ht="14.25" customHeight="1"/>
+    <row r="1011" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6574,10 +6612,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
-  <dimension ref="A1:C255"/>
+  <dimension ref="A1:C258"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6608,7 +6646,7 @@
         <v>181</v>
       </c>
       <c r="B5" t="s">
-        <v>504</v>
+        <v>498</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6645,18 +6683,18 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
       <c r="B10" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="B11" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -6677,10 +6715,10 @@
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
       <c r="B15" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -6749,10 +6787,10 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>558</v>
+        <v>551</v>
       </c>
       <c r="B24" t="s">
-        <v>562</v>
+        <v>555</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -6819,7 +6857,7 @@
         <v>99</v>
       </c>
       <c r="C33" t="s">
-        <v>617</v>
+        <v>608</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -6832,10 +6870,10 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="B35" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -6843,7 +6881,7 @@
         <v>185</v>
       </c>
       <c r="B37" t="s">
-        <v>620</v>
+        <v>611</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -6907,7 +6945,7 @@
         <v>205</v>
       </c>
       <c r="B45" t="s">
-        <v>502</v>
+        <v>496</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -6915,42 +6953,42 @@
         <v>206</v>
       </c>
       <c r="B46" t="s">
-        <v>621</v>
+        <v>612</v>
       </c>
       <c r="C46" t="s">
-        <v>617</v>
+        <v>608</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>608</v>
+        <v>599</v>
       </c>
       <c r="B47" t="s">
-        <v>622</v>
+        <v>613</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>559</v>
+        <v>552</v>
       </c>
       <c r="B48" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>581</v>
+        <v>574</v>
       </c>
       <c r="B49" t="s">
-        <v>582</v>
+        <v>655</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
       <c r="B50" t="s">
-        <v>623</v>
+        <v>614</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -6966,7 +7004,7 @@
         <v>122</v>
       </c>
       <c r="B53" t="s">
-        <v>624</v>
+        <v>615</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -6979,10 +7017,10 @@
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="B55" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -7014,7 +7052,7 @@
         <v>139</v>
       </c>
       <c r="B60" t="s">
-        <v>625</v>
+        <v>616</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -7022,7 +7060,7 @@
         <v>140</v>
       </c>
       <c r="B61" t="s">
-        <v>626</v>
+        <v>617</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -7030,7 +7068,7 @@
         <v>141</v>
       </c>
       <c r="B62" t="s">
-        <v>627</v>
+        <v>618</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -7038,7 +7076,7 @@
         <v>142</v>
       </c>
       <c r="B63" t="s">
-        <v>628</v>
+        <v>619</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -7046,7 +7084,7 @@
         <v>143</v>
       </c>
       <c r="B64" t="s">
-        <v>503</v>
+        <v>497</v>
       </c>
     </row>
     <row r="65" spans="1:3">
@@ -7054,10 +7092,10 @@
         <v>144</v>
       </c>
       <c r="B65" t="s">
-        <v>505</v>
+        <v>499</v>
       </c>
       <c r="C65" t="s">
-        <v>583</v>
+        <v>575</v>
       </c>
     </row>
     <row r="66" spans="1:3">
@@ -7065,15 +7103,15 @@
         <v>145</v>
       </c>
       <c r="B66" t="s">
-        <v>506</v>
+        <v>500</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
       <c r="B67" t="s">
-        <v>565</v>
+        <v>558</v>
       </c>
     </row>
     <row r="69" spans="1:3">
@@ -7105,7 +7143,7 @@
         <v>146</v>
       </c>
       <c r="B72" t="s">
-        <v>609</v>
+        <v>600</v>
       </c>
       <c r="C72" t="s">
         <v>129</v>
@@ -7124,7 +7162,7 @@
         <v>132</v>
       </c>
       <c r="B74" t="s">
-        <v>629</v>
+        <v>620</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -7137,10 +7175,10 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="B76" t="s">
-        <v>566</v>
+        <v>559</v>
       </c>
     </row>
     <row r="78" spans="1:3">
@@ -7193,515 +7231,515 @@
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>552</v>
+        <v>653</v>
       </c>
       <c r="B84" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86" t="s">
-        <v>160</v>
-      </c>
-      <c r="B86" t="s">
-        <v>164</v>
+        <v>654</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>545</v>
+      </c>
+      <c r="B85" t="s">
+        <v>560</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B87" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B88" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B89" t="s">
-        <v>630</v>
+        <v>166</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>584</v>
+        <v>163</v>
       </c>
       <c r="B90" t="s">
-        <v>585</v>
+        <v>621</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>551</v>
+        <v>576</v>
       </c>
       <c r="B91" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" t="s">
-        <v>193</v>
-      </c>
-      <c r="B93" t="s">
-        <v>194</v>
+        <v>577</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>544</v>
+      </c>
+      <c r="B92" t="s">
+        <v>622</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
       <c r="B94" t="s">
-        <v>169</v>
+        <v>194</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B95" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>550</v>
+        <v>168</v>
       </c>
       <c r="B96" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
-      <c r="A98" t="s">
-        <v>191</v>
-      </c>
-      <c r="B98" t="s">
-        <v>192</v>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
+        <v>543</v>
+      </c>
+      <c r="B97" t="s">
+        <v>561</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="B99" t="s">
-        <v>173</v>
-      </c>
-      <c r="C99" t="s">
-        <v>617</v>
+        <v>192</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="B100" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C100" t="s">
-        <v>617</v>
+        <v>608</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B101" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C101" t="s">
-        <v>617</v>
+        <v>608</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>204</v>
+        <v>172</v>
       </c>
       <c r="B102" t="s">
-        <v>203</v>
+        <v>175</v>
+      </c>
+      <c r="C102" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B103" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>177</v>
+        <v>201</v>
       </c>
       <c r="B104" t="s">
-        <v>178</v>
-      </c>
-      <c r="C104" t="s">
-        <v>617</v>
+        <v>202</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>536</v>
+        <v>177</v>
       </c>
       <c r="B105" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3">
-      <c r="A107" t="s">
-        <v>521</v>
-      </c>
-      <c r="B107" t="s">
-        <v>522</v>
+        <v>178</v>
+      </c>
+      <c r="C105" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" t="s">
+        <v>530</v>
+      </c>
+      <c r="B106" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>243</v>
+        <v>515</v>
       </c>
       <c r="B108" t="s">
-        <v>244</v>
+        <v>516</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B109" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="B110" t="s">
-        <v>588</v>
+        <v>246</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="B111" t="s">
-        <v>247</v>
+        <v>580</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>511</v>
+        <v>248</v>
       </c>
       <c r="B112" t="s">
-        <v>520</v>
+        <v>247</v>
       </c>
     </row>
     <row r="113" spans="1:2">
       <c r="A113" t="s">
-        <v>250</v>
+        <v>505</v>
       </c>
       <c r="B113" t="s">
-        <v>249</v>
+        <v>514</v>
       </c>
     </row>
     <row r="114" spans="1:2">
       <c r="A114" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B114" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="115" spans="1:2">
       <c r="A115" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B115" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="116" spans="1:2">
       <c r="A116" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B116" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="117" spans="1:2">
       <c r="A117" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B117" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="118" spans="1:2">
       <c r="A118" t="s">
-        <v>303</v>
+        <v>258</v>
       </c>
       <c r="B118" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
     </row>
     <row r="119" spans="1:2">
       <c r="A119" t="s">
-        <v>350</v>
+        <v>303</v>
       </c>
       <c r="B119" t="s">
-        <v>351</v>
+        <v>249</v>
       </c>
     </row>
     <row r="120" spans="1:2">
       <c r="A120" t="s">
-        <v>534</v>
+        <v>350</v>
       </c>
       <c r="B120" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2">
-      <c r="A122" t="s">
-        <v>523</v>
-      </c>
-      <c r="B122" t="s">
-        <v>524</v>
+        <v>351</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>528</v>
+      </c>
+      <c r="B121" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="123" spans="1:2">
       <c r="A123" t="s">
+        <v>517</v>
+      </c>
+      <c r="B123" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" t="s">
         <v>260</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B124" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="13.5" customHeight="1">
-      <c r="A124" t="s">
+    <row r="125" spans="1:2" ht="13.5" customHeight="1">
+      <c r="A125" t="s">
         <v>262</v>
       </c>
-      <c r="B124" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2">
-      <c r="A125" t="s">
-        <v>261</v>
-      </c>
       <c r="B125" t="s">
-        <v>264</v>
+        <v>581</v>
       </c>
     </row>
     <row r="126" spans="1:2">
       <c r="A126" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B126" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="127" spans="1:2">
       <c r="A127" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B127" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="128" spans="1:2">
       <c r="A128" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B128" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>512</v>
+        <v>270</v>
       </c>
       <c r="B129" t="s">
-        <v>598</v>
+        <v>269</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>271</v>
+        <v>506</v>
       </c>
       <c r="B130" t="s">
-        <v>272</v>
+        <v>590</v>
       </c>
     </row>
     <row r="131" spans="1:2">
       <c r="A131" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B131" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B132" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B133" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B134" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B135" t="s">
-        <v>636</v>
+        <v>286</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B136" t="s">
-        <v>285</v>
+        <v>627</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B137" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
       <c r="B138" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B139" t="s">
-        <v>249</v>
+        <v>301</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B140" t="s">
-        <v>306</v>
+        <v>249</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>549</v>
+        <v>305</v>
       </c>
       <c r="B141" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2">
-      <c r="A143" t="s">
-        <v>525</v>
-      </c>
-      <c r="B143" t="s">
-        <v>526</v>
+        <v>306</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2">
+      <c r="A142" t="s">
+        <v>542</v>
+      </c>
+      <c r="B142" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>293</v>
+        <v>519</v>
       </c>
       <c r="B144" t="s">
-        <v>297</v>
+        <v>520</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>513</v>
+        <v>293</v>
       </c>
       <c r="B145" t="s">
-        <v>599</v>
+        <v>297</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>294</v>
+        <v>507</v>
       </c>
       <c r="B146" t="s">
-        <v>298</v>
+        <v>591</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B147" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B148" t="s">
-        <v>590</v>
+        <v>299</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B149" t="s">
-        <v>249</v>
+        <v>582</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="B150" t="s">
-        <v>311</v>
+        <v>249</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B151" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="152" spans="1:2">
       <c r="A152" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B152" t="s">
         <v>309</v>
@@ -7709,785 +7747,809 @@
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B153" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>548</v>
+        <v>312</v>
       </c>
       <c r="B154" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2">
-      <c r="A156" t="s">
-        <v>527</v>
-      </c>
-      <c r="B156" t="s">
-        <v>528</v>
+        <v>313</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2">
+      <c r="A155" t="s">
+        <v>541</v>
+      </c>
+      <c r="B155" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>507</v>
+        <v>521</v>
       </c>
       <c r="B157" t="s">
-        <v>321</v>
+        <v>522</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>514</v>
+        <v>501</v>
       </c>
       <c r="B158" t="s">
-        <v>600</v>
+        <v>321</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>316</v>
+        <v>508</v>
       </c>
       <c r="B159" t="s">
-        <v>322</v>
+        <v>592</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B160" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B161" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B162" t="s">
-        <v>591</v>
+        <v>324</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B163" t="s">
-        <v>249</v>
+        <v>583</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="B164" t="s">
-        <v>326</v>
+        <v>249</v>
       </c>
     </row>
     <row r="165" spans="1:2">
       <c r="A165" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B165" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B166" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B167" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B168" t="s">
-        <v>257</v>
+        <v>332</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>547</v>
+        <v>333</v>
       </c>
       <c r="B169" t="s">
-        <v>571</v>
-      </c>
-    </row>
-    <row r="171" spans="1:2">
-      <c r="A171" t="s">
-        <v>529</v>
-      </c>
-      <c r="B171" t="s">
-        <v>530</v>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2">
+      <c r="A170" t="s">
+        <v>540</v>
+      </c>
+      <c r="B170" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>509</v>
+        <v>523</v>
       </c>
       <c r="B172" t="s">
-        <v>339</v>
+        <v>524</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" t="s">
-        <v>515</v>
+        <v>503</v>
       </c>
       <c r="B173" t="s">
-        <v>601</v>
+        <v>339</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" t="s">
-        <v>337</v>
+        <v>509</v>
       </c>
       <c r="B174" t="s">
-        <v>340</v>
+        <v>593</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B175" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" t="s">
-        <v>508</v>
+        <v>338</v>
       </c>
       <c r="B176" t="s">
-        <v>592</v>
+        <v>341</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>345</v>
+        <v>502</v>
       </c>
       <c r="B177" t="s">
-        <v>249</v>
+        <v>584</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B178" t="s">
-        <v>342</v>
+        <v>249</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B179" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B180" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B181" t="s">
-        <v>257</v>
+        <v>344</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" t="s">
-        <v>546</v>
+        <v>349</v>
       </c>
       <c r="B182" t="s">
-        <v>572</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3">
-      <c r="A184" t="s">
-        <v>577</v>
-      </c>
-      <c r="B184" t="s">
-        <v>580</v>
-      </c>
-      <c r="C184" t="s">
-        <v>615</v>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
+      <c r="A183" t="s">
+        <v>539</v>
+      </c>
+      <c r="B183" t="s">
+        <v>565</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="s">
-        <v>578</v>
+        <v>570</v>
       </c>
       <c r="B185" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="C185" t="s">
-        <v>616</v>
+        <v>606</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="s">
-        <v>614</v>
+        <v>571</v>
       </c>
       <c r="B186" t="s">
-        <v>632</v>
+        <v>572</v>
+      </c>
+      <c r="C186" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" t="s">
-        <v>366</v>
+        <v>605</v>
       </c>
       <c r="B187" t="s">
-        <v>352</v>
+        <v>623</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B188" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" t="s">
-        <v>516</v>
+        <v>367</v>
       </c>
       <c r="B189" t="s">
-        <v>602</v>
+        <v>353</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190" t="s">
-        <v>368</v>
+        <v>510</v>
       </c>
       <c r="B190" t="s">
-        <v>354</v>
+        <v>594</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B191" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B192" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B193" t="s">
-        <v>357</v>
-      </c>
-      <c r="C193" t="s">
-        <v>617</v>
+        <v>356</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B194" t="s">
-        <v>358</v>
+        <v>357</v>
+      </c>
+      <c r="C194" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B195" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B196" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B197" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B198" t="s">
-        <v>362</v>
-      </c>
-      <c r="C198" t="s">
-        <v>617</v>
+        <v>361</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B199" t="s">
-        <v>363</v>
+        <v>362</v>
+      </c>
+      <c r="C199" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B200" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B201" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>545</v>
+        <v>379</v>
       </c>
       <c r="B202" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3">
-      <c r="A204" t="s">
-        <v>637</v>
-      </c>
-      <c r="B204" t="s">
-        <v>638</v>
+        <v>365</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203" t="s">
+        <v>538</v>
+      </c>
+      <c r="B203" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
-        <v>386</v>
+        <v>628</v>
       </c>
       <c r="B205" t="s">
-        <v>404</v>
+        <v>629</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B206" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B207" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>517</v>
+        <v>388</v>
       </c>
       <c r="B208" t="s">
-        <v>603</v>
+        <v>402</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" t="s">
-        <v>405</v>
+        <v>511</v>
       </c>
       <c r="B209" t="s">
-        <v>403</v>
+        <v>595</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" t="s">
-        <v>389</v>
+        <v>405</v>
       </c>
       <c r="B210" t="s">
-        <v>395</v>
+        <v>403</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
-        <v>406</v>
+        <v>389</v>
       </c>
       <c r="B211" t="s">
-        <v>396</v>
-      </c>
-      <c r="C211" t="s">
-        <v>593</v>
+        <v>395</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" t="s">
-        <v>390</v>
+        <v>406</v>
       </c>
       <c r="B212" t="s">
-        <v>397</v>
+        <v>396</v>
+      </c>
+      <c r="C212" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B213" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B214" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B215" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B216" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" t="s">
-        <v>544</v>
+        <v>394</v>
       </c>
       <c r="B217" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3">
-      <c r="A219" t="s">
-        <v>531</v>
-      </c>
-      <c r="B219" t="s">
-        <v>532</v>
+        <v>397</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3">
+      <c r="A218" t="s">
+        <v>537</v>
+      </c>
+      <c r="B218" t="s">
+        <v>567</v>
       </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220" t="s">
-        <v>412</v>
+        <v>525</v>
       </c>
       <c r="B220" t="s">
-        <v>423</v>
+        <v>526</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B221" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" t="s">
-        <v>604</v>
+        <v>413</v>
       </c>
       <c r="B222" t="s">
-        <v>605</v>
+        <v>424</v>
       </c>
     </row>
     <row r="223" spans="1:3">
       <c r="A223" t="s">
-        <v>414</v>
+        <v>596</v>
       </c>
       <c r="B223" t="s">
-        <v>425</v>
+        <v>597</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B224" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B225" t="s">
-        <v>618</v>
+        <v>426</v>
       </c>
     </row>
     <row r="226" spans="1:2">
       <c r="A226" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B226" t="s">
-        <v>427</v>
+        <v>609</v>
       </c>
     </row>
     <row r="227" spans="1:2">
       <c r="A227" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B227" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="228" spans="1:2">
       <c r="A228" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B228" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="229" spans="1:2">
       <c r="A229" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B229" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="230" spans="1:2">
       <c r="A230" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B230" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="231" spans="1:2">
       <c r="A231" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B231" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="232" spans="1:2">
       <c r="A232" t="s">
-        <v>541</v>
+        <v>422</v>
       </c>
       <c r="B232" t="s">
-        <v>542</v>
+        <v>432</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2">
+      <c r="A233" t="s">
+        <v>534</v>
+      </c>
+      <c r="B233" t="s">
+        <v>535</v>
       </c>
     </row>
     <row r="234" spans="1:2">
       <c r="A234" t="s">
-        <v>533</v>
+        <v>637</v>
       </c>
       <c r="B234" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="235" spans="1:2">
-      <c r="A235" t="s">
-        <v>445</v>
-      </c>
-      <c r="B235" t="s">
-        <v>456</v>
+        <v>638</v>
       </c>
     </row>
     <row r="236" spans="1:2">
       <c r="A236" t="s">
-        <v>446</v>
+        <v>527</v>
       </c>
       <c r="B236" t="s">
-        <v>457</v>
+        <v>526</v>
       </c>
     </row>
     <row r="237" spans="1:2">
       <c r="A237" t="s">
-        <v>518</v>
+        <v>439</v>
       </c>
       <c r="B237" t="s">
-        <v>607</v>
+        <v>450</v>
       </c>
     </row>
     <row r="238" spans="1:2">
       <c r="A238" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="B238" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
     </row>
     <row r="239" spans="1:2">
       <c r="A239" t="s">
-        <v>448</v>
+        <v>512</v>
       </c>
       <c r="B239" t="s">
-        <v>459</v>
+        <v>598</v>
       </c>
     </row>
     <row r="240" spans="1:2">
       <c r="A240" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="B240" t="s">
-        <v>619</v>
+        <v>452</v>
       </c>
     </row>
     <row r="241" spans="1:2">
       <c r="A241" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="B241" t="s">
-        <v>427</v>
+        <v>453</v>
       </c>
     </row>
     <row r="242" spans="1:2">
       <c r="A242" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="B242" t="s">
-        <v>428</v>
+        <v>610</v>
       </c>
     </row>
     <row r="243" spans="1:2">
       <c r="A243" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="B243" t="s">
-        <v>460</v>
+        <v>427</v>
       </c>
     </row>
     <row r="244" spans="1:2">
       <c r="A244" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="B244" t="s">
-        <v>461</v>
+        <v>428</v>
       </c>
     </row>
     <row r="245" spans="1:2">
       <c r="A245" t="s">
+        <v>446</v>
+      </c>
+      <c r="B245" t="s">
         <v>454</v>
-      </c>
-      <c r="B245" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="246" spans="1:2">
       <c r="A246" t="s">
+        <v>447</v>
+      </c>
+      <c r="B246" t="s">
         <v>455</v>
-      </c>
-      <c r="B246" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="247" spans="1:2">
       <c r="A247" t="s">
-        <v>539</v>
+        <v>448</v>
       </c>
       <c r="B247" t="s">
-        <v>542</v>
+        <v>431</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2">
+      <c r="A248" t="s">
+        <v>449</v>
+      </c>
+      <c r="B248" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="249" spans="1:2">
       <c r="A249" t="s">
-        <v>433</v>
+        <v>533</v>
       </c>
       <c r="B249" t="s">
-        <v>438</v>
+        <v>535</v>
       </c>
     </row>
     <row r="250" spans="1:2">
       <c r="A250" t="s">
-        <v>434</v>
+        <v>644</v>
       </c>
       <c r="B250" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="251" spans="1:2">
-      <c r="A251" t="s">
-        <v>519</v>
-      </c>
-      <c r="B251" t="s">
-        <v>606</v>
+        <v>638</v>
       </c>
     </row>
     <row r="252" spans="1:2">
       <c r="A252" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B252" t="s">
-        <v>440</v>
+        <v>645</v>
       </c>
     </row>
     <row r="253" spans="1:2">
       <c r="A253" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B253" t="s">
-        <v>441</v>
+        <v>646</v>
       </c>
     </row>
     <row r="254" spans="1:2">
       <c r="A254" t="s">
-        <v>437</v>
+        <v>513</v>
       </c>
       <c r="B254" t="s">
-        <v>442</v>
+        <v>647</v>
       </c>
     </row>
     <row r="255" spans="1:2">
       <c r="A255" t="s">
-        <v>538</v>
+        <v>435</v>
       </c>
       <c r="B255" t="s">
-        <v>540</v>
+        <v>648</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2">
+      <c r="A256" t="s">
+        <v>436</v>
+      </c>
+      <c r="B256" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2">
+      <c r="A257" t="s">
+        <v>437</v>
+      </c>
+      <c r="B257" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2">
+      <c r="A258" t="s">
+        <v>532</v>
+      </c>
+      <c r="B258" t="s">
+        <v>651</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MoveInDate check, Asset Values check in IAQ
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.malyala\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1189A6EE-C5D3-412F-99E5-5B955288D299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455D2CDC-5C2F-4362-AB3A-3C210A4F8373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="674">
   <si>
     <t>Name</t>
   </si>
@@ -2008,6 +2008,60 @@
   </si>
   <si>
     <t>Assets Type and  value does not match that listed on the ICW.</t>
+  </si>
+  <si>
+    <t>AS_CheckDateWithMoveIn</t>
+  </si>
+  <si>
+    <t>Date listed on the Application Summary is not with in 120 days of Move-In date.</t>
+  </si>
+  <si>
+    <t>MID_CheckDateWithMoveIn</t>
+  </si>
+  <si>
+    <t>Date listed on the Member Information Document is not with in 120 days of Move-In date.</t>
+  </si>
+  <si>
+    <t>SCNE_CheckDateWithMoveIn</t>
+  </si>
+  <si>
+    <t>Date listed on the Self Certification of Non Employment is not with in 120 days of Move-In date.</t>
+  </si>
+  <si>
+    <t>ASC_CheckDateWithMoveIn</t>
+  </si>
+  <si>
+    <t>Date listed on the Asset Self Certification is not with in 120 days of Move-In date.</t>
+  </si>
+  <si>
+    <t>ASFA_CheckDateWithMoveIn</t>
+  </si>
+  <si>
+    <t>Date listed on the Affidavit of Student Financial Assistance is not with in 120 days of Move-In date.</t>
+  </si>
+  <si>
+    <t>SC_CheckDateWithMoveIn</t>
+  </si>
+  <si>
+    <t>Date listed on the Student Certification is not with in 120 days of Move-In date.</t>
+  </si>
+  <si>
+    <t>VAWA_CheckDateWithMoveIn</t>
+  </si>
+  <si>
+    <t>Date listed on the VAWA Acknowledgement is not with in 120 days of Move-In date.</t>
+  </si>
+  <si>
+    <t>SR_CheckDateWithMoveIn</t>
+  </si>
+  <si>
+    <t>Date listed on the screening is not with in 120 days of Move-In date.</t>
+  </si>
+  <si>
+    <t>CZI_CheckDateWithMoveIn</t>
+  </si>
+  <si>
+    <t>Date listed on the Certification of Zero Income is not with in 120 days of Move-In date.</t>
   </si>
 </sst>
 </file>
@@ -6612,10 +6666,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
-  <dimension ref="A1:C258"/>
+  <dimension ref="A1:C267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="A142" sqref="A142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6787,1768 +6841,1840 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
+        <v>656</v>
+      </c>
+      <c r="B24" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
         <v>551</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>555</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
-        <v>184</v>
-      </c>
-      <c r="B26" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>91</v>
+        <v>184</v>
       </c>
       <c r="B27" t="s">
-        <v>92</v>
+        <v>186</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B28" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B32" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B33" t="s">
-        <v>99</v>
-      </c>
-      <c r="C33" t="s">
-        <v>608</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B34" t="s">
-        <v>100</v>
+        <v>99</v>
+      </c>
+      <c r="C34" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>550</v>
+        <v>106</v>
       </c>
       <c r="B35" t="s">
-        <v>556</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>658</v>
+      </c>
+      <c r="B36" t="s">
+        <v>659</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>185</v>
+        <v>550</v>
       </c>
       <c r="B37" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
-        <v>107</v>
-      </c>
-      <c r="B38" t="s">
-        <v>108</v>
+        <v>556</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>117</v>
+        <v>185</v>
       </c>
       <c r="B39" t="s">
-        <v>118</v>
+        <v>611</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="B40" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B41" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B42" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B43" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B44" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>205</v>
+        <v>115</v>
       </c>
       <c r="B45" t="s">
-        <v>496</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>206</v>
+        <v>116</v>
       </c>
       <c r="B46" t="s">
-        <v>612</v>
-      </c>
-      <c r="C46" t="s">
-        <v>608</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>599</v>
+        <v>205</v>
       </c>
       <c r="B47" t="s">
-        <v>613</v>
+        <v>496</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>552</v>
+        <v>206</v>
       </c>
       <c r="B48" t="s">
-        <v>553</v>
+        <v>612</v>
+      </c>
+      <c r="C48" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>574</v>
+        <v>599</v>
       </c>
       <c r="B49" t="s">
-        <v>655</v>
+        <v>613</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="B50" t="s">
-        <v>614</v>
+        <v>553</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>574</v>
+      </c>
+      <c r="B51" t="s">
+        <v>655</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>159</v>
+        <v>549</v>
       </c>
       <c r="B52" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
-      <c r="A53" t="s">
-        <v>122</v>
-      </c>
-      <c r="B53" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>124</v>
+        <v>159</v>
       </c>
       <c r="B54" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>548</v>
+        <v>122</v>
       </c>
       <c r="B55" t="s">
-        <v>557</v>
+        <v>615</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>124</v>
+      </c>
+      <c r="B56" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>187</v>
+        <v>660</v>
       </c>
       <c r="B57" t="s">
-        <v>188</v>
+        <v>661</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>125</v>
+        <v>548</v>
       </c>
       <c r="B58" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" t="s">
-        <v>126</v>
-      </c>
-      <c r="B59" t="s">
-        <v>128</v>
+        <v>557</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
       <c r="B60" t="s">
-        <v>616</v>
+        <v>188</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="B61" t="s">
-        <v>617</v>
+        <v>127</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="B62" t="s">
-        <v>618</v>
+        <v>128</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B63" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B64" t="s">
-        <v>497</v>
+        <v>617</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B65" t="s">
-        <v>499</v>
-      </c>
-      <c r="C65" t="s">
-        <v>575</v>
+        <v>618</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B66" t="s">
-        <v>500</v>
+        <v>619</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>547</v>
+        <v>143</v>
       </c>
       <c r="B67" t="s">
-        <v>558</v>
+        <v>497</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>144</v>
+      </c>
+      <c r="B68" t="s">
+        <v>499</v>
+      </c>
+      <c r="C68" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B69" t="s">
-        <v>151</v>
+        <v>500</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>149</v>
+        <v>662</v>
       </c>
       <c r="B70" t="s">
-        <v>152</v>
+        <v>663</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>150</v>
+        <v>547</v>
       </c>
       <c r="B71" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" t="s">
-        <v>146</v>
-      </c>
-      <c r="B72" t="s">
-        <v>600</v>
-      </c>
-      <c r="C72" t="s">
-        <v>129</v>
+        <v>558</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B73" t="s">
-        <v>130</v>
+        <v>151</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="B74" t="s">
-        <v>620</v>
+        <v>152</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="B75" t="s">
-        <v>131</v>
+        <v>153</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>546</v>
+        <v>146</v>
       </c>
       <c r="B76" t="s">
-        <v>559</v>
+        <v>600</v>
+      </c>
+      <c r="C76" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>147</v>
+      </c>
+      <c r="B77" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>189</v>
+        <v>132</v>
       </c>
       <c r="B78" t="s">
-        <v>190</v>
+        <v>620</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B79" t="s">
-        <v>154</v>
+        <v>131</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>136</v>
+        <v>664</v>
       </c>
       <c r="B80" t="s">
-        <v>155</v>
+        <v>665</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>135</v>
+        <v>546</v>
       </c>
       <c r="B81" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" t="s">
-        <v>137</v>
-      </c>
-      <c r="B82" t="s">
-        <v>157</v>
+        <v>559</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>138</v>
+        <v>189</v>
       </c>
       <c r="B83" t="s">
-        <v>158</v>
+        <v>190</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>653</v>
+        <v>134</v>
       </c>
       <c r="B84" t="s">
-        <v>654</v>
+        <v>154</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>545</v>
+        <v>136</v>
       </c>
       <c r="B85" t="s">
-        <v>560</v>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>135</v>
+      </c>
+      <c r="B86" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>160</v>
+        <v>137</v>
       </c>
       <c r="B87" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
       <c r="B88" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>162</v>
+        <v>653</v>
       </c>
       <c r="B89" t="s">
-        <v>166</v>
+        <v>654</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>163</v>
+        <v>666</v>
       </c>
       <c r="B90" t="s">
-        <v>621</v>
+        <v>667</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>576</v>
+        <v>545</v>
       </c>
       <c r="B91" t="s">
-        <v>577</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" t="s">
-        <v>544</v>
-      </c>
-      <c r="B92" t="s">
-        <v>622</v>
+        <v>560</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>160</v>
+      </c>
+      <c r="B93" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>193</v>
+        <v>161</v>
       </c>
       <c r="B94" t="s">
-        <v>194</v>
+        <v>165</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B95" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B96" t="s">
-        <v>170</v>
+        <v>621</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>543</v>
+        <v>576</v>
       </c>
       <c r="B97" t="s">
-        <v>561</v>
+        <v>577</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
+        <v>672</v>
+      </c>
+      <c r="B98" t="s">
+        <v>673</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>191</v>
+        <v>544</v>
       </c>
       <c r="B99" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3">
-      <c r="A100" t="s">
-        <v>176</v>
-      </c>
-      <c r="B100" t="s">
-        <v>173</v>
-      </c>
-      <c r="C100" t="s">
-        <v>608</v>
+        <v>622</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>171</v>
+        <v>193</v>
       </c>
       <c r="B101" t="s">
-        <v>174</v>
-      </c>
-      <c r="C101" t="s">
-        <v>608</v>
+        <v>194</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B102" t="s">
-        <v>175</v>
-      </c>
-      <c r="C102" t="s">
-        <v>608</v>
+        <v>169</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>204</v>
+        <v>168</v>
       </c>
       <c r="B103" t="s">
-        <v>203</v>
+        <v>170</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>201</v>
+        <v>668</v>
       </c>
       <c r="B104" t="s">
-        <v>202</v>
+        <v>669</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>177</v>
+        <v>543</v>
       </c>
       <c r="B105" t="s">
-        <v>178</v>
-      </c>
-      <c r="C105" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3">
-      <c r="A106" t="s">
-        <v>530</v>
-      </c>
-      <c r="B106" t="s">
-        <v>531</v>
+        <v>561</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" t="s">
+        <v>191</v>
+      </c>
+      <c r="B107" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>515</v>
+        <v>176</v>
       </c>
       <c r="B108" t="s">
-        <v>516</v>
+        <v>173</v>
+      </c>
+      <c r="C108" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>243</v>
+        <v>171</v>
       </c>
       <c r="B109" t="s">
-        <v>244</v>
+        <v>174</v>
+      </c>
+      <c r="C109" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>245</v>
+        <v>172</v>
       </c>
       <c r="B110" t="s">
-        <v>246</v>
+        <v>175</v>
+      </c>
+      <c r="C110" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>259</v>
+        <v>204</v>
       </c>
       <c r="B111" t="s">
-        <v>580</v>
+        <v>203</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
+        <v>201</v>
+      </c>
+      <c r="B112" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" t="s">
+        <v>177</v>
+      </c>
+      <c r="B113" t="s">
+        <v>178</v>
+      </c>
+      <c r="C113" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" t="s">
+        <v>670</v>
+      </c>
+      <c r="B114" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" t="s">
+        <v>530</v>
+      </c>
+      <c r="B115" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" t="s">
+        <v>515</v>
+      </c>
+      <c r="B117" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" t="s">
+        <v>243</v>
+      </c>
+      <c r="B118" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" t="s">
+        <v>245</v>
+      </c>
+      <c r="B119" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" t="s">
+        <v>259</v>
+      </c>
+      <c r="B120" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" t="s">
         <v>248</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B121" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
-      <c r="A113" t="s">
+    <row r="122" spans="1:3">
+      <c r="A122" t="s">
         <v>505</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B122" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
-      <c r="A114" t="s">
+    <row r="123" spans="1:3">
+      <c r="A123" t="s">
         <v>250</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B123" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
-      <c r="A115" t="s">
+    <row r="124" spans="1:3">
+      <c r="A124" t="s">
         <v>251</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B124" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
-      <c r="A116" t="s">
+    <row r="125" spans="1:3">
+      <c r="A125" t="s">
         <v>252</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B125" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
-      <c r="A117" t="s">
+    <row r="126" spans="1:3">
+      <c r="A126" t="s">
         <v>256</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B126" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
-      <c r="A118" t="s">
+    <row r="127" spans="1:3">
+      <c r="A127" t="s">
         <v>258</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B127" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
-      <c r="A119" t="s">
+    <row r="128" spans="1:3">
+      <c r="A128" t="s">
         <v>303</v>
       </c>
-      <c r="B119" t="s">
+      <c r="B128" t="s">
         <v>249</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2">
-      <c r="A120" t="s">
-        <v>350</v>
-      </c>
-      <c r="B120" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2">
-      <c r="A121" t="s">
-        <v>528</v>
-      </c>
-      <c r="B121" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2">
-      <c r="A123" t="s">
-        <v>517</v>
-      </c>
-      <c r="B123" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2">
-      <c r="A124" t="s">
-        <v>260</v>
-      </c>
-      <c r="B124" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" ht="13.5" customHeight="1">
-      <c r="A125" t="s">
-        <v>262</v>
-      </c>
-      <c r="B125" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2">
-      <c r="A126" t="s">
-        <v>261</v>
-      </c>
-      <c r="B126" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2">
-      <c r="A127" t="s">
-        <v>266</v>
-      </c>
-      <c r="B127" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2">
-      <c r="A128" t="s">
-        <v>267</v>
-      </c>
-      <c r="B128" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>270</v>
+        <v>350</v>
       </c>
       <c r="B129" t="s">
-        <v>269</v>
+        <v>351</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>506</v>
+        <v>528</v>
       </c>
       <c r="B130" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2">
-      <c r="A131" t="s">
-        <v>271</v>
-      </c>
-      <c r="B131" t="s">
-        <v>272</v>
+        <v>529</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>273</v>
+        <v>517</v>
       </c>
       <c r="B132" t="s">
-        <v>274</v>
+        <v>518</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>278</v>
+        <v>260</v>
       </c>
       <c r="B133" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" ht="13.5" customHeight="1">
       <c r="A134" t="s">
-        <v>279</v>
+        <v>262</v>
       </c>
       <c r="B134" t="s">
-        <v>287</v>
+        <v>581</v>
       </c>
     </row>
     <row r="135" spans="1:2">
       <c r="A135" t="s">
-        <v>280</v>
+        <v>261</v>
       </c>
       <c r="B135" t="s">
-        <v>286</v>
+        <v>264</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="B136" t="s">
-        <v>627</v>
+        <v>265</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="B137" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
     </row>
     <row r="138" spans="1:2">
       <c r="A138" t="s">
-        <v>283</v>
+        <v>270</v>
       </c>
       <c r="B138" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>300</v>
+        <v>506</v>
       </c>
       <c r="B139" t="s">
-        <v>301</v>
+        <v>590</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>302</v>
+        <v>271</v>
       </c>
       <c r="B140" t="s">
-        <v>249</v>
+        <v>272</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>305</v>
+        <v>273</v>
       </c>
       <c r="B141" t="s">
-        <v>306</v>
+        <v>274</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>542</v>
+        <v>278</v>
       </c>
       <c r="B142" t="s">
-        <v>562</v>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2">
+      <c r="A143" t="s">
+        <v>279</v>
+      </c>
+      <c r="B143" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>519</v>
+        <v>280</v>
       </c>
       <c r="B144" t="s">
-        <v>520</v>
+        <v>286</v>
       </c>
     </row>
     <row r="145" spans="1:2">
       <c r="A145" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="B145" t="s">
-        <v>297</v>
+        <v>627</v>
       </c>
     </row>
     <row r="146" spans="1:2">
       <c r="A146" t="s">
-        <v>507</v>
+        <v>282</v>
       </c>
       <c r="B146" t="s">
-        <v>591</v>
+        <v>285</v>
       </c>
     </row>
     <row r="147" spans="1:2">
       <c r="A147" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="B147" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
     </row>
     <row r="148" spans="1:2">
       <c r="A148" t="s">
-        <v>295</v>
+        <v>300</v>
       </c>
       <c r="B148" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="149" spans="1:2">
       <c r="A149" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="B149" t="s">
-        <v>582</v>
+        <v>249</v>
       </c>
     </row>
     <row r="150" spans="1:2">
       <c r="A150" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B150" t="s">
-        <v>249</v>
+        <v>306</v>
       </c>
     </row>
     <row r="151" spans="1:2">
       <c r="A151" t="s">
-        <v>310</v>
+        <v>542</v>
       </c>
       <c r="B151" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2">
-      <c r="A152" t="s">
-        <v>307</v>
-      </c>
-      <c r="B152" t="s">
-        <v>309</v>
+        <v>562</v>
       </c>
     </row>
     <row r="153" spans="1:2">
       <c r="A153" t="s">
-        <v>308</v>
+        <v>519</v>
       </c>
       <c r="B153" t="s">
-        <v>309</v>
+        <v>520</v>
       </c>
     </row>
     <row r="154" spans="1:2">
       <c r="A154" t="s">
-        <v>312</v>
+        <v>293</v>
       </c>
       <c r="B154" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
     </row>
     <row r="155" spans="1:2">
       <c r="A155" t="s">
-        <v>541</v>
+        <v>507</v>
       </c>
       <c r="B155" t="s">
-        <v>563</v>
+        <v>591</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2">
+      <c r="A156" t="s">
+        <v>294</v>
+      </c>
+      <c r="B156" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="157" spans="1:2">
       <c r="A157" t="s">
-        <v>521</v>
+        <v>295</v>
       </c>
       <c r="B157" t="s">
-        <v>522</v>
+        <v>299</v>
       </c>
     </row>
     <row r="158" spans="1:2">
       <c r="A158" t="s">
-        <v>501</v>
+        <v>296</v>
       </c>
       <c r="B158" t="s">
-        <v>321</v>
+        <v>582</v>
       </c>
     </row>
     <row r="159" spans="1:2">
       <c r="A159" t="s">
-        <v>508</v>
+        <v>304</v>
       </c>
       <c r="B159" t="s">
-        <v>592</v>
+        <v>249</v>
       </c>
     </row>
     <row r="160" spans="1:2">
       <c r="A160" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="B160" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="B161" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="B162" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="B163" t="s">
-        <v>583</v>
+        <v>313</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>320</v>
+        <v>541</v>
       </c>
       <c r="B164" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="165" spans="1:2">
-      <c r="A165" t="s">
-        <v>325</v>
-      </c>
-      <c r="B165" t="s">
-        <v>326</v>
+        <v>563</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>327</v>
+        <v>521</v>
       </c>
       <c r="B166" t="s">
-        <v>328</v>
+        <v>522</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>330</v>
+        <v>501</v>
       </c>
       <c r="B167" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>331</v>
+        <v>508</v>
       </c>
       <c r="B168" t="s">
-        <v>332</v>
+        <v>592</v>
       </c>
     </row>
     <row r="169" spans="1:2">
       <c r="A169" t="s">
-        <v>333</v>
+        <v>316</v>
       </c>
       <c r="B169" t="s">
-        <v>257</v>
+        <v>322</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>540</v>
+        <v>317</v>
       </c>
       <c r="B170" t="s">
-        <v>564</v>
+        <v>323</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2">
+      <c r="A171" t="s">
+        <v>318</v>
+      </c>
+      <c r="B171" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>523</v>
+        <v>319</v>
       </c>
       <c r="B172" t="s">
-        <v>524</v>
+        <v>583</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" t="s">
-        <v>503</v>
+        <v>320</v>
       </c>
       <c r="B173" t="s">
-        <v>339</v>
+        <v>249</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" t="s">
-        <v>509</v>
+        <v>325</v>
       </c>
       <c r="B174" t="s">
-        <v>593</v>
+        <v>326</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="B175" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" t="s">
+        <v>330</v>
+      </c>
+      <c r="B176" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2">
+      <c r="A177" t="s">
+        <v>331</v>
+      </c>
+      <c r="B177" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2">
+      <c r="A178" t="s">
+        <v>333</v>
+      </c>
+      <c r="B178" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2">
+      <c r="A179" t="s">
+        <v>540</v>
+      </c>
+      <c r="B179" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2">
+      <c r="A181" t="s">
+        <v>523</v>
+      </c>
+      <c r="B181" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2">
+      <c r="A182" t="s">
+        <v>503</v>
+      </c>
+      <c r="B182" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2">
+      <c r="A183" t="s">
+        <v>509</v>
+      </c>
+      <c r="B183" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2">
+      <c r="A184" t="s">
+        <v>337</v>
+      </c>
+      <c r="B184" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2">
+      <c r="A185" t="s">
         <v>338</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B185" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="177" spans="1:3">
-      <c r="A177" t="s">
+    <row r="186" spans="1:2">
+      <c r="A186" t="s">
         <v>502</v>
       </c>
-      <c r="B177" t="s">
+      <c r="B186" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="178" spans="1:3">
-      <c r="A178" t="s">
+    <row r="187" spans="1:2">
+      <c r="A187" t="s">
         <v>345</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B187" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="179" spans="1:3">
-      <c r="A179" t="s">
+    <row r="188" spans="1:2">
+      <c r="A188" t="s">
         <v>346</v>
       </c>
-      <c r="B179" t="s">
+      <c r="B188" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="180" spans="1:3">
-      <c r="A180" t="s">
+    <row r="189" spans="1:2">
+      <c r="A189" t="s">
         <v>347</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B189" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="181" spans="1:3">
-      <c r="A181" t="s">
+    <row r="190" spans="1:2">
+      <c r="A190" t="s">
         <v>348</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B190" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="182" spans="1:3">
-      <c r="A182" t="s">
+    <row r="191" spans="1:2">
+      <c r="A191" t="s">
         <v>349</v>
       </c>
-      <c r="B182" t="s">
+      <c r="B191" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="183" spans="1:3">
-      <c r="A183" t="s">
+    <row r="192" spans="1:2">
+      <c r="A192" t="s">
         <v>539</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B192" t="s">
         <v>565</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3">
-      <c r="A185" t="s">
-        <v>570</v>
-      </c>
-      <c r="B185" t="s">
-        <v>573</v>
-      </c>
-      <c r="C185" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3">
-      <c r="A186" t="s">
-        <v>571</v>
-      </c>
-      <c r="B186" t="s">
-        <v>572</v>
-      </c>
-      <c r="C186" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3">
-      <c r="A187" t="s">
-        <v>605</v>
-      </c>
-      <c r="B187" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3">
-      <c r="A188" t="s">
-        <v>366</v>
-      </c>
-      <c r="B188" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3">
-      <c r="A189" t="s">
-        <v>367</v>
-      </c>
-      <c r="B189" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3">
-      <c r="A190" t="s">
-        <v>510</v>
-      </c>
-      <c r="B190" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3">
-      <c r="A191" t="s">
-        <v>368</v>
-      </c>
-      <c r="B191" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3">
-      <c r="A192" t="s">
-        <v>369</v>
-      </c>
-      <c r="B192" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3">
-      <c r="A193" t="s">
-        <v>370</v>
-      </c>
-      <c r="B193" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>371</v>
+        <v>570</v>
       </c>
       <c r="B194" t="s">
-        <v>357</v>
+        <v>573</v>
       </c>
       <c r="C194" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>372</v>
+        <v>571</v>
       </c>
       <c r="B195" t="s">
-        <v>358</v>
+        <v>572</v>
+      </c>
+      <c r="C195" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>373</v>
+        <v>605</v>
       </c>
       <c r="B196" t="s">
-        <v>359</v>
+        <v>623</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="B197" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="B198" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" t="s">
-        <v>376</v>
+        <v>510</v>
       </c>
       <c r="B199" t="s">
-        <v>362</v>
-      </c>
-      <c r="C199" t="s">
-        <v>608</v>
+        <v>594</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="B200" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
       <c r="B201" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="B202" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" t="s">
-        <v>538</v>
+        <v>371</v>
       </c>
       <c r="B203" t="s">
-        <v>566</v>
+        <v>357</v>
+      </c>
+      <c r="C203" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3">
+      <c r="A204" t="s">
+        <v>372</v>
+      </c>
+      <c r="B204" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
-        <v>628</v>
+        <v>373</v>
       </c>
       <c r="B205" t="s">
-        <v>629</v>
+        <v>359</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
       <c r="B206" t="s">
-        <v>404</v>
+        <v>360</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="B207" t="s">
-        <v>401</v>
+        <v>361</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="B208" t="s">
-        <v>402</v>
+        <v>362</v>
+      </c>
+      <c r="C208" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" t="s">
-        <v>511</v>
+        <v>377</v>
       </c>
       <c r="B209" t="s">
-        <v>595</v>
+        <v>363</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" t="s">
-        <v>405</v>
+        <v>378</v>
       </c>
       <c r="B210" t="s">
-        <v>403</v>
+        <v>364</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="B211" t="s">
-        <v>395</v>
+        <v>365</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" t="s">
-        <v>406</v>
+        <v>538</v>
       </c>
       <c r="B212" t="s">
-        <v>396</v>
-      </c>
-      <c r="C212" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3">
-      <c r="A213" t="s">
-        <v>390</v>
-      </c>
-      <c r="B213" t="s">
-        <v>397</v>
+        <v>566</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" t="s">
-        <v>392</v>
+        <v>628</v>
       </c>
       <c r="B214" t="s">
-        <v>398</v>
+        <v>629</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="B215" t="s">
-        <v>399</v>
+        <v>404</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="B216" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="B217" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" t="s">
-        <v>537</v>
+        <v>511</v>
       </c>
       <c r="B218" t="s">
-        <v>567</v>
+        <v>595</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3">
+      <c r="A219" t="s">
+        <v>405</v>
+      </c>
+      <c r="B219" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220" t="s">
-        <v>525</v>
+        <v>389</v>
       </c>
       <c r="B220" t="s">
-        <v>526</v>
+        <v>395</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="B221" t="s">
-        <v>423</v>
+        <v>396</v>
+      </c>
+      <c r="C221" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" t="s">
-        <v>413</v>
+        <v>390</v>
       </c>
       <c r="B222" t="s">
-        <v>424</v>
+        <v>397</v>
       </c>
     </row>
     <row r="223" spans="1:3">
       <c r="A223" t="s">
-        <v>596</v>
+        <v>392</v>
       </c>
       <c r="B223" t="s">
-        <v>597</v>
+        <v>398</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" t="s">
-        <v>414</v>
+        <v>391</v>
       </c>
       <c r="B224" t="s">
-        <v>425</v>
+        <v>399</v>
       </c>
     </row>
     <row r="225" spans="1:2">
       <c r="A225" t="s">
-        <v>415</v>
+        <v>393</v>
       </c>
       <c r="B225" t="s">
-        <v>426</v>
+        <v>400</v>
       </c>
     </row>
     <row r="226" spans="1:2">
       <c r="A226" t="s">
-        <v>416</v>
+        <v>394</v>
       </c>
       <c r="B226" t="s">
-        <v>609</v>
+        <v>397</v>
       </c>
     </row>
     <row r="227" spans="1:2">
       <c r="A227" t="s">
-        <v>417</v>
+        <v>537</v>
       </c>
       <c r="B227" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="228" spans="1:2">
-      <c r="A228" t="s">
-        <v>418</v>
-      </c>
-      <c r="B228" t="s">
-        <v>428</v>
+        <v>567</v>
       </c>
     </row>
     <row r="229" spans="1:2">
       <c r="A229" t="s">
-        <v>419</v>
+        <v>525</v>
       </c>
       <c r="B229" t="s">
-        <v>429</v>
+        <v>526</v>
       </c>
     </row>
     <row r="230" spans="1:2">
       <c r="A230" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="B230" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
     </row>
     <row r="231" spans="1:2">
       <c r="A231" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="B231" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
     </row>
     <row r="232" spans="1:2">
       <c r="A232" t="s">
-        <v>422</v>
+        <v>596</v>
       </c>
       <c r="B232" t="s">
-        <v>432</v>
+        <v>597</v>
       </c>
     </row>
     <row r="233" spans="1:2">
       <c r="A233" t="s">
-        <v>534</v>
+        <v>414</v>
       </c>
       <c r="B233" t="s">
-        <v>535</v>
+        <v>425</v>
       </c>
     </row>
     <row r="234" spans="1:2">
       <c r="A234" t="s">
-        <v>637</v>
+        <v>415</v>
       </c>
       <c r="B234" t="s">
-        <v>638</v>
+        <v>426</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2">
+      <c r="A235" t="s">
+        <v>416</v>
+      </c>
+      <c r="B235" t="s">
+        <v>609</v>
       </c>
     </row>
     <row r="236" spans="1:2">
       <c r="A236" t="s">
-        <v>527</v>
+        <v>417</v>
       </c>
       <c r="B236" t="s">
-        <v>526</v>
+        <v>427</v>
       </c>
     </row>
     <row r="237" spans="1:2">
       <c r="A237" t="s">
-        <v>439</v>
+        <v>418</v>
       </c>
       <c r="B237" t="s">
-        <v>450</v>
+        <v>428</v>
       </c>
     </row>
     <row r="238" spans="1:2">
       <c r="A238" t="s">
-        <v>440</v>
+        <v>419</v>
       </c>
       <c r="B238" t="s">
-        <v>451</v>
+        <v>429</v>
       </c>
     </row>
     <row r="239" spans="1:2">
       <c r="A239" t="s">
-        <v>512</v>
+        <v>420</v>
       </c>
       <c r="B239" t="s">
-        <v>598</v>
+        <v>430</v>
       </c>
     </row>
     <row r="240" spans="1:2">
       <c r="A240" t="s">
-        <v>441</v>
+        <v>421</v>
       </c>
       <c r="B240" t="s">
-        <v>452</v>
+        <v>431</v>
       </c>
     </row>
     <row r="241" spans="1:2">
       <c r="A241" t="s">
-        <v>442</v>
+        <v>422</v>
       </c>
       <c r="B241" t="s">
-        <v>453</v>
+        <v>432</v>
       </c>
     </row>
     <row r="242" spans="1:2">
       <c r="A242" t="s">
-        <v>443</v>
+        <v>534</v>
       </c>
       <c r="B242" t="s">
-        <v>610</v>
+        <v>535</v>
       </c>
     </row>
     <row r="243" spans="1:2">
       <c r="A243" t="s">
-        <v>444</v>
+        <v>637</v>
       </c>
       <c r="B243" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="244" spans="1:2">
-      <c r="A244" t="s">
-        <v>445</v>
-      </c>
-      <c r="B244" t="s">
-        <v>428</v>
+        <v>638</v>
       </c>
     </row>
     <row r="245" spans="1:2">
       <c r="A245" t="s">
-        <v>446</v>
+        <v>527</v>
       </c>
       <c r="B245" t="s">
-        <v>454</v>
+        <v>526</v>
       </c>
     </row>
     <row r="246" spans="1:2">
       <c r="A246" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="B246" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
     </row>
     <row r="247" spans="1:2">
       <c r="A247" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="B247" t="s">
-        <v>431</v>
+        <v>451</v>
       </c>
     </row>
     <row r="248" spans="1:2">
       <c r="A248" t="s">
-        <v>449</v>
+        <v>512</v>
       </c>
       <c r="B248" t="s">
-        <v>432</v>
+        <v>598</v>
       </c>
     </row>
     <row r="249" spans="1:2">
       <c r="A249" t="s">
-        <v>533</v>
+        <v>441</v>
       </c>
       <c r="B249" t="s">
-        <v>535</v>
+        <v>452</v>
       </c>
     </row>
     <row r="250" spans="1:2">
       <c r="A250" t="s">
-        <v>644</v>
+        <v>442</v>
       </c>
       <c r="B250" t="s">
-        <v>638</v>
+        <v>453</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2">
+      <c r="A251" t="s">
+        <v>443</v>
+      </c>
+      <c r="B251" t="s">
+        <v>610</v>
       </c>
     </row>
     <row r="252" spans="1:2">
       <c r="A252" t="s">
-        <v>433</v>
+        <v>444</v>
       </c>
       <c r="B252" t="s">
-        <v>645</v>
+        <v>427</v>
       </c>
     </row>
     <row r="253" spans="1:2">
       <c r="A253" t="s">
-        <v>434</v>
+        <v>445</v>
       </c>
       <c r="B253" t="s">
-        <v>646</v>
+        <v>428</v>
       </c>
     </row>
     <row r="254" spans="1:2">
       <c r="A254" t="s">
-        <v>513</v>
+        <v>446</v>
       </c>
       <c r="B254" t="s">
-        <v>647</v>
+        <v>454</v>
       </c>
     </row>
     <row r="255" spans="1:2">
       <c r="A255" t="s">
-        <v>435</v>
+        <v>447</v>
       </c>
       <c r="B255" t="s">
-        <v>648</v>
+        <v>455</v>
       </c>
     </row>
     <row r="256" spans="1:2">
       <c r="A256" t="s">
-        <v>436</v>
+        <v>448</v>
       </c>
       <c r="B256" t="s">
-        <v>649</v>
+        <v>431</v>
       </c>
     </row>
     <row r="257" spans="1:2">
       <c r="A257" t="s">
-        <v>437</v>
+        <v>449</v>
       </c>
       <c r="B257" t="s">
-        <v>650</v>
+        <v>432</v>
       </c>
     </row>
     <row r="258" spans="1:2">
       <c r="A258" t="s">
+        <v>533</v>
+      </c>
+      <c r="B258" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2">
+      <c r="A259" t="s">
+        <v>644</v>
+      </c>
+      <c r="B259" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2">
+      <c r="A261" t="s">
+        <v>433</v>
+      </c>
+      <c r="B261" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2">
+      <c r="A262" t="s">
+        <v>434</v>
+      </c>
+      <c r="B262" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2">
+      <c r="A263" t="s">
+        <v>513</v>
+      </c>
+      <c r="B263" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2">
+      <c r="A264" t="s">
+        <v>435</v>
+      </c>
+      <c r="B264" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2">
+      <c r="A265" t="s">
+        <v>436</v>
+      </c>
+      <c r="B265" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2">
+      <c r="A266" t="s">
+        <v>437</v>
+      </c>
+      <c r="B266" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2">
+      <c r="A267" t="s">
         <v>532</v>
       </c>
-      <c r="B258" t="s">
+      <c r="B267" t="s">
         <v>651</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added fuzzy logic for member names comparison and handling multiple EDCs
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.malyala\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455D2CDC-5C2F-4362-AB3A-3C210A4F8373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8509149-792A-4D5E-9935-10911214C2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="20190" windowHeight="9720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="674">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="676">
   <si>
     <t>Name</t>
   </si>
@@ -1986,9 +1986,6 @@
     <t>Date listed on the Verification of Reccurring Cash Contribution is not with in 120 days of Move-In date.</t>
   </si>
   <si>
-    <t xml:space="preserve">Amount listed on the Verification of Reccurring Cash Contribution and ICW do not match. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Verification of Reccurring Cash Contribution has not been signed. </t>
   </si>
   <si>
@@ -2062,6 +2059,15 @@
   </si>
   <si>
     <t>Date listed on the Certification of Zero Income is not with in 120 days of Move-In date.</t>
+  </si>
+  <si>
+    <t>FindAllMatches_Threshold</t>
+  </si>
+  <si>
+    <t>ICW check was removed from this check</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contributor and Amount listed on the Verification of Reccurring Cash Contribution and ICW do not match. </t>
   </si>
 </sst>
 </file>
@@ -5355,8 +5361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1011"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5557,10 +5563,10 @@
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B21" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1">
@@ -5683,7 +5689,14 @@
         <v>625</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A37" t="s">
+        <v>673</v>
+      </c>
+      <c r="B37" t="s">
+        <v>673</v>
+      </c>
+    </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
@@ -6668,8 +6681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
   <dimension ref="A1:C267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
-      <selection activeCell="A142" sqref="A142"/>
+    <sheetView tabSelected="1" topLeftCell="A258" workbookViewId="0">
+      <selection activeCell="B270" sqref="B270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6841,10 +6854,10 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
+        <v>655</v>
+      </c>
+      <c r="B24" t="s">
         <v>656</v>
-      </c>
-      <c r="B24" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -6932,10 +6945,10 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
+        <v>657</v>
+      </c>
+      <c r="B36" t="s">
         <v>658</v>
-      </c>
-      <c r="B36" t="s">
-        <v>659</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -6961,6 +6974,9 @@
       <c r="B40" t="s">
         <v>108</v>
       </c>
+      <c r="C40" t="s">
+        <v>608</v>
+      </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
@@ -6969,6 +6985,9 @@
       <c r="B41" t="s">
         <v>118</v>
       </c>
+      <c r="C41" t="s">
+        <v>608</v>
+      </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
@@ -6977,6 +6996,9 @@
       <c r="B42" t="s">
         <v>120</v>
       </c>
+      <c r="C42" t="s">
+        <v>608</v>
+      </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
@@ -6985,6 +7007,9 @@
       <c r="B43" t="s">
         <v>109</v>
       </c>
+      <c r="C43" t="s">
+        <v>608</v>
+      </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
@@ -6993,6 +7018,9 @@
       <c r="B44" t="s">
         <v>110</v>
       </c>
+      <c r="C44" t="s">
+        <v>608</v>
+      </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
@@ -7001,6 +7029,9 @@
       <c r="B45" t="s">
         <v>111</v>
       </c>
+      <c r="C45" t="s">
+        <v>608</v>
+      </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
@@ -7050,7 +7081,7 @@
         <v>574</v>
       </c>
       <c r="B51" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -7087,10 +7118,10 @@
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
+        <v>659</v>
+      </c>
+      <c r="B57" t="s">
         <v>660</v>
-      </c>
-      <c r="B57" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -7186,10 +7217,10 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
+        <v>661</v>
+      </c>
+      <c r="B70" t="s">
         <v>662</v>
-      </c>
-      <c r="B70" t="s">
-        <v>663</v>
       </c>
     </row>
     <row r="71" spans="1:3">
@@ -7261,10 +7292,10 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
+        <v>663</v>
+      </c>
+      <c r="B80" t="s">
         <v>664</v>
-      </c>
-      <c r="B80" t="s">
-        <v>665</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -7325,18 +7356,18 @@
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
+        <v>652</v>
+      </c>
+      <c r="B89" t="s">
         <v>653</v>
-      </c>
-      <c r="B89" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
+        <v>665</v>
+      </c>
+      <c r="B90" t="s">
         <v>666</v>
-      </c>
-      <c r="B90" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -7389,10 +7420,10 @@
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
+        <v>671</v>
+      </c>
+      <c r="B98" t="s">
         <v>672</v>
-      </c>
-      <c r="B98" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="99" spans="1:3">
@@ -7429,10 +7460,10 @@
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
+        <v>667</v>
+      </c>
+      <c r="B104" t="s">
         <v>668</v>
-      </c>
-      <c r="B104" t="s">
-        <v>669</v>
       </c>
     </row>
     <row r="105" spans="1:3">
@@ -7513,10 +7544,10 @@
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
+        <v>669</v>
+      </c>
+      <c r="B114" t="s">
         <v>670</v>
-      </c>
-      <c r="B114" t="s">
-        <v>671</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -7558,6 +7589,9 @@
       <c r="B120" t="s">
         <v>580</v>
       </c>
+      <c r="C120" t="s">
+        <v>674</v>
+      </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
@@ -7743,7 +7777,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
+    <row r="145" spans="1:3">
       <c r="A145" t="s">
         <v>281</v>
       </c>
@@ -7751,7 +7785,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
+    <row r="146" spans="1:3">
       <c r="A146" t="s">
         <v>282</v>
       </c>
@@ -7759,7 +7793,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
+    <row r="147" spans="1:3">
       <c r="A147" t="s">
         <v>283</v>
       </c>
@@ -7767,7 +7801,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
+    <row r="148" spans="1:3">
       <c r="A148" t="s">
         <v>300</v>
       </c>
@@ -7775,7 +7809,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
+    <row r="149" spans="1:3">
       <c r="A149" t="s">
         <v>302</v>
       </c>
@@ -7783,7 +7817,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="150" spans="1:2">
+    <row r="150" spans="1:3">
       <c r="A150" t="s">
         <v>305</v>
       </c>
@@ -7791,7 +7825,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
+    <row r="151" spans="1:3">
       <c r="A151" t="s">
         <v>542</v>
       </c>
@@ -7799,7 +7833,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="153" spans="1:2">
+    <row r="153" spans="1:3">
       <c r="A153" t="s">
         <v>519</v>
       </c>
@@ -7807,7 +7841,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="154" spans="1:2">
+    <row r="154" spans="1:3">
       <c r="A154" t="s">
         <v>293</v>
       </c>
@@ -7815,7 +7849,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="155" spans="1:2">
+    <row r="155" spans="1:3">
       <c r="A155" t="s">
         <v>507</v>
       </c>
@@ -7823,15 +7857,18 @@
         <v>591</v>
       </c>
     </row>
-    <row r="156" spans="1:2">
+    <row r="156" spans="1:3">
       <c r="A156" t="s">
         <v>294</v>
       </c>
       <c r="B156" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="157" spans="1:2">
+      <c r="C156" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
       <c r="A157" t="s">
         <v>295</v>
       </c>
@@ -7839,7 +7876,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="158" spans="1:2">
+    <row r="158" spans="1:3">
       <c r="A158" t="s">
         <v>296</v>
       </c>
@@ -7847,7 +7884,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="159" spans="1:2">
+    <row r="159" spans="1:3">
       <c r="A159" t="s">
         <v>304</v>
       </c>
@@ -7855,7 +7892,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="160" spans="1:2">
+    <row r="160" spans="1:3">
       <c r="A160" t="s">
         <v>310</v>
       </c>
@@ -8651,7 +8688,7 @@
         <v>435</v>
       </c>
       <c r="B264" t="s">
-        <v>648</v>
+        <v>675</v>
       </c>
     </row>
     <row r="265" spans="1:2">
@@ -8659,7 +8696,7 @@
         <v>436</v>
       </c>
       <c r="B265" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="266" spans="1:2">
@@ -8667,7 +8704,7 @@
         <v>437</v>
       </c>
       <c r="B266" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="267" spans="1:2">
@@ -8675,7 +8712,7 @@
         <v>532</v>
       </c>
       <c r="B267" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated code for the defects: 57333, 57384, 57187, 57328, 57461
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.malyala\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8509149-792A-4D5E-9935-10911214C2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A415F7-7B8A-4085-B55E-5A61BE1A81FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="20190" windowHeight="9720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="683">
   <si>
     <t>Name</t>
   </si>
@@ -2068,6 +2068,27 @@
   </si>
   <si>
     <t xml:space="preserve">Contributor and Amount listed on the Verification of Reccurring Cash Contribution and ICW do not match. </t>
+  </si>
+  <si>
+    <t>EDC_hourly_and_paycheck</t>
+  </si>
+  <si>
+    <t>Both hourly income and check stubs have been provided on the Exact Day Calculator. Manual review required.</t>
+  </si>
+  <si>
+    <t>Newly added</t>
+  </si>
+  <si>
+    <t>AS_HouseholdMemAbsent</t>
+  </si>
+  <si>
+    <t>household member is temporarily absent, need manual review.</t>
+  </si>
+  <si>
+    <t>PS_PaystubsMatchEDC</t>
+  </si>
+  <si>
+    <t>Paystubs do not match EDC with Employee Name, End date and Gross pay</t>
   </si>
 </sst>
 </file>
@@ -6679,10 +6700,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
-  <dimension ref="A1:C267"/>
+  <dimension ref="A1:C271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A258" workbookViewId="0">
-      <selection activeCell="B270" sqref="B270"/>
+    <sheetView tabSelected="1" topLeftCell="A225" workbookViewId="0">
+      <selection activeCell="C253" sqref="C253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6862,128 +6883,125 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
+        <v>679</v>
+      </c>
+      <c r="B25" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
         <v>551</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>555</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
-        <v>184</v>
-      </c>
-      <c r="B27" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>91</v>
+        <v>184</v>
       </c>
       <c r="B28" t="s">
-        <v>92</v>
+        <v>186</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B34" t="s">
-        <v>99</v>
-      </c>
-      <c r="C34" t="s">
-        <v>608</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B35" t="s">
-        <v>100</v>
+        <v>99</v>
+      </c>
+      <c r="C35" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>657</v>
+        <v>106</v>
       </c>
       <c r="B36" t="s">
-        <v>658</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
+        <v>657</v>
+      </c>
+      <c r="B37" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
         <v>550</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>556</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
-        <v>185</v>
-      </c>
-      <c r="B39" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>107</v>
+        <v>185</v>
       </c>
       <c r="B40" t="s">
-        <v>108</v>
-      </c>
-      <c r="C40" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B41" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C41" t="s">
         <v>608</v>
@@ -6991,10 +7009,10 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B42" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C42" t="s">
         <v>608</v>
@@ -7002,10 +7020,10 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B43" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="C43" t="s">
         <v>608</v>
@@ -7013,10 +7031,10 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B44" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C44" t="s">
         <v>608</v>
@@ -7024,10 +7042,10 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B45" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C45" t="s">
         <v>608</v>
@@ -7035,470 +7053,470 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B46" t="s">
-        <v>112</v>
+        <v>111</v>
+      </c>
+      <c r="C46" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>205</v>
+        <v>116</v>
       </c>
       <c r="B47" t="s">
-        <v>496</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
+        <v>205</v>
+      </c>
+      <c r="B48" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
         <v>206</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>612</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
-      <c r="A49" t="s">
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
         <v>599</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" t="s">
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
         <v>552</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
-      <c r="A51" t="s">
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
         <v>574</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
-      <c r="A52" t="s">
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
         <v>549</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
-      <c r="A54" t="s">
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
         <v>159</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
-      <c r="A55" t="s">
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
         <v>122</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B56" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
-      <c r="A56" t="s">
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
         <v>124</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
-      <c r="A57" t="s">
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
         <v>659</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B58" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
-      <c r="A58" t="s">
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
         <v>548</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
-      <c r="A60" t="s">
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
         <v>187</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
-      <c r="A61" t="s">
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
         <v>125</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
-      <c r="A62" t="s">
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
         <v>126</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
-      <c r="A63" t="s">
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
         <v>139</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B64" t="s">
         <v>616</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
-      <c r="A64" t="s">
-        <v>140</v>
-      </c>
-      <c r="B64" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B65" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B66" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B67" t="s">
-        <v>497</v>
+        <v>619</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B68" t="s">
-        <v>499</v>
-      </c>
-      <c r="C68" t="s">
-        <v>575</v>
+        <v>497</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B69" t="s">
-        <v>500</v>
+        <v>499</v>
+      </c>
+      <c r="C69" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>661</v>
+        <v>145</v>
       </c>
       <c r="B70" t="s">
-        <v>662</v>
+        <v>500</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
+        <v>661</v>
+      </c>
+      <c r="B71" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
         <v>547</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B72" t="s">
         <v>558</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" t="s">
-        <v>148</v>
-      </c>
-      <c r="B73" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B74" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B75" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B76" t="s">
-        <v>600</v>
-      </c>
-      <c r="C76" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B77" t="s">
-        <v>130</v>
+        <v>600</v>
+      </c>
+      <c r="C77" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="B78" t="s">
-        <v>620</v>
+        <v>130</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B79" t="s">
-        <v>131</v>
+        <v>620</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>663</v>
+        <v>133</v>
       </c>
       <c r="B80" t="s">
-        <v>664</v>
+        <v>131</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
+        <v>663</v>
+      </c>
+      <c r="B81" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
         <v>546</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B82" t="s">
         <v>559</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" t="s">
-        <v>189</v>
-      </c>
-      <c r="B83" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="84" spans="1:2">
       <c r="A84" t="s">
-        <v>134</v>
+        <v>189</v>
       </c>
       <c r="B84" t="s">
-        <v>154</v>
+        <v>190</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B85" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B86" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B87" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B88" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>652</v>
+        <v>138</v>
       </c>
       <c r="B89" t="s">
-        <v>653</v>
+        <v>158</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>665</v>
+        <v>652</v>
       </c>
       <c r="B90" t="s">
-        <v>666</v>
+        <v>653</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
+        <v>665</v>
+      </c>
+      <c r="B91" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
         <v>545</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B92" t="s">
         <v>560</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" t="s">
-        <v>160</v>
-      </c>
-      <c r="B93" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="94" spans="1:2">
       <c r="A94" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B94" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B95" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B96" t="s">
-        <v>621</v>
+        <v>166</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>576</v>
+        <v>163</v>
       </c>
       <c r="B97" t="s">
-        <v>577</v>
+        <v>621</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>671</v>
+        <v>576</v>
       </c>
       <c r="B98" t="s">
-        <v>672</v>
+        <v>577</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
+        <v>671</v>
+      </c>
+      <c r="B99" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
         <v>544</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B100" t="s">
         <v>622</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3">
-      <c r="A101" t="s">
-        <v>193</v>
-      </c>
-      <c r="B101" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
       <c r="B102" t="s">
-        <v>169</v>
+        <v>194</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B103" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>667</v>
+        <v>168</v>
       </c>
       <c r="B104" t="s">
-        <v>668</v>
+        <v>170</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
+        <v>667</v>
+      </c>
+      <c r="B105" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" t="s">
         <v>543</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B106" t="s">
         <v>561</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3">
-      <c r="A107" t="s">
-        <v>191</v>
-      </c>
-      <c r="B107" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="B108" t="s">
-        <v>173</v>
-      </c>
-      <c r="C108" t="s">
-        <v>608</v>
+        <v>192</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="B109" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C109" t="s">
         <v>608</v>
@@ -7506,10 +7524,10 @@
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B110" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C110" t="s">
         <v>608</v>
@@ -7517,1201 +7535,1237 @@
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>204</v>
+        <v>172</v>
       </c>
       <c r="B111" t="s">
-        <v>203</v>
+        <v>175</v>
+      </c>
+      <c r="C111" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B112" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>177</v>
+        <v>201</v>
       </c>
       <c r="B113" t="s">
-        <v>178</v>
-      </c>
-      <c r="C113" t="s">
-        <v>608</v>
+        <v>202</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>669</v>
+        <v>177</v>
       </c>
       <c r="B114" t="s">
-        <v>670</v>
+        <v>178</v>
+      </c>
+      <c r="C114" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
+        <v>669</v>
+      </c>
+      <c r="B115" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" t="s">
         <v>530</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B116" t="s">
         <v>531</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3">
-      <c r="A117" t="s">
-        <v>515</v>
-      </c>
-      <c r="B117" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>243</v>
+        <v>676</v>
       </c>
       <c r="B118" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3">
-      <c r="A119" t="s">
-        <v>245</v>
-      </c>
-      <c r="B119" t="s">
-        <v>246</v>
+        <v>677</v>
+      </c>
+      <c r="C118" t="s">
+        <v>678</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>259</v>
+        <v>515</v>
       </c>
       <c r="B120" t="s">
-        <v>580</v>
-      </c>
-      <c r="C120" t="s">
-        <v>674</v>
+        <v>516</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B121" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>505</v>
+        <v>245</v>
       </c>
       <c r="B122" t="s">
-        <v>514</v>
+        <v>246</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="B123" t="s">
-        <v>249</v>
+        <v>580</v>
+      </c>
+      <c r="C123" t="s">
+        <v>674</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B124" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>252</v>
+        <v>505</v>
       </c>
       <c r="B125" t="s">
-        <v>254</v>
+        <v>514</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B126" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="B127" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>303</v>
+        <v>252</v>
       </c>
       <c r="B128" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
     </row>
     <row r="129" spans="1:2">
       <c r="A129" t="s">
-        <v>350</v>
+        <v>256</v>
       </c>
       <c r="B129" t="s">
-        <v>351</v>
+        <v>255</v>
       </c>
     </row>
     <row r="130" spans="1:2">
       <c r="A130" t="s">
-        <v>528</v>
+        <v>258</v>
       </c>
       <c r="B130" t="s">
-        <v>529</v>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2">
+      <c r="A131" t="s">
+        <v>303</v>
+      </c>
+      <c r="B131" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="132" spans="1:2">
       <c r="A132" t="s">
-        <v>517</v>
+        <v>350</v>
       </c>
       <c r="B132" t="s">
-        <v>518</v>
+        <v>351</v>
       </c>
     </row>
     <row r="133" spans="1:2">
       <c r="A133" t="s">
-        <v>260</v>
+        <v>681</v>
       </c>
       <c r="B133" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" ht="13.5" customHeight="1">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2">
       <c r="A134" t="s">
-        <v>262</v>
+        <v>528</v>
       </c>
       <c r="B134" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2">
-      <c r="A135" t="s">
-        <v>261</v>
-      </c>
-      <c r="B135" t="s">
-        <v>264</v>
+        <v>529</v>
       </c>
     </row>
     <row r="136" spans="1:2">
       <c r="A136" t="s">
-        <v>266</v>
+        <v>517</v>
       </c>
       <c r="B136" t="s">
-        <v>265</v>
+        <v>518</v>
       </c>
     </row>
     <row r="137" spans="1:2">
       <c r="A137" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="B137" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" ht="13.5" customHeight="1">
       <c r="A138" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="B138" t="s">
-        <v>269</v>
+        <v>581</v>
       </c>
     </row>
     <row r="139" spans="1:2">
       <c r="A139" t="s">
-        <v>506</v>
+        <v>261</v>
       </c>
       <c r="B139" t="s">
-        <v>590</v>
+        <v>264</v>
       </c>
     </row>
     <row r="140" spans="1:2">
       <c r="A140" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B140" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
     </row>
     <row r="141" spans="1:2">
       <c r="A141" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="B141" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
     </row>
     <row r="142" spans="1:2">
       <c r="A142" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="B142" t="s">
-        <v>288</v>
+        <v>269</v>
       </c>
     </row>
     <row r="143" spans="1:2">
       <c r="A143" t="s">
-        <v>279</v>
+        <v>506</v>
       </c>
       <c r="B143" t="s">
-        <v>287</v>
+        <v>590</v>
       </c>
     </row>
     <row r="144" spans="1:2">
       <c r="A144" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="B144" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="B145" t="s">
-        <v>627</v>
+        <v>274</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B146" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B147" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="B148" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>302</v>
+        <v>281</v>
       </c>
       <c r="B149" t="s">
-        <v>249</v>
+        <v>627</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>305</v>
+        <v>282</v>
       </c>
       <c r="B150" t="s">
-        <v>306</v>
+        <v>285</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>542</v>
+        <v>283</v>
       </c>
       <c r="B151" t="s">
-        <v>562</v>
+        <v>284</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" t="s">
+        <v>300</v>
+      </c>
+      <c r="B152" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>519</v>
+        <v>302</v>
       </c>
       <c r="B153" t="s">
-        <v>520</v>
+        <v>249</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>293</v>
+        <v>305</v>
       </c>
       <c r="B154" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>507</v>
+        <v>542</v>
       </c>
       <c r="B155" t="s">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3">
-      <c r="A156" t="s">
-        <v>294</v>
-      </c>
-      <c r="B156" t="s">
-        <v>298</v>
-      </c>
-      <c r="C156" t="s">
-        <v>608</v>
+        <v>562</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>295</v>
+        <v>519</v>
       </c>
       <c r="B157" t="s">
-        <v>299</v>
+        <v>520</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B158" t="s">
-        <v>582</v>
+        <v>297</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
-        <v>304</v>
+        <v>507</v>
       </c>
       <c r="B159" t="s">
-        <v>249</v>
+        <v>591</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="B160" t="s">
-        <v>311</v>
+        <v>298</v>
+      </c>
+      <c r="C160" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="161" spans="1:2">
       <c r="A161" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="B161" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
     </row>
     <row r="162" spans="1:2">
       <c r="A162" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="B162" t="s">
-        <v>309</v>
+        <v>582</v>
       </c>
     </row>
     <row r="163" spans="1:2">
       <c r="A163" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="B163" t="s">
-        <v>313</v>
+        <v>249</v>
       </c>
     </row>
     <row r="164" spans="1:2">
       <c r="A164" t="s">
-        <v>541</v>
+        <v>310</v>
       </c>
       <c r="B164" t="s">
-        <v>563</v>
+        <v>311</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2">
+      <c r="A165" t="s">
+        <v>307</v>
+      </c>
+      <c r="B165" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="166" spans="1:2">
       <c r="A166" t="s">
-        <v>521</v>
+        <v>308</v>
       </c>
       <c r="B166" t="s">
-        <v>522</v>
+        <v>309</v>
       </c>
     </row>
     <row r="167" spans="1:2">
       <c r="A167" t="s">
-        <v>501</v>
+        <v>312</v>
       </c>
       <c r="B167" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
     </row>
     <row r="168" spans="1:2">
       <c r="A168" t="s">
-        <v>508</v>
+        <v>541</v>
       </c>
       <c r="B168" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="169" spans="1:2">
-      <c r="A169" t="s">
-        <v>316</v>
-      </c>
-      <c r="B169" t="s">
-        <v>322</v>
+        <v>563</v>
       </c>
     </row>
     <row r="170" spans="1:2">
       <c r="A170" t="s">
-        <v>317</v>
+        <v>521</v>
       </c>
       <c r="B170" t="s">
-        <v>323</v>
+        <v>522</v>
       </c>
     </row>
     <row r="171" spans="1:2">
       <c r="A171" t="s">
-        <v>318</v>
+        <v>501</v>
       </c>
       <c r="B171" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="172" spans="1:2">
       <c r="A172" t="s">
-        <v>319</v>
+        <v>508</v>
       </c>
       <c r="B172" t="s">
-        <v>583</v>
+        <v>592</v>
       </c>
     </row>
     <row r="173" spans="1:2">
       <c r="A173" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B173" t="s">
-        <v>249</v>
+        <v>322</v>
       </c>
     </row>
     <row r="174" spans="1:2">
       <c r="A174" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="B174" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="175" spans="1:2">
       <c r="A175" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="B175" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="176" spans="1:2">
       <c r="A176" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="B176" t="s">
-        <v>329</v>
+        <v>583</v>
       </c>
     </row>
     <row r="177" spans="1:2">
       <c r="A177" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="B177" t="s">
-        <v>332</v>
+        <v>249</v>
       </c>
     </row>
     <row r="178" spans="1:2">
       <c r="A178" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="B178" t="s">
-        <v>257</v>
+        <v>326</v>
       </c>
     </row>
     <row r="179" spans="1:2">
       <c r="A179" t="s">
-        <v>540</v>
+        <v>327</v>
       </c>
       <c r="B179" t="s">
-        <v>564</v>
+        <v>328</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2">
+      <c r="A180" t="s">
+        <v>330</v>
+      </c>
+      <c r="B180" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="181" spans="1:2">
       <c r="A181" t="s">
-        <v>523</v>
+        <v>331</v>
       </c>
       <c r="B181" t="s">
-        <v>524</v>
+        <v>332</v>
       </c>
     </row>
     <row r="182" spans="1:2">
       <c r="A182" t="s">
-        <v>503</v>
+        <v>333</v>
       </c>
       <c r="B182" t="s">
-        <v>339</v>
+        <v>257</v>
       </c>
     </row>
     <row r="183" spans="1:2">
       <c r="A183" t="s">
-        <v>509</v>
+        <v>540</v>
       </c>
       <c r="B183" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="184" spans="1:2">
-      <c r="A184" t="s">
-        <v>337</v>
-      </c>
-      <c r="B184" t="s">
-        <v>340</v>
+        <v>564</v>
       </c>
     </row>
     <row r="185" spans="1:2">
       <c r="A185" t="s">
-        <v>338</v>
+        <v>523</v>
       </c>
       <c r="B185" t="s">
-        <v>341</v>
+        <v>524</v>
       </c>
     </row>
     <row r="186" spans="1:2">
       <c r="A186" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B186" t="s">
-        <v>584</v>
+        <v>339</v>
       </c>
     </row>
     <row r="187" spans="1:2">
       <c r="A187" t="s">
-        <v>345</v>
+        <v>509</v>
       </c>
       <c r="B187" t="s">
-        <v>249</v>
+        <v>593</v>
       </c>
     </row>
     <row r="188" spans="1:2">
       <c r="A188" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="B188" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="189" spans="1:2">
       <c r="A189" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="B189" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="190" spans="1:2">
       <c r="A190" t="s">
-        <v>348</v>
+        <v>502</v>
       </c>
       <c r="B190" t="s">
-        <v>344</v>
+        <v>584</v>
       </c>
     </row>
     <row r="191" spans="1:2">
       <c r="A191" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="B191" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="192" spans="1:2">
       <c r="A192" t="s">
-        <v>539</v>
+        <v>346</v>
       </c>
       <c r="B192" t="s">
-        <v>565</v>
+        <v>342</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3">
+      <c r="A193" t="s">
+        <v>347</v>
+      </c>
+      <c r="B193" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>570</v>
+        <v>348</v>
       </c>
       <c r="B194" t="s">
-        <v>573</v>
-      </c>
-      <c r="C194" t="s">
-        <v>606</v>
+        <v>344</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>571</v>
+        <v>349</v>
       </c>
       <c r="B195" t="s">
-        <v>572</v>
-      </c>
-      <c r="C195" t="s">
-        <v>607</v>
+        <v>257</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>605</v>
+        <v>539</v>
       </c>
       <c r="B196" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3">
-      <c r="A197" t="s">
-        <v>366</v>
-      </c>
-      <c r="B197" t="s">
-        <v>352</v>
+        <v>565</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
-        <v>367</v>
+        <v>570</v>
       </c>
       <c r="B198" t="s">
-        <v>353</v>
+        <v>573</v>
+      </c>
+      <c r="C198" t="s">
+        <v>606</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" t="s">
-        <v>510</v>
+        <v>571</v>
       </c>
       <c r="B199" t="s">
-        <v>594</v>
+        <v>572</v>
+      </c>
+      <c r="C199" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>368</v>
+        <v>605</v>
       </c>
       <c r="B200" t="s">
-        <v>354</v>
+        <v>623</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B201" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B202" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" t="s">
-        <v>371</v>
+        <v>510</v>
       </c>
       <c r="B203" t="s">
-        <v>357</v>
-      </c>
-      <c r="C203" t="s">
-        <v>608</v>
+        <v>594</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B204" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B205" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B206" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B207" t="s">
-        <v>361</v>
+        <v>357</v>
+      </c>
+      <c r="C207" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B208" t="s">
-        <v>362</v>
-      </c>
-      <c r="C208" t="s">
-        <v>608</v>
+        <v>358</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B209" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="B210" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B211" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" t="s">
-        <v>538</v>
+        <v>376</v>
       </c>
       <c r="B212" t="s">
-        <v>566</v>
+        <v>362</v>
+      </c>
+      <c r="C212" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3">
+      <c r="A213" t="s">
+        <v>377</v>
+      </c>
+      <c r="B213" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" t="s">
-        <v>628</v>
+        <v>378</v>
       </c>
       <c r="B214" t="s">
-        <v>629</v>
+        <v>364</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="B215" t="s">
-        <v>404</v>
+        <v>365</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" t="s">
-        <v>387</v>
+        <v>538</v>
       </c>
       <c r="B216" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="217" spans="1:3">
-      <c r="A217" t="s">
-        <v>388</v>
-      </c>
-      <c r="B217" t="s">
-        <v>402</v>
+        <v>566</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" t="s">
-        <v>511</v>
+        <v>628</v>
       </c>
       <c r="B218" t="s">
-        <v>595</v>
+        <v>629</v>
       </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219" t="s">
-        <v>405</v>
+        <v>386</v>
       </c>
       <c r="B219" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B220" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" t="s">
-        <v>406</v>
+        <v>388</v>
       </c>
       <c r="B221" t="s">
-        <v>396</v>
-      </c>
-      <c r="C221" t="s">
-        <v>585</v>
+        <v>402</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" t="s">
-        <v>390</v>
+        <v>511</v>
       </c>
       <c r="B222" t="s">
-        <v>397</v>
+        <v>595</v>
       </c>
     </row>
     <row r="223" spans="1:3">
       <c r="A223" t="s">
-        <v>392</v>
+        <v>405</v>
       </c>
       <c r="B223" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B224" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="225" spans="1:2">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3">
       <c r="A225" t="s">
-        <v>393</v>
+        <v>406</v>
       </c>
       <c r="B225" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="226" spans="1:2">
+        <v>396</v>
+      </c>
+      <c r="C225" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3">
       <c r="A226" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="B226" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="227" spans="1:2">
+    <row r="227" spans="1:3">
       <c r="A227" t="s">
+        <v>392</v>
+      </c>
+      <c r="B227" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3">
+      <c r="A228" t="s">
+        <v>391</v>
+      </c>
+      <c r="B228" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3">
+      <c r="A229" t="s">
+        <v>393</v>
+      </c>
+      <c r="B229" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3">
+      <c r="A230" t="s">
+        <v>394</v>
+      </c>
+      <c r="B230" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3">
+      <c r="A231" t="s">
         <v>537</v>
       </c>
-      <c r="B227" t="s">
+      <c r="B231" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="229" spans="1:2">
-      <c r="A229" t="s">
+    <row r="233" spans="1:3">
+      <c r="A233" t="s">
         <v>525</v>
       </c>
-      <c r="B229" t="s">
+      <c r="B233" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="230" spans="1:2">
-      <c r="A230" t="s">
+    <row r="234" spans="1:3">
+      <c r="A234" t="s">
         <v>412</v>
       </c>
-      <c r="B230" t="s">
+      <c r="B234" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="231" spans="1:2">
-      <c r="A231" t="s">
+    <row r="235" spans="1:3">
+      <c r="A235" t="s">
         <v>413</v>
       </c>
-      <c r="B231" t="s">
+      <c r="B235" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="232" spans="1:2">
-      <c r="A232" t="s">
+    <row r="236" spans="1:3">
+      <c r="A236" t="s">
         <v>596</v>
       </c>
-      <c r="B232" t="s">
+      <c r="B236" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="233" spans="1:2">
-      <c r="A233" t="s">
+    <row r="237" spans="1:3">
+      <c r="A237" t="s">
         <v>414</v>
       </c>
-      <c r="B233" t="s">
+      <c r="B237" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="234" spans="1:2">
-      <c r="A234" t="s">
+      <c r="C237" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3">
+      <c r="A238" t="s">
         <v>415</v>
       </c>
-      <c r="B234" t="s">
+      <c r="B238" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="235" spans="1:2">
-      <c r="A235" t="s">
+    <row r="239" spans="1:3">
+      <c r="A239" t="s">
         <v>416</v>
       </c>
-      <c r="B235" t="s">
+      <c r="B239" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="236" spans="1:2">
-      <c r="A236" t="s">
+    <row r="240" spans="1:3">
+      <c r="A240" t="s">
         <v>417</v>
       </c>
-      <c r="B236" t="s">
+      <c r="B240" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="237" spans="1:2">
-      <c r="A237" t="s">
+    <row r="241" spans="1:3">
+      <c r="A241" t="s">
         <v>418</v>
       </c>
-      <c r="B237" t="s">
+      <c r="B241" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="238" spans="1:2">
-      <c r="A238" t="s">
+    <row r="242" spans="1:3">
+      <c r="A242" t="s">
         <v>419</v>
       </c>
-      <c r="B238" t="s">
+      <c r="B242" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="239" spans="1:2">
-      <c r="A239" t="s">
+    <row r="243" spans="1:3">
+      <c r="A243" t="s">
         <v>420</v>
       </c>
-      <c r="B239" t="s">
+      <c r="B243" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="240" spans="1:2">
-      <c r="A240" t="s">
+    <row r="244" spans="1:3">
+      <c r="A244" t="s">
         <v>421</v>
       </c>
-      <c r="B240" t="s">
+      <c r="B244" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="241" spans="1:2">
-      <c r="A241" t="s">
+    <row r="245" spans="1:3">
+      <c r="A245" t="s">
         <v>422</v>
       </c>
-      <c r="B241" t="s">
+      <c r="B245" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="242" spans="1:2">
-      <c r="A242" t="s">
+    <row r="246" spans="1:3">
+      <c r="A246" t="s">
         <v>534</v>
       </c>
-      <c r="B242" t="s">
+      <c r="B246" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="243" spans="1:2">
-      <c r="A243" t="s">
+    <row r="247" spans="1:3">
+      <c r="A247" t="s">
         <v>637</v>
       </c>
-      <c r="B243" t="s">
+      <c r="B247" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="245" spans="1:2">
-      <c r="A245" t="s">
+    <row r="249" spans="1:3">
+      <c r="A249" t="s">
         <v>527</v>
       </c>
-      <c r="B245" t="s">
+      <c r="B249" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="246" spans="1:2">
-      <c r="A246" t="s">
+    <row r="250" spans="1:3">
+      <c r="A250" t="s">
         <v>439</v>
       </c>
-      <c r="B246" t="s">
+      <c r="B250" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="247" spans="1:2">
-      <c r="A247" t="s">
+    <row r="251" spans="1:3">
+      <c r="A251" t="s">
         <v>440</v>
       </c>
-      <c r="B247" t="s">
+      <c r="B251" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="248" spans="1:2">
-      <c r="A248" t="s">
+    <row r="252" spans="1:3">
+      <c r="A252" t="s">
         <v>512</v>
       </c>
-      <c r="B248" t="s">
+      <c r="B252" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="249" spans="1:2">
-      <c r="A249" t="s">
+    <row r="253" spans="1:3">
+      <c r="A253" t="s">
         <v>441</v>
       </c>
-      <c r="B249" t="s">
+      <c r="B253" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="250" spans="1:2">
-      <c r="A250" t="s">
+      <c r="C253" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3">
+      <c r="A254" t="s">
         <v>442</v>
       </c>
-      <c r="B250" t="s">
+      <c r="B254" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="251" spans="1:2">
-      <c r="A251" t="s">
+    <row r="255" spans="1:3">
+      <c r="A255" t="s">
         <v>443</v>
       </c>
-      <c r="B251" t="s">
+      <c r="B255" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="252" spans="1:2">
-      <c r="A252" t="s">
+    <row r="256" spans="1:3">
+      <c r="A256" t="s">
         <v>444</v>
       </c>
-      <c r="B252" t="s">
+      <c r="B256" t="s">
         <v>427</v>
-      </c>
-    </row>
-    <row r="253" spans="1:2">
-      <c r="A253" t="s">
-        <v>445</v>
-      </c>
-      <c r="B253" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="254" spans="1:2">
-      <c r="A254" t="s">
-        <v>446</v>
-      </c>
-      <c r="B254" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="255" spans="1:2">
-      <c r="A255" t="s">
-        <v>447</v>
-      </c>
-      <c r="B255" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="256" spans="1:2">
-      <c r="A256" t="s">
-        <v>448</v>
-      </c>
-      <c r="B256" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="257" spans="1:2">
       <c r="A257" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="B257" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="258" spans="1:2">
       <c r="A258" t="s">
-        <v>533</v>
+        <v>446</v>
       </c>
       <c r="B258" t="s">
-        <v>535</v>
+        <v>454</v>
       </c>
     </row>
     <row r="259" spans="1:2">
       <c r="A259" t="s">
-        <v>644</v>
+        <v>447</v>
       </c>
       <c r="B259" t="s">
-        <v>638</v>
+        <v>455</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2">
+      <c r="A260" t="s">
+        <v>448</v>
+      </c>
+      <c r="B260" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="261" spans="1:2">
       <c r="A261" t="s">
-        <v>433</v>
+        <v>449</v>
       </c>
       <c r="B261" t="s">
-        <v>645</v>
+        <v>432</v>
       </c>
     </row>
     <row r="262" spans="1:2">
       <c r="A262" t="s">
-        <v>434</v>
+        <v>533</v>
       </c>
       <c r="B262" t="s">
-        <v>646</v>
+        <v>535</v>
       </c>
     </row>
     <row r="263" spans="1:2">
       <c r="A263" t="s">
-        <v>513</v>
+        <v>644</v>
       </c>
       <c r="B263" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="264" spans="1:2">
-      <c r="A264" t="s">
-        <v>435</v>
-      </c>
-      <c r="B264" t="s">
-        <v>675</v>
+        <v>638</v>
       </c>
     </row>
     <row r="265" spans="1:2">
       <c r="A265" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="B265" t="s">
-        <v>648</v>
+        <v>645</v>
       </c>
     </row>
     <row r="266" spans="1:2">
       <c r="A266" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="B266" t="s">
-        <v>649</v>
+        <v>646</v>
       </c>
     </row>
     <row r="267" spans="1:2">
       <c r="A267" t="s">
+        <v>513</v>
+      </c>
+      <c r="B267" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2">
+      <c r="A268" t="s">
+        <v>435</v>
+      </c>
+      <c r="B268" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2">
+      <c r="A269" t="s">
+        <v>436</v>
+      </c>
+      <c r="B269" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2">
+      <c r="A270" t="s">
+        <v>437</v>
+      </c>
+      <c r="B270" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2">
+      <c r="A271" t="s">
         <v>532</v>
       </c>
-      <c r="B267" t="s">
+      <c r="B271" t="s">
         <v>650</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Story: removing all Commented out business checks
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.malyala\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A415F7-7B8A-4085-B55E-5A61BE1A81FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68F9266-607D-4D66-AAEC-09BDE3A7F02F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="683">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="685">
   <si>
     <t>Name</t>
   </si>
@@ -2089,6 +2089,12 @@
   </si>
   <si>
     <t>Paystubs do not match EDC with Employee Name, End date and Gross pay</t>
+  </si>
+  <si>
+    <t>Business asked to remove</t>
+  </si>
+  <si>
+    <t>removed this check</t>
   </si>
 </sst>
 </file>
@@ -6702,8 +6708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
   <dimension ref="A1:C271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A225" workbookViewId="0">
-      <selection activeCell="C253" sqref="C253"/>
+    <sheetView tabSelected="1" topLeftCell="A246" workbookViewId="0">
+      <selection activeCell="B272" sqref="B272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6713,7 +6719,7 @@
     <col min="3" max="3" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="18.75">
+    <row r="1" spans="1:3" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6721,7 +6727,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>195</v>
       </c>
@@ -6729,7 +6735,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>181</v>
       </c>
@@ -6737,7 +6743,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -6745,7 +6751,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>180</v>
       </c>
@@ -6753,7 +6759,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>78</v>
       </c>
@@ -6761,15 +6767,18 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>207</v>
       </c>
       <c r="B9" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>568</v>
       </c>
@@ -6777,7 +6786,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>536</v>
       </c>
@@ -6785,7 +6794,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>182</v>
       </c>
@@ -6793,7 +6802,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -6801,7 +6810,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>578</v>
       </c>
@@ -6809,7 +6818,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -7243,6 +7252,9 @@
       <c r="B70" t="s">
         <v>500</v>
       </c>
+      <c r="C70" t="s">
+        <v>575</v>
+      </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
@@ -7613,6 +7625,9 @@
       <c r="B121" t="s">
         <v>244</v>
       </c>
+      <c r="C121" t="s">
+        <v>608</v>
+      </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
@@ -7673,7 +7688,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
+    <row r="129" spans="1:3">
       <c r="A129" t="s">
         <v>256</v>
       </c>
@@ -7681,7 +7696,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
+    <row r="130" spans="1:3">
       <c r="A130" t="s">
         <v>258</v>
       </c>
@@ -7689,7 +7704,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="131" spans="1:2">
+    <row r="131" spans="1:3">
       <c r="A131" t="s">
         <v>303</v>
       </c>
@@ -7697,7 +7712,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
+    <row r="132" spans="1:3">
       <c r="A132" t="s">
         <v>350</v>
       </c>
@@ -7705,7 +7720,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
+    <row r="133" spans="1:3">
       <c r="A133" t="s">
         <v>681</v>
       </c>
@@ -7713,7 +7728,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
+    <row r="134" spans="1:3">
       <c r="A134" t="s">
         <v>528</v>
       </c>
@@ -7721,7 +7736,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:3">
       <c r="A136" t="s">
         <v>517</v>
       </c>
@@ -7729,15 +7744,18 @@
         <v>518</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:3">
       <c r="A137" t="s">
         <v>260</v>
       </c>
       <c r="B137" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="138" spans="1:2" ht="13.5" customHeight="1">
+      <c r="C137" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" ht="13.5" customHeight="1">
       <c r="A138" t="s">
         <v>262</v>
       </c>
@@ -7745,7 +7763,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="139" spans="1:2">
+    <row r="139" spans="1:3">
       <c r="A139" t="s">
         <v>261</v>
       </c>
@@ -7753,7 +7771,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="140" spans="1:2">
+    <row r="140" spans="1:3">
       <c r="A140" t="s">
         <v>266</v>
       </c>
@@ -7761,7 +7779,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="141" spans="1:2">
+    <row r="141" spans="1:3">
       <c r="A141" t="s">
         <v>267</v>
       </c>
@@ -7769,15 +7787,18 @@
         <v>268</v>
       </c>
     </row>
-    <row r="142" spans="1:2">
+    <row r="142" spans="1:3">
       <c r="A142" t="s">
         <v>270</v>
       </c>
       <c r="B142" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="143" spans="1:2">
+      <c r="C142" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
       <c r="A143" t="s">
         <v>506</v>
       </c>
@@ -7785,7 +7806,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
+    <row r="144" spans="1:3">
       <c r="A144" t="s">
         <v>271</v>
       </c>
@@ -7824,6 +7845,9 @@
       <c r="B148" t="s">
         <v>286</v>
       </c>
+      <c r="C148" t="s">
+        <v>684</v>
+      </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
@@ -7840,6 +7864,9 @@
       <c r="B150" t="s">
         <v>285</v>
       </c>
+      <c r="C150" t="s">
+        <v>684</v>
+      </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
@@ -7896,6 +7923,9 @@
       <c r="B158" t="s">
         <v>297</v>
       </c>
+      <c r="C158" t="s">
+        <v>608</v>
+      </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
@@ -7916,7 +7946,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
+    <row r="161" spans="1:3">
       <c r="A161" t="s">
         <v>295</v>
       </c>
@@ -7924,7 +7954,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="162" spans="1:2">
+    <row r="162" spans="1:3">
       <c r="A162" t="s">
         <v>296</v>
       </c>
@@ -7932,7 +7962,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
+    <row r="163" spans="1:3">
       <c r="A163" t="s">
         <v>304</v>
       </c>
@@ -7940,7 +7970,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="164" spans="1:2">
+    <row r="164" spans="1:3">
       <c r="A164" t="s">
         <v>310</v>
       </c>
@@ -7948,7 +7978,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:3">
       <c r="A165" t="s">
         <v>307</v>
       </c>
@@ -7956,7 +7986,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:3">
       <c r="A166" t="s">
         <v>308</v>
       </c>
@@ -7964,7 +7994,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:3">
       <c r="A167" t="s">
         <v>312</v>
       </c>
@@ -7972,7 +8002,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="168" spans="1:2">
+    <row r="168" spans="1:3">
       <c r="A168" t="s">
         <v>541</v>
       </c>
@@ -7980,7 +8010,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
+    <row r="170" spans="1:3">
       <c r="A170" t="s">
         <v>521</v>
       </c>
@@ -7988,15 +8018,18 @@
         <v>522</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
+    <row r="171" spans="1:3">
       <c r="A171" t="s">
         <v>501</v>
       </c>
       <c r="B171" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="172" spans="1:2">
+      <c r="C171" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
       <c r="A172" t="s">
         <v>508</v>
       </c>
@@ -8004,15 +8037,18 @@
         <v>592</v>
       </c>
     </row>
-    <row r="173" spans="1:2">
+    <row r="173" spans="1:3">
       <c r="A173" t="s">
         <v>316</v>
       </c>
       <c r="B173" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="174" spans="1:2">
+      <c r="C173" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
       <c r="A174" t="s">
         <v>317</v>
       </c>
@@ -8020,7 +8056,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
+    <row r="175" spans="1:3">
       <c r="A175" t="s">
         <v>318</v>
       </c>
@@ -8028,7 +8064,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
+    <row r="176" spans="1:3">
       <c r="A176" t="s">
         <v>319</v>
       </c>
@@ -8036,7 +8072,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="177" spans="1:2">
+    <row r="177" spans="1:3">
       <c r="A177" t="s">
         <v>320</v>
       </c>
@@ -8044,15 +8080,18 @@
         <v>249</v>
       </c>
     </row>
-    <row r="178" spans="1:2">
+    <row r="178" spans="1:3">
       <c r="A178" t="s">
         <v>325</v>
       </c>
       <c r="B178" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="179" spans="1:2">
+      <c r="C178" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
       <c r="A179" t="s">
         <v>327</v>
       </c>
@@ -8060,7 +8099,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="180" spans="1:2">
+    <row r="180" spans="1:3">
       <c r="A180" t="s">
         <v>330</v>
       </c>
@@ -8068,7 +8107,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="181" spans="1:2">
+    <row r="181" spans="1:3">
       <c r="A181" t="s">
         <v>331</v>
       </c>
@@ -8076,7 +8115,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="182" spans="1:2">
+    <row r="182" spans="1:3">
       <c r="A182" t="s">
         <v>333</v>
       </c>
@@ -8084,7 +8123,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="183" spans="1:2">
+    <row r="183" spans="1:3">
       <c r="A183" t="s">
         <v>540</v>
       </c>
@@ -8092,7 +8131,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="185" spans="1:2">
+    <row r="185" spans="1:3">
       <c r="A185" t="s">
         <v>523</v>
       </c>
@@ -8100,15 +8139,18 @@
         <v>524</v>
       </c>
     </row>
-    <row r="186" spans="1:2">
+    <row r="186" spans="1:3">
       <c r="A186" t="s">
         <v>503</v>
       </c>
       <c r="B186" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="187" spans="1:2">
+      <c r="C186" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
       <c r="A187" t="s">
         <v>509</v>
       </c>
@@ -8116,15 +8158,18 @@
         <v>593</v>
       </c>
     </row>
-    <row r="188" spans="1:2">
+    <row r="188" spans="1:3">
       <c r="A188" t="s">
         <v>337</v>
       </c>
       <c r="B188" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="189" spans="1:2">
+      <c r="C188" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3">
       <c r="A189" t="s">
         <v>338</v>
       </c>
@@ -8132,7 +8177,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="190" spans="1:2">
+    <row r="190" spans="1:3">
       <c r="A190" t="s">
         <v>502</v>
       </c>
@@ -8140,7 +8185,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="191" spans="1:2">
+    <row r="191" spans="1:3">
       <c r="A191" t="s">
         <v>345</v>
       </c>
@@ -8148,7 +8193,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="192" spans="1:2">
+    <row r="192" spans="1:3">
       <c r="A192" t="s">
         <v>346</v>
       </c>
@@ -8233,6 +8278,9 @@
       <c r="B202" t="s">
         <v>353</v>
       </c>
+      <c r="C202" t="s">
+        <v>608</v>
+      </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" t="s">
@@ -8383,6 +8431,9 @@
       <c r="B221" t="s">
         <v>402</v>
       </c>
+      <c r="C221" t="s">
+        <v>608</v>
+      </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" t="s">
@@ -8399,6 +8450,9 @@
       <c r="B223" t="s">
         <v>403</v>
       </c>
+      <c r="C223" t="s">
+        <v>608</v>
+      </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" t="s">
@@ -8490,6 +8544,9 @@
       <c r="B235" t="s">
         <v>424</v>
       </c>
+      <c r="C235" t="s">
+        <v>608</v>
+      </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" t="s">
@@ -8517,6 +8574,9 @@
       <c r="B238" t="s">
         <v>426</v>
       </c>
+      <c r="C238" t="s">
+        <v>608</v>
+      </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239" t="s">
@@ -8613,6 +8673,9 @@
       <c r="B251" t="s">
         <v>451</v>
       </c>
+      <c r="C251" t="s">
+        <v>608</v>
+      </c>
     </row>
     <row r="252" spans="1:3">
       <c r="A252" t="s">
@@ -8640,6 +8703,9 @@
       <c r="B254" t="s">
         <v>453</v>
       </c>
+      <c r="C254" t="s">
+        <v>608</v>
+      </c>
     </row>
     <row r="255" spans="1:3">
       <c r="A255" t="s">
@@ -8657,7 +8723,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="257" spans="1:2">
+    <row r="257" spans="1:3">
       <c r="A257" t="s">
         <v>445</v>
       </c>
@@ -8665,7 +8731,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="258" spans="1:2">
+    <row r="258" spans="1:3">
       <c r="A258" t="s">
         <v>446</v>
       </c>
@@ -8673,7 +8739,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="259" spans="1:2">
+    <row r="259" spans="1:3">
       <c r="A259" t="s">
         <v>447</v>
       </c>
@@ -8681,7 +8747,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="260" spans="1:2">
+    <row r="260" spans="1:3">
       <c r="A260" t="s">
         <v>448</v>
       </c>
@@ -8689,7 +8755,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="261" spans="1:2">
+    <row r="261" spans="1:3">
       <c r="A261" t="s">
         <v>449</v>
       </c>
@@ -8697,7 +8763,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="262" spans="1:2">
+    <row r="262" spans="1:3">
       <c r="A262" t="s">
         <v>533</v>
       </c>
@@ -8705,7 +8771,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="263" spans="1:2">
+    <row r="263" spans="1:3">
       <c r="A263" t="s">
         <v>644</v>
       </c>
@@ -8713,7 +8779,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="265" spans="1:2">
+    <row r="265" spans="1:3">
       <c r="A265" t="s">
         <v>433</v>
       </c>
@@ -8721,15 +8787,18 @@
         <v>645</v>
       </c>
     </row>
-    <row r="266" spans="1:2">
+    <row r="266" spans="1:3">
       <c r="A266" t="s">
         <v>434</v>
       </c>
       <c r="B266" t="s">
         <v>646</v>
       </c>
-    </row>
-    <row r="267" spans="1:2">
+      <c r="C266" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3">
       <c r="A267" t="s">
         <v>513</v>
       </c>
@@ -8737,7 +8806,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="268" spans="1:2">
+    <row r="268" spans="1:3">
       <c r="A268" t="s">
         <v>435</v>
       </c>
@@ -8745,7 +8814,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="269" spans="1:2">
+    <row r="269" spans="1:3">
       <c r="A269" t="s">
         <v>436</v>
       </c>
@@ -8753,7 +8822,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="270" spans="1:2">
+    <row r="270" spans="1:3">
       <c r="A270" t="s">
         <v>437</v>
       </c>
@@ -8761,7 +8830,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="271" spans="1:2">
+    <row r="271" spans="1:3">
       <c r="A271" t="s">
         <v>532</v>
       </c>

</xml_diff>

<commit_message>
Updated code for ICW and VOE
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.malyala\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raluca.ilinca\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68F9266-607D-4D66-AAEC-09BDE3A7F02F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09ABBF56-1323-4089-BB4F-4999DAD33CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="22440" windowHeight="11715" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="832" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="688">
   <si>
     <t>Name</t>
   </si>
@@ -2095,6 +2095,15 @@
   </si>
   <si>
     <t>removed this check</t>
+  </si>
+  <si>
+    <t>TotalAssetLimit</t>
+  </si>
+  <si>
+    <t>ICW_AssetsOver52787</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assets exceed the asset limit, manual review is required. </t>
   </si>
 </sst>
 </file>
@@ -5388,8 +5397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1011"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5724,7 +5733,14 @@
         <v>673</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A38" t="s">
+        <v>685</v>
+      </c>
+      <c r="B38" t="s">
+        <v>685</v>
+      </c>
+    </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
@@ -6706,10 +6722,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
-  <dimension ref="A1:C271"/>
+  <dimension ref="A1:C272"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A246" workbookViewId="0">
-      <selection activeCell="B272" sqref="B272"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6794,234 +6810,231 @@
         <v>554</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>182</v>
-      </c>
-      <c r="B13" t="s">
-        <v>183</v>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>686</v>
+      </c>
+      <c r="B12" t="s">
+        <v>687</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>182</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>578</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>579</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>578</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>579</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B17" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>197</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>198</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B19" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>84</v>
+        <v>199</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>655</v>
+        <v>89</v>
       </c>
       <c r="B24" t="s">
-        <v>656</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>679</v>
+        <v>655</v>
       </c>
       <c r="B25" t="s">
-        <v>680</v>
+        <v>656</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
+        <v>679</v>
+      </c>
+      <c r="B26" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
         <v>551</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>555</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>184</v>
-      </c>
-      <c r="B28" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>91</v>
+        <v>184</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>186</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B35" t="s">
-        <v>99</v>
-      </c>
-      <c r="C35" t="s">
-        <v>608</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B36" t="s">
-        <v>100</v>
+        <v>99</v>
+      </c>
+      <c r="C36" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>657</v>
+        <v>106</v>
       </c>
       <c r="B37" t="s">
-        <v>658</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
+        <v>657</v>
+      </c>
+      <c r="B38" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
         <v>550</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>556</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" t="s">
-        <v>185</v>
-      </c>
-      <c r="B40" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>107</v>
+        <v>185</v>
       </c>
       <c r="B41" t="s">
-        <v>108</v>
-      </c>
-      <c r="C41" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B42" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C42" t="s">
         <v>608</v>
@@ -7029,10 +7042,10 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B43" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C43" t="s">
         <v>608</v>
@@ -7040,10 +7053,10 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B44" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="C44" t="s">
         <v>608</v>
@@ -7051,10 +7064,10 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C45" t="s">
         <v>608</v>
@@ -7062,10 +7075,10 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C46" t="s">
         <v>608</v>
@@ -7073,184 +7086,184 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B47" t="s">
-        <v>112</v>
+        <v>111</v>
+      </c>
+      <c r="C47" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>205</v>
+        <v>116</v>
       </c>
       <c r="B48" t="s">
-        <v>496</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B49" t="s">
-        <v>612</v>
-      </c>
-      <c r="C49" t="s">
-        <v>608</v>
+        <v>496</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>599</v>
+        <v>206</v>
       </c>
       <c r="B50" t="s">
-        <v>613</v>
+        <v>612</v>
+      </c>
+      <c r="C50" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>552</v>
+        <v>599</v>
       </c>
       <c r="B51" t="s">
-        <v>553</v>
+        <v>613</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>574</v>
+        <v>552</v>
       </c>
       <c r="B52" t="s">
-        <v>654</v>
+        <v>553</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
+        <v>574</v>
+      </c>
+      <c r="B53" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
         <v>549</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>614</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" t="s">
-        <v>159</v>
-      </c>
-      <c r="B55" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>122</v>
+        <v>159</v>
       </c>
       <c r="B56" t="s">
-        <v>615</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B57" t="s">
-        <v>123</v>
+        <v>615</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>659</v>
+        <v>124</v>
       </c>
       <c r="B58" t="s">
-        <v>660</v>
+        <v>123</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
+        <v>659</v>
+      </c>
+      <c r="B59" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
         <v>548</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B60" t="s">
         <v>557</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" t="s">
-        <v>187</v>
-      </c>
-      <c r="B61" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>125</v>
+        <v>187</v>
       </c>
       <c r="B62" t="s">
-        <v>127</v>
+        <v>188</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B63" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="B64" t="s">
-        <v>616</v>
+        <v>128</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B65" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B66" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B67" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B68" t="s">
-        <v>497</v>
+        <v>619</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B69" t="s">
-        <v>499</v>
-      </c>
-      <c r="C69" t="s">
-        <v>575</v>
+        <v>497</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B70" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C70" t="s">
         <v>575</v>
@@ -7258,288 +7271,288 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>661</v>
+        <v>145</v>
       </c>
       <c r="B71" t="s">
-        <v>662</v>
+        <v>500</v>
+      </c>
+      <c r="C71" t="s">
+        <v>575</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
+        <v>661</v>
+      </c>
+      <c r="B72" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
         <v>547</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B73" t="s">
         <v>558</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" t="s">
-        <v>148</v>
-      </c>
-      <c r="B74" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B75" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B76" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B77" t="s">
-        <v>600</v>
-      </c>
-      <c r="C77" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B78" t="s">
-        <v>130</v>
+        <v>600</v>
+      </c>
+      <c r="C78" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="B79" t="s">
-        <v>620</v>
+        <v>130</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B80" t="s">
-        <v>131</v>
+        <v>620</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>663</v>
+        <v>133</v>
       </c>
       <c r="B81" t="s">
-        <v>664</v>
+        <v>131</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
+        <v>663</v>
+      </c>
+      <c r="B82" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
         <v>546</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B83" t="s">
         <v>559</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" t="s">
-        <v>189</v>
-      </c>
-      <c r="B84" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>134</v>
+        <v>189</v>
       </c>
       <c r="B85" t="s">
-        <v>154</v>
+        <v>190</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B86" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B87" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B88" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B89" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>652</v>
+        <v>138</v>
       </c>
       <c r="B90" t="s">
-        <v>653</v>
+        <v>158</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>665</v>
+        <v>652</v>
       </c>
       <c r="B91" t="s">
-        <v>666</v>
+        <v>653</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
+        <v>665</v>
+      </c>
+      <c r="B92" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
         <v>545</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B93" t="s">
         <v>560</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" t="s">
-        <v>160</v>
-      </c>
-      <c r="B94" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B95" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B96" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B97" t="s">
-        <v>621</v>
+        <v>166</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>576</v>
+        <v>163</v>
       </c>
       <c r="B98" t="s">
-        <v>577</v>
+        <v>621</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>671</v>
+        <v>576</v>
       </c>
       <c r="B99" t="s">
-        <v>672</v>
+        <v>577</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
+        <v>671</v>
+      </c>
+      <c r="B100" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="s">
         <v>544</v>
       </c>
-      <c r="B100" t="s">
+      <c r="B101" t="s">
         <v>622</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3">
-      <c r="A102" t="s">
-        <v>193</v>
-      </c>
-      <c r="B102" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
       <c r="B103" t="s">
-        <v>169</v>
+        <v>194</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B104" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>667</v>
+        <v>168</v>
       </c>
       <c r="B105" t="s">
-        <v>668</v>
+        <v>170</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
+        <v>667</v>
+      </c>
+      <c r="B106" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" t="s">
         <v>543</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B107" t="s">
         <v>561</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
-      <c r="A108" t="s">
-        <v>191</v>
-      </c>
-      <c r="B108" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="B109" t="s">
-        <v>173</v>
-      </c>
-      <c r="C109" t="s">
-        <v>608</v>
+        <v>192</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="B110" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C110" t="s">
         <v>608</v>
@@ -7547,10 +7560,10 @@
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B111" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C111" t="s">
         <v>608</v>
@@ -7558,437 +7571,440 @@
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>204</v>
+        <v>172</v>
       </c>
       <c r="B112" t="s">
-        <v>203</v>
+        <v>175</v>
+      </c>
+      <c r="C112" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B113" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>177</v>
+        <v>201</v>
       </c>
       <c r="B114" t="s">
-        <v>178</v>
-      </c>
-      <c r="C114" t="s">
-        <v>608</v>
+        <v>202</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>669</v>
+        <v>177</v>
       </c>
       <c r="B115" t="s">
-        <v>670</v>
+        <v>178</v>
+      </c>
+      <c r="C115" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
+        <v>669</v>
+      </c>
+      <c r="B116" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" t="s">
         <v>530</v>
       </c>
-      <c r="B116" t="s">
+      <c r="B117" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="118" spans="1:3">
-      <c r="A118" t="s">
+    <row r="119" spans="1:3">
+      <c r="A119" t="s">
         <v>676</v>
       </c>
-      <c r="B118" t="s">
+      <c r="B119" t="s">
         <v>677</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C119" t="s">
         <v>678</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3">
-      <c r="A120" t="s">
-        <v>515</v>
-      </c>
-      <c r="B120" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>243</v>
+        <v>515</v>
       </c>
       <c r="B121" t="s">
-        <v>244</v>
-      </c>
-      <c r="C121" t="s">
-        <v>608</v>
+        <v>516</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B122" t="s">
-        <v>246</v>
+        <v>244</v>
+      </c>
+      <c r="C122" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="B123" t="s">
-        <v>580</v>
-      </c>
-      <c r="C123" t="s">
-        <v>674</v>
+        <v>246</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="B124" t="s">
-        <v>247</v>
+        <v>580</v>
+      </c>
+      <c r="C124" t="s">
+        <v>674</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>505</v>
+        <v>248</v>
       </c>
       <c r="B125" t="s">
-        <v>514</v>
+        <v>247</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>250</v>
+        <v>505</v>
       </c>
       <c r="B126" t="s">
-        <v>249</v>
+        <v>514</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B127" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B128" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B129" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B130" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>303</v>
+        <v>258</v>
       </c>
       <c r="B131" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>350</v>
+        <v>303</v>
       </c>
       <c r="B132" t="s">
-        <v>351</v>
+        <v>249</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>681</v>
+        <v>350</v>
       </c>
       <c r="B133" t="s">
-        <v>682</v>
+        <v>351</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
+        <v>681</v>
+      </c>
+      <c r="B134" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" t="s">
         <v>528</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B135" t="s">
         <v>529</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3">
-      <c r="A136" t="s">
-        <v>517</v>
-      </c>
-      <c r="B136" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
+        <v>517</v>
+      </c>
+      <c r="B137" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" t="s">
         <v>260</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B138" t="s">
         <v>263</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C138" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A138" t="s">
+    <row r="139" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A139" t="s">
         <v>262</v>
       </c>
-      <c r="B138" t="s">
+      <c r="B139" t="s">
         <v>581</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3">
-      <c r="A139" t="s">
-        <v>261</v>
-      </c>
-      <c r="B139" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B140" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B141" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B142" t="s">
-        <v>269</v>
-      </c>
-      <c r="C142" t="s">
-        <v>684</v>
+        <v>268</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>506</v>
+        <v>270</v>
       </c>
       <c r="B143" t="s">
-        <v>590</v>
+        <v>269</v>
+      </c>
+      <c r="C143" t="s">
+        <v>684</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>271</v>
+        <v>506</v>
       </c>
       <c r="B144" t="s">
-        <v>272</v>
+        <v>590</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B145" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B146" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B147" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B148" t="s">
-        <v>286</v>
-      </c>
-      <c r="C148" t="s">
-        <v>684</v>
+        <v>287</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B149" t="s">
-        <v>627</v>
+        <v>286</v>
+      </c>
+      <c r="C149" t="s">
+        <v>684</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B150" t="s">
-        <v>285</v>
-      </c>
-      <c r="C150" t="s">
-        <v>684</v>
+        <v>627</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B151" t="s">
-        <v>284</v>
+        <v>285</v>
+      </c>
+      <c r="C151" t="s">
+        <v>684</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
       <c r="B152" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B153" t="s">
-        <v>249</v>
+        <v>301</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B154" t="s">
-        <v>306</v>
+        <v>249</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
+        <v>305</v>
+      </c>
+      <c r="B155" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" t="s">
         <v>542</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B156" t="s">
         <v>562</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3">
-      <c r="A157" t="s">
-        <v>519</v>
-      </c>
-      <c r="B157" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
-        <v>293</v>
+        <v>519</v>
       </c>
       <c r="B158" t="s">
-        <v>297</v>
-      </c>
-      <c r="C158" t="s">
-        <v>608</v>
+        <v>520</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
-        <v>507</v>
+        <v>293</v>
       </c>
       <c r="B159" t="s">
-        <v>591</v>
+        <v>297</v>
+      </c>
+      <c r="C159" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" t="s">
-        <v>294</v>
+        <v>507</v>
       </c>
       <c r="B160" t="s">
-        <v>298</v>
-      </c>
-      <c r="C160" t="s">
-        <v>608</v>
+        <v>591</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B161" t="s">
-        <v>299</v>
+        <v>298</v>
+      </c>
+      <c r="C161" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B162" t="s">
-        <v>582</v>
+        <v>299</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B163" t="s">
-        <v>249</v>
+        <v>582</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="B164" t="s">
-        <v>311</v>
+        <v>249</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B165" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B166" t="s">
         <v>309</v>
@@ -7996,583 +8012,580 @@
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B167" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
+        <v>312</v>
+      </c>
+      <c r="B168" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
+      <c r="A169" t="s">
         <v>541</v>
       </c>
-      <c r="B168" t="s">
+      <c r="B169" t="s">
         <v>563</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3">
-      <c r="A170" t="s">
-        <v>521</v>
-      </c>
-      <c r="B170" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>501</v>
+        <v>521</v>
       </c>
       <c r="B171" t="s">
-        <v>321</v>
-      </c>
-      <c r="C171" t="s">
-        <v>608</v>
+        <v>522</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B172" t="s">
-        <v>592</v>
+        <v>321</v>
+      </c>
+      <c r="C172" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
-        <v>316</v>
+        <v>508</v>
       </c>
       <c r="B173" t="s">
-        <v>322</v>
-      </c>
-      <c r="C173" t="s">
-        <v>608</v>
+        <v>592</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B174" t="s">
-        <v>323</v>
+        <v>322</v>
+      </c>
+      <c r="C174" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B175" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B176" t="s">
-        <v>583</v>
+        <v>324</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B177" t="s">
-        <v>249</v>
+        <v>583</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="B178" t="s">
-        <v>326</v>
-      </c>
-      <c r="C178" t="s">
-        <v>608</v>
+        <v>249</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B179" t="s">
-        <v>328</v>
+        <v>326</v>
+      </c>
+      <c r="C179" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B180" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B181" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B182" t="s">
-        <v>257</v>
+        <v>332</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" t="s">
+        <v>333</v>
+      </c>
+      <c r="B183" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3">
+      <c r="A184" t="s">
         <v>540</v>
       </c>
-      <c r="B183" t="s">
+      <c r="B184" t="s">
         <v>564</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3">
-      <c r="A185" t="s">
-        <v>523</v>
-      </c>
-      <c r="B185" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="s">
-        <v>503</v>
+        <v>523</v>
       </c>
       <c r="B186" t="s">
-        <v>339</v>
-      </c>
-      <c r="C186" t="s">
-        <v>608</v>
+        <v>524</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="B187" t="s">
-        <v>593</v>
+        <v>339</v>
+      </c>
+      <c r="C187" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" t="s">
-        <v>337</v>
+        <v>509</v>
       </c>
       <c r="B188" t="s">
-        <v>340</v>
-      </c>
-      <c r="C188" t="s">
-        <v>608</v>
+        <v>593</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B189" t="s">
-        <v>341</v>
+        <v>340</v>
+      </c>
+      <c r="C189" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190" t="s">
-        <v>502</v>
+        <v>338</v>
       </c>
       <c r="B190" t="s">
-        <v>584</v>
+        <v>341</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" t="s">
-        <v>345</v>
+        <v>502</v>
       </c>
       <c r="B191" t="s">
-        <v>249</v>
+        <v>584</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B192" t="s">
-        <v>342</v>
+        <v>249</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B193" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B194" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B195" t="s">
-        <v>257</v>
+        <v>344</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
+        <v>349</v>
+      </c>
+      <c r="B196" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3">
+      <c r="A197" t="s">
         <v>539</v>
       </c>
-      <c r="B196" t="s">
+      <c r="B197" t="s">
         <v>565</v>
-      </c>
-    </row>
-    <row r="198" spans="1:3">
-      <c r="A198" t="s">
-        <v>570</v>
-      </c>
-      <c r="B198" t="s">
-        <v>573</v>
-      </c>
-      <c r="C198" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B199" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="C199" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>605</v>
+        <v>571</v>
       </c>
       <c r="B200" t="s">
-        <v>623</v>
+        <v>572</v>
+      </c>
+      <c r="C200" t="s">
+        <v>607</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" t="s">
-        <v>366</v>
+        <v>605</v>
       </c>
       <c r="B201" t="s">
-        <v>352</v>
+        <v>623</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B202" t="s">
-        <v>353</v>
-      </c>
-      <c r="C202" t="s">
-        <v>608</v>
+        <v>352</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" t="s">
-        <v>510</v>
+        <v>367</v>
       </c>
       <c r="B203" t="s">
-        <v>594</v>
+        <v>353</v>
+      </c>
+      <c r="C203" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
-        <v>368</v>
+        <v>510</v>
       </c>
       <c r="B204" t="s">
-        <v>354</v>
+        <v>594</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B205" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B206" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B207" t="s">
-        <v>357</v>
-      </c>
-      <c r="C207" t="s">
-        <v>608</v>
+        <v>356</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B208" t="s">
-        <v>358</v>
+        <v>357</v>
+      </c>
+      <c r="C208" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B209" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B210" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B211" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B212" t="s">
-        <v>362</v>
-      </c>
-      <c r="C212" t="s">
-        <v>608</v>
+        <v>361</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B213" t="s">
-        <v>363</v>
+        <v>362</v>
+      </c>
+      <c r="C213" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B214" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B215" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" t="s">
+        <v>379</v>
+      </c>
+      <c r="B216" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3">
+      <c r="A217" t="s">
         <v>538</v>
       </c>
-      <c r="B216" t="s">
+      <c r="B217" t="s">
         <v>566</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3">
-      <c r="A218" t="s">
-        <v>628</v>
-      </c>
-      <c r="B218" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219" t="s">
-        <v>386</v>
+        <v>628</v>
       </c>
       <c r="B219" t="s">
-        <v>404</v>
+        <v>629</v>
       </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B220" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B221" t="s">
-        <v>402</v>
-      </c>
-      <c r="C221" t="s">
-        <v>608</v>
+        <v>401</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" t="s">
-        <v>511</v>
+        <v>388</v>
       </c>
       <c r="B222" t="s">
-        <v>595</v>
+        <v>402</v>
+      </c>
+      <c r="C222" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="223" spans="1:3">
       <c r="A223" t="s">
-        <v>405</v>
+        <v>511</v>
       </c>
       <c r="B223" t="s">
-        <v>403</v>
-      </c>
-      <c r="C223" t="s">
-        <v>608</v>
+        <v>595</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" t="s">
-        <v>389</v>
+        <v>405</v>
       </c>
       <c r="B224" t="s">
-        <v>395</v>
+        <v>403</v>
+      </c>
+      <c r="C224" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" t="s">
-        <v>406</v>
+        <v>389</v>
       </c>
       <c r="B225" t="s">
-        <v>396</v>
-      </c>
-      <c r="C225" t="s">
-        <v>585</v>
+        <v>395</v>
       </c>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" t="s">
-        <v>390</v>
+        <v>406</v>
       </c>
       <c r="B226" t="s">
-        <v>397</v>
+        <v>396</v>
+      </c>
+      <c r="C226" t="s">
+        <v>585</v>
       </c>
     </row>
     <row r="227" spans="1:3">
       <c r="A227" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B227" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B228" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B229" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B230" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
     </row>
     <row r="231" spans="1:3">
       <c r="A231" t="s">
+        <v>394</v>
+      </c>
+      <c r="B231" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3">
+      <c r="A232" t="s">
         <v>537</v>
       </c>
-      <c r="B231" t="s">
+      <c r="B232" t="s">
         <v>567</v>
-      </c>
-    </row>
-    <row r="233" spans="1:3">
-      <c r="A233" t="s">
-        <v>525</v>
-      </c>
-      <c r="B233" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" t="s">
-        <v>412</v>
+        <v>525</v>
       </c>
       <c r="B234" t="s">
-        <v>423</v>
+        <v>526</v>
       </c>
     </row>
     <row r="235" spans="1:3">
       <c r="A235" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B235" t="s">
-        <v>424</v>
-      </c>
-      <c r="C235" t="s">
-        <v>608</v>
+        <v>423</v>
       </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" t="s">
-        <v>596</v>
+        <v>413</v>
       </c>
       <c r="B236" t="s">
-        <v>597</v>
+        <v>424</v>
+      </c>
+      <c r="C236" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" t="s">
-        <v>414</v>
+        <v>596</v>
       </c>
       <c r="B237" t="s">
-        <v>425</v>
-      </c>
-      <c r="C237" t="s">
-        <v>608</v>
+        <v>597</v>
       </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B238" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C238" t="s">
         <v>608</v>
@@ -8580,128 +8593,128 @@
     </row>
     <row r="239" spans="1:3">
       <c r="A239" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B239" t="s">
-        <v>609</v>
+        <v>426</v>
+      </c>
+      <c r="C239" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="240" spans="1:3">
       <c r="A240" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B240" t="s">
-        <v>427</v>
+        <v>609</v>
       </c>
     </row>
     <row r="241" spans="1:3">
       <c r="A241" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B241" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B242" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="243" spans="1:3">
       <c r="A243" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B243" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="244" spans="1:3">
       <c r="A244" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B244" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="245" spans="1:3">
       <c r="A245" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B245" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="246" spans="1:3">
       <c r="A246" t="s">
-        <v>534</v>
+        <v>422</v>
       </c>
       <c r="B246" t="s">
-        <v>535</v>
+        <v>432</v>
       </c>
     </row>
     <row r="247" spans="1:3">
       <c r="A247" t="s">
+        <v>534</v>
+      </c>
+      <c r="B247" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3">
+      <c r="A248" t="s">
         <v>637</v>
       </c>
-      <c r="B247" t="s">
+      <c r="B248" t="s">
         <v>638</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3">
-      <c r="A249" t="s">
-        <v>527</v>
-      </c>
-      <c r="B249" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="250" spans="1:3">
       <c r="A250" t="s">
-        <v>439</v>
+        <v>527</v>
       </c>
       <c r="B250" t="s">
-        <v>450</v>
+        <v>526</v>
       </c>
     </row>
     <row r="251" spans="1:3">
       <c r="A251" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B251" t="s">
-        <v>451</v>
-      </c>
-      <c r="C251" t="s">
-        <v>608</v>
+        <v>450</v>
       </c>
     </row>
     <row r="252" spans="1:3">
       <c r="A252" t="s">
-        <v>512</v>
+        <v>440</v>
       </c>
       <c r="B252" t="s">
-        <v>598</v>
+        <v>451</v>
+      </c>
+      <c r="C252" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="253" spans="1:3">
       <c r="A253" t="s">
-        <v>441</v>
+        <v>512</v>
       </c>
       <c r="B253" t="s">
-        <v>452</v>
-      </c>
-      <c r="C253" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
     </row>
     <row r="254" spans="1:3">
       <c r="A254" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B254" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C254" t="s">
         <v>608</v>
@@ -8709,132 +8722,143 @@
     </row>
     <row r="255" spans="1:3">
       <c r="A255" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B255" t="s">
-        <v>610</v>
+        <v>453</v>
+      </c>
+      <c r="C255" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="256" spans="1:3">
       <c r="A256" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B256" t="s">
-        <v>427</v>
+        <v>610</v>
       </c>
     </row>
     <row r="257" spans="1:3">
       <c r="A257" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B257" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="258" spans="1:3">
       <c r="A258" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B258" t="s">
-        <v>454</v>
+        <v>428</v>
       </c>
     </row>
     <row r="259" spans="1:3">
       <c r="A259" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B259" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="260" spans="1:3">
       <c r="A260" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B260" t="s">
-        <v>431</v>
+        <v>455</v>
       </c>
     </row>
     <row r="261" spans="1:3">
       <c r="A261" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B261" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="262" spans="1:3">
       <c r="A262" t="s">
-        <v>533</v>
+        <v>449</v>
       </c>
       <c r="B262" t="s">
-        <v>535</v>
+        <v>432</v>
       </c>
     </row>
     <row r="263" spans="1:3">
       <c r="A263" t="s">
+        <v>533</v>
+      </c>
+      <c r="B263" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3">
+      <c r="A264" t="s">
         <v>644</v>
       </c>
-      <c r="B263" t="s">
+      <c r="B264" t="s">
         <v>638</v>
-      </c>
-    </row>
-    <row r="265" spans="1:3">
-      <c r="A265" t="s">
-        <v>433</v>
-      </c>
-      <c r="B265" t="s">
-        <v>645</v>
       </c>
     </row>
     <row r="266" spans="1:3">
       <c r="A266" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B266" t="s">
-        <v>646</v>
-      </c>
-      <c r="C266" t="s">
-        <v>608</v>
+        <v>645</v>
       </c>
     </row>
     <row r="267" spans="1:3">
       <c r="A267" t="s">
-        <v>513</v>
+        <v>434</v>
       </c>
       <c r="B267" t="s">
-        <v>647</v>
+        <v>646</v>
+      </c>
+      <c r="C267" t="s">
+        <v>608</v>
       </c>
     </row>
     <row r="268" spans="1:3">
       <c r="A268" t="s">
-        <v>435</v>
+        <v>513</v>
       </c>
       <c r="B268" t="s">
-        <v>675</v>
+        <v>647</v>
       </c>
     </row>
     <row r="269" spans="1:3">
       <c r="A269" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B269" t="s">
-        <v>648</v>
+        <v>675</v>
       </c>
     </row>
     <row r="270" spans="1:3">
       <c r="A270" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B270" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="271" spans="1:3">
       <c r="A271" t="s">
+        <v>437</v>
+      </c>
+      <c r="B271" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3">
+      <c r="A272" t="s">
         <v>532</v>
       </c>
-      <c r="B271" t="s">
+      <c r="B272" t="s">
         <v>650</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1040, paystub and SEC change
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.malyala\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4EAD44A-019E-4CC8-9B9B-CC4ECB3AC2C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA791FA-DF4D-4C81-B31A-624C0AD7729F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2265" yWindow="2265" windowWidth="20190" windowHeight="8340" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="694">
   <si>
     <t>Name</t>
   </si>
@@ -1629,15 +1629,9 @@
     <t>PS_FindingError</t>
   </si>
   <si>
-    <t>Errors in Validating findings for Paystub</t>
-  </si>
-  <si>
     <t>SR_FindingError</t>
   </si>
   <si>
-    <t>Errors in Validating findings for Screening Document</t>
-  </si>
-  <si>
     <t>VRCC_FindingError</t>
   </si>
   <si>
@@ -1647,9 +1641,6 @@
     <t>SSBL_FindingError</t>
   </si>
   <si>
-    <t>Errors in Validating findings for Supplemental Security Income Letter</t>
-  </si>
-  <si>
     <t>ICW_FindingError</t>
   </si>
   <si>
@@ -1704,48 +1695,6 @@
     <t>The effective dates on the ICW, Application Summary, and Income &amp; Asset Questionnaire do not match as expected.</t>
   </si>
   <si>
-    <t>Errors in Validating findings for ICW</t>
-  </si>
-  <si>
-    <t>Errors in Validating findings for Application Summary</t>
-  </si>
-  <si>
-    <t>Errors in Validating findings for Member Information Document</t>
-  </si>
-  <si>
-    <t>Errors in Validating findings for Self Certification of Non Employment.</t>
-  </si>
-  <si>
-    <t>Errors in Validating findings for Asset Self Certification &amp; Worksheet</t>
-  </si>
-  <si>
-    <t>Errors in Validating findings for Affidavit of Student Financial Assistance</t>
-  </si>
-  <si>
-    <t>Errors in Validating findings for Student Certification</t>
-  </si>
-  <si>
-    <t>Errors in Validating findings for VAWA Acknowledgement</t>
-  </si>
-  <si>
-    <t>Errors in Validating findings for Verification of Employment</t>
-  </si>
-  <si>
-    <t>Errors in Validating findings for Offer Letter</t>
-  </si>
-  <si>
-    <t>Errors in Validating findings for Work Number</t>
-  </si>
-  <si>
-    <t>Errors in Validating findings for Verification Services</t>
-  </si>
-  <si>
-    <t>Errors in Validating findings for Self-Employment Certification</t>
-  </si>
-  <si>
-    <t>Errors in Validating findings for Child Support Payment History</t>
-  </si>
-  <si>
     <t>ICW_AssetsOver51600</t>
   </si>
   <si>
@@ -1884,9 +1833,6 @@
     <t>Income Types listed on Income &amp; Asset Questionnaire does not match the ICW</t>
   </si>
   <si>
-    <t>Errors in Validating findings for Income &amp; Asset Questionnaire</t>
-  </si>
-  <si>
     <t>Signature is missing from the Self Certification of Non Employment.</t>
   </si>
   <si>
@@ -1908,9 +1854,6 @@
     <t>Date is left blank on the Certification of Zero Income.</t>
   </si>
   <si>
-    <t>Errors in Validating findings for Certification of Zero Income.</t>
-  </si>
-  <si>
     <t>Supporting documents do not exist for Self-Employment Verification</t>
   </si>
   <si>
@@ -1992,9 +1935,6 @@
     <t xml:space="preserve">Verification of Reccurring Cash Contribution has not been dated appropriately. </t>
   </si>
   <si>
-    <t>Errors in Validating findings for Verification of Reccurring Cash Contribution</t>
-  </si>
-  <si>
     <t>LLM_ImageQuality</t>
   </si>
   <si>
@@ -2103,13 +2043,85 @@
     <t>PS_AssetsSavingsCount</t>
   </si>
   <si>
-    <t>Savings Account listed in Paystub do not match the count in ICW</t>
-  </si>
-  <si>
-    <t>Checking Account listed in Paystub do not the count in ICW</t>
-  </si>
-  <si>
     <t>newly added</t>
+  </si>
+  <si>
+    <t>Additional savings accounts have been listed on the Paystub that are not listed on the ICW.</t>
+  </si>
+  <si>
+    <t>Additional checking accounts have been listed on the Paystub that are not listed on the ICW.</t>
+  </si>
+  <si>
+    <t>Unable to validate findings for Self-Employment Certification. Needs manual review.</t>
+  </si>
+  <si>
+    <t>Unable to validate findings for ICW. Needs manual review.</t>
+  </si>
+  <si>
+    <t>Unable to validate findings for Application Summary. Needs manual review.</t>
+  </si>
+  <si>
+    <t>Unable to validate findings for Member Information Document. Needs manual review.</t>
+  </si>
+  <si>
+    <t>Unable to validate findings for Income &amp; Asset Questionnaire. Needs manual review.</t>
+  </si>
+  <si>
+    <t>Errors in Validating findings for Self Certification of Non Employment. Needs manual review.</t>
+  </si>
+  <si>
+    <t>Unable to validate findings for Asset Self Certification &amp; Worksheet. Needs manual review.</t>
+  </si>
+  <si>
+    <t>Unable to validate findings for Affidavit of Student Financial Assistance. Needs manual review.</t>
+  </si>
+  <si>
+    <t>Unable to validate findings for Student Certification. Needs manual review.</t>
+  </si>
+  <si>
+    <t>Errors in Validating findings for Certification of Zero Income. Needs manual review.</t>
+  </si>
+  <si>
+    <t>Unable to validate findings for VAWA Acknowledgement. Needs manual review.</t>
+  </si>
+  <si>
+    <t>Unable to validate findings for Screening Document. Needs manual review.</t>
+  </si>
+  <si>
+    <t>Unable to validate findings for Paystub. Needs manual review.</t>
+  </si>
+  <si>
+    <t>Unable to validate findings for Verification of Employment. Needs manual review.</t>
+  </si>
+  <si>
+    <t>Unable to validate findings for Offer Letter. Needs manual review.</t>
+  </si>
+  <si>
+    <t>Unable to validate findings for Work Number. Needs manual review.</t>
+  </si>
+  <si>
+    <t>Unable to validate findings for Verification Services. Needs manual review.</t>
+  </si>
+  <si>
+    <t>Unable to validate findings for Child Support Payment History. Needs manual review.</t>
+  </si>
+  <si>
+    <t>Unable to validate findings for Supplemental Security Income Letter. Needs manual review.</t>
+  </si>
+  <si>
+    <t>Unable to validate findings for Verification of Reccurring Cash Contribution. Needs manual review.</t>
+  </si>
+  <si>
+    <t>BusinessAskedToRemovePage2check but on different page</t>
+  </si>
+  <si>
+    <t>ICW_AssetsOver52787</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assets exceed the asset limit, manual review is required. </t>
+  </si>
+  <si>
+    <t>TotalAssetsLimit</t>
   </si>
 </sst>
 </file>
@@ -2620,7 +2632,7 @@
         <v>220</v>
       </c>
       <c r="B14" t="s">
-        <v>639</v>
+        <v>620</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
@@ -2658,7 +2670,7 @@
         <v>224</v>
       </c>
       <c r="B18" t="s">
-        <v>636</v>
+        <v>617</v>
       </c>
       <c r="C18" t="s">
         <v>239</v>
@@ -2680,7 +2692,7 @@
         <v>226</v>
       </c>
       <c r="B20" t="s">
-        <v>640</v>
+        <v>621</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
@@ -2696,7 +2708,7 @@
         <v>228</v>
       </c>
       <c r="B22" t="s">
-        <v>641</v>
+        <v>622</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
@@ -2763,7 +2775,7 @@
         <v>380</v>
       </c>
       <c r="B30" t="s">
-        <v>642</v>
+        <v>623</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
@@ -2795,7 +2807,7 @@
         <v>411</v>
       </c>
       <c r="B34" t="s">
-        <v>630</v>
+        <v>611</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
@@ -2843,7 +2855,7 @@
         <v>438</v>
       </c>
       <c r="B40" t="s">
-        <v>643</v>
+        <v>624</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
@@ -4358,10 +4370,10 @@
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>626</v>
+        <v>607</v>
       </c>
       <c r="B21" t="s">
-        <v>626</v>
+        <v>607</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
@@ -5403,8 +5415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1011"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5533,82 +5545,82 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>586</v>
+        <v>569</v>
       </c>
       <c r="B12" t="s">
-        <v>586</v>
+        <v>569</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>587</v>
+        <v>570</v>
       </c>
       <c r="B13" t="s">
-        <v>587</v>
+        <v>570</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>588</v>
+        <v>571</v>
       </c>
       <c r="B14" t="s">
-        <v>588</v>
+        <v>571</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>589</v>
+        <v>572</v>
       </c>
       <c r="B15" t="s">
-        <v>589</v>
+        <v>572</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>631</v>
+        <v>612</v>
       </c>
       <c r="B16" t="s">
-        <v>631</v>
+        <v>612</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
       <c r="B17" t="s">
-        <v>633</v>
+        <v>614</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>635</v>
+        <v>616</v>
       </c>
       <c r="B18" t="s">
-        <v>635</v>
+        <v>616</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>632</v>
+        <v>613</v>
       </c>
       <c r="B19" t="s">
-        <v>632</v>
+        <v>613</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>634</v>
+        <v>615</v>
       </c>
       <c r="B20" t="s">
-        <v>634</v>
+        <v>615</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>651</v>
+        <v>631</v>
       </c>
       <c r="B21" t="s">
-        <v>651</v>
+        <v>631</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1">
@@ -5685,61 +5697,68 @@
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1">
       <c r="A31" s="2" t="s">
-        <v>601</v>
+        <v>584</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>601</v>
+        <v>584</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>603</v>
+        <v>586</v>
       </c>
       <c r="B32" t="s">
-        <v>603</v>
+        <v>586</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
       <c r="A33" s="2" t="s">
-        <v>602</v>
+        <v>585</v>
       </c>
       <c r="B33" t="s">
-        <v>602</v>
+        <v>585</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>604</v>
+        <v>587</v>
       </c>
       <c r="B34" t="s">
-        <v>604</v>
+        <v>587</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>624</v>
+        <v>605</v>
       </c>
       <c r="B35" t="s">
-        <v>624</v>
+        <v>605</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>625</v>
+        <v>606</v>
       </c>
       <c r="B36" t="s">
-        <v>625</v>
+        <v>606</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>673</v>
+        <v>653</v>
       </c>
       <c r="B37" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
+        <v>653</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A38" t="s">
+        <v>693</v>
+      </c>
+      <c r="B38" t="s">
+        <v>693</v>
+      </c>
+    </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
@@ -6721,10 +6740,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
-  <dimension ref="A1:C273"/>
+  <dimension ref="A1:C274"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" workbookViewId="0">
-      <selection activeCell="A122" sqref="A122"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6790,1242 +6809,1245 @@
         <v>208</v>
       </c>
       <c r="C9" t="s">
-        <v>683</v>
+        <v>663</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>568</v>
+        <v>551</v>
       </c>
       <c r="B10" t="s">
-        <v>569</v>
+        <v>552</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>536</v>
+        <v>691</v>
       </c>
       <c r="B11" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
-        <v>182</v>
-      </c>
-      <c r="B13" t="s">
-        <v>183</v>
+        <v>692</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>533</v>
+      </c>
+      <c r="B12" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>182</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>578</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>579</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>561</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>562</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B17" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>197</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>198</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B19" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>84</v>
+        <v>199</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B21" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>655</v>
+        <v>89</v>
       </c>
       <c r="B24" t="s">
-        <v>656</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>679</v>
+        <v>635</v>
       </c>
       <c r="B25" t="s">
-        <v>680</v>
+        <v>636</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>551</v>
+        <v>659</v>
       </c>
       <c r="B26" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
-        <v>184</v>
-      </c>
-      <c r="B28" t="s">
-        <v>186</v>
+        <v>660</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>548</v>
+      </c>
+      <c r="B27" t="s">
+        <v>672</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>91</v>
+        <v>184</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>186</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B35" t="s">
-        <v>99</v>
-      </c>
-      <c r="C35" t="s">
-        <v>608</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B36" t="s">
-        <v>100</v>
+        <v>99</v>
+      </c>
+      <c r="C36" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>657</v>
+        <v>106</v>
       </c>
       <c r="B37" t="s">
-        <v>658</v>
+        <v>100</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>550</v>
+        <v>637</v>
       </c>
       <c r="B38" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" t="s">
-        <v>185</v>
-      </c>
-      <c r="B40" t="s">
-        <v>611</v>
+        <v>638</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>547</v>
+      </c>
+      <c r="B39" t="s">
+        <v>673</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>107</v>
+        <v>185</v>
       </c>
       <c r="B41" t="s">
-        <v>108</v>
-      </c>
-      <c r="C41" t="s">
-        <v>608</v>
+        <v>594</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B42" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C42" t="s">
-        <v>608</v>
+        <v>591</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B43" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C43" t="s">
-        <v>608</v>
+        <v>591</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B44" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="C44" t="s">
-        <v>608</v>
+        <v>591</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B45" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C45" t="s">
-        <v>608</v>
+        <v>591</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B46" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C46" t="s">
-        <v>608</v>
+        <v>591</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B47" t="s">
-        <v>112</v>
+        <v>111</v>
+      </c>
+      <c r="C47" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>205</v>
+        <v>116</v>
       </c>
       <c r="B48" t="s">
-        <v>496</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B49" t="s">
-        <v>612</v>
-      </c>
-      <c r="C49" t="s">
-        <v>608</v>
+        <v>496</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>599</v>
+        <v>206</v>
       </c>
       <c r="B50" t="s">
-        <v>613</v>
+        <v>595</v>
+      </c>
+      <c r="C50" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>552</v>
+        <v>582</v>
       </c>
       <c r="B51" t="s">
-        <v>553</v>
+        <v>596</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>574</v>
+        <v>549</v>
       </c>
       <c r="B52" t="s">
-        <v>654</v>
+        <v>550</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>549</v>
+        <v>557</v>
       </c>
       <c r="B53" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" t="s">
-        <v>159</v>
-      </c>
-      <c r="B55" t="s">
-        <v>121</v>
+        <v>634</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>546</v>
+      </c>
+      <c r="B54" t="s">
+        <v>674</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>122</v>
+        <v>159</v>
       </c>
       <c r="B56" t="s">
-        <v>615</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B57" t="s">
-        <v>123</v>
+        <v>597</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>659</v>
+        <v>124</v>
       </c>
       <c r="B58" t="s">
-        <v>660</v>
+        <v>123</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>548</v>
+        <v>639</v>
       </c>
       <c r="B59" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" t="s">
-        <v>187</v>
-      </c>
-      <c r="B61" t="s">
-        <v>188</v>
+        <v>640</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>545</v>
+      </c>
+      <c r="B60" t="s">
+        <v>675</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>125</v>
+        <v>187</v>
       </c>
       <c r="B62" t="s">
-        <v>127</v>
+        <v>188</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B63" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="B64" t="s">
-        <v>616</v>
+        <v>128</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B65" t="s">
-        <v>617</v>
+        <v>598</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B66" t="s">
-        <v>618</v>
+        <v>599</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B67" t="s">
-        <v>619</v>
+        <v>600</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B68" t="s">
-        <v>497</v>
+        <v>601</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B69" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C69" t="s">
-        <v>575</v>
+        <v>690</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B70" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C70" t="s">
-        <v>575</v>
+        <v>558</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>661</v>
+        <v>145</v>
       </c>
       <c r="B71" t="s">
-        <v>662</v>
+        <v>500</v>
+      </c>
+      <c r="C71" t="s">
+        <v>558</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>547</v>
+        <v>641</v>
       </c>
       <c r="B72" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" t="s">
-        <v>148</v>
-      </c>
-      <c r="B74" t="s">
-        <v>151</v>
+        <v>642</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>544</v>
+      </c>
+      <c r="B73" t="s">
+        <v>676</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B75" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B76" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B77" t="s">
-        <v>600</v>
-      </c>
-      <c r="C77" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B78" t="s">
-        <v>130</v>
+        <v>583</v>
+      </c>
+      <c r="C78" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="B79" t="s">
-        <v>620</v>
+        <v>130</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B80" t="s">
-        <v>131</v>
+        <v>602</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>663</v>
+        <v>133</v>
       </c>
       <c r="B81" t="s">
-        <v>664</v>
+        <v>131</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>546</v>
+        <v>643</v>
       </c>
       <c r="B82" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" t="s">
-        <v>189</v>
-      </c>
-      <c r="B84" t="s">
-        <v>190</v>
+        <v>644</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>543</v>
+      </c>
+      <c r="B83" t="s">
+        <v>677</v>
       </c>
     </row>
     <row r="85" spans="1:2">
       <c r="A85" t="s">
-        <v>134</v>
+        <v>189</v>
       </c>
       <c r="B85" t="s">
-        <v>154</v>
+        <v>190</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B86" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B87" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="88" spans="1:2">
       <c r="A88" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B88" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B89" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>652</v>
+        <v>138</v>
       </c>
       <c r="B90" t="s">
-        <v>653</v>
+        <v>158</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>665</v>
+        <v>632</v>
       </c>
       <c r="B91" t="s">
-        <v>666</v>
+        <v>633</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>545</v>
+        <v>645</v>
       </c>
       <c r="B92" t="s">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" t="s">
-        <v>160</v>
-      </c>
-      <c r="B94" t="s">
-        <v>164</v>
+        <v>646</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>542</v>
+      </c>
+      <c r="B93" t="s">
+        <v>678</v>
       </c>
     </row>
     <row r="95" spans="1:2">
       <c r="A95" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B95" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B96" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B97" t="s">
-        <v>621</v>
+        <v>166</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>576</v>
+        <v>163</v>
       </c>
       <c r="B98" t="s">
-        <v>577</v>
+        <v>603</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>671</v>
+        <v>559</v>
       </c>
       <c r="B99" t="s">
-        <v>672</v>
+        <v>560</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>544</v>
+        <v>651</v>
       </c>
       <c r="B100" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3">
-      <c r="A102" t="s">
-        <v>193</v>
-      </c>
-      <c r="B102" t="s">
-        <v>194</v>
+        <v>652</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="s">
+        <v>541</v>
+      </c>
+      <c r="B101" t="s">
+        <v>679</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
       <c r="B103" t="s">
-        <v>169</v>
+        <v>194</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B104" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>667</v>
+        <v>168</v>
       </c>
       <c r="B105" t="s">
-        <v>668</v>
+        <v>170</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>543</v>
+        <v>647</v>
       </c>
       <c r="B106" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
-      <c r="A108" t="s">
-        <v>191</v>
-      </c>
-      <c r="B108" t="s">
-        <v>192</v>
+        <v>648</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" t="s">
+        <v>540</v>
+      </c>
+      <c r="B107" t="s">
+        <v>680</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="B109" t="s">
-        <v>173</v>
-      </c>
-      <c r="C109" t="s">
-        <v>608</v>
+        <v>192</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="B110" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C110" t="s">
-        <v>608</v>
+        <v>591</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B111" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C111" t="s">
-        <v>608</v>
+        <v>591</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>204</v>
+        <v>172</v>
       </c>
       <c r="B112" t="s">
-        <v>203</v>
+        <v>175</v>
+      </c>
+      <c r="C112" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B113" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>177</v>
+        <v>201</v>
       </c>
       <c r="B114" t="s">
-        <v>178</v>
-      </c>
-      <c r="C114" t="s">
-        <v>608</v>
+        <v>202</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>669</v>
+        <v>177</v>
       </c>
       <c r="B115" t="s">
-        <v>670</v>
+        <v>178</v>
+      </c>
+      <c r="C115" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>530</v>
+        <v>649</v>
       </c>
       <c r="B116" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3">
-      <c r="A118" t="s">
-        <v>676</v>
-      </c>
-      <c r="B118" t="s">
-        <v>677</v>
-      </c>
-      <c r="C118" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3">
-      <c r="A120" t="s">
-        <v>515</v>
-      </c>
-      <c r="B120" t="s">
-        <v>516</v>
+        <v>650</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" t="s">
+        <v>529</v>
+      </c>
+      <c r="B117" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" t="s">
+        <v>656</v>
+      </c>
+      <c r="B119" t="s">
+        <v>657</v>
+      </c>
+      <c r="C119" t="s">
+        <v>658</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>685</v>
+        <v>515</v>
       </c>
       <c r="B121" t="s">
-        <v>688</v>
-      </c>
-      <c r="C121" t="s">
-        <v>689</v>
+        <v>516</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>686</v>
+        <v>665</v>
       </c>
       <c r="B122" t="s">
-        <v>687</v>
+        <v>669</v>
       </c>
       <c r="C122" t="s">
-        <v>689</v>
+        <v>667</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>243</v>
+        <v>666</v>
       </c>
       <c r="B123" t="s">
-        <v>244</v>
+        <v>668</v>
       </c>
       <c r="C123" t="s">
-        <v>608</v>
+        <v>667</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B124" t="s">
-        <v>246</v>
+        <v>244</v>
+      </c>
+      <c r="C124" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
       <c r="B125" t="s">
-        <v>580</v>
-      </c>
-      <c r="C125" t="s">
-        <v>674</v>
+        <v>246</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="B126" t="s">
-        <v>247</v>
+        <v>563</v>
+      </c>
+      <c r="C126" t="s">
+        <v>654</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>505</v>
+        <v>248</v>
       </c>
       <c r="B127" t="s">
-        <v>514</v>
+        <v>247</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>250</v>
+        <v>505</v>
       </c>
       <c r="B128" t="s">
-        <v>249</v>
+        <v>514</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B129" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B130" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B131" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B132" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>303</v>
+        <v>258</v>
       </c>
       <c r="B133" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>350</v>
+        <v>303</v>
       </c>
       <c r="B134" t="s">
-        <v>351</v>
+        <v>249</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>681</v>
+        <v>350</v>
       </c>
       <c r="B135" t="s">
-        <v>682</v>
+        <v>351</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
+        <v>661</v>
+      </c>
+      <c r="B136" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" t="s">
         <v>528</v>
       </c>
-      <c r="B136" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3">
-      <c r="A138" t="s">
-        <v>517</v>
-      </c>
-      <c r="B138" t="s">
-        <v>518</v>
+      <c r="B137" t="s">
+        <v>682</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
+        <v>517</v>
+      </c>
+      <c r="B139" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" t="s">
         <v>260</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B140" t="s">
         <v>263</v>
       </c>
-      <c r="C139" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A140" t="s">
+      <c r="C140" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A141" t="s">
         <v>262</v>
       </c>
-      <c r="B140" t="s">
-        <v>581</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3">
-      <c r="A141" t="s">
-        <v>261</v>
-      </c>
       <c r="B141" t="s">
-        <v>264</v>
+        <v>564</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B142" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B143" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B144" t="s">
-        <v>269</v>
-      </c>
-      <c r="C144" t="s">
-        <v>684</v>
+        <v>268</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>506</v>
+        <v>270</v>
       </c>
       <c r="B145" t="s">
-        <v>590</v>
+        <v>269</v>
+      </c>
+      <c r="C145" t="s">
+        <v>664</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>271</v>
+        <v>506</v>
       </c>
       <c r="B146" t="s">
-        <v>272</v>
+        <v>573</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B147" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B148" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B149" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B150" t="s">
-        <v>286</v>
-      </c>
-      <c r="C150" t="s">
-        <v>684</v>
+        <v>287</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B151" t="s">
-        <v>627</v>
+        <v>286</v>
+      </c>
+      <c r="C151" t="s">
+        <v>664</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B152" t="s">
-        <v>285</v>
-      </c>
-      <c r="C152" t="s">
-        <v>684</v>
+        <v>608</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B153" t="s">
-        <v>284</v>
+        <v>285</v>
+      </c>
+      <c r="C153" t="s">
+        <v>664</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
       <c r="B154" t="s">
-        <v>301</v>
+        <v>284</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B155" t="s">
-        <v>249</v>
+        <v>301</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B156" t="s">
-        <v>306</v>
+        <v>249</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>542</v>
+        <v>305</v>
       </c>
       <c r="B157" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3">
-      <c r="A159" t="s">
-        <v>519</v>
-      </c>
-      <c r="B159" t="s">
-        <v>520</v>
+        <v>306</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" t="s">
+        <v>539</v>
+      </c>
+      <c r="B158" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" t="s">
-        <v>293</v>
+        <v>519</v>
       </c>
       <c r="B160" t="s">
-        <v>297</v>
-      </c>
-      <c r="C160" t="s">
-        <v>608</v>
+        <v>520</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>507</v>
+        <v>293</v>
       </c>
       <c r="B161" t="s">
+        <v>297</v>
+      </c>
+      <c r="C161" t="s">
         <v>591</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>294</v>
+        <v>507</v>
       </c>
       <c r="B162" t="s">
-        <v>298</v>
-      </c>
-      <c r="C162" t="s">
-        <v>608</v>
+        <v>574</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B163" t="s">
-        <v>299</v>
+        <v>298</v>
+      </c>
+      <c r="C163" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B164" t="s">
-        <v>582</v>
+        <v>299</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="B165" t="s">
-        <v>249</v>
+        <v>565</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="B166" t="s">
-        <v>311</v>
+        <v>249</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B167" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B168" t="s">
         <v>309</v>
@@ -8033,846 +8055,854 @@
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B169" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>541</v>
+        <v>312</v>
       </c>
       <c r="B170" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3">
-      <c r="A172" t="s">
-        <v>521</v>
-      </c>
-      <c r="B172" t="s">
-        <v>522</v>
+        <v>313</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="A171" t="s">
+        <v>538</v>
+      </c>
+      <c r="B171" t="s">
+        <v>684</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
-        <v>501</v>
+        <v>521</v>
       </c>
       <c r="B173" t="s">
-        <v>321</v>
-      </c>
-      <c r="C173" t="s">
-        <v>608</v>
+        <v>522</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>508</v>
+        <v>501</v>
       </c>
       <c r="B174" t="s">
-        <v>592</v>
+        <v>321</v>
+      </c>
+      <c r="C174" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>316</v>
+        <v>508</v>
       </c>
       <c r="B175" t="s">
-        <v>322</v>
-      </c>
-      <c r="C175" t="s">
-        <v>608</v>
+        <v>575</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B176" t="s">
-        <v>323</v>
+        <v>322</v>
+      </c>
+      <c r="C176" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B177" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B178" t="s">
-        <v>583</v>
+        <v>324</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B179" t="s">
-        <v>249</v>
+        <v>566</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="B180" t="s">
-        <v>326</v>
-      </c>
-      <c r="C180" t="s">
-        <v>608</v>
+        <v>249</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B181" t="s">
-        <v>328</v>
+        <v>326</v>
+      </c>
+      <c r="C181" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B182" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B183" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B184" t="s">
-        <v>257</v>
+        <v>332</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="s">
-        <v>540</v>
+        <v>333</v>
       </c>
       <c r="B185" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3">
-      <c r="A187" t="s">
-        <v>523</v>
-      </c>
-      <c r="B187" t="s">
-        <v>524</v>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3">
+      <c r="A186" t="s">
+        <v>537</v>
+      </c>
+      <c r="B186" t="s">
+        <v>685</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" t="s">
-        <v>503</v>
+        <v>523</v>
       </c>
       <c r="B188" t="s">
-        <v>339</v>
-      </c>
-      <c r="C188" t="s">
-        <v>608</v>
+        <v>524</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" t="s">
-        <v>509</v>
+        <v>503</v>
       </c>
       <c r="B189" t="s">
-        <v>593</v>
+        <v>339</v>
+      </c>
+      <c r="C189" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190" t="s">
-        <v>337</v>
+        <v>509</v>
       </c>
       <c r="B190" t="s">
-        <v>340</v>
-      </c>
-      <c r="C190" t="s">
-        <v>608</v>
+        <v>576</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B191" t="s">
-        <v>341</v>
+        <v>340</v>
+      </c>
+      <c r="C191" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" t="s">
-        <v>502</v>
+        <v>338</v>
       </c>
       <c r="B192" t="s">
-        <v>584</v>
+        <v>341</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" t="s">
-        <v>345</v>
+        <v>502</v>
       </c>
       <c r="B193" t="s">
-        <v>249</v>
+        <v>567</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B194" t="s">
-        <v>342</v>
+        <v>249</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B195" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B196" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B197" t="s">
-        <v>257</v>
+        <v>344</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
-        <v>539</v>
+        <v>349</v>
       </c>
       <c r="B198" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3">
-      <c r="A200" t="s">
-        <v>570</v>
-      </c>
-      <c r="B200" t="s">
-        <v>573</v>
-      </c>
-      <c r="C200" t="s">
-        <v>606</v>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199" t="s">
+        <v>536</v>
+      </c>
+      <c r="B199" t="s">
+        <v>686</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" t="s">
-        <v>571</v>
+        <v>553</v>
       </c>
       <c r="B201" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
       <c r="C201" t="s">
-        <v>607</v>
+        <v>589</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>605</v>
+        <v>554</v>
       </c>
       <c r="B202" t="s">
-        <v>623</v>
+        <v>555</v>
+      </c>
+      <c r="C202" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" t="s">
-        <v>366</v>
+        <v>588</v>
       </c>
       <c r="B203" t="s">
-        <v>352</v>
+        <v>604</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B204" t="s">
-        <v>353</v>
-      </c>
-      <c r="C204" t="s">
-        <v>608</v>
+        <v>352</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
-        <v>510</v>
+        <v>367</v>
       </c>
       <c r="B205" t="s">
-        <v>594</v>
+        <v>353</v>
+      </c>
+      <c r="C205" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
-        <v>368</v>
+        <v>510</v>
       </c>
       <c r="B206" t="s">
-        <v>354</v>
+        <v>577</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B207" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B208" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B209" t="s">
-        <v>357</v>
-      </c>
-      <c r="C209" t="s">
-        <v>608</v>
+        <v>356</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B210" t="s">
-        <v>358</v>
+        <v>357</v>
+      </c>
+      <c r="C210" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B211" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B212" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B213" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B214" t="s">
-        <v>362</v>
-      </c>
-      <c r="C214" t="s">
-        <v>608</v>
+        <v>361</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B215" t="s">
-        <v>363</v>
+        <v>362</v>
+      </c>
+      <c r="C215" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B216" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B217" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" t="s">
-        <v>538</v>
+        <v>379</v>
       </c>
       <c r="B218" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3">
-      <c r="A220" t="s">
-        <v>628</v>
-      </c>
-      <c r="B220" t="s">
-        <v>629</v>
+        <v>365</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3">
+      <c r="A219" t="s">
+        <v>535</v>
+      </c>
+      <c r="B219" t="s">
+        <v>670</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" t="s">
-        <v>386</v>
+        <v>609</v>
       </c>
       <c r="B221" t="s">
-        <v>404</v>
+        <v>610</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B222" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
     </row>
     <row r="223" spans="1:3">
       <c r="A223" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B223" t="s">
-        <v>402</v>
-      </c>
-      <c r="C223" t="s">
-        <v>608</v>
+        <v>401</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" t="s">
-        <v>511</v>
+        <v>388</v>
       </c>
       <c r="B224" t="s">
-        <v>595</v>
+        <v>402</v>
+      </c>
+      <c r="C224" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" t="s">
-        <v>405</v>
+        <v>511</v>
       </c>
       <c r="B225" t="s">
-        <v>403</v>
-      </c>
-      <c r="C225" t="s">
-        <v>608</v>
+        <v>578</v>
       </c>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" t="s">
-        <v>389</v>
+        <v>405</v>
       </c>
       <c r="B226" t="s">
-        <v>395</v>
+        <v>403</v>
+      </c>
+      <c r="C226" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="227" spans="1:3">
       <c r="A227" t="s">
-        <v>406</v>
+        <v>389</v>
       </c>
       <c r="B227" t="s">
-        <v>396</v>
-      </c>
-      <c r="C227" t="s">
-        <v>585</v>
+        <v>395</v>
       </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" t="s">
-        <v>390</v>
+        <v>406</v>
       </c>
       <c r="B228" t="s">
-        <v>397</v>
+        <v>396</v>
+      </c>
+      <c r="C228" t="s">
+        <v>568</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B229" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B230" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="231" spans="1:3">
       <c r="A231" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B231" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B232" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
     </row>
     <row r="233" spans="1:3">
       <c r="A233" t="s">
-        <v>537</v>
+        <v>394</v>
       </c>
       <c r="B233" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3">
-      <c r="A235" t="s">
-        <v>525</v>
-      </c>
-      <c r="B235" t="s">
-        <v>526</v>
+        <v>397</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3">
+      <c r="A234" t="s">
+        <v>534</v>
+      </c>
+      <c r="B234" t="s">
+        <v>687</v>
       </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" t="s">
-        <v>412</v>
+        <v>525</v>
       </c>
       <c r="B236" t="s">
-        <v>423</v>
+        <v>526</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B237" t="s">
-        <v>424</v>
-      </c>
-      <c r="C237" t="s">
-        <v>608</v>
+        <v>423</v>
       </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" t="s">
-        <v>596</v>
+        <v>413</v>
       </c>
       <c r="B238" t="s">
-        <v>597</v>
+        <v>424</v>
+      </c>
+      <c r="C238" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239" t="s">
-        <v>414</v>
+        <v>579</v>
       </c>
       <c r="B239" t="s">
-        <v>425</v>
-      </c>
-      <c r="C239" t="s">
-        <v>608</v>
+        <v>580</v>
       </c>
     </row>
     <row r="240" spans="1:3">
       <c r="A240" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B240" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C240" t="s">
-        <v>608</v>
+        <v>591</v>
       </c>
     </row>
     <row r="241" spans="1:3">
       <c r="A241" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B241" t="s">
-        <v>609</v>
+        <v>426</v>
+      </c>
+      <c r="C241" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B242" t="s">
-        <v>427</v>
+        <v>592</v>
       </c>
     </row>
     <row r="243" spans="1:3">
       <c r="A243" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B243" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="244" spans="1:3">
       <c r="A244" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B244" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="245" spans="1:3">
       <c r="A245" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B245" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="246" spans="1:3">
       <c r="A246" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B246" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="247" spans="1:3">
       <c r="A247" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B247" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="248" spans="1:3">
       <c r="A248" t="s">
-        <v>534</v>
+        <v>422</v>
       </c>
       <c r="B248" t="s">
-        <v>535</v>
+        <v>432</v>
       </c>
     </row>
     <row r="249" spans="1:3">
       <c r="A249" t="s">
-        <v>637</v>
+        <v>532</v>
       </c>
       <c r="B249" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="251" spans="1:3">
-      <c r="A251" t="s">
-        <v>527</v>
-      </c>
-      <c r="B251" t="s">
-        <v>526</v>
+        <v>688</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3">
+      <c r="A250" t="s">
+        <v>618</v>
+      </c>
+      <c r="B250" t="s">
+        <v>619</v>
       </c>
     </row>
     <row r="252" spans="1:3">
       <c r="A252" t="s">
-        <v>439</v>
+        <v>527</v>
       </c>
       <c r="B252" t="s">
-        <v>450</v>
+        <v>526</v>
       </c>
     </row>
     <row r="253" spans="1:3">
       <c r="A253" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B253" t="s">
-        <v>451</v>
-      </c>
-      <c r="C253" t="s">
-        <v>608</v>
+        <v>450</v>
       </c>
     </row>
     <row r="254" spans="1:3">
       <c r="A254" t="s">
-        <v>512</v>
+        <v>440</v>
       </c>
       <c r="B254" t="s">
-        <v>598</v>
+        <v>451</v>
+      </c>
+      <c r="C254" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="255" spans="1:3">
       <c r="A255" t="s">
-        <v>441</v>
+        <v>512</v>
       </c>
       <c r="B255" t="s">
-        <v>452</v>
-      </c>
-      <c r="C255" t="s">
-        <v>608</v>
+        <v>581</v>
       </c>
     </row>
     <row r="256" spans="1:3">
       <c r="A256" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B256" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C256" t="s">
-        <v>608</v>
+        <v>591</v>
       </c>
     </row>
     <row r="257" spans="1:3">
       <c r="A257" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B257" t="s">
-        <v>610</v>
+        <v>453</v>
+      </c>
+      <c r="C257" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="258" spans="1:3">
       <c r="A258" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B258" t="s">
-        <v>427</v>
+        <v>593</v>
       </c>
     </row>
     <row r="259" spans="1:3">
       <c r="A259" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B259" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="260" spans="1:3">
       <c r="A260" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B260" t="s">
-        <v>454</v>
+        <v>428</v>
       </c>
     </row>
     <row r="261" spans="1:3">
       <c r="A261" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B261" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="262" spans="1:3">
       <c r="A262" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B262" t="s">
-        <v>431</v>
+        <v>455</v>
       </c>
     </row>
     <row r="263" spans="1:3">
       <c r="A263" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B263" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="264" spans="1:3">
       <c r="A264" t="s">
-        <v>533</v>
+        <v>449</v>
       </c>
       <c r="B264" t="s">
-        <v>535</v>
+        <v>432</v>
       </c>
     </row>
     <row r="265" spans="1:3">
       <c r="A265" t="s">
-        <v>644</v>
+        <v>531</v>
       </c>
       <c r="B265" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="267" spans="1:3">
-      <c r="A267" t="s">
-        <v>433</v>
-      </c>
-      <c r="B267" t="s">
-        <v>645</v>
+        <v>688</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3">
+      <c r="A266" t="s">
+        <v>625</v>
+      </c>
+      <c r="B266" t="s">
+        <v>619</v>
       </c>
     </row>
     <row r="268" spans="1:3">
       <c r="A268" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B268" t="s">
-        <v>646</v>
-      </c>
-      <c r="C268" t="s">
-        <v>608</v>
+        <v>626</v>
       </c>
     </row>
     <row r="269" spans="1:3">
       <c r="A269" t="s">
-        <v>513</v>
+        <v>434</v>
       </c>
       <c r="B269" t="s">
-        <v>647</v>
+        <v>627</v>
+      </c>
+      <c r="C269" t="s">
+        <v>591</v>
       </c>
     </row>
     <row r="270" spans="1:3">
       <c r="A270" t="s">
-        <v>435</v>
+        <v>513</v>
       </c>
       <c r="B270" t="s">
-        <v>675</v>
+        <v>628</v>
       </c>
     </row>
     <row r="271" spans="1:3">
       <c r="A271" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B271" t="s">
-        <v>648</v>
+        <v>655</v>
       </c>
     </row>
     <row r="272" spans="1:3">
       <c r="A272" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B272" t="s">
-        <v>649</v>
+        <v>629</v>
       </c>
     </row>
     <row r="273" spans="1:2">
       <c r="A273" t="s">
-        <v>532</v>
+        <v>437</v>
       </c>
       <c r="B273" t="s">
-        <v>650</v>
+        <v>630</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2">
+      <c r="A274" t="s">
+        <v>530</v>
+      </c>
+      <c r="B274" t="s">
+        <v>689</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code updates for 57278, 57674
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.malyala\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA791FA-DF4D-4C81-B31A-624C0AD7729F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418CC419-8DBB-4746-ACE2-3ADD45EC9FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2265" yWindow="2265" windowWidth="20190" windowHeight="8340" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="843" uniqueCount="694">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="695">
   <si>
     <t>Name</t>
   </si>
@@ -429,9 +429,6 @@
     <t>Unit is blank on the Asset Self Certification.</t>
   </si>
   <si>
-    <t>Affidavit of student financial Assistance</t>
-  </si>
-  <si>
     <t>Not every field in Part 4 have been answered on the Affidavit of Student Financial Assistance.</t>
   </si>
   <si>
@@ -2122,6 +2119,12 @@
   </si>
   <si>
     <t>TotalAssetsLimit</t>
+  </si>
+  <si>
+    <t>ASFA_AssistanceMarkedYes</t>
+  </si>
+  <si>
+    <t>Removed this check as we replace this with below check to see if assitance is mared yes in an arrays 1, 2, 3</t>
   </si>
 </sst>
 </file>
@@ -2580,202 +2583,202 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B7" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B12" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B13" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B14" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B15" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B16" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B18" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C18" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B19" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C19" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B20" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B21" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B22" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B23" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B24" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B25" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C26" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B27" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
+        <v>313</v>
+      </c>
+      <c r="B28" t="s">
         <v>314</v>
-      </c>
-      <c r="B28" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
+        <v>334</v>
+      </c>
+      <c r="B29" t="s">
         <v>335</v>
-      </c>
-      <c r="B29" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B30" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
@@ -2788,74 +2791,74 @@
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
+        <v>381</v>
+      </c>
+      <c r="B32" t="s">
         <v>382</v>
-      </c>
-      <c r="B32" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
       <c r="A33" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B33" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B34" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
       <c r="A35" t="s">
+        <v>408</v>
+      </c>
+      <c r="B35" t="s">
         <v>409</v>
-      </c>
-      <c r="B35" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1">
       <c r="A36" t="s">
+        <v>456</v>
+      </c>
+      <c r="B36" t="s">
         <v>457</v>
-      </c>
-      <c r="B36" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B37" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1">
       <c r="A38" t="s">
+        <v>406</v>
+      </c>
+      <c r="B38" t="s">
         <v>407</v>
-      </c>
-      <c r="B38" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1">
       <c r="A39" t="s">
+        <v>459</v>
+      </c>
+      <c r="B39" t="s">
         <v>460</v>
-      </c>
-      <c r="B39" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B40" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3842,242 +3845,242 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>471</v>
+      </c>
+      <c r="B1" t="s">
         <v>472</v>
-      </c>
-      <c r="B1" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B5" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B6" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B7" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B9" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B10" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
+        <v>478</v>
+      </c>
+      <c r="B11" t="s">
         <v>479</v>
-      </c>
-      <c r="B11" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B12" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B13" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B14" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B15" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
+        <v>481</v>
+      </c>
+      <c r="B16" t="s">
         <v>482</v>
-      </c>
-      <c r="B16" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B17" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B19" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B20" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
+        <v>486</v>
+      </c>
+      <c r="B22" t="s">
         <v>487</v>
-      </c>
-      <c r="B22" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B23" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B24" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B25" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B26" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B27" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B28" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B29" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B30" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -4085,79 +4088,79 @@
         <v>1040</v>
       </c>
       <c r="B31" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B32" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B33" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B34" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B35" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B36" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B37" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B38" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B39" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B40" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
   </sheetData>
@@ -4365,15 +4368,15 @@
         <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B21" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
@@ -5415,7 +5418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1011"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+    <sheetView topLeftCell="A32" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
@@ -5537,90 +5540,90 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B12" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B13" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B14" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B15" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B16" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B17" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B18" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B19" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B20" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B21" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1">
@@ -5633,130 +5636,130 @@
     </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B23" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B27" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B28" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B29" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B30" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1">
       <c r="A31" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B32" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
       <c r="A33" s="2" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B33" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B34" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B35" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B36" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B37" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B38" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
@@ -6740,10 +6743,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
-  <dimension ref="A1:C274"/>
+  <dimension ref="A1:C275"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6763,18 +6766,18 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" t="s">
         <v>195</v>
-      </c>
-      <c r="B3" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B5" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -6787,10 +6790,10 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -6803,45 +6806,45 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
+        <v>206</v>
+      </c>
+      <c r="B9" t="s">
         <v>207</v>
       </c>
-      <c r="B9" t="s">
-        <v>208</v>
-      </c>
       <c r="C9" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
+        <v>550</v>
+      </c>
+      <c r="B10" t="s">
         <v>551</v>
-      </c>
-      <c r="B10" t="s">
-        <v>552</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
+        <v>690</v>
+      </c>
+      <c r="B11" t="s">
         <v>691</v>
-      </c>
-      <c r="B11" t="s">
-        <v>692</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B12" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
+        <v>181</v>
+      </c>
+      <c r="B14" t="s">
         <v>182</v>
-      </c>
-      <c r="B14" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -6854,10 +6857,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
+        <v>560</v>
+      </c>
+      <c r="B16" t="s">
         <v>561</v>
-      </c>
-      <c r="B16" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -6878,18 +6881,18 @@
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
+        <v>196</v>
+      </c>
+      <c r="B19" t="s">
         <v>197</v>
-      </c>
-      <c r="B19" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B20" t="s">
         <v>199</v>
-      </c>
-      <c r="B20" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -6926,34 +6929,34 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
+        <v>634</v>
+      </c>
+      <c r="B25" t="s">
         <v>635</v>
-      </c>
-      <c r="B25" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
+        <v>658</v>
+      </c>
+      <c r="B26" t="s">
         <v>659</v>
-      </c>
-      <c r="B26" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B27" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B29" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -7012,7 +7015,7 @@
         <v>99</v>
       </c>
       <c r="C36" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -7025,26 +7028,26 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
+        <v>636</v>
+      </c>
+      <c r="B38" t="s">
         <v>637</v>
-      </c>
-      <c r="B38" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B39" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B41" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -7055,7 +7058,7 @@
         <v>108</v>
       </c>
       <c r="C42" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -7066,7 +7069,7 @@
         <v>118</v>
       </c>
       <c r="C43" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -7077,7 +7080,7 @@
         <v>120</v>
       </c>
       <c r="C44" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -7088,7 +7091,7 @@
         <v>109</v>
       </c>
       <c r="C45" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -7099,7 +7102,7 @@
         <v>110</v>
       </c>
       <c r="C46" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -7110,7 +7113,7 @@
         <v>111</v>
       </c>
       <c r="C47" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -7123,58 +7126,58 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B49" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B50" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C50" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="B51" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
+        <v>548</v>
+      </c>
+      <c r="B52" t="s">
         <v>549</v>
-      </c>
-      <c r="B52" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B53" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B54" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B56" t="s">
         <v>121</v>
@@ -7185,7 +7188,7 @@
         <v>122</v>
       </c>
       <c r="B57" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -7198,26 +7201,26 @@
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
+        <v>638</v>
+      </c>
+      <c r="B59" t="s">
         <v>639</v>
-      </c>
-      <c r="B59" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="B60" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
+        <v>186</v>
+      </c>
+      <c r="B62" t="s">
         <v>187</v>
-      </c>
-      <c r="B62" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -7238,182 +7241,182 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B65" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B66" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B67" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B68" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B69" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C69" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B70" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C70" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B71" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C71" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
+        <v>640</v>
+      </c>
+      <c r="B72" t="s">
         <v>641</v>
-      </c>
-      <c r="B72" t="s">
-        <v>642</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B73" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B75" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B76" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B77" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B78" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="C78" t="s">
-        <v>129</v>
+        <v>694</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>147</v>
+        <v>693</v>
       </c>
       <c r="B79" t="s">
-        <v>130</v>
+        <v>582</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="B80" t="s">
-        <v>602</v>
+        <v>129</v>
       </c>
     </row>
     <row r="81" spans="1:2">
       <c r="A81" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B81" t="s">
-        <v>131</v>
+        <v>601</v>
       </c>
     </row>
     <row r="82" spans="1:2">
       <c r="A82" t="s">
-        <v>643</v>
+        <v>132</v>
       </c>
       <c r="B82" t="s">
-        <v>644</v>
+        <v>130</v>
       </c>
     </row>
     <row r="83" spans="1:2">
       <c r="A83" t="s">
-        <v>543</v>
+        <v>642</v>
       </c>
       <c r="B83" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
-      <c r="A85" t="s">
-        <v>189</v>
-      </c>
-      <c r="B85" t="s">
-        <v>190</v>
+        <v>643</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>542</v>
+      </c>
+      <c r="B84" t="s">
+        <v>676</v>
       </c>
     </row>
     <row r="86" spans="1:2">
       <c r="A86" t="s">
-        <v>134</v>
+        <v>188</v>
       </c>
       <c r="B86" t="s">
-        <v>154</v>
+        <v>189</v>
       </c>
     </row>
     <row r="87" spans="1:2">
       <c r="A87" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B87" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -7421,197 +7424,197 @@
         <v>135</v>
       </c>
       <c r="B88" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="89" spans="1:2">
       <c r="A89" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B89" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="90" spans="1:2">
       <c r="A90" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B90" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="91" spans="1:2">
       <c r="A91" t="s">
-        <v>632</v>
+        <v>137</v>
       </c>
       <c r="B91" t="s">
-        <v>633</v>
+        <v>157</v>
       </c>
     </row>
     <row r="92" spans="1:2">
       <c r="A92" t="s">
-        <v>645</v>
+        <v>631</v>
       </c>
       <c r="B92" t="s">
-        <v>646</v>
+        <v>632</v>
       </c>
     </row>
     <row r="93" spans="1:2">
       <c r="A93" t="s">
-        <v>542</v>
+        <v>644</v>
       </c>
       <c r="B93" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="A95" t="s">
-        <v>160</v>
-      </c>
-      <c r="B95" t="s">
-        <v>164</v>
+        <v>645</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>541</v>
+      </c>
+      <c r="B94" t="s">
+        <v>677</v>
       </c>
     </row>
     <row r="96" spans="1:2">
       <c r="A96" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B96" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B97" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B98" t="s">
-        <v>603</v>
+        <v>165</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>559</v>
+        <v>162</v>
       </c>
       <c r="B99" t="s">
-        <v>560</v>
+        <v>602</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>651</v>
+        <v>558</v>
       </c>
       <c r="B100" t="s">
-        <v>652</v>
+        <v>559</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>541</v>
+        <v>650</v>
       </c>
       <c r="B101" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3">
-      <c r="A103" t="s">
-        <v>193</v>
-      </c>
-      <c r="B103" t="s">
-        <v>194</v>
+        <v>651</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" t="s">
+        <v>540</v>
+      </c>
+      <c r="B102" t="s">
+        <v>678</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>167</v>
+        <v>192</v>
       </c>
       <c r="B104" t="s">
-        <v>169</v>
+        <v>193</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
+        <v>166</v>
+      </c>
+      <c r="B105" t="s">
         <v>168</v>
-      </c>
-      <c r="B105" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>647</v>
+        <v>167</v>
       </c>
       <c r="B106" t="s">
-        <v>648</v>
+        <v>169</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>540</v>
+        <v>646</v>
       </c>
       <c r="B107" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3">
-      <c r="A109" t="s">
-        <v>191</v>
-      </c>
-      <c r="B109" t="s">
-        <v>192</v>
+        <v>647</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" t="s">
+        <v>539</v>
+      </c>
+      <c r="B108" t="s">
+        <v>679</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="B110" t="s">
-        <v>173</v>
-      </c>
-      <c r="C110" t="s">
-        <v>591</v>
+        <v>191</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B111" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C111" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B112" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C112" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>204</v>
+        <v>171</v>
       </c>
       <c r="B113" t="s">
-        <v>203</v>
+        <v>174</v>
+      </c>
+      <c r="C113" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B114" t="s">
         <v>202</v>
@@ -7619,287 +7622,287 @@
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>177</v>
+        <v>200</v>
       </c>
       <c r="B115" t="s">
-        <v>178</v>
-      </c>
-      <c r="C115" t="s">
-        <v>591</v>
+        <v>201</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>649</v>
+        <v>176</v>
       </c>
       <c r="B116" t="s">
-        <v>650</v>
+        <v>177</v>
+      </c>
+      <c r="C116" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>529</v>
+        <v>648</v>
       </c>
       <c r="B117" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3">
-      <c r="A119" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" t="s">
+        <v>528</v>
+      </c>
+      <c r="B118" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" t="s">
+        <v>655</v>
+      </c>
+      <c r="B120" t="s">
         <v>656</v>
       </c>
-      <c r="B119" t="s">
+      <c r="C120" t="s">
         <v>657</v>
-      </c>
-      <c r="C119" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3">
-      <c r="A121" t="s">
-        <v>515</v>
-      </c>
-      <c r="B121" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>665</v>
+        <v>514</v>
       </c>
       <c r="B122" t="s">
-        <v>669</v>
-      </c>
-      <c r="C122" t="s">
-        <v>667</v>
+        <v>515</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="B123" t="s">
         <v>668</v>
       </c>
       <c r="C123" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>243</v>
+        <v>665</v>
       </c>
       <c r="B124" t="s">
-        <v>244</v>
+        <v>667</v>
       </c>
       <c r="C124" t="s">
-        <v>591</v>
+        <v>666</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B125" t="s">
-        <v>246</v>
+        <v>243</v>
+      </c>
+      <c r="C125" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="B126" t="s">
-        <v>563</v>
-      </c>
-      <c r="C126" t="s">
-        <v>654</v>
+        <v>245</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
       <c r="B127" t="s">
-        <v>247</v>
+        <v>562</v>
+      </c>
+      <c r="C127" t="s">
+        <v>653</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>505</v>
+        <v>247</v>
       </c>
       <c r="B128" t="s">
-        <v>514</v>
+        <v>246</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>250</v>
+        <v>504</v>
       </c>
       <c r="B129" t="s">
-        <v>249</v>
+        <v>513</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B130" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
+        <v>250</v>
+      </c>
+      <c r="B131" t="s">
         <v>252</v>
-      </c>
-      <c r="B131" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B132" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B133" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>303</v>
+        <v>257</v>
       </c>
       <c r="B134" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>350</v>
+        <v>302</v>
       </c>
       <c r="B135" t="s">
-        <v>351</v>
+        <v>248</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>661</v>
+        <v>349</v>
       </c>
       <c r="B136" t="s">
-        <v>662</v>
+        <v>350</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>528</v>
+        <v>660</v>
       </c>
       <c r="B137" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3">
-      <c r="A139" t="s">
-        <v>517</v>
-      </c>
-      <c r="B139" t="s">
-        <v>518</v>
+        <v>661</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" t="s">
+        <v>527</v>
+      </c>
+      <c r="B138" t="s">
+        <v>681</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>260</v>
+        <v>516</v>
       </c>
       <c r="B140" t="s">
-        <v>263</v>
-      </c>
-      <c r="C140" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" ht="13.5" customHeight="1">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
       <c r="A141" t="s">
+        <v>259</v>
+      </c>
+      <c r="B141" t="s">
         <v>262</v>
       </c>
-      <c r="B141" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3">
+      <c r="C141" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" ht="13.5" customHeight="1">
       <c r="A142" t="s">
         <v>261</v>
       </c>
       <c r="B142" t="s">
-        <v>264</v>
+        <v>563</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B143" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B144" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B145" t="s">
-        <v>269</v>
-      </c>
-      <c r="C145" t="s">
-        <v>664</v>
+        <v>267</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>506</v>
+        <v>269</v>
       </c>
       <c r="B146" t="s">
-        <v>573</v>
+        <v>268</v>
+      </c>
+      <c r="C146" t="s">
+        <v>663</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>271</v>
+        <v>505</v>
       </c>
       <c r="B147" t="s">
-        <v>272</v>
+        <v>572</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B148" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="B149" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B150" t="s">
         <v>287</v>
@@ -7907,653 +7910,653 @@
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B151" t="s">
         <v>286</v>
       </c>
-      <c r="C151" t="s">
-        <v>664</v>
-      </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B152" t="s">
-        <v>608</v>
+        <v>285</v>
+      </c>
+      <c r="C152" t="s">
+        <v>663</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B153" t="s">
-        <v>285</v>
-      </c>
-      <c r="C153" t="s">
-        <v>664</v>
+        <v>607</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B154" t="s">
         <v>284</v>
       </c>
+      <c r="C154" t="s">
+        <v>663</v>
+      </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="B155" t="s">
-        <v>301</v>
+        <v>283</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B156" t="s">
-        <v>249</v>
+        <v>300</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B157" t="s">
-        <v>306</v>
+        <v>248</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
-        <v>539</v>
+        <v>304</v>
       </c>
       <c r="B158" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3">
-      <c r="A160" t="s">
-        <v>519</v>
-      </c>
-      <c r="B160" t="s">
-        <v>520</v>
+        <v>305</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159" t="s">
+        <v>538</v>
+      </c>
+      <c r="B159" t="s">
+        <v>682</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>293</v>
+        <v>518</v>
       </c>
       <c r="B161" t="s">
-        <v>297</v>
-      </c>
-      <c r="C161" t="s">
-        <v>591</v>
+        <v>519</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>507</v>
+        <v>292</v>
       </c>
       <c r="B162" t="s">
-        <v>574</v>
+        <v>296</v>
+      </c>
+      <c r="C162" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>294</v>
+        <v>506</v>
       </c>
       <c r="B163" t="s">
-        <v>298</v>
-      </c>
-      <c r="C163" t="s">
-        <v>591</v>
+        <v>573</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B164" t="s">
-        <v>299</v>
+        <v>297</v>
+      </c>
+      <c r="C164" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B165" t="s">
-        <v>565</v>
+        <v>298</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="B166" t="s">
-        <v>249</v>
+        <v>564</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="B167" t="s">
-        <v>311</v>
+        <v>248</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B168" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
+        <v>306</v>
+      </c>
+      <c r="B169" t="s">
         <v>308</v>
-      </c>
-      <c r="B169" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B170" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>538</v>
+        <v>311</v>
       </c>
       <c r="B171" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3">
-      <c r="A173" t="s">
-        <v>521</v>
-      </c>
-      <c r="B173" t="s">
-        <v>522</v>
+        <v>312</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172" t="s">
+        <v>537</v>
+      </c>
+      <c r="B172" t="s">
+        <v>683</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>501</v>
+        <v>520</v>
       </c>
       <c r="B174" t="s">
-        <v>321</v>
-      </c>
-      <c r="C174" t="s">
-        <v>591</v>
+        <v>521</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
       <c r="B175" t="s">
-        <v>575</v>
+        <v>320</v>
+      </c>
+      <c r="C175" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>316</v>
+        <v>507</v>
       </c>
       <c r="B176" t="s">
-        <v>322</v>
-      </c>
-      <c r="C176" t="s">
-        <v>591</v>
+        <v>574</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B177" t="s">
-        <v>323</v>
+        <v>321</v>
+      </c>
+      <c r="C177" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B178" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B179" t="s">
-        <v>566</v>
+        <v>323</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B180" t="s">
-        <v>249</v>
+        <v>565</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="B181" t="s">
-        <v>326</v>
-      </c>
-      <c r="C181" t="s">
-        <v>591</v>
+        <v>248</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B182" t="s">
-        <v>328</v>
+        <v>325</v>
+      </c>
+      <c r="C182" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B183" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B184" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B185" t="s">
-        <v>257</v>
+        <v>331</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="s">
-        <v>537</v>
+        <v>332</v>
       </c>
       <c r="B186" t="s">
-        <v>685</v>
-      </c>
-    </row>
-    <row r="188" spans="1:3">
-      <c r="A188" t="s">
-        <v>523</v>
-      </c>
-      <c r="B188" t="s">
-        <v>524</v>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3">
+      <c r="A187" t="s">
+        <v>536</v>
+      </c>
+      <c r="B187" t="s">
+        <v>684</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" t="s">
-        <v>503</v>
+        <v>522</v>
       </c>
       <c r="B189" t="s">
-        <v>339</v>
-      </c>
-      <c r="C189" t="s">
-        <v>591</v>
+        <v>523</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190" t="s">
-        <v>509</v>
+        <v>502</v>
       </c>
       <c r="B190" t="s">
-        <v>576</v>
+        <v>338</v>
+      </c>
+      <c r="C190" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" t="s">
-        <v>337</v>
+        <v>508</v>
       </c>
       <c r="B191" t="s">
-        <v>340</v>
-      </c>
-      <c r="C191" t="s">
-        <v>591</v>
+        <v>575</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B192" t="s">
-        <v>341</v>
+        <v>339</v>
+      </c>
+      <c r="C192" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" t="s">
-        <v>502</v>
+        <v>337</v>
       </c>
       <c r="B193" t="s">
-        <v>567</v>
+        <v>340</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>345</v>
+        <v>501</v>
       </c>
       <c r="B194" t="s">
-        <v>249</v>
+        <v>566</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B195" t="s">
-        <v>342</v>
+        <v>248</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B196" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B197" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B198" t="s">
-        <v>257</v>
+        <v>343</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" t="s">
-        <v>536</v>
+        <v>348</v>
       </c>
       <c r="B199" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3">
-      <c r="A201" t="s">
-        <v>553</v>
-      </c>
-      <c r="B201" t="s">
-        <v>556</v>
-      </c>
-      <c r="C201" t="s">
-        <v>589</v>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3">
+      <c r="A200" t="s">
+        <v>535</v>
+      </c>
+      <c r="B200" t="s">
+        <v>685</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B202" t="s">
         <v>555</v>
       </c>
       <c r="C202" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" t="s">
-        <v>588</v>
+        <v>553</v>
       </c>
       <c r="B203" t="s">
-        <v>604</v>
+        <v>554</v>
+      </c>
+      <c r="C203" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
-        <v>366</v>
+        <v>587</v>
       </c>
       <c r="B204" t="s">
-        <v>352</v>
+        <v>603</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B205" t="s">
-        <v>353</v>
-      </c>
-      <c r="C205" t="s">
-        <v>591</v>
+        <v>351</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
-        <v>510</v>
+        <v>366</v>
       </c>
       <c r="B206" t="s">
-        <v>577</v>
+        <v>352</v>
+      </c>
+      <c r="C206" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" t="s">
-        <v>368</v>
+        <v>509</v>
       </c>
       <c r="B207" t="s">
-        <v>354</v>
+        <v>576</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B208" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B209" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B210" t="s">
-        <v>357</v>
-      </c>
-      <c r="C210" t="s">
-        <v>591</v>
+        <v>355</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B211" t="s">
-        <v>358</v>
+        <v>356</v>
+      </c>
+      <c r="C211" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B212" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B213" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B214" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B215" t="s">
-        <v>362</v>
-      </c>
-      <c r="C215" t="s">
-        <v>591</v>
+        <v>360</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B216" t="s">
-        <v>363</v>
+        <v>361</v>
+      </c>
+      <c r="C216" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B217" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B218" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219" t="s">
-        <v>535</v>
+        <v>378</v>
       </c>
       <c r="B219" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="221" spans="1:3">
-      <c r="A221" t="s">
-        <v>609</v>
-      </c>
-      <c r="B221" t="s">
-        <v>610</v>
+        <v>364</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3">
+      <c r="A220" t="s">
+        <v>534</v>
+      </c>
+      <c r="B220" t="s">
+        <v>669</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" t="s">
-        <v>386</v>
+        <v>608</v>
       </c>
       <c r="B222" t="s">
-        <v>404</v>
+        <v>609</v>
       </c>
     </row>
     <row r="223" spans="1:3">
       <c r="A223" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B223" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B224" t="s">
-        <v>402</v>
-      </c>
-      <c r="C224" t="s">
-        <v>591</v>
+        <v>400</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" t="s">
-        <v>511</v>
+        <v>387</v>
       </c>
       <c r="B225" t="s">
-        <v>578</v>
+        <v>401</v>
+      </c>
+      <c r="C225" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" t="s">
-        <v>405</v>
+        <v>510</v>
       </c>
       <c r="B226" t="s">
-        <v>403</v>
-      </c>
-      <c r="C226" t="s">
-        <v>591</v>
+        <v>577</v>
       </c>
     </row>
     <row r="227" spans="1:3">
       <c r="A227" t="s">
-        <v>389</v>
+        <v>404</v>
       </c>
       <c r="B227" t="s">
-        <v>395</v>
+        <v>402</v>
+      </c>
+      <c r="C227" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" t="s">
-        <v>406</v>
+        <v>388</v>
       </c>
       <c r="B228" t="s">
-        <v>396</v>
-      </c>
-      <c r="C228" t="s">
-        <v>568</v>
+        <v>394</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" t="s">
-        <v>390</v>
+        <v>405</v>
       </c>
       <c r="B229" t="s">
-        <v>397</v>
+        <v>395</v>
+      </c>
+      <c r="C229" t="s">
+        <v>567</v>
       </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B230" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="231" spans="1:3">
@@ -8561,348 +8564,356 @@
         <v>391</v>
       </c>
       <c r="B231" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B232" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="233" spans="1:3">
       <c r="A233" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B233" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" t="s">
-        <v>534</v>
+        <v>393</v>
       </c>
       <c r="B234" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3">
-      <c r="A236" t="s">
-        <v>525</v>
-      </c>
-      <c r="B236" t="s">
-        <v>526</v>
+        <v>396</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3">
+      <c r="A235" t="s">
+        <v>533</v>
+      </c>
+      <c r="B235" t="s">
+        <v>686</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" t="s">
-        <v>412</v>
+        <v>524</v>
       </c>
       <c r="B237" t="s">
-        <v>423</v>
+        <v>525</v>
       </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B238" t="s">
-        <v>424</v>
-      </c>
-      <c r="C238" t="s">
-        <v>591</v>
+        <v>422</v>
       </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239" t="s">
-        <v>579</v>
+        <v>412</v>
       </c>
       <c r="B239" t="s">
-        <v>580</v>
+        <v>423</v>
+      </c>
+      <c r="C239" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="240" spans="1:3">
       <c r="A240" t="s">
-        <v>414</v>
+        <v>578</v>
       </c>
       <c r="B240" t="s">
-        <v>425</v>
-      </c>
-      <c r="C240" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="241" spans="1:3">
       <c r="A241" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B241" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C241" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B242" t="s">
-        <v>592</v>
+        <v>425</v>
+      </c>
+      <c r="C242" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="243" spans="1:3">
       <c r="A243" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B243" t="s">
-        <v>427</v>
+        <v>591</v>
       </c>
     </row>
     <row r="244" spans="1:3">
       <c r="A244" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B244" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="245" spans="1:3">
       <c r="A245" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B245" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="246" spans="1:3">
       <c r="A246" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B246" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="247" spans="1:3">
       <c r="A247" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B247" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="248" spans="1:3">
       <c r="A248" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B248" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="249" spans="1:3">
       <c r="A249" t="s">
-        <v>532</v>
+        <v>421</v>
       </c>
       <c r="B249" t="s">
-        <v>688</v>
+        <v>431</v>
       </c>
     </row>
     <row r="250" spans="1:3">
       <c r="A250" t="s">
+        <v>531</v>
+      </c>
+      <c r="B250" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3">
+      <c r="A251" t="s">
+        <v>617</v>
+      </c>
+      <c r="B251" t="s">
         <v>618</v>
-      </c>
-      <c r="B250" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="252" spans="1:3">
-      <c r="A252" t="s">
-        <v>527</v>
-      </c>
-      <c r="B252" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="253" spans="1:3">
       <c r="A253" t="s">
-        <v>439</v>
+        <v>526</v>
       </c>
       <c r="B253" t="s">
-        <v>450</v>
+        <v>525</v>
       </c>
     </row>
     <row r="254" spans="1:3">
       <c r="A254" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B254" t="s">
-        <v>451</v>
-      </c>
-      <c r="C254" t="s">
-        <v>591</v>
+        <v>449</v>
       </c>
     </row>
     <row r="255" spans="1:3">
       <c r="A255" t="s">
-        <v>512</v>
+        <v>439</v>
       </c>
       <c r="B255" t="s">
-        <v>581</v>
+        <v>450</v>
+      </c>
+      <c r="C255" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="256" spans="1:3">
       <c r="A256" t="s">
-        <v>441</v>
+        <v>511</v>
       </c>
       <c r="B256" t="s">
-        <v>452</v>
-      </c>
-      <c r="C256" t="s">
-        <v>591</v>
+        <v>580</v>
       </c>
     </row>
     <row r="257" spans="1:3">
       <c r="A257" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B257" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C257" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="258" spans="1:3">
       <c r="A258" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B258" t="s">
-        <v>593</v>
+        <v>452</v>
+      </c>
+      <c r="C258" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="259" spans="1:3">
       <c r="A259" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B259" t="s">
-        <v>427</v>
+        <v>592</v>
       </c>
     </row>
     <row r="260" spans="1:3">
       <c r="A260" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B260" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="261" spans="1:3">
       <c r="A261" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B261" t="s">
-        <v>454</v>
+        <v>427</v>
       </c>
     </row>
     <row r="262" spans="1:3">
       <c r="A262" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B262" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="263" spans="1:3">
       <c r="A263" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B263" t="s">
-        <v>431</v>
+        <v>454</v>
       </c>
     </row>
     <row r="264" spans="1:3">
       <c r="A264" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B264" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="265" spans="1:3">
       <c r="A265" t="s">
-        <v>531</v>
+        <v>448</v>
       </c>
       <c r="B265" t="s">
-        <v>688</v>
+        <v>431</v>
       </c>
     </row>
     <row r="266" spans="1:3">
       <c r="A266" t="s">
-        <v>625</v>
+        <v>530</v>
       </c>
       <c r="B266" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="268" spans="1:3">
-      <c r="A268" t="s">
-        <v>433</v>
-      </c>
-      <c r="B268" t="s">
-        <v>626</v>
+        <v>687</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3">
+      <c r="A267" t="s">
+        <v>624</v>
+      </c>
+      <c r="B267" t="s">
+        <v>618</v>
       </c>
     </row>
     <row r="269" spans="1:3">
       <c r="A269" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B269" t="s">
-        <v>627</v>
-      </c>
-      <c r="C269" t="s">
-        <v>591</v>
+        <v>625</v>
       </c>
     </row>
     <row r="270" spans="1:3">
       <c r="A270" t="s">
-        <v>513</v>
+        <v>433</v>
       </c>
       <c r="B270" t="s">
-        <v>628</v>
+        <v>626</v>
+      </c>
+      <c r="C270" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="271" spans="1:3">
       <c r="A271" t="s">
-        <v>435</v>
+        <v>512</v>
       </c>
       <c r="B271" t="s">
-        <v>655</v>
+        <v>627</v>
       </c>
     </row>
     <row r="272" spans="1:3">
       <c r="A272" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B272" t="s">
-        <v>629</v>
+        <v>654</v>
       </c>
     </row>
     <row r="273" spans="1:2">
       <c r="A273" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B273" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="274" spans="1:2">
       <c r="A274" t="s">
-        <v>530</v>
+        <v>436</v>
       </c>
       <c r="B274" t="s">
-        <v>689</v>
+        <v>629</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2">
+      <c r="A275" t="s">
+        <v>529</v>
+      </c>
+      <c r="B275" t="s">
+        <v>688</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated code for VOE, SC
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.malyala\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raluca.ilinca.AzureAI-Jump2\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418CC419-8DBB-4746-ACE2-3ADD45EC9FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBD76AB-4D0C-4DE2-93AE-07349EEAF609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28200" windowHeight="13530" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="695">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="702">
   <si>
     <t>Name</t>
   </si>
@@ -1518,9 +1518,6 @@
     <t>VAWA Acknowledgement</t>
   </si>
   <si>
-    <t>C:\Users\harika.malyala\Documents\AZApplicationReview\Prompts\</t>
-  </si>
-  <si>
     <t>Replace_JArraayInJSON</t>
   </si>
   <si>
@@ -1938,9 +1935,6 @@
     <t>SC_AllFullTimeStudents</t>
   </si>
   <si>
-    <t>All household members have been or will be students for the next five months. Manual review required.</t>
-  </si>
-  <si>
     <t>Assets Type and  value does not match that listed on the ICW.</t>
   </si>
   <si>
@@ -2125,6 +2119,33 @@
   </si>
   <si>
     <t>Removed this check as we replace this with below check to see if assitance is mared yes in an arrays 1, 2, 3</t>
+  </si>
+  <si>
+    <t>MID_MinorLessThan50Percent</t>
+  </si>
+  <si>
+    <t>A minor will live in the household less than 50% of the time. Manual review required.</t>
+  </si>
+  <si>
+    <t>VOE_PayIncrease</t>
+  </si>
+  <si>
+    <t>Anticipated increase in the base pay over the next 12 months. Manual review required.</t>
+  </si>
+  <si>
+    <t>The applicant has indicated all household contains all students by selecting 2 or 3 to Part A on the Student Certification. Manual review required.</t>
+  </si>
+  <si>
+    <t>C:\Users\raluca.ilinca.AzureAI-Jump2\Documents\AZApplicationReview\Prompts\</t>
+  </si>
+  <si>
+    <t>Updated by Raluca</t>
+  </si>
+  <si>
+    <t>Removed this check - Raluca</t>
+  </si>
+  <si>
+    <t>Newly added by Raluca</t>
   </si>
 </sst>
 </file>
@@ -2502,8 +2523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2586,7 +2607,7 @@
         <v>209</v>
       </c>
       <c r="B7" t="s">
-        <v>492</v>
+        <v>698</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -2635,7 +2656,7 @@
         <v>219</v>
       </c>
       <c r="B14" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
@@ -2673,7 +2694,7 @@
         <v>223</v>
       </c>
       <c r="B18" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C18" t="s">
         <v>238</v>
@@ -2695,7 +2716,7 @@
         <v>225</v>
       </c>
       <c r="B20" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
@@ -2711,7 +2732,7 @@
         <v>227</v>
       </c>
       <c r="B22" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
@@ -2778,7 +2799,7 @@
         <v>379</v>
       </c>
       <c r="B30" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
@@ -2810,7 +2831,7 @@
         <v>410</v>
       </c>
       <c r="B34" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
@@ -2858,7 +2879,7 @@
         <v>437</v>
       </c>
       <c r="B40" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
@@ -4368,15 +4389,15 @@
         <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B21" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
@@ -5548,82 +5569,82 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B12" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B13" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B14" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B15" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B16" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B17" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B18" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B19" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B20" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B21" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1">
@@ -5684,82 +5705,82 @@
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B29" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B30" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1">
       <c r="A31" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B32" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
       <c r="A33" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B33" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B34" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B35" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B36" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B37" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B38" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
@@ -6743,16 +6764,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
-  <dimension ref="A1:C275"/>
+  <dimension ref="A1:C277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A149" workbookViewId="0">
+      <selection activeCell="C161" sqref="C161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="126.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="153.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6777,7 +6798,7 @@
         <v>180</v>
       </c>
       <c r="B5" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -6812,31 +6833,31 @@
         <v>207</v>
       </c>
       <c r="C9" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
+        <v>549</v>
+      </c>
+      <c r="B10" t="s">
         <v>550</v>
-      </c>
-      <c r="B10" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B11" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B12" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -6857,10 +6878,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
+        <v>559</v>
+      </c>
+      <c r="B16" t="s">
         <v>560</v>
-      </c>
-      <c r="B16" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -6929,26 +6950,26 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B25" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B26" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B27" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -7015,7 +7036,7 @@
         <v>99</v>
       </c>
       <c r="C36" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -7028,1892 +7049,1920 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B38" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B39" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" t="s">
-        <v>184</v>
-      </c>
-      <c r="B41" t="s">
-        <v>593</v>
+        <v>670</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>693</v>
+      </c>
+      <c r="B40" t="s">
+        <v>694</v>
+      </c>
+      <c r="C40" t="s">
+        <v>701</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>107</v>
+        <v>184</v>
       </c>
       <c r="B42" t="s">
-        <v>108</v>
-      </c>
-      <c r="C42" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B43" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C43" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B44" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C44" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B45" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="C45" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B46" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C46" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C47" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B48" t="s">
-        <v>112</v>
+        <v>111</v>
+      </c>
+      <c r="C48" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>204</v>
+        <v>116</v>
       </c>
       <c r="B49" t="s">
-        <v>495</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B50" t="s">
-        <v>594</v>
-      </c>
-      <c r="C50" t="s">
-        <v>590</v>
+        <v>494</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>581</v>
+        <v>205</v>
       </c>
       <c r="B51" t="s">
-        <v>595</v>
+        <v>593</v>
+      </c>
+      <c r="C51" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>548</v>
+        <v>580</v>
       </c>
       <c r="B52" t="s">
-        <v>549</v>
+        <v>594</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>556</v>
+        <v>547</v>
       </c>
       <c r="B53" t="s">
-        <v>633</v>
+        <v>548</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>545</v>
+        <v>555</v>
       </c>
       <c r="B54" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" t="s">
-        <v>158</v>
-      </c>
-      <c r="B56" t="s">
-        <v>121</v>
+        <v>631</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>544</v>
+      </c>
+      <c r="B55" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>122</v>
+        <v>158</v>
       </c>
       <c r="B57" t="s">
-        <v>596</v>
+        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B58" t="s">
-        <v>123</v>
+        <v>595</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>638</v>
+        <v>124</v>
       </c>
       <c r="B59" t="s">
-        <v>639</v>
+        <v>123</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>544</v>
+        <v>636</v>
       </c>
       <c r="B60" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" t="s">
-        <v>186</v>
-      </c>
-      <c r="B62" t="s">
-        <v>187</v>
+        <v>637</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>543</v>
+      </c>
+      <c r="B61" t="s">
+        <v>672</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>125</v>
+        <v>186</v>
       </c>
       <c r="B63" t="s">
-        <v>127</v>
+        <v>187</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B64" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B65" t="s">
-        <v>597</v>
+        <v>128</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B66" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B67" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B68" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B69" t="s">
-        <v>496</v>
-      </c>
-      <c r="C69" t="s">
-        <v>689</v>
+        <v>599</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B70" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C70" t="s">
-        <v>557</v>
+        <v>687</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B71" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C71" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>640</v>
+        <v>144</v>
       </c>
       <c r="B72" t="s">
-        <v>641</v>
+        <v>498</v>
+      </c>
+      <c r="C72" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>543</v>
+        <v>638</v>
       </c>
       <c r="B73" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" t="s">
-        <v>147</v>
-      </c>
-      <c r="B75" t="s">
-        <v>150</v>
+        <v>639</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>542</v>
+      </c>
+      <c r="B74" t="s">
+        <v>673</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B76" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B77" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B78" t="s">
-        <v>582</v>
-      </c>
-      <c r="C78" t="s">
-        <v>694</v>
+        <v>152</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>693</v>
+        <v>145</v>
       </c>
       <c r="B79" t="s">
-        <v>582</v>
+        <v>581</v>
+      </c>
+      <c r="C79" t="s">
+        <v>692</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
+        <v>691</v>
+      </c>
+      <c r="B80" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
         <v>146</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B81" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
-      <c r="A81" t="s">
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
         <v>131</v>
       </c>
-      <c r="B81" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" t="s">
+      <c r="B82" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
         <v>132</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B83" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
-      <c r="A83" t="s">
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>640</v>
+      </c>
+      <c r="B84" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>541</v>
+      </c>
+      <c r="B85" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>188</v>
+      </c>
+      <c r="B87" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>133</v>
+      </c>
+      <c r="B88" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>135</v>
+      </c>
+      <c r="B89" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>134</v>
+      </c>
+      <c r="B90" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>136</v>
+      </c>
+      <c r="B91" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>137</v>
+      </c>
+      <c r="B92" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>630</v>
+      </c>
+      <c r="B93" t="s">
+        <v>697</v>
+      </c>
+      <c r="C93" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
         <v>642</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B94" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
-      <c r="A84" t="s">
-        <v>542</v>
-      </c>
-      <c r="B84" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86" t="s">
-        <v>188</v>
-      </c>
-      <c r="B86" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" t="s">
-        <v>133</v>
-      </c>
-      <c r="B87" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2">
-      <c r="A88" t="s">
-        <v>135</v>
-      </c>
-      <c r="B88" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89" t="s">
-        <v>134</v>
-      </c>
-      <c r="B89" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" t="s">
-        <v>136</v>
-      </c>
-      <c r="B90" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" t="s">
-        <v>137</v>
-      </c>
-      <c r="B91" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" t="s">
-        <v>631</v>
-      </c>
-      <c r="B92" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" t="s">
-        <v>644</v>
-      </c>
-      <c r="B93" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" t="s">
-        <v>541</v>
-      </c>
-      <c r="B94" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
-      <c r="A96" t="s">
-        <v>159</v>
-      </c>
-      <c r="B96" t="s">
-        <v>163</v>
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
+        <v>540</v>
+      </c>
+      <c r="B95" t="s">
+        <v>675</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B97" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B98" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B99" t="s">
-        <v>602</v>
+        <v>165</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>558</v>
+        <v>162</v>
       </c>
       <c r="B100" t="s">
-        <v>559</v>
+        <v>601</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>650</v>
+        <v>557</v>
       </c>
       <c r="B101" t="s">
-        <v>651</v>
+        <v>558</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>540</v>
+        <v>648</v>
       </c>
       <c r="B102" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
-      <c r="A104" t="s">
-        <v>192</v>
-      </c>
-      <c r="B104" t="s">
-        <v>193</v>
+        <v>649</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" t="s">
+        <v>539</v>
+      </c>
+      <c r="B103" t="s">
+        <v>676</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>166</v>
+        <v>192</v>
       </c>
       <c r="B105" t="s">
-        <v>168</v>
+        <v>193</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B106" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>646</v>
+        <v>167</v>
       </c>
       <c r="B107" t="s">
-        <v>647</v>
+        <v>169</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>539</v>
+        <v>644</v>
       </c>
       <c r="B108" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3">
-      <c r="A110" t="s">
-        <v>190</v>
-      </c>
-      <c r="B110" t="s">
-        <v>191</v>
+        <v>645</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" t="s">
+        <v>538</v>
+      </c>
+      <c r="B109" t="s">
+        <v>677</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="B111" t="s">
-        <v>172</v>
-      </c>
-      <c r="C111" t="s">
-        <v>590</v>
+        <v>191</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="B112" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C112" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B113" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C113" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>203</v>
+        <v>171</v>
       </c>
       <c r="B114" t="s">
-        <v>202</v>
+        <v>174</v>
+      </c>
+      <c r="C114" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B115" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
       <c r="B116" t="s">
-        <v>177</v>
-      </c>
-      <c r="C116" t="s">
-        <v>590</v>
+        <v>201</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>648</v>
+        <v>176</v>
       </c>
       <c r="B117" t="s">
-        <v>649</v>
+        <v>177</v>
+      </c>
+      <c r="C117" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>528</v>
+        <v>646</v>
       </c>
       <c r="B118" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3">
-      <c r="A120" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" t="s">
+        <v>527</v>
+      </c>
+      <c r="B119" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" t="s">
+        <v>653</v>
+      </c>
+      <c r="B121" t="s">
+        <v>654</v>
+      </c>
+      <c r="C121" t="s">
         <v>655</v>
-      </c>
-      <c r="B120" t="s">
-        <v>656</v>
-      </c>
-      <c r="C120" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3">
-      <c r="A122" t="s">
-        <v>514</v>
-      </c>
-      <c r="B122" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>664</v>
+        <v>513</v>
       </c>
       <c r="B123" t="s">
-        <v>668</v>
-      </c>
-      <c r="C123" t="s">
-        <v>666</v>
+        <v>514</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="B124" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C124" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>242</v>
+        <v>663</v>
       </c>
       <c r="B125" t="s">
-        <v>243</v>
+        <v>665</v>
       </c>
       <c r="C125" t="s">
-        <v>590</v>
+        <v>664</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B126" t="s">
-        <v>245</v>
+        <v>243</v>
+      </c>
+      <c r="C126" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="B127" t="s">
-        <v>562</v>
-      </c>
-      <c r="C127" t="s">
-        <v>653</v>
+        <v>245</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="B128" t="s">
-        <v>246</v>
+        <v>561</v>
+      </c>
+      <c r="C128" t="s">
+        <v>651</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>504</v>
+        <v>247</v>
       </c>
       <c r="B129" t="s">
-        <v>513</v>
+        <v>246</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>249</v>
+        <v>503</v>
       </c>
       <c r="B130" t="s">
-        <v>248</v>
+        <v>512</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B131" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B132" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B133" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B134" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>302</v>
+        <v>257</v>
       </c>
       <c r="B135" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>349</v>
+        <v>302</v>
       </c>
       <c r="B136" t="s">
-        <v>350</v>
+        <v>248</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>660</v>
+        <v>349</v>
       </c>
       <c r="B137" t="s">
-        <v>661</v>
+        <v>350</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>527</v>
+        <v>658</v>
       </c>
       <c r="B138" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3">
-      <c r="A140" t="s">
-        <v>516</v>
-      </c>
-      <c r="B140" t="s">
-        <v>517</v>
+        <v>659</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" t="s">
+        <v>526</v>
+      </c>
+      <c r="B139" t="s">
+        <v>679</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
+        <v>515</v>
+      </c>
+      <c r="B141" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" t="s">
         <v>259</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B142" t="s">
         <v>262</v>
       </c>
-      <c r="C141" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A142" t="s">
+      <c r="C142" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A143" t="s">
         <v>261</v>
       </c>
-      <c r="B142" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3">
-      <c r="A143" t="s">
-        <v>260</v>
-      </c>
       <c r="B143" t="s">
-        <v>263</v>
+        <v>562</v>
+      </c>
+      <c r="C143" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B144" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B145" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B146" t="s">
-        <v>268</v>
-      </c>
-      <c r="C146" t="s">
-        <v>663</v>
+        <v>267</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>505</v>
+        <v>269</v>
       </c>
       <c r="B147" t="s">
-        <v>572</v>
+        <v>268</v>
+      </c>
+      <c r="C147" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>270</v>
+        <v>504</v>
       </c>
       <c r="B148" t="s">
-        <v>271</v>
+        <v>571</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B149" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B150" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B151" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B152" t="s">
-        <v>285</v>
-      </c>
-      <c r="C152" t="s">
-        <v>663</v>
+        <v>286</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B153" t="s">
-        <v>607</v>
+        <v>285</v>
+      </c>
+      <c r="C153" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B154" t="s">
-        <v>284</v>
-      </c>
-      <c r="C154" t="s">
-        <v>663</v>
+        <v>606</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B155" t="s">
-        <v>283</v>
+        <v>284</v>
+      </c>
+      <c r="C155" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
-        <v>299</v>
+        <v>282</v>
       </c>
       <c r="B156" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B157" t="s">
-        <v>248</v>
+        <v>300</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B158" t="s">
-        <v>305</v>
+        <v>248</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
-        <v>538</v>
+        <v>304</v>
       </c>
       <c r="B159" t="s">
-        <v>682</v>
+        <v>305</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160" t="s">
+        <v>537</v>
+      </c>
+      <c r="B160" t="s">
+        <v>680</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>518</v>
+        <v>695</v>
       </c>
       <c r="B161" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3">
-      <c r="A162" t="s">
-        <v>292</v>
-      </c>
-      <c r="B162" t="s">
-        <v>296</v>
-      </c>
-      <c r="C162" t="s">
-        <v>590</v>
+        <v>696</v>
+      </c>
+      <c r="C161" t="s">
+        <v>701</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>506</v>
+        <v>517</v>
       </c>
       <c r="B163" t="s">
-        <v>573</v>
+        <v>518</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B164" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C164" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
-        <v>294</v>
+        <v>505</v>
       </c>
       <c r="B165" t="s">
-        <v>298</v>
+        <v>572</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B166" t="s">
-        <v>564</v>
+        <v>297</v>
+      </c>
+      <c r="C166" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B167" t="s">
-        <v>248</v>
+        <v>298</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="B168" t="s">
-        <v>310</v>
+        <v>563</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B169" t="s">
-        <v>308</v>
+        <v>248</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B170" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B171" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
-        <v>537</v>
+        <v>307</v>
       </c>
       <c r="B172" t="s">
-        <v>683</v>
+        <v>308</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173" t="s">
+        <v>311</v>
+      </c>
+      <c r="B173" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>520</v>
+        <v>536</v>
       </c>
       <c r="B174" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3">
-      <c r="A175" t="s">
-        <v>500</v>
-      </c>
-      <c r="B175" t="s">
-        <v>320</v>
-      </c>
-      <c r="C175" t="s">
-        <v>590</v>
+        <v>681</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>507</v>
+        <v>519</v>
       </c>
       <c r="B176" t="s">
-        <v>574</v>
+        <v>520</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>315</v>
+        <v>499</v>
       </c>
       <c r="B177" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C177" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>316</v>
+        <v>506</v>
       </c>
       <c r="B178" t="s">
-        <v>322</v>
+        <v>573</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B179" t="s">
-        <v>323</v>
+        <v>321</v>
+      </c>
+      <c r="C179" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B180" t="s">
-        <v>565</v>
+        <v>322</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B181" t="s">
-        <v>248</v>
+        <v>323</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="B182" t="s">
-        <v>325</v>
-      </c>
-      <c r="C182" t="s">
-        <v>590</v>
+        <v>564</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="B183" t="s">
-        <v>327</v>
+        <v>248</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B184" t="s">
-        <v>328</v>
+        <v>325</v>
+      </c>
+      <c r="C184" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B185" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B186" t="s">
-        <v>256</v>
+        <v>328</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" t="s">
-        <v>536</v>
+        <v>330</v>
       </c>
       <c r="B187" t="s">
-        <v>684</v>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188" t="s">
+        <v>332</v>
+      </c>
+      <c r="B188" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" t="s">
-        <v>522</v>
+        <v>535</v>
       </c>
       <c r="B189" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3">
-      <c r="A190" t="s">
-        <v>502</v>
-      </c>
-      <c r="B190" t="s">
-        <v>338</v>
-      </c>
-      <c r="C190" t="s">
-        <v>590</v>
+        <v>682</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" t="s">
-        <v>508</v>
+        <v>521</v>
       </c>
       <c r="B191" t="s">
-        <v>575</v>
+        <v>522</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" t="s">
-        <v>336</v>
+        <v>501</v>
       </c>
       <c r="B192" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C192" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" t="s">
-        <v>337</v>
+        <v>507</v>
       </c>
       <c r="B193" t="s">
-        <v>340</v>
+        <v>574</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>501</v>
+        <v>336</v>
       </c>
       <c r="B194" t="s">
-        <v>566</v>
+        <v>339</v>
+      </c>
+      <c r="C194" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="B195" t="s">
-        <v>248</v>
+        <v>340</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>345</v>
+        <v>500</v>
       </c>
       <c r="B196" t="s">
-        <v>341</v>
+        <v>565</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B197" t="s">
-        <v>342</v>
+        <v>248</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B198" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B199" t="s">
-        <v>256</v>
+        <v>342</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>535</v>
+        <v>347</v>
       </c>
       <c r="B200" t="s">
-        <v>685</v>
+        <v>343</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201" t="s">
+        <v>348</v>
+      </c>
+      <c r="B201" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>552</v>
+        <v>534</v>
       </c>
       <c r="B202" t="s">
-        <v>555</v>
-      </c>
-      <c r="C202" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3">
-      <c r="A203" t="s">
-        <v>553</v>
-      </c>
-      <c r="B203" t="s">
-        <v>554</v>
-      </c>
-      <c r="C203" t="s">
-        <v>589</v>
+        <v>683</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
+        <v>551</v>
+      </c>
+      <c r="B204" t="s">
+        <v>554</v>
+      </c>
+      <c r="C204" t="s">
         <v>587</v>
-      </c>
-      <c r="B204" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
-        <v>365</v>
+        <v>552</v>
       </c>
       <c r="B205" t="s">
-        <v>351</v>
+        <v>553</v>
+      </c>
+      <c r="C205" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
-        <v>366</v>
+        <v>586</v>
       </c>
       <c r="B206" t="s">
-        <v>352</v>
-      </c>
-      <c r="C206" t="s">
-        <v>590</v>
+        <v>602</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" t="s">
-        <v>509</v>
+        <v>365</v>
       </c>
       <c r="B207" t="s">
-        <v>576</v>
+        <v>351</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B208" t="s">
-        <v>353</v>
+        <v>352</v>
+      </c>
+      <c r="C208" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" t="s">
-        <v>368</v>
+        <v>508</v>
       </c>
       <c r="B209" t="s">
-        <v>354</v>
+        <v>575</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B210" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B211" t="s">
-        <v>356</v>
-      </c>
-      <c r="C211" t="s">
-        <v>590</v>
+        <v>354</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B212" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B213" t="s">
-        <v>358</v>
+        <v>356</v>
+      </c>
+      <c r="C213" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B214" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B215" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B216" t="s">
-        <v>361</v>
-      </c>
-      <c r="C216" t="s">
-        <v>590</v>
+        <v>359</v>
       </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B217" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B218" t="s">
-        <v>363</v>
+        <v>361</v>
+      </c>
+      <c r="C218" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B219" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220" t="s">
-        <v>534</v>
+        <v>377</v>
       </c>
       <c r="B220" t="s">
-        <v>669</v>
+        <v>363</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3">
+      <c r="A221" t="s">
+        <v>378</v>
+      </c>
+      <c r="B221" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" t="s">
-        <v>608</v>
+        <v>533</v>
       </c>
       <c r="B222" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3">
-      <c r="A223" t="s">
-        <v>385</v>
-      </c>
-      <c r="B223" t="s">
-        <v>403</v>
+        <v>667</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" t="s">
-        <v>386</v>
+        <v>607</v>
       </c>
       <c r="B224" t="s">
-        <v>400</v>
+        <v>608</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B225" t="s">
-        <v>401</v>
-      </c>
-      <c r="C225" t="s">
-        <v>590</v>
+        <v>403</v>
       </c>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" t="s">
-        <v>510</v>
+        <v>386</v>
       </c>
       <c r="B226" t="s">
-        <v>577</v>
+        <v>400</v>
       </c>
     </row>
     <row r="227" spans="1:3">
       <c r="A227" t="s">
-        <v>404</v>
+        <v>387</v>
       </c>
       <c r="B227" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C227" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" t="s">
-        <v>388</v>
+        <v>509</v>
       </c>
       <c r="B228" t="s">
-        <v>394</v>
+        <v>576</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B229" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C229" t="s">
-        <v>567</v>
+        <v>589</v>
       </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B230" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="231" spans="1:3">
       <c r="A231" t="s">
-        <v>391</v>
+        <v>405</v>
       </c>
       <c r="B231" t="s">
-        <v>397</v>
+        <v>395</v>
+      </c>
+      <c r="C231" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B232" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="233" spans="1:3">
       <c r="A233" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B233" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B234" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="235" spans="1:3">
       <c r="A235" t="s">
-        <v>533</v>
+        <v>392</v>
       </c>
       <c r="B235" t="s">
-        <v>686</v>
+        <v>399</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3">
+      <c r="A236" t="s">
+        <v>393</v>
+      </c>
+      <c r="B236" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" t="s">
-        <v>524</v>
+        <v>532</v>
       </c>
       <c r="B237" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3">
-      <c r="A238" t="s">
-        <v>411</v>
-      </c>
-      <c r="B238" t="s">
-        <v>422</v>
+        <v>684</v>
       </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239" t="s">
-        <v>412</v>
+        <v>523</v>
       </c>
       <c r="B239" t="s">
-        <v>423</v>
-      </c>
-      <c r="C239" t="s">
-        <v>590</v>
+        <v>524</v>
       </c>
     </row>
     <row r="240" spans="1:3">
       <c r="A240" t="s">
-        <v>578</v>
+        <v>411</v>
       </c>
       <c r="B240" t="s">
-        <v>579</v>
+        <v>422</v>
       </c>
     </row>
     <row r="241" spans="1:3">
       <c r="A241" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B241" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C241" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" t="s">
-        <v>414</v>
+        <v>577</v>
       </c>
       <c r="B242" t="s">
-        <v>425</v>
-      </c>
-      <c r="C242" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="243" spans="1:3">
       <c r="A243" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B243" t="s">
-        <v>591</v>
+        <v>424</v>
+      </c>
+      <c r="C243" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="244" spans="1:3">
       <c r="A244" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B244" t="s">
-        <v>426</v>
+        <v>425</v>
+      </c>
+      <c r="C244" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="245" spans="1:3">
       <c r="A245" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B245" t="s">
-        <v>427</v>
+        <v>590</v>
       </c>
     </row>
     <row r="246" spans="1:3">
       <c r="A246" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B246" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="247" spans="1:3">
       <c r="A247" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B247" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="248" spans="1:3">
       <c r="A248" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B248" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="249" spans="1:3">
       <c r="A249" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B249" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="250" spans="1:3">
       <c r="A250" t="s">
-        <v>531</v>
+        <v>420</v>
       </c>
       <c r="B250" t="s">
-        <v>687</v>
+        <v>430</v>
       </c>
     </row>
     <row r="251" spans="1:3">
       <c r="A251" t="s">
-        <v>617</v>
+        <v>421</v>
       </c>
       <c r="B251" t="s">
-        <v>618</v>
+        <v>431</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3">
+      <c r="A252" t="s">
+        <v>530</v>
+      </c>
+      <c r="B252" t="s">
+        <v>685</v>
       </c>
     </row>
     <row r="253" spans="1:3">
       <c r="A253" t="s">
-        <v>526</v>
+        <v>616</v>
       </c>
       <c r="B253" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="254" spans="1:3">
-      <c r="A254" t="s">
-        <v>438</v>
-      </c>
-      <c r="B254" t="s">
-        <v>449</v>
+        <v>617</v>
       </c>
     </row>
     <row r="255" spans="1:3">
       <c r="A255" t="s">
-        <v>439</v>
+        <v>525</v>
       </c>
       <c r="B255" t="s">
-        <v>450</v>
-      </c>
-      <c r="C255" t="s">
-        <v>590</v>
+        <v>524</v>
       </c>
     </row>
     <row r="256" spans="1:3">
       <c r="A256" t="s">
-        <v>511</v>
+        <v>438</v>
       </c>
       <c r="B256" t="s">
-        <v>580</v>
+        <v>449</v>
       </c>
     </row>
     <row r="257" spans="1:3">
       <c r="A257" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B257" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C257" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="258" spans="1:3">
       <c r="A258" t="s">
-        <v>441</v>
+        <v>510</v>
       </c>
       <c r="B258" t="s">
-        <v>452</v>
-      </c>
-      <c r="C258" t="s">
-        <v>590</v>
+        <v>579</v>
       </c>
     </row>
     <row r="259" spans="1:3">
       <c r="A259" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B259" t="s">
-        <v>592</v>
+        <v>451</v>
+      </c>
+      <c r="C259" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="260" spans="1:3">
       <c r="A260" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B260" t="s">
-        <v>426</v>
+        <v>452</v>
+      </c>
+      <c r="C260" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="261" spans="1:3">
       <c r="A261" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B261" t="s">
-        <v>427</v>
+        <v>591</v>
       </c>
     </row>
     <row r="262" spans="1:3">
       <c r="A262" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B262" t="s">
-        <v>453</v>
+        <v>426</v>
       </c>
     </row>
     <row r="263" spans="1:3">
       <c r="A263" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B263" t="s">
-        <v>454</v>
+        <v>427</v>
       </c>
     </row>
     <row r="264" spans="1:3">
       <c r="A264" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B264" t="s">
-        <v>430</v>
+        <v>453</v>
       </c>
     </row>
     <row r="265" spans="1:3">
       <c r="A265" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B265" t="s">
-        <v>431</v>
+        <v>454</v>
       </c>
     </row>
     <row r="266" spans="1:3">
       <c r="A266" t="s">
-        <v>530</v>
+        <v>447</v>
       </c>
       <c r="B266" t="s">
-        <v>687</v>
+        <v>430</v>
       </c>
     </row>
     <row r="267" spans="1:3">
       <c r="A267" t="s">
-        <v>624</v>
+        <v>448</v>
       </c>
       <c r="B267" t="s">
-        <v>618</v>
+        <v>431</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3">
+      <c r="A268" t="s">
+        <v>529</v>
+      </c>
+      <c r="B268" t="s">
+        <v>685</v>
       </c>
     </row>
     <row r="269" spans="1:3">
       <c r="A269" t="s">
-        <v>432</v>
+        <v>623</v>
       </c>
       <c r="B269" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="270" spans="1:3">
-      <c r="A270" t="s">
-        <v>433</v>
-      </c>
-      <c r="B270" t="s">
-        <v>626</v>
-      </c>
-      <c r="C270" t="s">
-        <v>590</v>
+        <v>617</v>
       </c>
     </row>
     <row r="271" spans="1:3">
       <c r="A271" t="s">
-        <v>512</v>
+        <v>432</v>
       </c>
       <c r="B271" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
     </row>
     <row r="272" spans="1:3">
       <c r="A272" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B272" t="s">
-        <v>654</v>
+        <v>625</v>
+      </c>
+      <c r="C272" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="273" spans="1:2">
       <c r="A273" t="s">
-        <v>435</v>
+        <v>511</v>
       </c>
       <c r="B273" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="274" spans="1:2">
       <c r="A274" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B274" t="s">
-        <v>629</v>
+        <v>652</v>
       </c>
     </row>
     <row r="275" spans="1:2">
       <c r="A275" t="s">
-        <v>529</v>
+        <v>435</v>
       </c>
       <c r="B275" t="s">
-        <v>688</v>
+        <v>627</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2">
+      <c r="A276" t="s">
+        <v>436</v>
+      </c>
+      <c r="B276" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2">
+      <c r="A277" t="s">
+        <v>528</v>
+      </c>
+      <c r="B277" t="s">
+        <v>686</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates for Raluca’s assigned user stories
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.malyala\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raluca.ilinca.AzureAI-Jump2\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{418CC419-8DBB-4746-ACE2-3ADD45EC9FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F35D323-08E0-45FF-A8BB-7E1730EFB64D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="22440" windowHeight="11715" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="845" uniqueCount="695">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="702">
   <si>
     <t>Name</t>
   </si>
@@ -1518,9 +1518,6 @@
     <t>VAWA Acknowledgement</t>
   </si>
   <si>
-    <t>C:\Users\harika.malyala\Documents\AZApplicationReview\Prompts\</t>
-  </si>
-  <si>
     <t>Replace_JArraayInJSON</t>
   </si>
   <si>
@@ -1938,9 +1935,6 @@
     <t>SC_AllFullTimeStudents</t>
   </si>
   <si>
-    <t>All household members have been or will be students for the next five months. Manual review required.</t>
-  </si>
-  <si>
     <t>Assets Type and  value does not match that listed on the ICW.</t>
   </si>
   <si>
@@ -2125,6 +2119,33 @@
   </si>
   <si>
     <t>Removed this check as we replace this with below check to see if assitance is mared yes in an arrays 1, 2, 3</t>
+  </si>
+  <si>
+    <t>C:\Users\raluca.ilinca.AzureAI-Jump2\Documents\AZApplicationReview\Prompts\</t>
+  </si>
+  <si>
+    <t>Newly added by Raluca</t>
+  </si>
+  <si>
+    <t>MID_MinorLessThan50Percent</t>
+  </si>
+  <si>
+    <t>A minor will live in the household less than 50% of the time. Manual review required.</t>
+  </si>
+  <si>
+    <t>The applicant has indicated all household contains all students by selecting 2 or 3 to Part A on the Student Certification. Manual review required.</t>
+  </si>
+  <si>
+    <t>Raluca removed this check</t>
+  </si>
+  <si>
+    <t>VOE_PayIncrease</t>
+  </si>
+  <si>
+    <t>Anticipated increase in the base pay over the next 12 months. Manual review required.</t>
+  </si>
+  <si>
+    <t>Raluca updated this check</t>
   </si>
 </sst>
 </file>
@@ -2502,8 +2523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2586,7 +2607,7 @@
         <v>209</v>
       </c>
       <c r="B7" t="s">
-        <v>492</v>
+        <v>693</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -2635,7 +2656,7 @@
         <v>219</v>
       </c>
       <c r="B14" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
@@ -2673,7 +2694,7 @@
         <v>223</v>
       </c>
       <c r="B18" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C18" t="s">
         <v>238</v>
@@ -2695,7 +2716,7 @@
         <v>225</v>
       </c>
       <c r="B20" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
@@ -2711,7 +2732,7 @@
         <v>227</v>
       </c>
       <c r="B22" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
@@ -2778,7 +2799,7 @@
         <v>379</v>
       </c>
       <c r="B30" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
@@ -2810,7 +2831,7 @@
         <v>410</v>
       </c>
       <c r="B34" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
@@ -2858,7 +2879,7 @@
         <v>437</v>
       </c>
       <c r="B40" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
@@ -4172,7 +4193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -4368,15 +4389,15 @@
         <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B21" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
@@ -5418,7 +5439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1011"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
@@ -5548,82 +5569,82 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B12" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B13" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B14" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B15" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B16" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B17" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B18" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B19" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B20" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B21" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1">
@@ -5684,82 +5705,82 @@
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B29" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B30" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1">
       <c r="A31" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B32" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
       <c r="A33" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B33" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B34" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B35" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B36" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B37" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B38" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
@@ -6743,16 +6764,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
-  <dimension ref="A1:C275"/>
+  <dimension ref="A1:C277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
+      <selection activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="126.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="153.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6777,7 +6798,7 @@
         <v>180</v>
       </c>
       <c r="B5" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -6812,31 +6833,31 @@
         <v>207</v>
       </c>
       <c r="C9" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
+        <v>549</v>
+      </c>
+      <c r="B10" t="s">
         <v>550</v>
-      </c>
-      <c r="B10" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B11" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B12" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -6857,10 +6878,10 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
+        <v>559</v>
+      </c>
+      <c r="B16" t="s">
         <v>560</v>
-      </c>
-      <c r="B16" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -6929,26 +6950,26 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B25" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B26" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="B27" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -7015,7 +7036,7 @@
         <v>99</v>
       </c>
       <c r="C36" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -7028,1892 +7049,1920 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B38" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B39" t="s">
-        <v>672</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" t="s">
-        <v>184</v>
-      </c>
-      <c r="B41" t="s">
-        <v>593</v>
+        <v>670</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>695</v>
+      </c>
+      <c r="B40" t="s">
+        <v>696</v>
+      </c>
+      <c r="C40" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>107</v>
+        <v>184</v>
       </c>
       <c r="B42" t="s">
-        <v>108</v>
-      </c>
-      <c r="C42" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B43" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C43" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B44" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C44" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B45" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="C45" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B46" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C46" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B47" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C47" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B48" t="s">
-        <v>112</v>
+        <v>111</v>
+      </c>
+      <c r="C48" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>204</v>
+        <v>116</v>
       </c>
       <c r="B49" t="s">
-        <v>495</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B50" t="s">
-        <v>594</v>
-      </c>
-      <c r="C50" t="s">
-        <v>590</v>
+        <v>494</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>581</v>
+        <v>205</v>
       </c>
       <c r="B51" t="s">
-        <v>595</v>
+        <v>593</v>
+      </c>
+      <c r="C51" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>548</v>
+        <v>580</v>
       </c>
       <c r="B52" t="s">
-        <v>549</v>
+        <v>594</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>556</v>
+        <v>547</v>
       </c>
       <c r="B53" t="s">
-        <v>633</v>
+        <v>548</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>545</v>
+        <v>555</v>
       </c>
       <c r="B54" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" t="s">
-        <v>158</v>
-      </c>
-      <c r="B56" t="s">
-        <v>121</v>
+        <v>631</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>544</v>
+      </c>
+      <c r="B55" t="s">
+        <v>671</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>122</v>
+        <v>158</v>
       </c>
       <c r="B57" t="s">
-        <v>596</v>
+        <v>121</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B58" t="s">
-        <v>123</v>
+        <v>595</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>638</v>
+        <v>124</v>
       </c>
       <c r="B59" t="s">
-        <v>639</v>
+        <v>123</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>544</v>
+        <v>636</v>
       </c>
       <c r="B60" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" t="s">
-        <v>186</v>
-      </c>
-      <c r="B62" t="s">
-        <v>187</v>
+        <v>637</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>543</v>
+      </c>
+      <c r="B61" t="s">
+        <v>672</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>125</v>
+        <v>186</v>
       </c>
       <c r="B63" t="s">
-        <v>127</v>
+        <v>187</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B64" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B65" t="s">
-        <v>597</v>
+        <v>128</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B66" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B67" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B68" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B69" t="s">
-        <v>496</v>
-      </c>
-      <c r="C69" t="s">
-        <v>689</v>
+        <v>599</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B70" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C70" t="s">
-        <v>557</v>
+        <v>687</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B71" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C71" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>640</v>
+        <v>144</v>
       </c>
       <c r="B72" t="s">
-        <v>641</v>
+        <v>498</v>
+      </c>
+      <c r="C72" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>543</v>
+        <v>638</v>
       </c>
       <c r="B73" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" t="s">
-        <v>147</v>
-      </c>
-      <c r="B75" t="s">
-        <v>150</v>
+        <v>639</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>542</v>
+      </c>
+      <c r="B74" t="s">
+        <v>673</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B76" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B77" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B78" t="s">
-        <v>582</v>
-      </c>
-      <c r="C78" t="s">
-        <v>694</v>
+        <v>152</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>693</v>
+        <v>145</v>
       </c>
       <c r="B79" t="s">
-        <v>582</v>
+        <v>581</v>
+      </c>
+      <c r="C79" t="s">
+        <v>692</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
+        <v>691</v>
+      </c>
+      <c r="B80" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
         <v>146</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B81" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
-      <c r="A81" t="s">
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
         <v>131</v>
       </c>
-      <c r="B81" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
-      <c r="A82" t="s">
+      <c r="B82" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
         <v>132</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B83" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
-      <c r="A83" t="s">
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>640</v>
+      </c>
+      <c r="B84" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>541</v>
+      </c>
+      <c r="B85" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>188</v>
+      </c>
+      <c r="B87" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>133</v>
+      </c>
+      <c r="B88" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>135</v>
+      </c>
+      <c r="B89" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>134</v>
+      </c>
+      <c r="B90" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>136</v>
+      </c>
+      <c r="B91" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>137</v>
+      </c>
+      <c r="B92" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>630</v>
+      </c>
+      <c r="B93" t="s">
+        <v>697</v>
+      </c>
+      <c r="C93" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
         <v>642</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B94" t="s">
         <v>643</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
-      <c r="A84" t="s">
-        <v>542</v>
-      </c>
-      <c r="B84" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
-      <c r="A86" t="s">
-        <v>188</v>
-      </c>
-      <c r="B86" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" t="s">
-        <v>133</v>
-      </c>
-      <c r="B87" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2">
-      <c r="A88" t="s">
-        <v>135</v>
-      </c>
-      <c r="B88" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89" t="s">
-        <v>134</v>
-      </c>
-      <c r="B89" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" t="s">
-        <v>136</v>
-      </c>
-      <c r="B90" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" t="s">
-        <v>137</v>
-      </c>
-      <c r="B91" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" t="s">
-        <v>631</v>
-      </c>
-      <c r="B92" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" t="s">
-        <v>644</v>
-      </c>
-      <c r="B93" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
-      <c r="A94" t="s">
-        <v>541</v>
-      </c>
-      <c r="B94" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
-      <c r="A96" t="s">
-        <v>159</v>
-      </c>
-      <c r="B96" t="s">
-        <v>163</v>
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
+        <v>540</v>
+      </c>
+      <c r="B95" t="s">
+        <v>675</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B97" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B98" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B99" t="s">
-        <v>602</v>
+        <v>165</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>558</v>
+        <v>162</v>
       </c>
       <c r="B100" t="s">
-        <v>559</v>
+        <v>601</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>650</v>
+        <v>557</v>
       </c>
       <c r="B101" t="s">
-        <v>651</v>
+        <v>558</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>540</v>
+        <v>648</v>
       </c>
       <c r="B102" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
-      <c r="A104" t="s">
-        <v>192</v>
-      </c>
-      <c r="B104" t="s">
-        <v>193</v>
+        <v>649</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" t="s">
+        <v>539</v>
+      </c>
+      <c r="B103" t="s">
+        <v>676</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>166</v>
+        <v>192</v>
       </c>
       <c r="B105" t="s">
-        <v>168</v>
+        <v>193</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B106" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>646</v>
+        <v>167</v>
       </c>
       <c r="B107" t="s">
-        <v>647</v>
+        <v>169</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>539</v>
+        <v>644</v>
       </c>
       <c r="B108" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3">
-      <c r="A110" t="s">
-        <v>190</v>
-      </c>
-      <c r="B110" t="s">
-        <v>191</v>
+        <v>645</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" t="s">
+        <v>538</v>
+      </c>
+      <c r="B109" t="s">
+        <v>677</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="B111" t="s">
-        <v>172</v>
-      </c>
-      <c r="C111" t="s">
-        <v>590</v>
+        <v>191</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="B112" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C112" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B113" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C113" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>203</v>
+        <v>171</v>
       </c>
       <c r="B114" t="s">
-        <v>202</v>
+        <v>174</v>
+      </c>
+      <c r="C114" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B115" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
       <c r="B116" t="s">
-        <v>177</v>
-      </c>
-      <c r="C116" t="s">
-        <v>590</v>
+        <v>201</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>648</v>
+        <v>176</v>
       </c>
       <c r="B117" t="s">
-        <v>649</v>
+        <v>177</v>
+      </c>
+      <c r="C117" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>528</v>
+        <v>646</v>
       </c>
       <c r="B118" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3">
-      <c r="A120" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" t="s">
+        <v>527</v>
+      </c>
+      <c r="B119" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" t="s">
+        <v>653</v>
+      </c>
+      <c r="B121" t="s">
+        <v>654</v>
+      </c>
+      <c r="C121" t="s">
         <v>655</v>
-      </c>
-      <c r="B120" t="s">
-        <v>656</v>
-      </c>
-      <c r="C120" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3">
-      <c r="A122" t="s">
-        <v>514</v>
-      </c>
-      <c r="B122" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>664</v>
+        <v>513</v>
       </c>
       <c r="B123" t="s">
-        <v>668</v>
-      </c>
-      <c r="C123" t="s">
-        <v>666</v>
+        <v>514</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="B124" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C124" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>242</v>
+        <v>663</v>
       </c>
       <c r="B125" t="s">
-        <v>243</v>
+        <v>665</v>
       </c>
       <c r="C125" t="s">
-        <v>590</v>
+        <v>664</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B126" t="s">
-        <v>245</v>
+        <v>243</v>
+      </c>
+      <c r="C126" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="B127" t="s">
-        <v>562</v>
-      </c>
-      <c r="C127" t="s">
-        <v>653</v>
+        <v>245</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="B128" t="s">
-        <v>246</v>
+        <v>561</v>
+      </c>
+      <c r="C128" t="s">
+        <v>651</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>504</v>
+        <v>247</v>
       </c>
       <c r="B129" t="s">
-        <v>513</v>
+        <v>246</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>249</v>
+        <v>503</v>
       </c>
       <c r="B130" t="s">
-        <v>248</v>
+        <v>512</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B131" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B132" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B133" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B134" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>302</v>
+        <v>257</v>
       </c>
       <c r="B135" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>349</v>
+        <v>302</v>
       </c>
       <c r="B136" t="s">
-        <v>350</v>
+        <v>248</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>660</v>
+        <v>349</v>
       </c>
       <c r="B137" t="s">
-        <v>661</v>
+        <v>350</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>527</v>
+        <v>658</v>
       </c>
       <c r="B138" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="140" spans="1:3">
-      <c r="A140" t="s">
-        <v>516</v>
-      </c>
-      <c r="B140" t="s">
-        <v>517</v>
+        <v>659</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" t="s">
+        <v>526</v>
+      </c>
+      <c r="B139" t="s">
+        <v>679</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
+        <v>515</v>
+      </c>
+      <c r="B141" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" t="s">
         <v>259</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B142" t="s">
         <v>262</v>
       </c>
-      <c r="C141" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="142" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A142" t="s">
+      <c r="C142" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A143" t="s">
         <v>261</v>
       </c>
-      <c r="B142" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3">
-      <c r="A143" t="s">
-        <v>260</v>
-      </c>
       <c r="B143" t="s">
-        <v>263</v>
+        <v>562</v>
+      </c>
+      <c r="C143" t="s">
+        <v>698</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B144" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B145" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B146" t="s">
-        <v>268</v>
-      </c>
-      <c r="C146" t="s">
-        <v>663</v>
+        <v>267</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>505</v>
+        <v>269</v>
       </c>
       <c r="B147" t="s">
-        <v>572</v>
+        <v>268</v>
+      </c>
+      <c r="C147" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>270</v>
+        <v>504</v>
       </c>
       <c r="B148" t="s">
-        <v>271</v>
+        <v>571</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B149" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B150" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B151" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B152" t="s">
-        <v>285</v>
-      </c>
-      <c r="C152" t="s">
-        <v>663</v>
+        <v>286</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B153" t="s">
-        <v>607</v>
+        <v>285</v>
+      </c>
+      <c r="C153" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B154" t="s">
-        <v>284</v>
-      </c>
-      <c r="C154" t="s">
-        <v>663</v>
+        <v>606</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B155" t="s">
-        <v>283</v>
+        <v>284</v>
+      </c>
+      <c r="C155" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
-        <v>299</v>
+        <v>282</v>
       </c>
       <c r="B156" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B157" t="s">
-        <v>248</v>
+        <v>300</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B158" t="s">
-        <v>305</v>
+        <v>248</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
-        <v>538</v>
+        <v>304</v>
       </c>
       <c r="B159" t="s">
-        <v>682</v>
+        <v>305</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160" t="s">
+        <v>537</v>
+      </c>
+      <c r="B160" t="s">
+        <v>680</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>518</v>
+        <v>699</v>
       </c>
       <c r="B161" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3">
-      <c r="A162" t="s">
-        <v>292</v>
-      </c>
-      <c r="B162" t="s">
-        <v>296</v>
-      </c>
-      <c r="C162" t="s">
-        <v>590</v>
+        <v>700</v>
+      </c>
+      <c r="C161" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>506</v>
+        <v>517</v>
       </c>
       <c r="B163" t="s">
-        <v>573</v>
+        <v>518</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B164" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C164" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
-        <v>294</v>
+        <v>505</v>
       </c>
       <c r="B165" t="s">
-        <v>298</v>
+        <v>572</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B166" t="s">
-        <v>564</v>
+        <v>297</v>
+      </c>
+      <c r="C166" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B167" t="s">
-        <v>248</v>
+        <v>298</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="B168" t="s">
-        <v>310</v>
+        <v>563</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B169" t="s">
-        <v>308</v>
+        <v>248</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B170" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B171" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
-        <v>537</v>
+        <v>307</v>
       </c>
       <c r="B172" t="s">
-        <v>683</v>
+        <v>308</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173" t="s">
+        <v>311</v>
+      </c>
+      <c r="B173" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>520</v>
+        <v>536</v>
       </c>
       <c r="B174" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3">
-      <c r="A175" t="s">
-        <v>500</v>
-      </c>
-      <c r="B175" t="s">
-        <v>320</v>
-      </c>
-      <c r="C175" t="s">
-        <v>590</v>
+        <v>681</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>507</v>
+        <v>519</v>
       </c>
       <c r="B176" t="s">
-        <v>574</v>
+        <v>520</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>315</v>
+        <v>499</v>
       </c>
       <c r="B177" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C177" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>316</v>
+        <v>506</v>
       </c>
       <c r="B178" t="s">
-        <v>322</v>
+        <v>573</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="B179" t="s">
-        <v>323</v>
+        <v>321</v>
+      </c>
+      <c r="C179" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B180" t="s">
-        <v>565</v>
+        <v>322</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B181" t="s">
-        <v>248</v>
+        <v>323</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="B182" t="s">
-        <v>325</v>
-      </c>
-      <c r="C182" t="s">
-        <v>590</v>
+        <v>564</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="B183" t="s">
-        <v>327</v>
+        <v>248</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B184" t="s">
-        <v>328</v>
+        <v>325</v>
+      </c>
+      <c r="C184" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B185" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="B186" t="s">
-        <v>256</v>
+        <v>328</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" t="s">
-        <v>536</v>
+        <v>330</v>
       </c>
       <c r="B187" t="s">
-        <v>684</v>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3">
+      <c r="A188" t="s">
+        <v>332</v>
+      </c>
+      <c r="B188" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" t="s">
-        <v>522</v>
+        <v>535</v>
       </c>
       <c r="B189" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3">
-      <c r="A190" t="s">
-        <v>502</v>
-      </c>
-      <c r="B190" t="s">
-        <v>338</v>
-      </c>
-      <c r="C190" t="s">
-        <v>590</v>
+        <v>682</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" t="s">
-        <v>508</v>
+        <v>521</v>
       </c>
       <c r="B191" t="s">
-        <v>575</v>
+        <v>522</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" t="s">
-        <v>336</v>
+        <v>501</v>
       </c>
       <c r="B192" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C192" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" t="s">
-        <v>337</v>
+        <v>507</v>
       </c>
       <c r="B193" t="s">
-        <v>340</v>
+        <v>574</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>501</v>
+        <v>336</v>
       </c>
       <c r="B194" t="s">
-        <v>566</v>
+        <v>339</v>
+      </c>
+      <c r="C194" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="B195" t="s">
-        <v>248</v>
+        <v>340</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>345</v>
+        <v>500</v>
       </c>
       <c r="B196" t="s">
-        <v>341</v>
+        <v>565</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="B197" t="s">
-        <v>342</v>
+        <v>248</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B198" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B199" t="s">
-        <v>256</v>
+        <v>342</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>535</v>
+        <v>347</v>
       </c>
       <c r="B200" t="s">
-        <v>685</v>
+        <v>343</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3">
+      <c r="A201" t="s">
+        <v>348</v>
+      </c>
+      <c r="B201" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>552</v>
+        <v>534</v>
       </c>
       <c r="B202" t="s">
-        <v>555</v>
-      </c>
-      <c r="C202" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3">
-      <c r="A203" t="s">
-        <v>553</v>
-      </c>
-      <c r="B203" t="s">
-        <v>554</v>
-      </c>
-      <c r="C203" t="s">
-        <v>589</v>
+        <v>683</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
+        <v>551</v>
+      </c>
+      <c r="B204" t="s">
+        <v>554</v>
+      </c>
+      <c r="C204" t="s">
         <v>587</v>
-      </c>
-      <c r="B204" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
-        <v>365</v>
+        <v>552</v>
       </c>
       <c r="B205" t="s">
-        <v>351</v>
+        <v>553</v>
+      </c>
+      <c r="C205" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
-        <v>366</v>
+        <v>586</v>
       </c>
       <c r="B206" t="s">
-        <v>352</v>
-      </c>
-      <c r="C206" t="s">
-        <v>590</v>
+        <v>602</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" t="s">
-        <v>509</v>
+        <v>365</v>
       </c>
       <c r="B207" t="s">
-        <v>576</v>
+        <v>351</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B208" t="s">
-        <v>353</v>
+        <v>352</v>
+      </c>
+      <c r="C208" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" t="s">
-        <v>368</v>
+        <v>508</v>
       </c>
       <c r="B209" t="s">
-        <v>354</v>
+        <v>575</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B210" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="B211" t="s">
-        <v>356</v>
-      </c>
-      <c r="C211" t="s">
-        <v>590</v>
+        <v>354</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B212" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B213" t="s">
-        <v>358</v>
+        <v>356</v>
+      </c>
+      <c r="C213" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="B214" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B215" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B216" t="s">
-        <v>361</v>
-      </c>
-      <c r="C216" t="s">
-        <v>590</v>
+        <v>359</v>
       </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B217" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B218" t="s">
-        <v>363</v>
+        <v>361</v>
+      </c>
+      <c r="C218" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="B219" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220" t="s">
-        <v>534</v>
+        <v>377</v>
       </c>
       <c r="B220" t="s">
-        <v>669</v>
+        <v>363</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3">
+      <c r="A221" t="s">
+        <v>378</v>
+      </c>
+      <c r="B221" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" t="s">
-        <v>608</v>
+        <v>533</v>
       </c>
       <c r="B222" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3">
-      <c r="A223" t="s">
-        <v>385</v>
-      </c>
-      <c r="B223" t="s">
-        <v>403</v>
+        <v>667</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" t="s">
-        <v>386</v>
+        <v>607</v>
       </c>
       <c r="B224" t="s">
-        <v>400</v>
+        <v>608</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B225" t="s">
-        <v>401</v>
-      </c>
-      <c r="C225" t="s">
-        <v>590</v>
+        <v>403</v>
       </c>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" t="s">
-        <v>510</v>
+        <v>386</v>
       </c>
       <c r="B226" t="s">
-        <v>577</v>
+        <v>400</v>
       </c>
     </row>
     <row r="227" spans="1:3">
       <c r="A227" t="s">
-        <v>404</v>
+        <v>387</v>
       </c>
       <c r="B227" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C227" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" t="s">
-        <v>388</v>
+        <v>509</v>
       </c>
       <c r="B228" t="s">
-        <v>394</v>
+        <v>576</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B229" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C229" t="s">
-        <v>567</v>
+        <v>589</v>
       </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B230" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="231" spans="1:3">
       <c r="A231" t="s">
-        <v>391</v>
+        <v>405</v>
       </c>
       <c r="B231" t="s">
-        <v>397</v>
+        <v>395</v>
+      </c>
+      <c r="C231" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B232" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="233" spans="1:3">
       <c r="A233" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B233" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B234" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="235" spans="1:3">
       <c r="A235" t="s">
-        <v>533</v>
+        <v>392</v>
       </c>
       <c r="B235" t="s">
-        <v>686</v>
+        <v>399</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3">
+      <c r="A236" t="s">
+        <v>393</v>
+      </c>
+      <c r="B236" t="s">
+        <v>396</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" t="s">
-        <v>524</v>
+        <v>532</v>
       </c>
       <c r="B237" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3">
-      <c r="A238" t="s">
-        <v>411</v>
-      </c>
-      <c r="B238" t="s">
-        <v>422</v>
+        <v>684</v>
       </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239" t="s">
-        <v>412</v>
+        <v>523</v>
       </c>
       <c r="B239" t="s">
-        <v>423</v>
-      </c>
-      <c r="C239" t="s">
-        <v>590</v>
+        <v>524</v>
       </c>
     </row>
     <row r="240" spans="1:3">
       <c r="A240" t="s">
-        <v>578</v>
+        <v>411</v>
       </c>
       <c r="B240" t="s">
-        <v>579</v>
+        <v>422</v>
       </c>
     </row>
     <row r="241" spans="1:3">
       <c r="A241" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B241" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C241" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" t="s">
-        <v>414</v>
+        <v>577</v>
       </c>
       <c r="B242" t="s">
-        <v>425</v>
-      </c>
-      <c r="C242" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="243" spans="1:3">
       <c r="A243" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B243" t="s">
-        <v>591</v>
+        <v>424</v>
+      </c>
+      <c r="C243" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="244" spans="1:3">
       <c r="A244" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B244" t="s">
-        <v>426</v>
+        <v>425</v>
+      </c>
+      <c r="C244" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="245" spans="1:3">
       <c r="A245" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B245" t="s">
-        <v>427</v>
+        <v>590</v>
       </c>
     </row>
     <row r="246" spans="1:3">
       <c r="A246" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B246" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="247" spans="1:3">
       <c r="A247" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B247" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="248" spans="1:3">
       <c r="A248" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B248" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="249" spans="1:3">
       <c r="A249" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B249" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="250" spans="1:3">
       <c r="A250" t="s">
-        <v>531</v>
+        <v>420</v>
       </c>
       <c r="B250" t="s">
-        <v>687</v>
+        <v>430</v>
       </c>
     </row>
     <row r="251" spans="1:3">
       <c r="A251" t="s">
-        <v>617</v>
+        <v>421</v>
       </c>
       <c r="B251" t="s">
-        <v>618</v>
+        <v>431</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3">
+      <c r="A252" t="s">
+        <v>530</v>
+      </c>
+      <c r="B252" t="s">
+        <v>685</v>
       </c>
     </row>
     <row r="253" spans="1:3">
       <c r="A253" t="s">
-        <v>526</v>
+        <v>616</v>
       </c>
       <c r="B253" t="s">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="254" spans="1:3">
-      <c r="A254" t="s">
-        <v>438</v>
-      </c>
-      <c r="B254" t="s">
-        <v>449</v>
+        <v>617</v>
       </c>
     </row>
     <row r="255" spans="1:3">
       <c r="A255" t="s">
-        <v>439</v>
+        <v>525</v>
       </c>
       <c r="B255" t="s">
-        <v>450</v>
-      </c>
-      <c r="C255" t="s">
-        <v>590</v>
+        <v>524</v>
       </c>
     </row>
     <row r="256" spans="1:3">
       <c r="A256" t="s">
-        <v>511</v>
+        <v>438</v>
       </c>
       <c r="B256" t="s">
-        <v>580</v>
+        <v>449</v>
       </c>
     </row>
     <row r="257" spans="1:3">
       <c r="A257" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B257" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C257" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="258" spans="1:3">
       <c r="A258" t="s">
-        <v>441</v>
+        <v>510</v>
       </c>
       <c r="B258" t="s">
-        <v>452</v>
-      </c>
-      <c r="C258" t="s">
-        <v>590</v>
+        <v>579</v>
       </c>
     </row>
     <row r="259" spans="1:3">
       <c r="A259" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B259" t="s">
-        <v>592</v>
+        <v>451</v>
+      </c>
+      <c r="C259" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="260" spans="1:3">
       <c r="A260" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B260" t="s">
-        <v>426</v>
+        <v>452</v>
+      </c>
+      <c r="C260" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="261" spans="1:3">
       <c r="A261" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B261" t="s">
-        <v>427</v>
+        <v>591</v>
       </c>
     </row>
     <row r="262" spans="1:3">
       <c r="A262" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B262" t="s">
-        <v>453</v>
+        <v>426</v>
       </c>
     </row>
     <row r="263" spans="1:3">
       <c r="A263" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B263" t="s">
-        <v>454</v>
+        <v>427</v>
       </c>
     </row>
     <row r="264" spans="1:3">
       <c r="A264" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B264" t="s">
-        <v>430</v>
+        <v>453</v>
       </c>
     </row>
     <row r="265" spans="1:3">
       <c r="A265" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B265" t="s">
-        <v>431</v>
+        <v>454</v>
       </c>
     </row>
     <row r="266" spans="1:3">
       <c r="A266" t="s">
-        <v>530</v>
+        <v>447</v>
       </c>
       <c r="B266" t="s">
-        <v>687</v>
+        <v>430</v>
       </c>
     </row>
     <row r="267" spans="1:3">
       <c r="A267" t="s">
-        <v>624</v>
+        <v>448</v>
       </c>
       <c r="B267" t="s">
-        <v>618</v>
+        <v>431</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3">
+      <c r="A268" t="s">
+        <v>529</v>
+      </c>
+      <c r="B268" t="s">
+        <v>685</v>
       </c>
     </row>
     <row r="269" spans="1:3">
       <c r="A269" t="s">
-        <v>432</v>
+        <v>623</v>
       </c>
       <c r="B269" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="270" spans="1:3">
-      <c r="A270" t="s">
-        <v>433</v>
-      </c>
-      <c r="B270" t="s">
-        <v>626</v>
-      </c>
-      <c r="C270" t="s">
-        <v>590</v>
+        <v>617</v>
       </c>
     </row>
     <row r="271" spans="1:3">
       <c r="A271" t="s">
-        <v>512</v>
+        <v>432</v>
       </c>
       <c r="B271" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
     </row>
     <row r="272" spans="1:3">
       <c r="A272" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B272" t="s">
-        <v>654</v>
+        <v>625</v>
+      </c>
+      <c r="C272" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="273" spans="1:2">
       <c r="A273" t="s">
-        <v>435</v>
+        <v>511</v>
       </c>
       <c r="B273" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="274" spans="1:2">
       <c r="A274" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B274" t="s">
-        <v>629</v>
+        <v>652</v>
       </c>
     </row>
     <row r="275" spans="1:2">
       <c r="A275" t="s">
-        <v>529</v>
+        <v>435</v>
       </c>
       <c r="B275" t="s">
-        <v>688</v>
+        <v>627</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2">
+      <c r="A276" t="s">
+        <v>436</v>
+      </c>
+      <c r="B276" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2">
+      <c r="A277" t="s">
+        <v>528</v>
+      </c>
+      <c r="B277" t="s">
+        <v>686</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update to config file to match dev branch config
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raluca.ilinca.AzureAI-Jump2\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.malyala\Desktop\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F35D323-08E0-45FF-A8BB-7E1730EFB64D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B1BFC1-F95F-406E-80DD-E8DDEF7C0110}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="22440" windowHeight="11715" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="708">
   <si>
     <t>Name</t>
   </si>
@@ -2146,6 +2146,24 @@
   </si>
   <si>
     <t>Raluca updated this check</t>
+  </si>
+  <si>
+    <t>PS_MultipleIncomeDocsExists</t>
+  </si>
+  <si>
+    <t>Multiple employment documents provided for same employment. Can't determine which employment document to use to validate Exact Day Calculator. Manual review required.</t>
+  </si>
+  <si>
+    <t>VOE_MultipleIncomeDocsExists</t>
+  </si>
+  <si>
+    <t>OL_MultipleIncomeDocsExists</t>
+  </si>
+  <si>
+    <t>WN_MultipleIncomeDocsExists</t>
+  </si>
+  <si>
+    <t>VS_MultipleIncomeDocsExists</t>
   </si>
 </sst>
 </file>
@@ -6764,10 +6782,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
-  <dimension ref="A1:C277"/>
+  <dimension ref="A1:C282"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" topLeftCell="A261" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7057,21 +7075,21 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>545</v>
+        <v>695</v>
       </c>
       <c r="B39" t="s">
-        <v>670</v>
+        <v>696</v>
+      </c>
+      <c r="C39" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>695</v>
+        <v>545</v>
       </c>
       <c r="B40" t="s">
-        <v>696</v>
-      </c>
-      <c r="C40" t="s">
-        <v>694</v>
+        <v>670</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -7843,231 +7861,228 @@
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
+        <v>702</v>
+      </c>
+      <c r="B139" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" t="s">
         <v>526</v>
       </c>
-      <c r="B139" t="s">
+      <c r="B140" t="s">
         <v>679</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3">
-      <c r="A141" t="s">
-        <v>515</v>
-      </c>
-      <c r="B141" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>259</v>
+        <v>515</v>
       </c>
       <c r="B142" t="s">
-        <v>262</v>
-      </c>
-      <c r="C142" t="s">
-        <v>661</v>
+        <v>516</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="13.5" customHeight="1">
       <c r="A143" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B143" t="s">
-        <v>562</v>
+        <v>262</v>
       </c>
       <c r="C143" t="s">
-        <v>698</v>
+        <v>661</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B144" t="s">
-        <v>263</v>
+        <v>562</v>
+      </c>
+      <c r="C144" t="s">
+        <v>698</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B145" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B146" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B147" t="s">
-        <v>268</v>
-      </c>
-      <c r="C147" t="s">
-        <v>661</v>
+        <v>267</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>504</v>
+        <v>269</v>
       </c>
       <c r="B148" t="s">
-        <v>571</v>
+        <v>268</v>
+      </c>
+      <c r="C148" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>270</v>
+        <v>504</v>
       </c>
       <c r="B149" t="s">
-        <v>271</v>
+        <v>571</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B150" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B151" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B152" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B153" t="s">
-        <v>285</v>
-      </c>
-      <c r="C153" t="s">
-        <v>661</v>
+        <v>286</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B154" t="s">
-        <v>606</v>
+        <v>285</v>
+      </c>
+      <c r="C154" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B155" t="s">
-        <v>284</v>
-      </c>
-      <c r="C155" t="s">
-        <v>661</v>
+        <v>606</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B156" t="s">
-        <v>283</v>
+        <v>284</v>
+      </c>
+      <c r="C156" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>299</v>
+        <v>282</v>
       </c>
       <c r="B157" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B158" t="s">
-        <v>248</v>
+        <v>300</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B159" t="s">
-        <v>305</v>
+        <v>248</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" t="s">
-        <v>537</v>
+        <v>304</v>
       </c>
       <c r="B160" t="s">
-        <v>680</v>
+        <v>305</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
+        <v>704</v>
+      </c>
+      <c r="B161" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162" t="s">
         <v>699</v>
       </c>
-      <c r="B161" t="s">
+      <c r="B162" t="s">
         <v>700</v>
       </c>
-      <c r="C161" t="s">
+      <c r="C162" t="s">
         <v>694</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>517</v>
+        <v>537</v>
       </c>
       <c r="B163" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3">
-      <c r="A164" t="s">
-        <v>292</v>
-      </c>
-      <c r="B164" t="s">
-        <v>296</v>
-      </c>
-      <c r="C164" t="s">
-        <v>589</v>
+        <v>680</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
-        <v>505</v>
+        <v>517</v>
       </c>
       <c r="B165" t="s">
-        <v>572</v>
+        <v>518</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B166" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C166" t="s">
         <v>589</v>
@@ -8075,378 +8090,378 @@
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
-        <v>294</v>
+        <v>505</v>
       </c>
       <c r="B167" t="s">
-        <v>298</v>
+        <v>572</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B168" t="s">
-        <v>563</v>
+        <v>297</v>
+      </c>
+      <c r="C168" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B169" t="s">
-        <v>248</v>
+        <v>298</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="B170" t="s">
-        <v>310</v>
+        <v>563</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="B171" t="s">
-        <v>308</v>
+        <v>248</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="B172" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="B173" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>536</v>
+        <v>307</v>
       </c>
       <c r="B174" t="s">
-        <v>681</v>
+        <v>308</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
+      <c r="A175" t="s">
+        <v>311</v>
+      </c>
+      <c r="B175" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>519</v>
+        <v>705</v>
       </c>
       <c r="B176" t="s">
-        <v>520</v>
+        <v>703</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>499</v>
+        <v>536</v>
       </c>
       <c r="B177" t="s">
-        <v>320</v>
-      </c>
-      <c r="C177" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3">
-      <c r="A178" t="s">
-        <v>506</v>
-      </c>
-      <c r="B178" t="s">
-        <v>573</v>
+        <v>681</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>315</v>
+        <v>519</v>
       </c>
       <c r="B179" t="s">
-        <v>321</v>
-      </c>
-      <c r="C179" t="s">
-        <v>589</v>
+        <v>520</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>316</v>
+        <v>499</v>
       </c>
       <c r="B180" t="s">
-        <v>322</v>
+        <v>320</v>
+      </c>
+      <c r="C180" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
-        <v>317</v>
+        <v>506</v>
       </c>
       <c r="B181" t="s">
-        <v>323</v>
+        <v>573</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B182" t="s">
-        <v>564</v>
+        <v>321</v>
+      </c>
+      <c r="C182" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B183" t="s">
-        <v>248</v>
+        <v>322</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="B184" t="s">
-        <v>325</v>
-      </c>
-      <c r="C184" t="s">
-        <v>589</v>
+        <v>323</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="B185" t="s">
-        <v>327</v>
+        <v>564</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="B186" t="s">
-        <v>328</v>
+        <v>248</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="B187" t="s">
-        <v>331</v>
+        <v>325</v>
+      </c>
+      <c r="C187" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="B188" t="s">
-        <v>256</v>
+        <v>327</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" t="s">
-        <v>535</v>
+        <v>329</v>
       </c>
       <c r="B189" t="s">
-        <v>682</v>
+        <v>328</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190" t="s">
+        <v>330</v>
+      </c>
+      <c r="B190" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" t="s">
-        <v>521</v>
+        <v>332</v>
       </c>
       <c r="B191" t="s">
-        <v>522</v>
+        <v>256</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" t="s">
-        <v>501</v>
+        <v>706</v>
       </c>
       <c r="B192" t="s">
-        <v>338</v>
-      </c>
-      <c r="C192" t="s">
-        <v>589</v>
+        <v>703</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" t="s">
-        <v>507</v>
+        <v>535</v>
       </c>
       <c r="B193" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3">
-      <c r="A194" t="s">
-        <v>336</v>
-      </c>
-      <c r="B194" t="s">
-        <v>339</v>
-      </c>
-      <c r="C194" t="s">
-        <v>589</v>
+        <v>682</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>337</v>
+        <v>521</v>
       </c>
       <c r="B195" t="s">
-        <v>340</v>
+        <v>522</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="B196" t="s">
-        <v>565</v>
+        <v>338</v>
+      </c>
+      <c r="C196" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
-        <v>344</v>
+        <v>507</v>
       </c>
       <c r="B197" t="s">
-        <v>248</v>
+        <v>574</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="B198" t="s">
-        <v>341</v>
+        <v>339</v>
+      </c>
+      <c r="C198" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="B199" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>347</v>
+        <v>500</v>
       </c>
       <c r="B200" t="s">
-        <v>343</v>
+        <v>565</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B201" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>534</v>
+        <v>345</v>
       </c>
       <c r="B202" t="s">
-        <v>683</v>
+        <v>341</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3">
+      <c r="A203" t="s">
+        <v>346</v>
+      </c>
+      <c r="B203" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
-        <v>551</v>
+        <v>347</v>
       </c>
       <c r="B204" t="s">
-        <v>554</v>
-      </c>
-      <c r="C204" t="s">
-        <v>587</v>
+        <v>343</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
-        <v>552</v>
+        <v>348</v>
       </c>
       <c r="B205" t="s">
-        <v>553</v>
-      </c>
-      <c r="C205" t="s">
-        <v>588</v>
+        <v>256</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
-        <v>586</v>
+        <v>707</v>
       </c>
       <c r="B206" t="s">
-        <v>602</v>
+        <v>703</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" t="s">
-        <v>365</v>
+        <v>534</v>
       </c>
       <c r="B207" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3">
-      <c r="A208" t="s">
-        <v>366</v>
-      </c>
-      <c r="B208" t="s">
-        <v>352</v>
-      </c>
-      <c r="C208" t="s">
-        <v>589</v>
+        <v>683</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" t="s">
-        <v>508</v>
+        <v>551</v>
       </c>
       <c r="B209" t="s">
-        <v>575</v>
+        <v>554</v>
+      </c>
+      <c r="C209" t="s">
+        <v>587</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" t="s">
-        <v>367</v>
+        <v>552</v>
       </c>
       <c r="B210" t="s">
-        <v>353</v>
+        <v>553</v>
+      </c>
+      <c r="C210" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
-        <v>368</v>
+        <v>586</v>
       </c>
       <c r="B211" t="s">
-        <v>354</v>
+        <v>602</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B212" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B213" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C213" t="s">
         <v>589</v>
@@ -8454,42 +8469,42 @@
     </row>
     <row r="214" spans="1:3">
       <c r="A214" t="s">
-        <v>371</v>
+        <v>508</v>
       </c>
       <c r="B214" t="s">
-        <v>357</v>
+        <v>575</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="B215" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="B216" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B217" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="B218" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
       <c r="C218" t="s">
         <v>589</v>
@@ -8497,471 +8512,514 @@
     </row>
     <row r="219" spans="1:3">
       <c r="A219" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="B219" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="B220" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="B221" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" t="s">
-        <v>533</v>
+        <v>374</v>
       </c>
       <c r="B222" t="s">
-        <v>667</v>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3">
+      <c r="A223" t="s">
+        <v>375</v>
+      </c>
+      <c r="B223" t="s">
+        <v>361</v>
+      </c>
+      <c r="C223" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" t="s">
-        <v>607</v>
+        <v>376</v>
       </c>
       <c r="B224" t="s">
-        <v>608</v>
+        <v>362</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="B225" t="s">
-        <v>403</v>
+        <v>363</v>
       </c>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="B226" t="s">
-        <v>400</v>
+        <v>364</v>
       </c>
     </row>
     <row r="227" spans="1:3">
       <c r="A227" t="s">
-        <v>387</v>
+        <v>533</v>
       </c>
       <c r="B227" t="s">
-        <v>401</v>
-      </c>
-      <c r="C227" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="228" spans="1:3">
-      <c r="A228" t="s">
-        <v>509</v>
-      </c>
-      <c r="B228" t="s">
-        <v>576</v>
+        <v>667</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" t="s">
-        <v>404</v>
+        <v>607</v>
       </c>
       <c r="B229" t="s">
-        <v>402</v>
-      </c>
-      <c r="C229" t="s">
-        <v>589</v>
+        <v>608</v>
       </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="B230" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
     </row>
     <row r="231" spans="1:3">
       <c r="A231" t="s">
-        <v>405</v>
+        <v>386</v>
       </c>
       <c r="B231" t="s">
-        <v>395</v>
-      </c>
-      <c r="C231" t="s">
-        <v>566</v>
+        <v>400</v>
       </c>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B232" t="s">
-        <v>396</v>
+        <v>401</v>
+      </c>
+      <c r="C232" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="233" spans="1:3">
       <c r="A233" t="s">
-        <v>391</v>
+        <v>509</v>
       </c>
       <c r="B233" t="s">
-        <v>397</v>
+        <v>576</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" t="s">
-        <v>390</v>
+        <v>404</v>
       </c>
       <c r="B234" t="s">
-        <v>398</v>
+        <v>402</v>
+      </c>
+      <c r="C234" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="235" spans="1:3">
       <c r="A235" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="B235" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" t="s">
-        <v>393</v>
+        <v>405</v>
       </c>
       <c r="B236" t="s">
-        <v>396</v>
+        <v>395</v>
+      </c>
+      <c r="C236" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" t="s">
-        <v>532</v>
+        <v>389</v>
       </c>
       <c r="B237" t="s">
-        <v>684</v>
+        <v>396</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3">
+      <c r="A238" t="s">
+        <v>391</v>
+      </c>
+      <c r="B238" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239" t="s">
-        <v>523</v>
+        <v>390</v>
       </c>
       <c r="B239" t="s">
-        <v>524</v>
+        <v>398</v>
       </c>
     </row>
     <row r="240" spans="1:3">
       <c r="A240" t="s">
-        <v>411</v>
+        <v>392</v>
       </c>
       <c r="B240" t="s">
-        <v>422</v>
+        <v>399</v>
       </c>
     </row>
     <row r="241" spans="1:3">
       <c r="A241" t="s">
-        <v>412</v>
+        <v>393</v>
       </c>
       <c r="B241" t="s">
-        <v>423</v>
-      </c>
-      <c r="C241" t="s">
-        <v>589</v>
+        <v>396</v>
       </c>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" t="s">
-        <v>577</v>
+        <v>532</v>
       </c>
       <c r="B242" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3">
-      <c r="A243" t="s">
-        <v>413</v>
-      </c>
-      <c r="B243" t="s">
-        <v>424</v>
-      </c>
-      <c r="C243" t="s">
-        <v>589</v>
+        <v>684</v>
       </c>
     </row>
     <row r="244" spans="1:3">
       <c r="A244" t="s">
-        <v>414</v>
+        <v>523</v>
       </c>
       <c r="B244" t="s">
-        <v>425</v>
-      </c>
-      <c r="C244" t="s">
-        <v>589</v>
+        <v>524</v>
       </c>
     </row>
     <row r="245" spans="1:3">
       <c r="A245" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="B245" t="s">
-        <v>590</v>
+        <v>422</v>
       </c>
     </row>
     <row r="246" spans="1:3">
       <c r="A246" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="B246" t="s">
-        <v>426</v>
+        <v>423</v>
+      </c>
+      <c r="C246" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="247" spans="1:3">
       <c r="A247" t="s">
-        <v>417</v>
+        <v>577</v>
       </c>
       <c r="B247" t="s">
-        <v>427</v>
+        <v>578</v>
       </c>
     </row>
     <row r="248" spans="1:3">
       <c r="A248" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="B248" t="s">
-        <v>428</v>
+        <v>424</v>
+      </c>
+      <c r="C248" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="249" spans="1:3">
       <c r="A249" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="B249" t="s">
-        <v>429</v>
+        <v>425</v>
+      </c>
+      <c r="C249" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="250" spans="1:3">
       <c r="A250" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="B250" t="s">
-        <v>430</v>
+        <v>590</v>
       </c>
     </row>
     <row r="251" spans="1:3">
       <c r="A251" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="B251" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
     </row>
     <row r="252" spans="1:3">
       <c r="A252" t="s">
-        <v>530</v>
+        <v>417</v>
       </c>
       <c r="B252" t="s">
-        <v>685</v>
+        <v>427</v>
       </c>
     </row>
     <row r="253" spans="1:3">
       <c r="A253" t="s">
-        <v>616</v>
+        <v>418</v>
       </c>
       <c r="B253" t="s">
-        <v>617</v>
+        <v>428</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3">
+      <c r="A254" t="s">
+        <v>419</v>
+      </c>
+      <c r="B254" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="255" spans="1:3">
       <c r="A255" t="s">
-        <v>525</v>
+        <v>420</v>
       </c>
       <c r="B255" t="s">
-        <v>524</v>
+        <v>430</v>
       </c>
     </row>
     <row r="256" spans="1:3">
       <c r="A256" t="s">
-        <v>438</v>
+        <v>421</v>
       </c>
       <c r="B256" t="s">
-        <v>449</v>
+        <v>431</v>
       </c>
     </row>
     <row r="257" spans="1:3">
       <c r="A257" t="s">
-        <v>439</v>
+        <v>530</v>
       </c>
       <c r="B257" t="s">
-        <v>450</v>
-      </c>
-      <c r="C257" t="s">
-        <v>589</v>
+        <v>685</v>
       </c>
     </row>
     <row r="258" spans="1:3">
       <c r="A258" t="s">
-        <v>510</v>
+        <v>616</v>
       </c>
       <c r="B258" t="s">
-        <v>579</v>
-      </c>
-    </row>
-    <row r="259" spans="1:3">
-      <c r="A259" t="s">
-        <v>440</v>
-      </c>
-      <c r="B259" t="s">
-        <v>451</v>
-      </c>
-      <c r="C259" t="s">
-        <v>589</v>
+        <v>617</v>
       </c>
     </row>
     <row r="260" spans="1:3">
       <c r="A260" t="s">
-        <v>441</v>
+        <v>525</v>
       </c>
       <c r="B260" t="s">
-        <v>452</v>
-      </c>
-      <c r="C260" t="s">
-        <v>589</v>
+        <v>524</v>
       </c>
     </row>
     <row r="261" spans="1:3">
       <c r="A261" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="B261" t="s">
-        <v>591</v>
+        <v>449</v>
       </c>
     </row>
     <row r="262" spans="1:3">
       <c r="A262" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B262" t="s">
-        <v>426</v>
+        <v>450</v>
+      </c>
+      <c r="C262" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="263" spans="1:3">
       <c r="A263" t="s">
-        <v>444</v>
+        <v>510</v>
       </c>
       <c r="B263" t="s">
-        <v>427</v>
+        <v>579</v>
       </c>
     </row>
     <row r="264" spans="1:3">
       <c r="A264" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="B264" t="s">
-        <v>453</v>
+        <v>451</v>
+      </c>
+      <c r="C264" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="265" spans="1:3">
       <c r="A265" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="B265" t="s">
-        <v>454</v>
+        <v>452</v>
+      </c>
+      <c r="C265" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="266" spans="1:3">
       <c r="A266" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="B266" t="s">
-        <v>430</v>
+        <v>591</v>
       </c>
     </row>
     <row r="267" spans="1:3">
       <c r="A267" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="B267" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
     </row>
     <row r="268" spans="1:3">
       <c r="A268" t="s">
-        <v>529</v>
+        <v>444</v>
       </c>
       <c r="B268" t="s">
-        <v>685</v>
+        <v>427</v>
       </c>
     </row>
     <row r="269" spans="1:3">
       <c r="A269" t="s">
-        <v>623</v>
+        <v>445</v>
       </c>
       <c r="B269" t="s">
-        <v>617</v>
+        <v>453</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3">
+      <c r="A270" t="s">
+        <v>446</v>
+      </c>
+      <c r="B270" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="271" spans="1:3">
       <c r="A271" t="s">
-        <v>432</v>
+        <v>447</v>
       </c>
       <c r="B271" t="s">
-        <v>624</v>
+        <v>430</v>
       </c>
     </row>
     <row r="272" spans="1:3">
       <c r="A272" t="s">
+        <v>448</v>
+      </c>
+      <c r="B272" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3">
+      <c r="A273" t="s">
+        <v>529</v>
+      </c>
+      <c r="B273" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3">
+      <c r="A274" t="s">
+        <v>623</v>
+      </c>
+      <c r="B274" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3">
+      <c r="A276" t="s">
+        <v>432</v>
+      </c>
+      <c r="B276" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3">
+      <c r="A277" t="s">
         <v>433</v>
       </c>
-      <c r="B272" t="s">
+      <c r="B277" t="s">
         <v>625</v>
       </c>
-      <c r="C272" t="s">
+      <c r="C277" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="273" spans="1:2">
-      <c r="A273" t="s">
+    <row r="278" spans="1:3">
+      <c r="A278" t="s">
         <v>511</v>
       </c>
-      <c r="B273" t="s">
+      <c r="B278" t="s">
         <v>626</v>
       </c>
     </row>
-    <row r="274" spans="1:2">
-      <c r="A274" t="s">
+    <row r="279" spans="1:3">
+      <c r="A279" t="s">
         <v>434</v>
       </c>
-      <c r="B274" t="s">
+      <c r="B279" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="275" spans="1:2">
-      <c r="A275" t="s">
+    <row r="280" spans="1:3">
+      <c r="A280" t="s">
         <v>435</v>
       </c>
-      <c r="B275" t="s">
+      <c r="B280" t="s">
         <v>627</v>
       </c>
     </row>
-    <row r="276" spans="1:2">
-      <c r="A276" t="s">
+    <row r="281" spans="1:3">
+      <c r="A281" t="s">
         <v>436</v>
       </c>
-      <c r="B276" t="s">
+      <c r="B281" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="277" spans="1:2">
-      <c r="A277" t="s">
+    <row r="282" spans="1:3">
+      <c r="A282" t="s">
         <v>528</v>
       </c>
-      <c r="B277" t="s">
+      <c r="B282" t="s">
         <v>686</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes for User Story 57681 and 57470
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.malyala\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raluca.ilinca.AzureAI-Jump2\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600F8B92-FB0B-44B4-9888-E0D84C7A352F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9749C163-A098-46C9-A234-7FE4E3AF3693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="22440" windowHeight="11715" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="701">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="704">
   <si>
     <t>Name</t>
   </si>
@@ -1518,9 +1518,6 @@
     <t>VAWA Acknowledgement</t>
   </si>
   <si>
-    <t>C:\Users\harika.malyala\Documents\AZApplicationReview\Prompts\</t>
-  </si>
-  <si>
     <t>Replace_JArraayInJSON</t>
   </si>
   <si>
@@ -1938,9 +1935,6 @@
     <t>SC_AllFullTimeStudents</t>
   </si>
   <si>
-    <t>All household members have been or will be students for the next five months. Manual review required.</t>
-  </si>
-  <si>
     <t>Assets Type and  value does not match that listed on the ICW.</t>
   </si>
   <si>
@@ -2127,22 +2121,37 @@
     <t>Removed this check as we replace this with below check to see if assitance is mared yes in an arrays 1, 2, 3</t>
   </si>
   <si>
-    <t>PS_MultipleIncomeDocsExists</t>
-  </si>
-  <si>
-    <t>Multiple employment documents provided for same employment. Can't determine which employment document to use to validate Exact Day Calculator. Manual review required.</t>
-  </si>
-  <si>
-    <t>VOE_MultipleIncomeDocsExists</t>
-  </si>
-  <si>
-    <t>OL_MultipleIncomeDocsExists</t>
-  </si>
-  <si>
-    <t>WN_MultipleIncomeDocsExists</t>
-  </si>
-  <si>
-    <t>VS_MultipleIncomeDocsExists</t>
+    <t>C:\Users\raluca.ilinca.AzureAI-Jump2\Documents\AZApplicationReview\Prompts\</t>
+  </si>
+  <si>
+    <t>Newly added by Raluca</t>
+  </si>
+  <si>
+    <t>MID_MinorLessThan50Percent</t>
+  </si>
+  <si>
+    <t>A minor will live in the household less than 50% of the time. Manual review required.</t>
+  </si>
+  <si>
+    <t>The applicant has indicated all household contains all students by selecting 2 or 3 to Part A on the Student Certification. Manual review required.</t>
+  </si>
+  <si>
+    <t>Raluca removed this check</t>
+  </si>
+  <si>
+    <t>VOE_PayIncrease</t>
+  </si>
+  <si>
+    <t>Anticipated increase in the base pay over the next 12 months. Manual review required.</t>
+  </si>
+  <si>
+    <t>Raluca updated this check</t>
+  </si>
+  <si>
+    <t>ICW_LiveInAttendant</t>
+  </si>
+  <si>
+    <t>Live-In Attendant documented on the ICW, manual review required.</t>
   </si>
 </sst>
 </file>
@@ -2520,8 +2529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1002"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2604,7 +2613,7 @@
         <v>209</v>
       </c>
       <c r="B7" t="s">
-        <v>492</v>
+        <v>693</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -2653,7 +2662,7 @@
         <v>219</v>
       </c>
       <c r="B14" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
@@ -2691,7 +2700,7 @@
         <v>223</v>
       </c>
       <c r="B18" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C18" t="s">
         <v>238</v>
@@ -2713,7 +2722,7 @@
         <v>225</v>
       </c>
       <c r="B20" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
@@ -2729,7 +2738,7 @@
         <v>227</v>
       </c>
       <c r="B22" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
@@ -2796,7 +2805,7 @@
         <v>379</v>
       </c>
       <c r="B30" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
@@ -2828,7 +2837,7 @@
         <v>410</v>
       </c>
       <c r="B34" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
@@ -2876,7 +2885,7 @@
         <v>437</v>
       </c>
       <c r="B40" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
@@ -4190,7 +4199,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
@@ -4386,15 +4395,15 @@
         <v>57</v>
       </c>
       <c r="B20" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B21" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
@@ -5436,7 +5445,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1011"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
@@ -5566,82 +5575,82 @@
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B12" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B13" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B14" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B15" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B16" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B17" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B18" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B19" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B20" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B21" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1">
@@ -5702,82 +5711,82 @@
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B29" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B30" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="14.25" customHeight="1">
       <c r="A31" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B32" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
       <c r="A33" s="2" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="B33" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
       <c r="A34" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="B34" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
       <c r="A35" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B35" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1">
       <c r="A36" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B36" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="14.25" customHeight="1">
       <c r="A37" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="B37" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="14.25" customHeight="1">
       <c r="A38" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B38" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
@@ -6761,16 +6770,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
-  <dimension ref="A1:C280"/>
+  <dimension ref="A1:C278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="B160" sqref="B160"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="126.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="153.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6795,7 +6804,7 @@
         <v>180</v>
       </c>
       <c r="B5" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -6830,1277 +6839,1292 @@
         <v>207</v>
       </c>
       <c r="C9" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
+        <v>549</v>
+      </c>
+      <c r="B10" t="s">
         <v>550</v>
-      </c>
-      <c r="B10" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="B11" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B12" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
-        <v>181</v>
-      </c>
-      <c r="B14" t="s">
-        <v>182</v>
+        <v>668</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>702</v>
+      </c>
+      <c r="B13" t="s">
+        <v>703</v>
+      </c>
+      <c r="C13" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>181</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>560</v>
+        <v>79</v>
       </c>
       <c r="B16" t="s">
-        <v>561</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>559</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>560</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B18" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>196</v>
+        <v>82</v>
       </c>
       <c r="B19" t="s">
-        <v>197</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B20" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>634</v>
+        <v>89</v>
       </c>
       <c r="B25" t="s">
-        <v>635</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>658</v>
+        <v>632</v>
       </c>
       <c r="B26" t="s">
-        <v>659</v>
+        <v>633</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>547</v>
+        <v>656</v>
       </c>
       <c r="B27" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
-        <v>183</v>
-      </c>
-      <c r="B29" t="s">
-        <v>185</v>
+        <v>657</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>546</v>
+      </c>
+      <c r="B28" t="s">
+        <v>669</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>91</v>
+        <v>183</v>
       </c>
       <c r="B30" t="s">
-        <v>92</v>
+        <v>185</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B31" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B36" t="s">
-        <v>99</v>
-      </c>
-      <c r="C36" t="s">
-        <v>590</v>
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B37" t="s">
-        <v>100</v>
+        <v>99</v>
+      </c>
+      <c r="C37" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>636</v>
+        <v>106</v>
       </c>
       <c r="B38" t="s">
-        <v>637</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>546</v>
+        <v>634</v>
       </c>
       <c r="B39" t="s">
-        <v>672</v>
+        <v>635</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>545</v>
+      </c>
+      <c r="B40" t="s">
+        <v>670</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>184</v>
+        <v>695</v>
       </c>
       <c r="B41" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
-        <v>107</v>
-      </c>
-      <c r="B42" t="s">
-        <v>108</v>
-      </c>
-      <c r="C42" t="s">
-        <v>590</v>
+        <v>696</v>
+      </c>
+      <c r="C41" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>117</v>
+        <v>184</v>
       </c>
       <c r="B43" t="s">
-        <v>118</v>
-      </c>
-      <c r="C43" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="B44" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C44" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B45" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="C45" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B46" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="C46" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C47" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B48" t="s">
-        <v>112</v>
+        <v>110</v>
+      </c>
+      <c r="C48" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>204</v>
+        <v>115</v>
       </c>
       <c r="B49" t="s">
-        <v>495</v>
+        <v>111</v>
+      </c>
+      <c r="C49" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>205</v>
+        <v>116</v>
       </c>
       <c r="B50" t="s">
-        <v>594</v>
-      </c>
-      <c r="C50" t="s">
-        <v>590</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>581</v>
+        <v>204</v>
       </c>
       <c r="B51" t="s">
-        <v>595</v>
+        <v>494</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>548</v>
+        <v>205</v>
       </c>
       <c r="B52" t="s">
-        <v>549</v>
+        <v>593</v>
+      </c>
+      <c r="C52" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>556</v>
+        <v>580</v>
       </c>
       <c r="B53" t="s">
-        <v>633</v>
+        <v>594</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="B54" t="s">
-        <v>673</v>
+        <v>548</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>555</v>
+      </c>
+      <c r="B55" t="s">
+        <v>631</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>158</v>
+        <v>544</v>
       </c>
       <c r="B56" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" t="s">
-        <v>122</v>
-      </c>
-      <c r="B57" t="s">
-        <v>596</v>
+        <v>671</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>124</v>
+        <v>158</v>
       </c>
       <c r="B58" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>638</v>
+        <v>122</v>
       </c>
       <c r="B59" t="s">
-        <v>639</v>
+        <v>595</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>544</v>
+        <v>124</v>
       </c>
       <c r="B60" t="s">
-        <v>674</v>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>636</v>
+      </c>
+      <c r="B61" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>186</v>
+        <v>543</v>
       </c>
       <c r="B62" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" t="s">
-        <v>125</v>
-      </c>
-      <c r="B63" t="s">
-        <v>127</v>
+        <v>672</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>126</v>
+        <v>186</v>
       </c>
       <c r="B64" t="s">
-        <v>128</v>
+        <v>187</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="B65" t="s">
-        <v>597</v>
+        <v>127</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="B66" t="s">
-        <v>598</v>
+        <v>128</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B67" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B68" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B69" t="s">
-        <v>496</v>
-      </c>
-      <c r="C69" t="s">
-        <v>689</v>
+        <v>598</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B70" t="s">
-        <v>498</v>
-      </c>
-      <c r="C70" t="s">
-        <v>557</v>
+        <v>599</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B71" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="C71" t="s">
-        <v>557</v>
+        <v>687</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>640</v>
+        <v>143</v>
       </c>
       <c r="B72" t="s">
-        <v>641</v>
+        <v>497</v>
+      </c>
+      <c r="C72" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>543</v>
+        <v>144</v>
       </c>
       <c r="B73" t="s">
-        <v>675</v>
+        <v>498</v>
+      </c>
+      <c r="C73" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>638</v>
+      </c>
+      <c r="B74" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>147</v>
+        <v>542</v>
       </c>
       <c r="B75" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" t="s">
-        <v>148</v>
-      </c>
-      <c r="B76" t="s">
-        <v>151</v>
+        <v>673</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B77" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B78" t="s">
-        <v>582</v>
-      </c>
-      <c r="C78" t="s">
-        <v>694</v>
+        <v>151</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>693</v>
+        <v>149</v>
       </c>
       <c r="B79" t="s">
-        <v>582</v>
+        <v>152</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
+        <v>145</v>
+      </c>
+      <c r="B80" t="s">
+        <v>581</v>
+      </c>
+      <c r="C80" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>691</v>
+      </c>
+      <c r="B81" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
         <v>146</v>
       </c>
-      <c r="B80" t="s">
+      <c r="B82" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
-      <c r="A81" t="s">
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
         <v>131</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B83" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>132</v>
+      </c>
+      <c r="B84" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>640</v>
+      </c>
+      <c r="B85" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>541</v>
+      </c>
+      <c r="B86" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>188</v>
+      </c>
+      <c r="B88" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>133</v>
+      </c>
+      <c r="B89" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>135</v>
+      </c>
+      <c r="B90" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>134</v>
+      </c>
+      <c r="B91" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>136</v>
+      </c>
+      <c r="B92" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>137</v>
+      </c>
+      <c r="B93" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
+        <v>630</v>
+      </c>
+      <c r="B94" t="s">
+        <v>697</v>
+      </c>
+      <c r="C94" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
+        <v>642</v>
+      </c>
+      <c r="B95" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" t="s">
+        <v>540</v>
+      </c>
+      <c r="B96" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>159</v>
+      </c>
+      <c r="B98" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>160</v>
+      </c>
+      <c r="B99" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>161</v>
+      </c>
+      <c r="B100" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>162</v>
+      </c>
+      <c r="B101" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
-      <c r="A82" t="s">
-        <v>132</v>
-      </c>
-      <c r="B82" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
-      <c r="A83" t="s">
-        <v>642</v>
-      </c>
-      <c r="B83" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
-      <c r="A84" t="s">
-        <v>542</v>
-      </c>
-      <c r="B84" t="s">
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>557</v>
+      </c>
+      <c r="B102" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>648</v>
+      </c>
+      <c r="B103" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>539</v>
+      </c>
+      <c r="B104" t="s">
         <v>676</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
-      <c r="A86" t="s">
-        <v>188</v>
-      </c>
-      <c r="B86" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
-      <c r="A87" t="s">
-        <v>133</v>
-      </c>
-      <c r="B87" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2">
-      <c r="A88" t="s">
-        <v>135</v>
-      </c>
-      <c r="B88" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2">
-      <c r="A89" t="s">
-        <v>134</v>
-      </c>
-      <c r="B89" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
-      <c r="A90" t="s">
-        <v>136</v>
-      </c>
-      <c r="B90" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
-      <c r="A91" t="s">
-        <v>137</v>
-      </c>
-      <c r="B91" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
-      <c r="A92" t="s">
-        <v>631</v>
-      </c>
-      <c r="B92" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
-      <c r="A93" t="s">
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>192</v>
+      </c>
+      <c r="B106" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>166</v>
+      </c>
+      <c r="B107" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>167</v>
+      </c>
+      <c r="B108" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
         <v>644</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B109" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
-      <c r="A94" t="s">
-        <v>541</v>
-      </c>
-      <c r="B94" t="s">
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>538</v>
+      </c>
+      <c r="B110" t="s">
         <v>677</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
-      <c r="A96" t="s">
-        <v>159</v>
-      </c>
-      <c r="B96" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3">
-      <c r="A97" t="s">
-        <v>160</v>
-      </c>
-      <c r="B97" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
-      <c r="A98" t="s">
-        <v>161</v>
-      </c>
-      <c r="B98" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3">
-      <c r="A99" t="s">
-        <v>162</v>
-      </c>
-      <c r="B99" t="s">
-        <v>602</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3">
-      <c r="A100" t="s">
-        <v>558</v>
-      </c>
-      <c r="B100" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3">
-      <c r="A101" t="s">
-        <v>650</v>
-      </c>
-      <c r="B101" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3">
-      <c r="A102" t="s">
-        <v>540</v>
-      </c>
-      <c r="B102" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
-      <c r="A104" t="s">
-        <v>192</v>
-      </c>
-      <c r="B104" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3">
-      <c r="A105" t="s">
-        <v>166</v>
-      </c>
-      <c r="B105" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3">
-      <c r="A106" t="s">
-        <v>167</v>
-      </c>
-      <c r="B106" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3">
-      <c r="A107" t="s">
-        <v>646</v>
-      </c>
-      <c r="B107" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
-      <c r="A108" t="s">
-        <v>539</v>
-      </c>
-      <c r="B108" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3">
-      <c r="A110" t="s">
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
         <v>190</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B112" t="s">
         <v>191</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3">
-      <c r="A111" t="s">
-        <v>175</v>
-      </c>
-      <c r="B111" t="s">
-        <v>172</v>
-      </c>
-      <c r="C111" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3">
-      <c r="A112" t="s">
-        <v>170</v>
-      </c>
-      <c r="B112" t="s">
-        <v>173</v>
-      </c>
-      <c r="C112" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B113" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C113" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>203</v>
+        <v>170</v>
       </c>
       <c r="B114" t="s">
-        <v>202</v>
+        <v>173</v>
+      </c>
+      <c r="C114" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>200</v>
+        <v>171</v>
       </c>
       <c r="B115" t="s">
-        <v>201</v>
+        <v>174</v>
+      </c>
+      <c r="C115" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>176</v>
+        <v>203</v>
       </c>
       <c r="B116" t="s">
-        <v>177</v>
-      </c>
-      <c r="C116" t="s">
-        <v>590</v>
+        <v>202</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>648</v>
+        <v>200</v>
       </c>
       <c r="B117" t="s">
-        <v>649</v>
+        <v>201</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>528</v>
+        <v>176</v>
       </c>
       <c r="B118" t="s">
-        <v>680</v>
+        <v>177</v>
+      </c>
+      <c r="C118" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" t="s">
+        <v>646</v>
+      </c>
+      <c r="B119" t="s">
+        <v>647</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>655</v>
+        <v>527</v>
       </c>
       <c r="B120" t="s">
-        <v>656</v>
-      </c>
-      <c r="C120" t="s">
-        <v>657</v>
+        <v>678</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>514</v>
+        <v>653</v>
       </c>
       <c r="B122" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3">
-      <c r="A123" t="s">
-        <v>664</v>
-      </c>
-      <c r="B123" t="s">
-        <v>668</v>
-      </c>
-      <c r="C123" t="s">
-        <v>666</v>
+        <v>654</v>
+      </c>
+      <c r="C122" t="s">
+        <v>655</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>665</v>
+        <v>513</v>
       </c>
       <c r="B124" t="s">
-        <v>667</v>
-      </c>
-      <c r="C124" t="s">
-        <v>666</v>
+        <v>514</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>242</v>
+        <v>662</v>
       </c>
       <c r="B125" t="s">
-        <v>243</v>
+        <v>666</v>
       </c>
       <c r="C125" t="s">
-        <v>590</v>
+        <v>664</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>244</v>
+        <v>663</v>
       </c>
       <c r="B126" t="s">
-        <v>245</v>
+        <v>665</v>
+      </c>
+      <c r="C126" t="s">
+        <v>664</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="B127" t="s">
-        <v>562</v>
+        <v>243</v>
       </c>
       <c r="C127" t="s">
-        <v>653</v>
+        <v>589</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B128" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>504</v>
+        <v>258</v>
       </c>
       <c r="B129" t="s">
-        <v>513</v>
+        <v>561</v>
+      </c>
+      <c r="C129" t="s">
+        <v>651</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B130" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>250</v>
+        <v>503</v>
       </c>
       <c r="B131" t="s">
-        <v>252</v>
+        <v>512</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B132" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="B133" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B134" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>302</v>
+        <v>255</v>
       </c>
       <c r="B135" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>349</v>
+        <v>257</v>
       </c>
       <c r="B136" t="s">
-        <v>350</v>
+        <v>256</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>660</v>
+        <v>302</v>
       </c>
       <c r="B137" t="s">
-        <v>661</v>
+        <v>248</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>695</v>
+        <v>349</v>
       </c>
       <c r="B138" t="s">
-        <v>696</v>
+        <v>350</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>527</v>
+        <v>658</v>
       </c>
       <c r="B139" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3">
-      <c r="A141" t="s">
-        <v>516</v>
-      </c>
-      <c r="B141" t="s">
-        <v>517</v>
+        <v>659</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" t="s">
+        <v>526</v>
+      </c>
+      <c r="B140" t="s">
+        <v>679</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
+        <v>515</v>
+      </c>
+      <c r="B142" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" t="s">
         <v>259</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B143" t="s">
         <v>262</v>
       </c>
-      <c r="C142" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="143" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A143" t="s">
+      <c r="C143" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A144" t="s">
         <v>261</v>
       </c>
-      <c r="B143" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3">
-      <c r="A144" t="s">
-        <v>260</v>
-      </c>
       <c r="B144" t="s">
-        <v>263</v>
+        <v>562</v>
+      </c>
+      <c r="C144" t="s">
+        <v>698</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B145" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B146" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B147" t="s">
-        <v>268</v>
-      </c>
-      <c r="C147" t="s">
-        <v>663</v>
+        <v>267</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>505</v>
+        <v>269</v>
       </c>
       <c r="B148" t="s">
-        <v>572</v>
+        <v>268</v>
+      </c>
+      <c r="C148" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>270</v>
+        <v>504</v>
       </c>
       <c r="B149" t="s">
-        <v>271</v>
+        <v>571</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B150" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B151" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B152" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B153" t="s">
-        <v>285</v>
-      </c>
-      <c r="C153" t="s">
-        <v>663</v>
+        <v>286</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B154" t="s">
-        <v>607</v>
+        <v>285</v>
+      </c>
+      <c r="C154" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B155" t="s">
-        <v>284</v>
-      </c>
-      <c r="C155" t="s">
-        <v>663</v>
+        <v>606</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B156" t="s">
-        <v>283</v>
+        <v>284</v>
+      </c>
+      <c r="C156" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>299</v>
+        <v>282</v>
       </c>
       <c r="B157" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B158" t="s">
-        <v>248</v>
+        <v>300</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B159" t="s">
-        <v>305</v>
+        <v>248</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" t="s">
-        <v>697</v>
+        <v>304</v>
       </c>
       <c r="B160" t="s">
-        <v>696</v>
+        <v>305</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B161" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3">
-      <c r="A163" t="s">
-        <v>518</v>
-      </c>
-      <c r="B163" t="s">
-        <v>519</v>
+        <v>680</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162" t="s">
+        <v>699</v>
+      </c>
+      <c r="B162" t="s">
+        <v>700</v>
+      </c>
+      <c r="C162" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>292</v>
+        <v>517</v>
       </c>
       <c r="B164" t="s">
-        <v>296</v>
-      </c>
-      <c r="C164" t="s">
-        <v>590</v>
+        <v>518</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
-        <v>506</v>
+        <v>292</v>
       </c>
       <c r="B165" t="s">
-        <v>573</v>
+        <v>296</v>
+      </c>
+      <c r="C165" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
-        <v>293</v>
+        <v>505</v>
       </c>
       <c r="B166" t="s">
-        <v>297</v>
-      </c>
-      <c r="C166" t="s">
-        <v>590</v>
+        <v>572</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B167" t="s">
-        <v>298</v>
+        <v>297</v>
+      </c>
+      <c r="C167" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B168" t="s">
-        <v>564</v>
+        <v>298</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="B169" t="s">
-        <v>248</v>
+        <v>563</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="B170" t="s">
-        <v>310</v>
+        <v>248</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="B171" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B172" t="s">
         <v>308</v>
@@ -8108,53 +8132,53 @@
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B173" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>698</v>
+        <v>311</v>
       </c>
       <c r="B174" t="s">
-        <v>696</v>
+        <v>312</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B175" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
+        <v>519</v>
+      </c>
+      <c r="B177" t="s">
         <v>520</v>
-      </c>
-      <c r="B177" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B178" t="s">
         <v>320</v>
       </c>
       <c r="C178" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B179" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -8165,7 +8189,7 @@
         <v>321</v>
       </c>
       <c r="C180" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="181" spans="1:3">
@@ -8189,7 +8213,7 @@
         <v>318</v>
       </c>
       <c r="B183" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -8208,7 +8232,7 @@
         <v>325</v>
       </c>
       <c r="C185" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -8245,698 +8269,698 @@
     </row>
     <row r="190" spans="1:3">
       <c r="A190" t="s">
-        <v>699</v>
+        <v>535</v>
       </c>
       <c r="B190" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3">
-      <c r="A191" t="s">
-        <v>536</v>
-      </c>
-      <c r="B191" t="s">
-        <v>684</v>
+        <v>682</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3">
+      <c r="A192" t="s">
+        <v>521</v>
+      </c>
+      <c r="B192" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" t="s">
-        <v>522</v>
+        <v>501</v>
       </c>
       <c r="B193" t="s">
-        <v>523</v>
+        <v>338</v>
+      </c>
+      <c r="C193" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>502</v>
+        <v>507</v>
       </c>
       <c r="B194" t="s">
-        <v>338</v>
-      </c>
-      <c r="C194" t="s">
-        <v>590</v>
+        <v>574</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>508</v>
+        <v>336</v>
       </c>
       <c r="B195" t="s">
-        <v>575</v>
+        <v>339</v>
+      </c>
+      <c r="C195" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B196" t="s">
-        <v>339</v>
-      </c>
-      <c r="C196" t="s">
-        <v>590</v>
+        <v>340</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
-        <v>337</v>
+        <v>500</v>
       </c>
       <c r="B197" t="s">
-        <v>340</v>
+        <v>565</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
-        <v>501</v>
+        <v>344</v>
       </c>
       <c r="B198" t="s">
-        <v>566</v>
+        <v>248</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="B199" t="s">
-        <v>248</v>
+        <v>341</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B200" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B201" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="B202" t="s">
-        <v>343</v>
+        <v>256</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" t="s">
-        <v>348</v>
+        <v>534</v>
       </c>
       <c r="B203" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="204" spans="1:3">
-      <c r="A204" t="s">
-        <v>700</v>
-      </c>
-      <c r="B204" t="s">
-        <v>696</v>
+        <v>683</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
-        <v>535</v>
+        <v>551</v>
       </c>
       <c r="B205" t="s">
-        <v>685</v>
+        <v>554</v>
+      </c>
+      <c r="C205" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
+      <c r="A206" t="s">
+        <v>552</v>
+      </c>
+      <c r="B206" t="s">
+        <v>553</v>
+      </c>
+      <c r="C206" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" t="s">
-        <v>552</v>
+        <v>586</v>
       </c>
       <c r="B207" t="s">
-        <v>555</v>
-      </c>
-      <c r="C207" t="s">
-        <v>588</v>
+        <v>602</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>553</v>
+        <v>365</v>
       </c>
       <c r="B208" t="s">
-        <v>554</v>
-      </c>
-      <c r="C208" t="s">
-        <v>589</v>
+        <v>351</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" t="s">
-        <v>587</v>
+        <v>366</v>
       </c>
       <c r="B209" t="s">
-        <v>603</v>
+        <v>352</v>
+      </c>
+      <c r="C209" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" t="s">
-        <v>365</v>
+        <v>508</v>
       </c>
       <c r="B210" t="s">
-        <v>351</v>
+        <v>575</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B211" t="s">
-        <v>352</v>
-      </c>
-      <c r="C211" t="s">
-        <v>590</v>
+        <v>353</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" t="s">
-        <v>509</v>
+        <v>368</v>
       </c>
       <c r="B212" t="s">
-        <v>576</v>
+        <v>354</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B213" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B214" t="s">
-        <v>354</v>
+        <v>356</v>
+      </c>
+      <c r="C214" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B215" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="B216" t="s">
-        <v>356</v>
-      </c>
-      <c r="C216" t="s">
-        <v>590</v>
+        <v>358</v>
       </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B217" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="B218" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="B219" t="s">
-        <v>359</v>
+        <v>361</v>
+      </c>
+      <c r="C219" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B220" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="B221" t="s">
-        <v>361</v>
-      </c>
-      <c r="C221" t="s">
-        <v>590</v>
+        <v>363</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B222" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="223" spans="1:3">
       <c r="A223" t="s">
-        <v>377</v>
+        <v>533</v>
       </c>
       <c r="B223" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3">
-      <c r="A224" t="s">
-        <v>378</v>
-      </c>
-      <c r="B224" t="s">
-        <v>364</v>
+        <v>667</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" t="s">
-        <v>534</v>
+        <v>607</v>
       </c>
       <c r="B225" t="s">
-        <v>669</v>
+        <v>608</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3">
+      <c r="A226" t="s">
+        <v>385</v>
+      </c>
+      <c r="B226" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="227" spans="1:3">
       <c r="A227" t="s">
-        <v>608</v>
+        <v>386</v>
       </c>
       <c r="B227" t="s">
-        <v>609</v>
+        <v>400</v>
       </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B228" t="s">
-        <v>403</v>
+        <v>401</v>
+      </c>
+      <c r="C228" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" t="s">
-        <v>386</v>
+        <v>509</v>
       </c>
       <c r="B229" t="s">
-        <v>400</v>
+        <v>576</v>
       </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" t="s">
-        <v>387</v>
+        <v>404</v>
       </c>
       <c r="B230" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C230" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="231" spans="1:3">
       <c r="A231" t="s">
-        <v>510</v>
+        <v>388</v>
       </c>
       <c r="B231" t="s">
-        <v>577</v>
+        <v>394</v>
       </c>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B232" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="C232" t="s">
-        <v>590</v>
+        <v>566</v>
       </c>
     </row>
     <row r="233" spans="1:3">
       <c r="A233" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B233" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
       <c r="B234" t="s">
-        <v>395</v>
-      </c>
-      <c r="C234" t="s">
-        <v>567</v>
+        <v>397</v>
       </c>
     </row>
     <row r="235" spans="1:3">
       <c r="A235" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B235" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="B236" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="B237" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" t="s">
-        <v>392</v>
+        <v>532</v>
       </c>
       <c r="B238" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="239" spans="1:3">
-      <c r="A239" t="s">
-        <v>393</v>
-      </c>
-      <c r="B239" t="s">
-        <v>396</v>
+        <v>684</v>
       </c>
     </row>
     <row r="240" spans="1:3">
       <c r="A240" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="B240" t="s">
-        <v>686</v>
+        <v>524</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3">
+      <c r="A241" t="s">
+        <v>411</v>
+      </c>
+      <c r="B241" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" t="s">
-        <v>524</v>
+        <v>412</v>
       </c>
       <c r="B242" t="s">
-        <v>525</v>
+        <v>423</v>
+      </c>
+      <c r="C242" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="243" spans="1:3">
       <c r="A243" t="s">
-        <v>411</v>
+        <v>577</v>
       </c>
       <c r="B243" t="s">
-        <v>422</v>
+        <v>578</v>
       </c>
     </row>
     <row r="244" spans="1:3">
       <c r="A244" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B244" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C244" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="245" spans="1:3">
       <c r="A245" t="s">
-        <v>578</v>
+        <v>414</v>
       </c>
       <c r="B245" t="s">
-        <v>579</v>
+        <v>425</v>
+      </c>
+      <c r="C245" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="246" spans="1:3">
       <c r="A246" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="B246" t="s">
-        <v>424</v>
-      </c>
-      <c r="C246" t="s">
         <v>590</v>
       </c>
     </row>
     <row r="247" spans="1:3">
       <c r="A247" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="B247" t="s">
-        <v>425</v>
-      </c>
-      <c r="C247" t="s">
-        <v>590</v>
+        <v>426</v>
       </c>
     </row>
     <row r="248" spans="1:3">
       <c r="A248" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="B248" t="s">
-        <v>591</v>
+        <v>427</v>
       </c>
     </row>
     <row r="249" spans="1:3">
       <c r="A249" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="B249" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
     </row>
     <row r="250" spans="1:3">
       <c r="A250" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="B250" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
     </row>
     <row r="251" spans="1:3">
       <c r="A251" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="B251" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="252" spans="1:3">
       <c r="A252" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="B252" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
     </row>
     <row r="253" spans="1:3">
       <c r="A253" t="s">
-        <v>420</v>
+        <v>530</v>
       </c>
       <c r="B253" t="s">
-        <v>430</v>
+        <v>685</v>
       </c>
     </row>
     <row r="254" spans="1:3">
       <c r="A254" t="s">
-        <v>421</v>
+        <v>616</v>
       </c>
       <c r="B254" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="255" spans="1:3">
-      <c r="A255" t="s">
-        <v>531</v>
-      </c>
-      <c r="B255" t="s">
-        <v>687</v>
+        <v>617</v>
       </c>
     </row>
     <row r="256" spans="1:3">
       <c r="A256" t="s">
-        <v>617</v>
+        <v>525</v>
       </c>
       <c r="B256" t="s">
-        <v>618</v>
+        <v>524</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3">
+      <c r="A257" t="s">
+        <v>438</v>
+      </c>
+      <c r="B257" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="258" spans="1:3">
       <c r="A258" t="s">
-        <v>526</v>
+        <v>439</v>
       </c>
       <c r="B258" t="s">
-        <v>525</v>
+        <v>450</v>
+      </c>
+      <c r="C258" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="259" spans="1:3">
       <c r="A259" t="s">
-        <v>438</v>
+        <v>510</v>
       </c>
       <c r="B259" t="s">
-        <v>449</v>
+        <v>579</v>
       </c>
     </row>
     <row r="260" spans="1:3">
       <c r="A260" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B260" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C260" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="261" spans="1:3">
       <c r="A261" t="s">
-        <v>511</v>
+        <v>441</v>
       </c>
       <c r="B261" t="s">
-        <v>580</v>
+        <v>452</v>
+      </c>
+      <c r="C261" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="262" spans="1:3">
       <c r="A262" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="B262" t="s">
-        <v>451</v>
-      </c>
-      <c r="C262" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="263" spans="1:3">
       <c r="A263" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="B263" t="s">
-        <v>452</v>
-      </c>
-      <c r="C263" t="s">
-        <v>590</v>
+        <v>426</v>
       </c>
     </row>
     <row r="264" spans="1:3">
       <c r="A264" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="B264" t="s">
-        <v>592</v>
+        <v>427</v>
       </c>
     </row>
     <row r="265" spans="1:3">
       <c r="A265" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="B265" t="s">
-        <v>426</v>
+        <v>453</v>
       </c>
     </row>
     <row r="266" spans="1:3">
       <c r="A266" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="B266" t="s">
-        <v>427</v>
+        <v>454</v>
       </c>
     </row>
     <row r="267" spans="1:3">
       <c r="A267" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="B267" t="s">
-        <v>453</v>
+        <v>430</v>
       </c>
     </row>
     <row r="268" spans="1:3">
       <c r="A268" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="B268" t="s">
-        <v>454</v>
+        <v>431</v>
       </c>
     </row>
     <row r="269" spans="1:3">
       <c r="A269" t="s">
-        <v>447</v>
+        <v>529</v>
       </c>
       <c r="B269" t="s">
-        <v>430</v>
+        <v>685</v>
       </c>
     </row>
     <row r="270" spans="1:3">
       <c r="A270" t="s">
-        <v>448</v>
+        <v>623</v>
       </c>
       <c r="B270" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="271" spans="1:3">
-      <c r="A271" t="s">
-        <v>530</v>
-      </c>
-      <c r="B271" t="s">
-        <v>687</v>
+        <v>617</v>
       </c>
     </row>
     <row r="272" spans="1:3">
       <c r="A272" t="s">
+        <v>432</v>
+      </c>
+      <c r="B272" t="s">
         <v>624</v>
       </c>
-      <c r="B272" t="s">
-        <v>618</v>
+    </row>
+    <row r="273" spans="1:3">
+      <c r="A273" t="s">
+        <v>433</v>
+      </c>
+      <c r="B273" t="s">
+        <v>625</v>
+      </c>
+      <c r="C273" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="274" spans="1:3">
       <c r="A274" t="s">
-        <v>432</v>
+        <v>511</v>
       </c>
       <c r="B274" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
     <row r="275" spans="1:3">
       <c r="A275" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B275" t="s">
-        <v>626</v>
-      </c>
-      <c r="C275" t="s">
-        <v>590</v>
+        <v>652</v>
       </c>
     </row>
     <row r="276" spans="1:3">
       <c r="A276" t="s">
-        <v>512</v>
+        <v>435</v>
       </c>
       <c r="B276" t="s">
         <v>627</v>
@@ -8944,34 +8968,18 @@
     </row>
     <row r="277" spans="1:3">
       <c r="A277" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="B277" t="s">
-        <v>654</v>
+        <v>628</v>
       </c>
     </row>
     <row r="278" spans="1:3">
       <c r="A278" t="s">
-        <v>435</v>
+        <v>528</v>
       </c>
       <c r="B278" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="279" spans="1:3">
-      <c r="A279" t="s">
-        <v>436</v>
-      </c>
-      <c r="B279" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="280" spans="1:3">
-      <c r="A280" t="s">
-        <v>529</v>
-      </c>
-      <c r="B280" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes for 57748 and 57772  user stories
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.malyala\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raluca.ilinca.AzureAI-Jump2\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F40FF6-1446-4057-93D9-CD0CEB6B400E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A76F8E-684F-42B4-AEA2-17E8FBFC69BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28200" windowHeight="13530" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="719">
   <si>
     <t>Name</t>
   </si>
@@ -2191,6 +2191,12 @@
   </si>
   <si>
     <t>Errors in Validating findings for Annual Student Certification since there is Home unit . Needs manual review.</t>
+  </si>
+  <si>
+    <t>ICW_UnbornChildDOBListedInThePast</t>
+  </si>
+  <si>
+    <t>There is a Unborn Child listed on the ICW but has a date of birth listed in the past.</t>
   </si>
 </sst>
 </file>
@@ -6817,10 +6823,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
-  <dimension ref="A1:C286"/>
+  <dimension ref="A1:C287"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6924,245 +6930,245 @@
         <v>693</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
-        <v>181</v>
-      </c>
-      <c r="B15" t="s">
-        <v>182</v>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>717</v>
+      </c>
+      <c r="B14" t="s">
+        <v>718</v>
+      </c>
+      <c r="C14" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>181</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>559</v>
+        <v>79</v>
       </c>
       <c r="B17" t="s">
-        <v>560</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>559</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>560</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>196</v>
+        <v>82</v>
       </c>
       <c r="B20" t="s">
-        <v>197</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B21" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>84</v>
+        <v>198</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>199</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B25" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>632</v>
+        <v>89</v>
       </c>
       <c r="B26" t="s">
-        <v>633</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>656</v>
+        <v>632</v>
       </c>
       <c r="B27" t="s">
-        <v>657</v>
+        <v>633</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
+        <v>656</v>
+      </c>
+      <c r="B28" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
         <v>546</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>669</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" t="s">
-        <v>183</v>
-      </c>
-      <c r="B30" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>91</v>
+        <v>183</v>
       </c>
       <c r="B31" t="s">
-        <v>92</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B32" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B37" t="s">
-        <v>99</v>
-      </c>
-      <c r="C37" t="s">
-        <v>589</v>
+        <v>98</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B38" t="s">
-        <v>100</v>
+        <v>99</v>
+      </c>
+      <c r="C38" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>634</v>
+        <v>106</v>
       </c>
       <c r="B39" t="s">
-        <v>635</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>545</v>
+        <v>634</v>
       </c>
       <c r="B40" t="s">
-        <v>670</v>
+        <v>635</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
+        <v>545</v>
+      </c>
+      <c r="B41" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
         <v>694</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
         <v>695</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>693</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" t="s">
-        <v>184</v>
-      </c>
-      <c r="B43" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>107</v>
+        <v>184</v>
       </c>
       <c r="B44" t="s">
-        <v>108</v>
-      </c>
-      <c r="C44" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B45" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C45" t="s">
         <v>589</v>
@@ -7170,10 +7176,10 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B46" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C46" t="s">
         <v>589</v>
@@ -7181,10 +7187,10 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="B47" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="C47" t="s">
         <v>589</v>
@@ -7192,10 +7198,10 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B48" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C48" t="s">
         <v>589</v>
@@ -7203,10 +7209,10 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B49" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C49" t="s">
         <v>589</v>
@@ -7214,187 +7220,187 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B50" t="s">
-        <v>112</v>
+        <v>111</v>
+      </c>
+      <c r="C50" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>204</v>
+        <v>116</v>
       </c>
       <c r="B51" t="s">
-        <v>494</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B52" t="s">
-        <v>593</v>
-      </c>
-      <c r="C52" t="s">
-        <v>589</v>
+        <v>494</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>580</v>
+        <v>205</v>
       </c>
       <c r="B53" t="s">
-        <v>594</v>
+        <v>593</v>
+      </c>
+      <c r="C53" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>547</v>
+        <v>580</v>
       </c>
       <c r="B54" t="s">
-        <v>548</v>
+        <v>594</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
       <c r="B55" t="s">
-        <v>631</v>
+        <v>548</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
+        <v>555</v>
+      </c>
+      <c r="B56" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
         <v>544</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>671</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" t="s">
-        <v>158</v>
-      </c>
-      <c r="B58" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>122</v>
+        <v>158</v>
       </c>
       <c r="B59" t="s">
-        <v>595</v>
+        <v>121</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B60" t="s">
-        <v>123</v>
+        <v>595</v>
       </c>
     </row>
     <row r="61" spans="1:3">
       <c r="A61" t="s">
-        <v>636</v>
+        <v>124</v>
       </c>
       <c r="B61" t="s">
-        <v>637</v>
+        <v>123</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
+        <v>636</v>
+      </c>
+      <c r="B62" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
         <v>543</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B63" t="s">
         <v>672</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" t="s">
-        <v>186</v>
-      </c>
-      <c r="B64" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>125</v>
+        <v>186</v>
       </c>
       <c r="B65" t="s">
-        <v>127</v>
+        <v>187</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B66" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B67" t="s">
-        <v>596</v>
+        <v>128</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B68" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B69" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B70" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B71" t="s">
-        <v>495</v>
-      </c>
-      <c r="C71" t="s">
-        <v>687</v>
+        <v>599</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B72" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C72" t="s">
-        <v>556</v>
+        <v>687</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B73" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C73" t="s">
         <v>556</v>
@@ -7402,321 +7408,321 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>638</v>
+        <v>144</v>
       </c>
       <c r="B74" t="s">
-        <v>639</v>
+        <v>498</v>
+      </c>
+      <c r="C74" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
+        <v>638</v>
+      </c>
+      <c r="B75" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
         <v>542</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B76" t="s">
         <v>673</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" t="s">
-        <v>147</v>
-      </c>
-      <c r="B77" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B78" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B79" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B80" t="s">
-        <v>581</v>
-      </c>
-      <c r="C80" t="s">
-        <v>692</v>
+        <v>152</v>
       </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>691</v>
+        <v>145</v>
       </c>
       <c r="B81" t="s">
         <v>581</v>
       </c>
+      <c r="C81" t="s">
+        <v>692</v>
+      </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>146</v>
+        <v>691</v>
       </c>
       <c r="B82" t="s">
-        <v>129</v>
+        <v>581</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="B83" t="s">
-        <v>600</v>
+        <v>129</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B84" t="s">
-        <v>130</v>
+        <v>600</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>640</v>
+        <v>132</v>
       </c>
       <c r="B85" t="s">
-        <v>641</v>
+        <v>130</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
+        <v>640</v>
+      </c>
+      <c r="B86" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
         <v>541</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B87" t="s">
         <v>674</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88" t="s">
-        <v>188</v>
-      </c>
-      <c r="B88" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>133</v>
+        <v>188</v>
       </c>
       <c r="B89" t="s">
-        <v>153</v>
+        <v>189</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B90" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B91" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B92" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B93" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>630</v>
+        <v>137</v>
       </c>
       <c r="B94" t="s">
-        <v>696</v>
-      </c>
-      <c r="C94" t="s">
-        <v>700</v>
+        <v>157</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>642</v>
+        <v>630</v>
       </c>
       <c r="B95" t="s">
-        <v>643</v>
+        <v>696</v>
+      </c>
+      <c r="C95" t="s">
+        <v>700</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
+        <v>642</v>
+      </c>
+      <c r="B96" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
         <v>540</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B97" t="s">
         <v>675</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
-      <c r="A98" t="s">
-        <v>712</v>
-      </c>
-      <c r="B98" t="s">
-        <v>713</v>
-      </c>
-      <c r="C98" t="s">
-        <v>714</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="B99" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="C99" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
-      <c r="A101" t="s">
-        <v>159</v>
-      </c>
-      <c r="B101" t="s">
-        <v>163</v>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
+        <v>715</v>
+      </c>
+      <c r="B100" t="s">
+        <v>716</v>
+      </c>
+      <c r="C100" t="s">
+        <v>714</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B102" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B103" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B104" t="s">
-        <v>601</v>
+        <v>165</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>557</v>
+        <v>162</v>
       </c>
       <c r="B105" t="s">
-        <v>558</v>
+        <v>601</v>
       </c>
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>648</v>
+        <v>557</v>
       </c>
       <c r="B106" t="s">
-        <v>649</v>
+        <v>558</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
+        <v>648</v>
+      </c>
+      <c r="B107" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" t="s">
         <v>539</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B108" t="s">
         <v>676</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3">
-      <c r="A109" t="s">
-        <v>192</v>
-      </c>
-      <c r="B109" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>166</v>
+        <v>192</v>
       </c>
       <c r="B110" t="s">
-        <v>168</v>
+        <v>193</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B111" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>644</v>
+        <v>167</v>
       </c>
       <c r="B112" t="s">
-        <v>645</v>
+        <v>169</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
+        <v>644</v>
+      </c>
+      <c r="B113" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" t="s">
         <v>538</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B114" t="s">
         <v>677</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3">
-      <c r="A115" t="s">
-        <v>190</v>
-      </c>
-      <c r="B115" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="B116" t="s">
-        <v>172</v>
-      </c>
-      <c r="C116" t="s">
-        <v>589</v>
+        <v>191</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="B117" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C117" t="s">
         <v>589</v>
@@ -7724,10 +7730,10 @@
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B118" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C118" t="s">
         <v>589</v>
@@ -7735,83 +7741,83 @@
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>203</v>
+        <v>171</v>
       </c>
       <c r="B119" t="s">
-        <v>202</v>
+        <v>174</v>
+      </c>
+      <c r="C119" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="B120" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
       <c r="B121" t="s">
-        <v>177</v>
-      </c>
-      <c r="C121" t="s">
-        <v>589</v>
+        <v>201</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>646</v>
+        <v>176</v>
       </c>
       <c r="B122" t="s">
-        <v>647</v>
+        <v>177</v>
+      </c>
+      <c r="C122" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
+        <v>646</v>
+      </c>
+      <c r="B123" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" t="s">
         <v>527</v>
       </c>
-      <c r="B123" t="s">
+      <c r="B124" t="s">
         <v>678</v>
       </c>
     </row>
-    <row r="125" spans="1:3">
-      <c r="A125" t="s">
+    <row r="126" spans="1:3">
+      <c r="A126" t="s">
         <v>653</v>
       </c>
-      <c r="B125" t="s">
+      <c r="B126" t="s">
         <v>654</v>
       </c>
-      <c r="C125" t="s">
+      <c r="C126" t="s">
         <v>655</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3">
-      <c r="A127" t="s">
-        <v>513</v>
-      </c>
-      <c r="B127" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>662</v>
+        <v>513</v>
       </c>
       <c r="B128" t="s">
-        <v>666</v>
-      </c>
-      <c r="C128" t="s">
-        <v>664</v>
+        <v>514</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B129" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="C129" t="s">
         <v>664</v>
@@ -7819,405 +7825,408 @@
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>242</v>
+        <v>663</v>
       </c>
       <c r="B130" t="s">
-        <v>243</v>
+        <v>665</v>
       </c>
       <c r="C130" t="s">
-        <v>589</v>
+        <v>664</v>
       </c>
     </row>
     <row r="131" spans="1:3">
       <c r="A131" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B131" t="s">
-        <v>245</v>
+        <v>243</v>
+      </c>
+      <c r="C131" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="B132" t="s">
-        <v>561</v>
-      </c>
-      <c r="C132" t="s">
-        <v>651</v>
+        <v>245</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="B133" t="s">
-        <v>246</v>
+        <v>561</v>
+      </c>
+      <c r="C133" t="s">
+        <v>651</v>
       </c>
     </row>
     <row r="134" spans="1:3">
       <c r="A134" t="s">
-        <v>503</v>
+        <v>247</v>
       </c>
       <c r="B134" t="s">
-        <v>512</v>
+        <v>246</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>249</v>
+        <v>503</v>
       </c>
       <c r="B135" t="s">
-        <v>248</v>
+        <v>512</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B136" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B137" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B138" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B139" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>302</v>
+        <v>257</v>
       </c>
       <c r="B140" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>349</v>
+        <v>302</v>
       </c>
       <c r="B141" t="s">
-        <v>350</v>
+        <v>248</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>658</v>
+        <v>349</v>
       </c>
       <c r="B142" t="s">
-        <v>659</v>
+        <v>350</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>703</v>
+        <v>658</v>
       </c>
       <c r="B143" t="s">
-        <v>704</v>
+        <v>659</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
+        <v>703</v>
+      </c>
+      <c r="B144" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" t="s">
         <v>526</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B145" t="s">
         <v>679</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3">
-      <c r="A146" t="s">
-        <v>515</v>
-      </c>
-      <c r="B146" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
+        <v>515</v>
+      </c>
+      <c r="B147" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" t="s">
         <v>259</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B148" t="s">
         <v>262</v>
       </c>
-      <c r="C147" t="s">
+      <c r="C148" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="148" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A148" t="s">
+    <row r="149" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A149" t="s">
         <v>261</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B149" t="s">
         <v>562</v>
       </c>
-      <c r="C148" t="s">
+      <c r="C149" t="s">
         <v>697</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3">
-      <c r="A149" t="s">
-        <v>260</v>
-      </c>
-      <c r="B149" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B150" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B151" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B152" t="s">
-        <v>268</v>
-      </c>
-      <c r="C152" t="s">
-        <v>661</v>
+        <v>267</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>504</v>
+        <v>269</v>
       </c>
       <c r="B153" t="s">
-        <v>571</v>
+        <v>268</v>
+      </c>
+      <c r="C153" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>270</v>
+        <v>504</v>
       </c>
       <c r="B154" t="s">
-        <v>271</v>
+        <v>571</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B155" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B156" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B157" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B158" t="s">
-        <v>285</v>
-      </c>
-      <c r="C158" t="s">
-        <v>661</v>
+        <v>286</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B159" t="s">
-        <v>606</v>
+        <v>285</v>
+      </c>
+      <c r="C159" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B160" t="s">
-        <v>284</v>
-      </c>
-      <c r="C160" t="s">
-        <v>661</v>
+        <v>606</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B161" t="s">
-        <v>283</v>
+        <v>284</v>
+      </c>
+      <c r="C161" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>299</v>
+        <v>282</v>
       </c>
       <c r="B162" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B163" t="s">
-        <v>248</v>
+        <v>300</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B164" t="s">
-        <v>305</v>
+        <v>248</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
-        <v>705</v>
+        <v>304</v>
       </c>
       <c r="B165" t="s">
-        <v>704</v>
+        <v>305</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
-        <v>537</v>
+        <v>705</v>
       </c>
       <c r="B166" t="s">
-        <v>680</v>
+        <v>704</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
+        <v>537</v>
+      </c>
+      <c r="B167" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="A168" t="s">
         <v>698</v>
       </c>
-      <c r="B167" t="s">
+      <c r="B168" t="s">
         <v>699</v>
       </c>
-      <c r="C167" t="s">
+      <c r="C168" t="s">
         <v>693</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3">
-      <c r="A169" t="s">
-        <v>517</v>
-      </c>
-      <c r="B169" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>292</v>
+        <v>517</v>
       </c>
       <c r="B170" t="s">
-        <v>296</v>
-      </c>
-      <c r="C170" t="s">
-        <v>589</v>
+        <v>518</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>505</v>
+        <v>292</v>
       </c>
       <c r="B171" t="s">
-        <v>572</v>
+        <v>296</v>
+      </c>
+      <c r="C171" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
-        <v>293</v>
+        <v>505</v>
       </c>
       <c r="B172" t="s">
-        <v>297</v>
-      </c>
-      <c r="C172" t="s">
-        <v>589</v>
+        <v>572</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B173" t="s">
-        <v>298</v>
+        <v>297</v>
+      </c>
+      <c r="C173" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B174" t="s">
-        <v>563</v>
+        <v>298</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="B175" t="s">
-        <v>248</v>
+        <v>563</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="B176" t="s">
-        <v>310</v>
+        <v>248</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="B177" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B178" t="s">
         <v>308</v>
@@ -8225,607 +8234,604 @@
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B179" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>706</v>
+        <v>311</v>
       </c>
       <c r="B180" t="s">
-        <v>704</v>
+        <v>312</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
+        <v>706</v>
+      </c>
+      <c r="B181" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3">
+      <c r="A182" t="s">
         <v>536</v>
       </c>
-      <c r="B181" t="s">
+      <c r="B182" t="s">
         <v>681</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3">
-      <c r="A183" t="s">
-        <v>519</v>
-      </c>
-      <c r="B183" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" t="s">
-        <v>499</v>
+        <v>519</v>
       </c>
       <c r="B184" t="s">
-        <v>320</v>
-      </c>
-      <c r="C184" t="s">
-        <v>589</v>
+        <v>520</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="B185" t="s">
-        <v>573</v>
+        <v>320</v>
+      </c>
+      <c r="C185" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="s">
-        <v>315</v>
+        <v>506</v>
       </c>
       <c r="B186" t="s">
-        <v>321</v>
-      </c>
-      <c r="C186" t="s">
-        <v>589</v>
+        <v>573</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B187" t="s">
-        <v>322</v>
+        <v>321</v>
+      </c>
+      <c r="C187" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B188" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B189" t="s">
-        <v>564</v>
+        <v>323</v>
       </c>
     </row>
     <row r="190" spans="1:3">
       <c r="A190" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B190" t="s">
-        <v>248</v>
+        <v>564</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B191" t="s">
-        <v>325</v>
-      </c>
-      <c r="C191" t="s">
-        <v>589</v>
+        <v>248</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B192" t="s">
-        <v>327</v>
+        <v>325</v>
+      </c>
+      <c r="C192" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="193" spans="1:3">
       <c r="A193" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B193" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B194" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B195" t="s">
-        <v>256</v>
+        <v>331</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>707</v>
+        <v>332</v>
       </c>
       <c r="B196" t="s">
-        <v>704</v>
+        <v>256</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
+        <v>707</v>
+      </c>
+      <c r="B197" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3">
+      <c r="A198" t="s">
         <v>535</v>
       </c>
-      <c r="B197" t="s">
+      <c r="B198" t="s">
         <v>682</v>
-      </c>
-    </row>
-    <row r="199" spans="1:3">
-      <c r="A199" t="s">
-        <v>521</v>
-      </c>
-      <c r="B199" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>501</v>
+        <v>521</v>
       </c>
       <c r="B200" t="s">
-        <v>338</v>
-      </c>
-      <c r="C200" t="s">
-        <v>589</v>
+        <v>522</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="B201" t="s">
-        <v>574</v>
+        <v>338</v>
+      </c>
+      <c r="C201" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>336</v>
+        <v>507</v>
       </c>
       <c r="B202" t="s">
-        <v>339</v>
-      </c>
-      <c r="C202" t="s">
-        <v>589</v>
+        <v>574</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B203" t="s">
-        <v>340</v>
+        <v>339</v>
+      </c>
+      <c r="C203" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
-        <v>500</v>
+        <v>337</v>
       </c>
       <c r="B204" t="s">
-        <v>565</v>
+        <v>340</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
-        <v>344</v>
+        <v>500</v>
       </c>
       <c r="B205" t="s">
-        <v>248</v>
+        <v>565</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B206" t="s">
-        <v>341</v>
+        <v>248</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B207" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B208" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B209" t="s">
-        <v>256</v>
+        <v>343</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" t="s">
-        <v>708</v>
+        <v>348</v>
       </c>
       <c r="B210" t="s">
-        <v>704</v>
+        <v>256</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
+        <v>708</v>
+      </c>
+      <c r="B211" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3">
+      <c r="A212" t="s">
         <v>534</v>
       </c>
-      <c r="B211" t="s">
+      <c r="B212" t="s">
         <v>683</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3">
-      <c r="A213" t="s">
-        <v>551</v>
-      </c>
-      <c r="B213" t="s">
-        <v>554</v>
-      </c>
-      <c r="C213" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B214" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C214" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" t="s">
-        <v>586</v>
+        <v>552</v>
       </c>
       <c r="B215" t="s">
-        <v>602</v>
+        <v>553</v>
+      </c>
+      <c r="C215" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" t="s">
-        <v>365</v>
+        <v>586</v>
       </c>
       <c r="B216" t="s">
-        <v>351</v>
+        <v>602</v>
       </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B217" t="s">
-        <v>352</v>
-      </c>
-      <c r="C217" t="s">
-        <v>589</v>
+        <v>351</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" t="s">
-        <v>508</v>
+        <v>366</v>
       </c>
       <c r="B218" t="s">
-        <v>575</v>
+        <v>352</v>
+      </c>
+      <c r="C218" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219" t="s">
-        <v>367</v>
+        <v>508</v>
       </c>
       <c r="B219" t="s">
-        <v>353</v>
+        <v>575</v>
       </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B220" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B221" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B222" t="s">
-        <v>356</v>
-      </c>
-      <c r="C222" t="s">
-        <v>589</v>
+        <v>355</v>
       </c>
     </row>
     <row r="223" spans="1:3">
       <c r="A223" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B223" t="s">
-        <v>357</v>
+        <v>356</v>
+      </c>
+      <c r="C223" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B224" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B225" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B226" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="227" spans="1:3">
       <c r="A227" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B227" t="s">
-        <v>361</v>
-      </c>
-      <c r="C227" t="s">
-        <v>589</v>
+        <v>360</v>
       </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B228" t="s">
-        <v>362</v>
+        <v>361</v>
+      </c>
+      <c r="C228" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B229" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B230" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="231" spans="1:3">
       <c r="A231" t="s">
+        <v>378</v>
+      </c>
+      <c r="B231" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3">
+      <c r="A232" t="s">
         <v>533</v>
       </c>
-      <c r="B231" t="s">
+      <c r="B232" t="s">
         <v>667</v>
-      </c>
-    </row>
-    <row r="233" spans="1:3">
-      <c r="A233" t="s">
-        <v>607</v>
-      </c>
-      <c r="B233" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" t="s">
-        <v>385</v>
+        <v>607</v>
       </c>
       <c r="B234" t="s">
-        <v>403</v>
+        <v>608</v>
       </c>
     </row>
     <row r="235" spans="1:3">
       <c r="A235" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B235" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B236" t="s">
-        <v>401</v>
-      </c>
-      <c r="C236" t="s">
-        <v>589</v>
+        <v>400</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" t="s">
-        <v>509</v>
+        <v>387</v>
       </c>
       <c r="B237" t="s">
-        <v>576</v>
+        <v>401</v>
+      </c>
+      <c r="C237" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" t="s">
-        <v>404</v>
+        <v>509</v>
       </c>
       <c r="B238" t="s">
-        <v>402</v>
-      </c>
-      <c r="C238" t="s">
-        <v>589</v>
+        <v>576</v>
       </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239" t="s">
-        <v>388</v>
+        <v>404</v>
       </c>
       <c r="B239" t="s">
-        <v>394</v>
+        <v>402</v>
+      </c>
+      <c r="C239" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="240" spans="1:3">
       <c r="A240" t="s">
-        <v>405</v>
+        <v>388</v>
       </c>
       <c r="B240" t="s">
-        <v>395</v>
-      </c>
-      <c r="C240" t="s">
-        <v>566</v>
+        <v>394</v>
       </c>
     </row>
     <row r="241" spans="1:3">
       <c r="A241" t="s">
-        <v>389</v>
+        <v>405</v>
       </c>
       <c r="B241" t="s">
-        <v>396</v>
+        <v>395</v>
+      </c>
+      <c r="C241" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B242" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="243" spans="1:3">
       <c r="A243" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B243" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="244" spans="1:3">
       <c r="A244" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B244" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="245" spans="1:3">
       <c r="A245" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B245" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
     </row>
     <row r="246" spans="1:3">
       <c r="A246" t="s">
+        <v>393</v>
+      </c>
+      <c r="B246" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3">
+      <c r="A247" t="s">
         <v>532</v>
       </c>
-      <c r="B246" t="s">
+      <c r="B247" t="s">
         <v>684</v>
-      </c>
-    </row>
-    <row r="248" spans="1:3">
-      <c r="A248" t="s">
-        <v>523</v>
-      </c>
-      <c r="B248" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="249" spans="1:3">
       <c r="A249" t="s">
-        <v>411</v>
+        <v>523</v>
       </c>
       <c r="B249" t="s">
-        <v>422</v>
+        <v>524</v>
       </c>
     </row>
     <row r="250" spans="1:3">
       <c r="A250" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B250" t="s">
-        <v>423</v>
-      </c>
-      <c r="C250" t="s">
-        <v>589</v>
+        <v>422</v>
       </c>
     </row>
     <row r="251" spans="1:3">
       <c r="A251" t="s">
-        <v>577</v>
+        <v>412</v>
       </c>
       <c r="B251" t="s">
-        <v>578</v>
+        <v>423</v>
+      </c>
+      <c r="C251" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="252" spans="1:3">
       <c r="A252" t="s">
-        <v>413</v>
+        <v>577</v>
       </c>
       <c r="B252" t="s">
-        <v>424</v>
-      </c>
-      <c r="C252" t="s">
-        <v>589</v>
+        <v>578</v>
       </c>
     </row>
     <row r="253" spans="1:3">
       <c r="A253" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B253" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C253" t="s">
         <v>589</v>
@@ -8833,128 +8839,128 @@
     </row>
     <row r="254" spans="1:3">
       <c r="A254" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B254" t="s">
-        <v>590</v>
+        <v>425</v>
+      </c>
+      <c r="C254" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="255" spans="1:3">
       <c r="A255" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B255" t="s">
-        <v>426</v>
+        <v>590</v>
       </c>
     </row>
     <row r="256" spans="1:3">
       <c r="A256" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B256" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="257" spans="1:3">
       <c r="A257" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B257" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="258" spans="1:3">
       <c r="A258" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B258" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="259" spans="1:3">
       <c r="A259" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B259" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="260" spans="1:3">
       <c r="A260" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B260" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="261" spans="1:3">
       <c r="A261" t="s">
-        <v>530</v>
+        <v>421</v>
       </c>
       <c r="B261" t="s">
-        <v>685</v>
+        <v>431</v>
       </c>
     </row>
     <row r="262" spans="1:3">
       <c r="A262" t="s">
+        <v>530</v>
+      </c>
+      <c r="B262" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3">
+      <c r="A263" t="s">
         <v>616</v>
       </c>
-      <c r="B262" t="s">
+      <c r="B263" t="s">
         <v>617</v>
-      </c>
-    </row>
-    <row r="264" spans="1:3">
-      <c r="A264" t="s">
-        <v>525</v>
-      </c>
-      <c r="B264" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="265" spans="1:3">
       <c r="A265" t="s">
-        <v>438</v>
+        <v>525</v>
       </c>
       <c r="B265" t="s">
-        <v>449</v>
+        <v>524</v>
       </c>
     </row>
     <row r="266" spans="1:3">
       <c r="A266" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B266" t="s">
-        <v>450</v>
-      </c>
-      <c r="C266" t="s">
-        <v>589</v>
+        <v>449</v>
       </c>
     </row>
     <row r="267" spans="1:3">
       <c r="A267" t="s">
-        <v>510</v>
+        <v>439</v>
       </c>
       <c r="B267" t="s">
-        <v>579</v>
+        <v>450</v>
+      </c>
+      <c r="C267" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="268" spans="1:3">
       <c r="A268" t="s">
-        <v>440</v>
+        <v>510</v>
       </c>
       <c r="B268" t="s">
-        <v>451</v>
-      </c>
-      <c r="C268" t="s">
-        <v>589</v>
+        <v>579</v>
       </c>
     </row>
     <row r="269" spans="1:3">
       <c r="A269" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B269" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C269" t="s">
         <v>589</v>
@@ -8962,132 +8968,143 @@
     </row>
     <row r="270" spans="1:3">
       <c r="A270" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B270" t="s">
-        <v>591</v>
+        <v>452</v>
+      </c>
+      <c r="C270" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="271" spans="1:3">
       <c r="A271" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B271" t="s">
-        <v>426</v>
+        <v>591</v>
       </c>
     </row>
     <row r="272" spans="1:3">
       <c r="A272" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B272" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="273" spans="1:3">
       <c r="A273" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B273" t="s">
-        <v>453</v>
+        <v>427</v>
       </c>
     </row>
     <row r="274" spans="1:3">
       <c r="A274" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B274" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="275" spans="1:3">
       <c r="A275" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B275" t="s">
-        <v>430</v>
+        <v>454</v>
       </c>
     </row>
     <row r="276" spans="1:3">
       <c r="A276" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B276" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="277" spans="1:3">
       <c r="A277" t="s">
-        <v>529</v>
+        <v>448</v>
       </c>
       <c r="B277" t="s">
-        <v>685</v>
+        <v>431</v>
       </c>
     </row>
     <row r="278" spans="1:3">
       <c r="A278" t="s">
+        <v>529</v>
+      </c>
+      <c r="B278" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3">
+      <c r="A279" t="s">
         <v>623</v>
       </c>
-      <c r="B278" t="s">
+      <c r="B279" t="s">
         <v>617</v>
-      </c>
-    </row>
-    <row r="280" spans="1:3">
-      <c r="A280" t="s">
-        <v>432</v>
-      </c>
-      <c r="B280" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="281" spans="1:3">
       <c r="A281" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B281" t="s">
-        <v>625</v>
-      </c>
-      <c r="C281" t="s">
-        <v>589</v>
+        <v>624</v>
       </c>
     </row>
     <row r="282" spans="1:3">
       <c r="A282" t="s">
-        <v>511</v>
+        <v>433</v>
       </c>
       <c r="B282" t="s">
-        <v>626</v>
+        <v>625</v>
+      </c>
+      <c r="C282" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="283" spans="1:3">
       <c r="A283" t="s">
-        <v>434</v>
+        <v>511</v>
       </c>
       <c r="B283" t="s">
-        <v>652</v>
+        <v>626</v>
       </c>
     </row>
     <row r="284" spans="1:3">
       <c r="A284" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B284" t="s">
-        <v>627</v>
+        <v>652</v>
       </c>
     </row>
     <row r="285" spans="1:3">
       <c r="A285" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B285" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="286" spans="1:3">
       <c r="A286" t="s">
+        <v>436</v>
+      </c>
+      <c r="B286" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3">
+      <c r="A287" t="s">
         <v>528</v>
       </c>
-      <c r="B286" t="s">
+      <c r="B287" t="s">
         <v>686</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes for 57812 (Added Housing Disclosure check), 57773 (Added checks for the number of adults that signed the following docs: VAWA, ASC, SC, and AS), and 57764 (Changes in EDC - added a variable to count the number of PS on the EDC and then check if the number of PS listed and the required number of PS for HOME Unit are equal)
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raluca.ilinca.AzureAI-Jump2\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A76F8E-684F-42B4-AEA2-17E8FBFC69BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C42B86-236A-4DA5-ADEB-323FB25D606D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28200" windowHeight="13530" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="22440" windowHeight="11715" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="731">
   <si>
     <t>Name</t>
   </si>
@@ -2169,9 +2169,6 @@
     <t>VS_MultipleIncomeDocsExists</t>
   </si>
   <si>
-    <t>C:\Users\harika.malyala\Documents\AZApplicationReview\Prompts\</t>
-  </si>
-  <si>
     <t>AnnualSC</t>
   </si>
   <si>
@@ -2197,6 +2194,45 @@
   </si>
   <si>
     <t>There is a Unborn Child listed on the ICW but has a date of birth listed in the past.</t>
+  </si>
+  <si>
+    <t>AS_NotAllAdultsSigned</t>
+  </si>
+  <si>
+    <t>Not all adults in the household have signed the Application Summary.</t>
+  </si>
+  <si>
+    <t>ASC_NotAllAdultsSigned</t>
+  </si>
+  <si>
+    <t>Not all adults in the household have signed the Asset Self Certification.</t>
+  </si>
+  <si>
+    <t>SC_NotAllAdultsSigned</t>
+  </si>
+  <si>
+    <t>Not all adults in the household have signed the SC.</t>
+  </si>
+  <si>
+    <t>VAWA_NotAllAdultsSigned</t>
+  </si>
+  <si>
+    <t>Not all adults in the household have signed the VAWA.</t>
+  </si>
+  <si>
+    <t>C:\Users\raluca.ilinca.AzureAI-Jump2\Documents\AZApplicationReview\Prompts\</t>
+  </si>
+  <si>
+    <t>The Housing History Disclosure form is a required document but missing from the application.</t>
+  </si>
+  <si>
+    <t>HousingDisclosureExists</t>
+  </si>
+  <si>
+    <t>EDC_NoOfRequiredPSNotSupplied</t>
+  </si>
+  <si>
+    <t>This is a HOME unit, but 2 months of paystubs were not provided as required.</t>
   </si>
 </sst>
 </file>
@@ -2574,8 +2610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2583,7 +2619,8 @@
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
     <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2658,7 +2695,7 @@
         <v>209</v>
       </c>
       <c r="B7" t="s">
-        <v>709</v>
+        <v>726</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -2704,10 +2741,10 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>709</v>
+      </c>
+      <c r="B14" t="s">
         <v>710</v>
-      </c>
-      <c r="B14" t="s">
-        <v>711</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
@@ -2869,7 +2906,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="14.25" customHeight="1">
+    <row r="33" spans="1:4" ht="14.25" customHeight="1">
       <c r="A33" t="s">
         <v>381</v>
       </c>
@@ -2877,7 +2914,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="14.25" customHeight="1">
+    <row r="34" spans="1:4" ht="14.25" customHeight="1">
       <c r="A34" t="s">
         <v>383</v>
       </c>
@@ -2885,7 +2922,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="14.25" customHeight="1">
+    <row r="35" spans="1:4" ht="14.25" customHeight="1">
       <c r="A35" t="s">
         <v>410</v>
       </c>
@@ -2893,7 +2930,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="14.25" customHeight="1">
+    <row r="36" spans="1:4" ht="14.25" customHeight="1">
       <c r="A36" t="s">
         <v>408</v>
       </c>
@@ -2901,7 +2938,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="14.25" customHeight="1">
+    <row r="37" spans="1:4" ht="14.25" customHeight="1">
       <c r="A37" t="s">
         <v>456</v>
       </c>
@@ -2909,7 +2946,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="14.25" customHeight="1">
+    <row r="38" spans="1:4" ht="14.25" customHeight="1">
       <c r="A38" t="s">
         <v>458</v>
       </c>
@@ -2917,7 +2954,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="14.25" customHeight="1">
+    <row r="39" spans="1:4" ht="14.25" customHeight="1">
       <c r="A39" t="s">
         <v>406</v>
       </c>
@@ -2925,7 +2962,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="14.25" customHeight="1">
+    <row r="40" spans="1:4" ht="14.25" customHeight="1">
       <c r="A40" t="s">
         <v>459</v>
       </c>
@@ -2933,7 +2970,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="14.25" customHeight="1">
+    <row r="41" spans="1:4" ht="14.25" customHeight="1">
       <c r="A41" t="s">
         <v>437</v>
       </c>
@@ -2941,13 +2978,23 @@
         <v>622</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="44" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="45" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="46" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="47" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:4" ht="14.25" customHeight="1">
+      <c r="A42" t="s">
+        <v>485</v>
+      </c>
+      <c r="B42" t="s">
+        <v>485</v>
+      </c>
+      <c r="D42" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:4" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:4" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>
@@ -3914,13 +3961,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80DB68E2-2057-45AB-A45E-3EB9CF844C19}">
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -6823,10 +6871,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
-  <dimension ref="A1:C287"/>
+  <dimension ref="A1:C294"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="C133" sqref="C133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6854,354 +6902,343 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>180</v>
+        <v>728</v>
       </c>
       <c r="B5" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B6" t="s">
-        <v>71</v>
+        <v>727</v>
+      </c>
+      <c r="C5" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B7" t="s">
-        <v>178</v>
+        <v>496</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>206</v>
+        <v>179</v>
       </c>
       <c r="B9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C9" t="s">
-        <v>660</v>
+        <v>178</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>549</v>
+        <v>78</v>
       </c>
       <c r="B10" t="s">
-        <v>550</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>688</v>
+        <v>206</v>
       </c>
       <c r="B11" t="s">
-        <v>689</v>
+        <v>207</v>
+      </c>
+      <c r="C11" t="s">
+        <v>660</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>531</v>
+        <v>549</v>
       </c>
       <c r="B12" t="s">
-        <v>668</v>
+        <v>550</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>701</v>
+        <v>688</v>
       </c>
       <c r="B13" t="s">
-        <v>702</v>
-      </c>
-      <c r="C13" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>717</v>
+        <v>531</v>
       </c>
       <c r="B14" t="s">
-        <v>718</v>
-      </c>
-      <c r="C14" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>701</v>
+      </c>
+      <c r="B15" t="s">
+        <v>702</v>
+      </c>
+      <c r="C15" t="s">
         <v>693</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" t="s">
+        <v>716</v>
+      </c>
+      <c r="B16" t="s">
+        <v>717</v>
+      </c>
+      <c r="C16" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
         <v>181</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
         <v>79</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" t="s">
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
         <v>559</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
         <v>80</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
         <v>82</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B22" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
         <v>196</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" t="s">
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
         <v>198</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B24" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" t="s">
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
         <v>84</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B25" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" t="s">
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
         <v>86</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" t="s">
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
         <v>81</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B27" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" t="s">
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
         <v>89</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B28" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" t="s">
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
         <v>632</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B29" t="s">
         <v>633</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" t="s">
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
         <v>656</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B30" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" t="s">
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
         <v>546</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B31" t="s">
         <v>669</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="A31" t="s">
-        <v>183</v>
-      </c>
-      <c r="B31" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>91</v>
+        <v>718</v>
       </c>
       <c r="B32" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
-        <v>93</v>
-      </c>
-      <c r="B33" t="s">
-        <v>94</v>
+        <v>719</v>
+      </c>
+      <c r="C32" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>101</v>
+        <v>183</v>
       </c>
       <c r="B34" t="s">
-        <v>95</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="B35" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B36" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B37" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B38" t="s">
-        <v>99</v>
-      </c>
-      <c r="C38" t="s">
-        <v>589</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B39" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>634</v>
+        <v>104</v>
       </c>
       <c r="B40" t="s">
-        <v>635</v>
+        <v>98</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>545</v>
+        <v>105</v>
       </c>
       <c r="B41" t="s">
-        <v>670</v>
+        <v>99</v>
+      </c>
+      <c r="C41" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>694</v>
+        <v>106</v>
       </c>
       <c r="B42" t="s">
-        <v>695</v>
-      </c>
-      <c r="C42" t="s">
-        <v>693</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>634</v>
+      </c>
+      <c r="B43" t="s">
+        <v>635</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>184</v>
+        <v>545</v>
       </c>
       <c r="B44" t="s">
-        <v>592</v>
+        <v>670</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>107</v>
+        <v>694</v>
       </c>
       <c r="B45" t="s">
-        <v>108</v>
+        <v>695</v>
       </c>
       <c r="C45" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" t="s">
-        <v>117</v>
-      </c>
-      <c r="B46" t="s">
-        <v>118</v>
-      </c>
-      <c r="C46" t="s">
-        <v>589</v>
+        <v>693</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>119</v>
+        <v>184</v>
       </c>
       <c r="B47" t="s">
-        <v>120</v>
-      </c>
-      <c r="C47" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B48" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C48" t="s">
         <v>589</v>
@@ -7209,10 +7246,10 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B49" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C49" t="s">
         <v>589</v>
@@ -7220,10 +7257,10 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="B50" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="C50" t="s">
         <v>589</v>
@@ -7231,26 +7268,32 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B51" t="s">
-        <v>112</v>
+        <v>109</v>
+      </c>
+      <c r="C51" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>204</v>
+        <v>114</v>
       </c>
       <c r="B52" t="s">
-        <v>494</v>
+        <v>110</v>
+      </c>
+      <c r="C52" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>205</v>
+        <v>115</v>
       </c>
       <c r="B53" t="s">
-        <v>593</v>
+        <v>111</v>
       </c>
       <c r="C53" t="s">
         <v>589</v>
@@ -7258,1088 +7301,1097 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>580</v>
+        <v>116</v>
       </c>
       <c r="B54" t="s">
-        <v>594</v>
+        <v>112</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>547</v>
+        <v>204</v>
       </c>
       <c r="B55" t="s">
-        <v>548</v>
+        <v>494</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>555</v>
+        <v>205</v>
       </c>
       <c r="B56" t="s">
-        <v>631</v>
+        <v>593</v>
+      </c>
+      <c r="C56" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>544</v>
+        <v>580</v>
       </c>
       <c r="B57" t="s">
-        <v>671</v>
+        <v>594</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>547</v>
+      </c>
+      <c r="B58" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>158</v>
+        <v>555</v>
       </c>
       <c r="B59" t="s">
-        <v>121</v>
+        <v>631</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>122</v>
+        <v>544</v>
       </c>
       <c r="B60" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" t="s">
-        <v>124</v>
-      </c>
-      <c r="B61" t="s">
-        <v>123</v>
+        <v>671</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>636</v>
+        <v>158</v>
       </c>
       <c r="B62" t="s">
-        <v>637</v>
+        <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" t="s">
-        <v>543</v>
+        <v>122</v>
       </c>
       <c r="B63" t="s">
-        <v>672</v>
+        <v>595</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>124</v>
+      </c>
+      <c r="B64" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>186</v>
+        <v>636</v>
       </c>
       <c r="B65" t="s">
-        <v>187</v>
+        <v>637</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>125</v>
+        <v>543</v>
       </c>
       <c r="B66" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" t="s">
-        <v>126</v>
-      </c>
-      <c r="B67" t="s">
-        <v>128</v>
+        <v>672</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>138</v>
+        <v>186</v>
       </c>
       <c r="B68" t="s">
-        <v>596</v>
+        <v>187</v>
       </c>
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="B69" t="s">
-        <v>597</v>
+        <v>127</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="B70" t="s">
-        <v>598</v>
+        <v>128</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B71" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B72" t="s">
-        <v>495</v>
-      </c>
-      <c r="C72" t="s">
-        <v>687</v>
+        <v>597</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B73" t="s">
-        <v>497</v>
-      </c>
-      <c r="C73" t="s">
-        <v>556</v>
+        <v>598</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B74" t="s">
-        <v>498</v>
-      </c>
-      <c r="C74" t="s">
-        <v>556</v>
+        <v>599</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>638</v>
+        <v>142</v>
       </c>
       <c r="B75" t="s">
-        <v>639</v>
+        <v>495</v>
+      </c>
+      <c r="C75" t="s">
+        <v>687</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>542</v>
+        <v>143</v>
       </c>
       <c r="B76" t="s">
-        <v>673</v>
+        <v>497</v>
+      </c>
+      <c r="C76" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>144</v>
+      </c>
+      <c r="B77" t="s">
+        <v>498</v>
+      </c>
+      <c r="C77" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>147</v>
+        <v>638</v>
       </c>
       <c r="B78" t="s">
-        <v>150</v>
+        <v>639</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>148</v>
+        <v>542</v>
       </c>
       <c r="B79" t="s">
-        <v>151</v>
+        <v>673</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>149</v>
+        <v>720</v>
       </c>
       <c r="B80" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" t="s">
-        <v>145</v>
-      </c>
-      <c r="B81" t="s">
-        <v>581</v>
-      </c>
-      <c r="C81" t="s">
-        <v>692</v>
+        <v>721</v>
+      </c>
+      <c r="C80" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>691</v>
+        <v>147</v>
       </c>
       <c r="B82" t="s">
-        <v>581</v>
+        <v>150</v>
       </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B83" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="B84" t="s">
-        <v>600</v>
+        <v>152</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="B85" t="s">
-        <v>130</v>
+        <v>581</v>
+      </c>
+      <c r="C85" t="s">
+        <v>692</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>640</v>
+        <v>691</v>
       </c>
       <c r="B86" t="s">
-        <v>641</v>
+        <v>581</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>541</v>
+        <v>146</v>
       </c>
       <c r="B87" t="s">
-        <v>674</v>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>131</v>
+      </c>
+      <c r="B88" t="s">
+        <v>600</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>188</v>
+        <v>132</v>
       </c>
       <c r="B89" t="s">
-        <v>189</v>
+        <v>130</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>133</v>
+        <v>640</v>
       </c>
       <c r="B90" t="s">
-        <v>153</v>
+        <v>641</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>135</v>
+        <v>541</v>
       </c>
       <c r="B91" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="A92" t="s">
-        <v>134</v>
-      </c>
-      <c r="B92" t="s">
-        <v>155</v>
+        <v>674</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>136</v>
+        <v>188</v>
       </c>
       <c r="B93" t="s">
-        <v>156</v>
+        <v>189</v>
       </c>
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B94" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>630</v>
+        <v>135</v>
       </c>
       <c r="B95" t="s">
-        <v>696</v>
-      </c>
-      <c r="C95" t="s">
-        <v>700</v>
+        <v>154</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>642</v>
+        <v>134</v>
       </c>
       <c r="B96" t="s">
-        <v>643</v>
+        <v>155</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>540</v>
+        <v>136</v>
       </c>
       <c r="B97" t="s">
-        <v>675</v>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
+        <v>137</v>
+      </c>
+      <c r="B98" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>712</v>
+        <v>630</v>
       </c>
       <c r="B99" t="s">
-        <v>713</v>
+        <v>696</v>
       </c>
       <c r="C99" t="s">
-        <v>714</v>
+        <v>700</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>715</v>
+        <v>642</v>
       </c>
       <c r="B100" t="s">
-        <v>716</v>
-      </c>
-      <c r="C100" t="s">
-        <v>714</v>
+        <v>643</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="s">
+        <v>540</v>
+      </c>
+      <c r="B101" t="s">
+        <v>675</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>159</v>
+        <v>722</v>
       </c>
       <c r="B102" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3">
-      <c r="A103" t="s">
-        <v>160</v>
-      </c>
-      <c r="B103" t="s">
-        <v>164</v>
+        <v>723</v>
+      </c>
+      <c r="C102" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>161</v>
+        <v>711</v>
       </c>
       <c r="B104" t="s">
-        <v>165</v>
+        <v>712</v>
+      </c>
+      <c r="C104" t="s">
+        <v>713</v>
       </c>
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>162</v>
+        <v>714</v>
       </c>
       <c r="B105" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3">
-      <c r="A106" t="s">
-        <v>557</v>
-      </c>
-      <c r="B106" t="s">
-        <v>558</v>
+        <v>715</v>
+      </c>
+      <c r="C105" t="s">
+        <v>713</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>648</v>
+        <v>159</v>
       </c>
       <c r="B107" t="s">
-        <v>649</v>
+        <v>163</v>
       </c>
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>539</v>
+        <v>160</v>
       </c>
       <c r="B108" t="s">
-        <v>676</v>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" t="s">
+        <v>161</v>
+      </c>
+      <c r="B109" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>192</v>
+        <v>162</v>
       </c>
       <c r="B110" t="s">
-        <v>193</v>
+        <v>601</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>166</v>
+        <v>557</v>
       </c>
       <c r="B111" t="s">
-        <v>168</v>
+        <v>558</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>167</v>
+        <v>648</v>
       </c>
       <c r="B112" t="s">
-        <v>169</v>
+        <v>649</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>644</v>
+        <v>539</v>
       </c>
       <c r="B113" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3">
-      <c r="A114" t="s">
-        <v>538</v>
-      </c>
-      <c r="B114" t="s">
-        <v>677</v>
+        <v>676</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" t="s">
+        <v>192</v>
+      </c>
+      <c r="B115" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="B116" t="s">
-        <v>191</v>
+        <v>168</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="B117" t="s">
-        <v>172</v>
-      </c>
-      <c r="C117" t="s">
-        <v>589</v>
+        <v>169</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>170</v>
+        <v>644</v>
       </c>
       <c r="B118" t="s">
-        <v>173</v>
-      </c>
-      <c r="C118" t="s">
-        <v>589</v>
+        <v>645</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>171</v>
+        <v>538</v>
       </c>
       <c r="B119" t="s">
-        <v>174</v>
-      </c>
-      <c r="C119" t="s">
-        <v>589</v>
+        <v>677</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>203</v>
+        <v>724</v>
       </c>
       <c r="B120" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3">
-      <c r="A121" t="s">
-        <v>200</v>
-      </c>
-      <c r="B121" t="s">
-        <v>201</v>
+        <v>725</v>
+      </c>
+      <c r="C120" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="B122" t="s">
-        <v>177</v>
-      </c>
-      <c r="C122" t="s">
-        <v>589</v>
+        <v>191</v>
       </c>
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>646</v>
+        <v>175</v>
       </c>
       <c r="B123" t="s">
-        <v>647</v>
+        <v>172</v>
+      </c>
+      <c r="C123" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>527</v>
+        <v>170</v>
       </c>
       <c r="B124" t="s">
-        <v>678</v>
+        <v>173</v>
+      </c>
+      <c r="C124" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" t="s">
+        <v>171</v>
+      </c>
+      <c r="B125" t="s">
+        <v>174</v>
+      </c>
+      <c r="C125" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>653</v>
+        <v>203</v>
       </c>
       <c r="B126" t="s">
-        <v>654</v>
-      </c>
-      <c r="C126" t="s">
-        <v>655</v>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" t="s">
+        <v>200</v>
+      </c>
+      <c r="B127" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>513</v>
+        <v>176</v>
       </c>
       <c r="B128" t="s">
-        <v>514</v>
+        <v>177</v>
+      </c>
+      <c r="C128" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>662</v>
+        <v>646</v>
       </c>
       <c r="B129" t="s">
-        <v>666</v>
-      </c>
-      <c r="C129" t="s">
-        <v>664</v>
+        <v>647</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>663</v>
+        <v>527</v>
       </c>
       <c r="B130" t="s">
-        <v>665</v>
-      </c>
-      <c r="C130" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3">
-      <c r="A131" t="s">
-        <v>242</v>
-      </c>
-      <c r="B131" t="s">
-        <v>243</v>
-      </c>
-      <c r="C131" t="s">
-        <v>589</v>
+        <v>678</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
-        <v>244</v>
+        <v>653</v>
       </c>
       <c r="B132" t="s">
-        <v>245</v>
+        <v>654</v>
+      </c>
+      <c r="C132" t="s">
+        <v>655</v>
       </c>
     </row>
     <row r="133" spans="1:3">
       <c r="A133" t="s">
-        <v>258</v>
+        <v>729</v>
       </c>
       <c r="B133" t="s">
-        <v>561</v>
+        <v>730</v>
       </c>
       <c r="C133" t="s">
-        <v>651</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3">
-      <c r="A134" t="s">
-        <v>247</v>
-      </c>
-      <c r="B134" t="s">
-        <v>246</v>
+        <v>693</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>503</v>
+        <v>513</v>
       </c>
       <c r="B135" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>249</v>
+        <v>662</v>
       </c>
       <c r="B136" t="s">
-        <v>248</v>
+        <v>666</v>
+      </c>
+      <c r="C136" t="s">
+        <v>664</v>
       </c>
     </row>
     <row r="137" spans="1:3">
       <c r="A137" t="s">
-        <v>250</v>
+        <v>663</v>
       </c>
       <c r="B137" t="s">
-        <v>252</v>
+        <v>665</v>
+      </c>
+      <c r="C137" t="s">
+        <v>664</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="B138" t="s">
-        <v>253</v>
+        <v>243</v>
+      </c>
+      <c r="C138" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="B139" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B140" t="s">
-        <v>256</v>
+        <v>561</v>
+      </c>
+      <c r="C140" t="s">
+        <v>651</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>302</v>
+        <v>247</v>
       </c>
       <c r="B141" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>349</v>
+        <v>503</v>
       </c>
       <c r="B142" t="s">
-        <v>350</v>
+        <v>512</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>658</v>
+        <v>249</v>
       </c>
       <c r="B143" t="s">
-        <v>659</v>
+        <v>248</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>703</v>
+        <v>250</v>
       </c>
       <c r="B144" t="s">
-        <v>704</v>
+        <v>252</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>526</v>
+        <v>251</v>
       </c>
       <c r="B145" t="s">
-        <v>679</v>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" t="s">
+        <v>255</v>
+      </c>
+      <c r="B146" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>515</v>
+        <v>257</v>
       </c>
       <c r="B147" t="s">
-        <v>516</v>
+        <v>256</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>259</v>
+        <v>302</v>
       </c>
       <c r="B148" t="s">
-        <v>262</v>
-      </c>
-      <c r="C148" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" ht="13.5" customHeight="1">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>261</v>
+        <v>349</v>
       </c>
       <c r="B149" t="s">
-        <v>562</v>
-      </c>
-      <c r="C149" t="s">
-        <v>697</v>
+        <v>350</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>260</v>
+        <v>658</v>
       </c>
       <c r="B150" t="s">
-        <v>263</v>
+        <v>659</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>265</v>
+        <v>703</v>
       </c>
       <c r="B151" t="s">
-        <v>264</v>
+        <v>704</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>266</v>
+        <v>526</v>
       </c>
       <c r="B152" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3">
-      <c r="A153" t="s">
-        <v>269</v>
-      </c>
-      <c r="B153" t="s">
-        <v>268</v>
-      </c>
-      <c r="C153" t="s">
-        <v>661</v>
+        <v>679</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>504</v>
+        <v>515</v>
       </c>
       <c r="B154" t="s">
-        <v>571</v>
+        <v>516</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="B155" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3">
+        <v>262</v>
+      </c>
+      <c r="C155" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" ht="13.5" customHeight="1">
       <c r="A156" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="B156" t="s">
-        <v>273</v>
+        <v>562</v>
+      </c>
+      <c r="C156" t="s">
+        <v>697</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>277</v>
+        <v>260</v>
       </c>
       <c r="B157" t="s">
-        <v>287</v>
+        <v>263</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="B158" t="s">
-        <v>286</v>
+        <v>264</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="B159" t="s">
-        <v>285</v>
-      </c>
-      <c r="C159" t="s">
-        <v>661</v>
+        <v>267</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="B160" t="s">
-        <v>606</v>
+        <v>268</v>
+      </c>
+      <c r="C160" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>281</v>
+        <v>504</v>
       </c>
       <c r="B161" t="s">
-        <v>284</v>
-      </c>
-      <c r="C161" t="s">
-        <v>661</v>
+        <v>571</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
       <c r="B162" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>299</v>
+        <v>272</v>
       </c>
       <c r="B163" t="s">
-        <v>300</v>
+        <v>273</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>301</v>
+        <v>277</v>
       </c>
       <c r="B164" t="s">
-        <v>248</v>
+        <v>287</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
-        <v>304</v>
+        <v>278</v>
       </c>
       <c r="B165" t="s">
-        <v>305</v>
+        <v>286</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
-        <v>705</v>
+        <v>279</v>
       </c>
       <c r="B166" t="s">
-        <v>704</v>
+        <v>285</v>
+      </c>
+      <c r="C166" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
-        <v>537</v>
+        <v>280</v>
       </c>
       <c r="B167" t="s">
-        <v>680</v>
+        <v>606</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
-        <v>698</v>
+        <v>281</v>
       </c>
       <c r="B168" t="s">
-        <v>699</v>
+        <v>284</v>
       </c>
       <c r="C168" t="s">
-        <v>693</v>
+        <v>661</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
+      <c r="A169" t="s">
+        <v>282</v>
+      </c>
+      <c r="B169" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>517</v>
+        <v>299</v>
       </c>
       <c r="B170" t="s">
-        <v>518</v>
+        <v>300</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
       <c r="B171" t="s">
-        <v>296</v>
-      </c>
-      <c r="C171" t="s">
-        <v>589</v>
+        <v>248</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
-        <v>505</v>
+        <v>304</v>
       </c>
       <c r="B172" t="s">
-        <v>572</v>
+        <v>305</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
-        <v>293</v>
+        <v>705</v>
       </c>
       <c r="B173" t="s">
-        <v>297</v>
-      </c>
-      <c r="C173" t="s">
-        <v>589</v>
+        <v>704</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>294</v>
+        <v>537</v>
       </c>
       <c r="B174" t="s">
-        <v>298</v>
+        <v>680</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>295</v>
+        <v>698</v>
       </c>
       <c r="B175" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3">
-      <c r="A176" t="s">
-        <v>303</v>
-      </c>
-      <c r="B176" t="s">
-        <v>248</v>
+        <v>699</v>
+      </c>
+      <c r="C175" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>309</v>
+        <v>517</v>
       </c>
       <c r="B177" t="s">
-        <v>310</v>
+        <v>518</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="B178" t="s">
-        <v>308</v>
+        <v>296</v>
+      </c>
+      <c r="C178" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="179" spans="1:3">
       <c r="A179" t="s">
-        <v>307</v>
+        <v>505</v>
       </c>
       <c r="B179" t="s">
-        <v>308</v>
+        <v>572</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>311</v>
+        <v>293</v>
       </c>
       <c r="B180" t="s">
-        <v>312</v>
+        <v>297</v>
+      </c>
+      <c r="C180" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
-        <v>706</v>
+        <v>294</v>
       </c>
       <c r="B181" t="s">
-        <v>704</v>
+        <v>298</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" t="s">
-        <v>536</v>
+        <v>295</v>
       </c>
       <c r="B182" t="s">
-        <v>681</v>
+        <v>563</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3">
+      <c r="A183" t="s">
+        <v>303</v>
+      </c>
+      <c r="B183" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" t="s">
-        <v>519</v>
+        <v>309</v>
       </c>
       <c r="B184" t="s">
-        <v>520</v>
+        <v>310</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="s">
-        <v>499</v>
+        <v>306</v>
       </c>
       <c r="B185" t="s">
-        <v>320</v>
-      </c>
-      <c r="C185" t="s">
-        <v>589</v>
+        <v>308</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="s">
-        <v>506</v>
+        <v>307</v>
       </c>
       <c r="B186" t="s">
-        <v>573</v>
+        <v>308</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B187" t="s">
-        <v>321</v>
-      </c>
-      <c r="C187" t="s">
-        <v>589</v>
+        <v>312</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" t="s">
-        <v>316</v>
+        <v>706</v>
       </c>
       <c r="B188" t="s">
-        <v>322</v>
+        <v>704</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" t="s">
-        <v>317</v>
+        <v>536</v>
       </c>
       <c r="B189" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3">
-      <c r="A190" t="s">
-        <v>318</v>
-      </c>
-      <c r="B190" t="s">
-        <v>564</v>
+        <v>681</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" t="s">
-        <v>319</v>
+        <v>519</v>
       </c>
       <c r="B191" t="s">
-        <v>248</v>
+        <v>520</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" t="s">
-        <v>324</v>
+        <v>499</v>
       </c>
       <c r="B192" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="C192" t="s">
         <v>589</v>
@@ -8347,764 +8399,826 @@
     </row>
     <row r="193" spans="1:3">
       <c r="A193" t="s">
-        <v>326</v>
+        <v>506</v>
       </c>
       <c r="B193" t="s">
-        <v>327</v>
+        <v>573</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
       <c r="B194" t="s">
-        <v>328</v>
+        <v>321</v>
+      </c>
+      <c r="C194" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="B195" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="B196" t="s">
-        <v>256</v>
+        <v>323</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
-        <v>707</v>
+        <v>318</v>
       </c>
       <c r="B197" t="s">
-        <v>704</v>
+        <v>564</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
-        <v>535</v>
+        <v>319</v>
       </c>
       <c r="B198" t="s">
-        <v>682</v>
+        <v>248</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3">
+      <c r="A199" t="s">
+        <v>324</v>
+      </c>
+      <c r="B199" t="s">
+        <v>325</v>
+      </c>
+      <c r="C199" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>521</v>
+        <v>326</v>
       </c>
       <c r="B200" t="s">
-        <v>522</v>
+        <v>327</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" t="s">
-        <v>501</v>
+        <v>329</v>
       </c>
       <c r="B201" t="s">
-        <v>338</v>
-      </c>
-      <c r="C201" t="s">
-        <v>589</v>
+        <v>328</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>507</v>
+        <v>330</v>
       </c>
       <c r="B202" t="s">
-        <v>574</v>
+        <v>331</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B203" t="s">
-        <v>339</v>
-      </c>
-      <c r="C203" t="s">
-        <v>589</v>
+        <v>256</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
-        <v>337</v>
+        <v>707</v>
       </c>
       <c r="B204" t="s">
-        <v>340</v>
+        <v>704</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
-        <v>500</v>
+        <v>535</v>
       </c>
       <c r="B205" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="206" spans="1:3">
-      <c r="A206" t="s">
-        <v>344</v>
-      </c>
-      <c r="B206" t="s">
-        <v>248</v>
+        <v>682</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" t="s">
-        <v>345</v>
+        <v>521</v>
       </c>
       <c r="B207" t="s">
-        <v>341</v>
+        <v>522</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>346</v>
+        <v>501</v>
       </c>
       <c r="B208" t="s">
-        <v>342</v>
+        <v>338</v>
+      </c>
+      <c r="C208" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" t="s">
-        <v>347</v>
+        <v>507</v>
       </c>
       <c r="B209" t="s">
-        <v>343</v>
+        <v>574</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="B210" t="s">
-        <v>256</v>
+        <v>339</v>
+      </c>
+      <c r="C210" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
-        <v>708</v>
+        <v>337</v>
       </c>
       <c r="B211" t="s">
-        <v>704</v>
+        <v>340</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" t="s">
-        <v>534</v>
+        <v>500</v>
       </c>
       <c r="B212" t="s">
-        <v>683</v>
+        <v>565</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3">
+      <c r="A213" t="s">
+        <v>344</v>
+      </c>
+      <c r="B213" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" t="s">
-        <v>551</v>
+        <v>345</v>
       </c>
       <c r="B214" t="s">
-        <v>554</v>
-      </c>
-      <c r="C214" t="s">
-        <v>587</v>
+        <v>341</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" t="s">
-        <v>552</v>
+        <v>346</v>
       </c>
       <c r="B215" t="s">
-        <v>553</v>
-      </c>
-      <c r="C215" t="s">
-        <v>588</v>
+        <v>342</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" t="s">
-        <v>586</v>
+        <v>347</v>
       </c>
       <c r="B216" t="s">
-        <v>602</v>
+        <v>343</v>
       </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" t="s">
-        <v>365</v>
+        <v>348</v>
       </c>
       <c r="B217" t="s">
-        <v>351</v>
+        <v>256</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" t="s">
-        <v>366</v>
+        <v>708</v>
       </c>
       <c r="B218" t="s">
-        <v>352</v>
-      </c>
-      <c r="C218" t="s">
-        <v>589</v>
+        <v>704</v>
       </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219" t="s">
-        <v>508</v>
+        <v>534</v>
       </c>
       <c r="B219" t="s">
-        <v>575</v>
-      </c>
-    </row>
-    <row r="220" spans="1:3">
-      <c r="A220" t="s">
-        <v>367</v>
-      </c>
-      <c r="B220" t="s">
-        <v>353</v>
+        <v>683</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" t="s">
-        <v>368</v>
+        <v>551</v>
       </c>
       <c r="B221" t="s">
-        <v>354</v>
+        <v>554</v>
+      </c>
+      <c r="C221" t="s">
+        <v>587</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" t="s">
-        <v>369</v>
+        <v>552</v>
       </c>
       <c r="B222" t="s">
-        <v>355</v>
+        <v>553</v>
+      </c>
+      <c r="C222" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="223" spans="1:3">
       <c r="A223" t="s">
-        <v>370</v>
+        <v>586</v>
       </c>
       <c r="B223" t="s">
-        <v>356</v>
-      </c>
-      <c r="C223" t="s">
-        <v>589</v>
+        <v>602</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="B224" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="B225" t="s">
-        <v>358</v>
+        <v>352</v>
+      </c>
+      <c r="C225" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" t="s">
-        <v>373</v>
+        <v>508</v>
       </c>
       <c r="B226" t="s">
-        <v>359</v>
+        <v>575</v>
       </c>
     </row>
     <row r="227" spans="1:3">
       <c r="A227" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="B227" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="B228" t="s">
-        <v>361</v>
-      </c>
-      <c r="C228" t="s">
-        <v>589</v>
+        <v>354</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="B229" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="B230" t="s">
-        <v>363</v>
+        <v>356</v>
+      </c>
+      <c r="C230" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="231" spans="1:3">
       <c r="A231" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="B231" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" t="s">
-        <v>533</v>
+        <v>372</v>
       </c>
       <c r="B232" t="s">
-        <v>667</v>
+        <v>358</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3">
+      <c r="A233" t="s">
+        <v>373</v>
+      </c>
+      <c r="B233" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" t="s">
-        <v>607</v>
+        <v>374</v>
       </c>
       <c r="B234" t="s">
-        <v>608</v>
+        <v>360</v>
       </c>
     </row>
     <row r="235" spans="1:3">
       <c r="A235" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="B235" t="s">
-        <v>403</v>
+        <v>361</v>
+      </c>
+      <c r="C235" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="B236" t="s">
-        <v>400</v>
+        <v>362</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="B237" t="s">
-        <v>401</v>
-      </c>
-      <c r="C237" t="s">
-        <v>589</v>
+        <v>363</v>
       </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" t="s">
-        <v>509</v>
+        <v>378</v>
       </c>
       <c r="B238" t="s">
-        <v>576</v>
+        <v>364</v>
       </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239" t="s">
-        <v>404</v>
+        <v>533</v>
       </c>
       <c r="B239" t="s">
-        <v>402</v>
-      </c>
-      <c r="C239" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="240" spans="1:3">
-      <c r="A240" t="s">
-        <v>388</v>
-      </c>
-      <c r="B240" t="s">
-        <v>394</v>
+        <v>667</v>
       </c>
     </row>
     <row r="241" spans="1:3">
       <c r="A241" t="s">
-        <v>405</v>
+        <v>607</v>
       </c>
       <c r="B241" t="s">
-        <v>395</v>
-      </c>
-      <c r="C241" t="s">
-        <v>566</v>
+        <v>608</v>
       </c>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="B242" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
     </row>
     <row r="243" spans="1:3">
       <c r="A243" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="B243" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
     </row>
     <row r="244" spans="1:3">
       <c r="A244" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="B244" t="s">
-        <v>398</v>
+        <v>401</v>
+      </c>
+      <c r="C244" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="245" spans="1:3">
       <c r="A245" t="s">
-        <v>392</v>
+        <v>509</v>
       </c>
       <c r="B245" t="s">
-        <v>399</v>
+        <v>576</v>
       </c>
     </row>
     <row r="246" spans="1:3">
       <c r="A246" t="s">
-        <v>393</v>
+        <v>404</v>
       </c>
       <c r="B246" t="s">
-        <v>396</v>
+        <v>402</v>
+      </c>
+      <c r="C246" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="247" spans="1:3">
       <c r="A247" t="s">
-        <v>532</v>
+        <v>388</v>
       </c>
       <c r="B247" t="s">
-        <v>684</v>
+        <v>394</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3">
+      <c r="A248" t="s">
+        <v>405</v>
+      </c>
+      <c r="B248" t="s">
+        <v>395</v>
+      </c>
+      <c r="C248" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="249" spans="1:3">
       <c r="A249" t="s">
-        <v>523</v>
+        <v>389</v>
       </c>
       <c r="B249" t="s">
-        <v>524</v>
+        <v>396</v>
       </c>
     </row>
     <row r="250" spans="1:3">
       <c r="A250" t="s">
-        <v>411</v>
+        <v>391</v>
       </c>
       <c r="B250" t="s">
-        <v>422</v>
+        <v>397</v>
       </c>
     </row>
     <row r="251" spans="1:3">
       <c r="A251" t="s">
-        <v>412</v>
+        <v>390</v>
       </c>
       <c r="B251" t="s">
-        <v>423</v>
-      </c>
-      <c r="C251" t="s">
-        <v>589</v>
+        <v>398</v>
       </c>
     </row>
     <row r="252" spans="1:3">
       <c r="A252" t="s">
-        <v>577</v>
+        <v>392</v>
       </c>
       <c r="B252" t="s">
-        <v>578</v>
+        <v>399</v>
       </c>
     </row>
     <row r="253" spans="1:3">
       <c r="A253" t="s">
-        <v>413</v>
+        <v>393</v>
       </c>
       <c r="B253" t="s">
-        <v>424</v>
-      </c>
-      <c r="C253" t="s">
-        <v>589</v>
+        <v>396</v>
       </c>
     </row>
     <row r="254" spans="1:3">
       <c r="A254" t="s">
-        <v>414</v>
+        <v>532</v>
       </c>
       <c r="B254" t="s">
-        <v>425</v>
-      </c>
-      <c r="C254" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="255" spans="1:3">
-      <c r="A255" t="s">
-        <v>415</v>
-      </c>
-      <c r="B255" t="s">
-        <v>590</v>
+        <v>684</v>
       </c>
     </row>
     <row r="256" spans="1:3">
       <c r="A256" t="s">
-        <v>416</v>
+        <v>523</v>
       </c>
       <c r="B256" t="s">
-        <v>426</v>
+        <v>524</v>
       </c>
     </row>
     <row r="257" spans="1:3">
       <c r="A257" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="B257" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
     </row>
     <row r="258" spans="1:3">
       <c r="A258" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="B258" t="s">
-        <v>428</v>
+        <v>423</v>
+      </c>
+      <c r="C258" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="259" spans="1:3">
       <c r="A259" t="s">
-        <v>419</v>
+        <v>577</v>
       </c>
       <c r="B259" t="s">
-        <v>429</v>
+        <v>578</v>
       </c>
     </row>
     <row r="260" spans="1:3">
       <c r="A260" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="B260" t="s">
-        <v>430</v>
+        <v>424</v>
+      </c>
+      <c r="C260" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="261" spans="1:3">
       <c r="A261" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="B261" t="s">
-        <v>431</v>
+        <v>425</v>
+      </c>
+      <c r="C261" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="262" spans="1:3">
       <c r="A262" t="s">
-        <v>530</v>
+        <v>415</v>
       </c>
       <c r="B262" t="s">
-        <v>685</v>
+        <v>590</v>
       </c>
     </row>
     <row r="263" spans="1:3">
       <c r="A263" t="s">
-        <v>616</v>
+        <v>416</v>
       </c>
       <c r="B263" t="s">
-        <v>617</v>
+        <v>426</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3">
+      <c r="A264" t="s">
+        <v>417</v>
+      </c>
+      <c r="B264" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="265" spans="1:3">
       <c r="A265" t="s">
-        <v>525</v>
+        <v>418</v>
       </c>
       <c r="B265" t="s">
-        <v>524</v>
+        <v>428</v>
       </c>
     </row>
     <row r="266" spans="1:3">
       <c r="A266" t="s">
-        <v>438</v>
+        <v>419</v>
       </c>
       <c r="B266" t="s">
-        <v>449</v>
+        <v>429</v>
       </c>
     </row>
     <row r="267" spans="1:3">
       <c r="A267" t="s">
-        <v>439</v>
+        <v>420</v>
       </c>
       <c r="B267" t="s">
-        <v>450</v>
-      </c>
-      <c r="C267" t="s">
-        <v>589</v>
+        <v>430</v>
       </c>
     </row>
     <row r="268" spans="1:3">
       <c r="A268" t="s">
-        <v>510</v>
+        <v>421</v>
       </c>
       <c r="B268" t="s">
-        <v>579</v>
+        <v>431</v>
       </c>
     </row>
     <row r="269" spans="1:3">
       <c r="A269" t="s">
-        <v>440</v>
+        <v>530</v>
       </c>
       <c r="B269" t="s">
-        <v>451</v>
-      </c>
-      <c r="C269" t="s">
-        <v>589</v>
+        <v>685</v>
       </c>
     </row>
     <row r="270" spans="1:3">
       <c r="A270" t="s">
-        <v>441</v>
+        <v>616</v>
       </c>
       <c r="B270" t="s">
-        <v>452</v>
-      </c>
-      <c r="C270" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="271" spans="1:3">
-      <c r="A271" t="s">
-        <v>442</v>
-      </c>
-      <c r="B271" t="s">
-        <v>591</v>
+        <v>617</v>
       </c>
     </row>
     <row r="272" spans="1:3">
       <c r="A272" t="s">
-        <v>443</v>
+        <v>525</v>
       </c>
       <c r="B272" t="s">
-        <v>426</v>
+        <v>524</v>
       </c>
     </row>
     <row r="273" spans="1:3">
       <c r="A273" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="B273" t="s">
-        <v>427</v>
+        <v>449</v>
       </c>
     </row>
     <row r="274" spans="1:3">
       <c r="A274" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="B274" t="s">
-        <v>453</v>
+        <v>450</v>
+      </c>
+      <c r="C274" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="275" spans="1:3">
       <c r="A275" t="s">
-        <v>446</v>
+        <v>510</v>
       </c>
       <c r="B275" t="s">
-        <v>454</v>
+        <v>579</v>
       </c>
     </row>
     <row r="276" spans="1:3">
       <c r="A276" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="B276" t="s">
-        <v>430</v>
+        <v>451</v>
+      </c>
+      <c r="C276" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="277" spans="1:3">
       <c r="A277" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="B277" t="s">
-        <v>431</v>
+        <v>452</v>
+      </c>
+      <c r="C277" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="278" spans="1:3">
       <c r="A278" t="s">
-        <v>529</v>
+        <v>442</v>
       </c>
       <c r="B278" t="s">
-        <v>685</v>
+        <v>591</v>
       </c>
     </row>
     <row r="279" spans="1:3">
       <c r="A279" t="s">
-        <v>623</v>
+        <v>443</v>
       </c>
       <c r="B279" t="s">
-        <v>617</v>
+        <v>426</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3">
+      <c r="A280" t="s">
+        <v>444</v>
+      </c>
+      <c r="B280" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="281" spans="1:3">
       <c r="A281" t="s">
-        <v>432</v>
+        <v>445</v>
       </c>
       <c r="B281" t="s">
-        <v>624</v>
+        <v>453</v>
       </c>
     </row>
     <row r="282" spans="1:3">
       <c r="A282" t="s">
-        <v>433</v>
+        <v>446</v>
       </c>
       <c r="B282" t="s">
-        <v>625</v>
-      </c>
-      <c r="C282" t="s">
-        <v>589</v>
+        <v>454</v>
       </c>
     </row>
     <row r="283" spans="1:3">
       <c r="A283" t="s">
-        <v>511</v>
+        <v>447</v>
       </c>
       <c r="B283" t="s">
-        <v>626</v>
+        <v>430</v>
       </c>
     </row>
     <row r="284" spans="1:3">
       <c r="A284" t="s">
-        <v>434</v>
+        <v>448</v>
       </c>
       <c r="B284" t="s">
-        <v>652</v>
+        <v>431</v>
       </c>
     </row>
     <row r="285" spans="1:3">
       <c r="A285" t="s">
-        <v>435</v>
+        <v>529</v>
       </c>
       <c r="B285" t="s">
-        <v>627</v>
+        <v>685</v>
       </c>
     </row>
     <row r="286" spans="1:3">
       <c r="A286" t="s">
+        <v>623</v>
+      </c>
+      <c r="B286" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3">
+      <c r="A288" t="s">
+        <v>432</v>
+      </c>
+      <c r="B288" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3">
+      <c r="A289" t="s">
+        <v>433</v>
+      </c>
+      <c r="B289" t="s">
+        <v>625</v>
+      </c>
+      <c r="C289" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3">
+      <c r="A290" t="s">
+        <v>511</v>
+      </c>
+      <c r="B290" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3">
+      <c r="A291" t="s">
+        <v>434</v>
+      </c>
+      <c r="B291" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3">
+      <c r="A292" t="s">
+        <v>435</v>
+      </c>
+      <c r="B292" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3">
+      <c r="A293" t="s">
         <v>436</v>
       </c>
-      <c r="B286" t="s">
+      <c r="B293" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="287" spans="1:3">
-      <c r="A287" t="s">
+    <row r="294" spans="1:3">
+      <c r="A294" t="s">
         <v>528</v>
       </c>
-      <c r="B287" t="s">
+      <c r="B294" t="s">
         <v>686</v>
       </c>
     </row>

</xml_diff>

<commit_message>
57443 - Added the finding for Unsupported Income Type in the ICW, 57817 - Added the check for Dominium Employee, 57818 - Checks for Pay Stubs and Hourly Income (need to check with Colin on these ones)
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raluca.ilinca.AzureAI-Jump2\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C42B86-236A-4DA5-ADEB-323FB25D606D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1ACC35-0215-461D-8E3E-BA0372AEC65B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="22440" windowHeight="11715" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="738">
   <si>
     <t>Name</t>
   </si>
@@ -2233,6 +2233,27 @@
   </si>
   <si>
     <t>This is a HOME unit, but 2 months of paystubs were not provided as required.</t>
+  </si>
+  <si>
+    <t>ICW_DominiumEmployee</t>
+  </si>
+  <si>
+    <t>Applicant is a Dominium employee, manual review is required.</t>
+  </si>
+  <si>
+    <t>SupportedIncomeTypes</t>
+  </si>
+  <si>
+    <t>Not supported Income Type. Needs manual review.</t>
+  </si>
+  <si>
+    <t>ICW_NotSupportedIncomeTypes</t>
+  </si>
+  <si>
+    <t>EDC_BothHourlyIncomeAndPSDocumented</t>
+  </si>
+  <si>
+    <t>Both hourly income and check stub income have been documented on the same Exact Day Calculator. Manual review is required.</t>
   </si>
 </sst>
 </file>
@@ -5546,8 +5567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1011"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5890,7 +5911,14 @@
         <v>690</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A39" t="s">
+        <v>733</v>
+      </c>
+      <c r="B39" t="s">
+        <v>733</v>
+      </c>
+    </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
@@ -6871,10 +6899,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
-  <dimension ref="A1:C294"/>
+  <dimension ref="A1:C297"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="C133" sqref="C133"/>
+    <sheetView tabSelected="1" topLeftCell="B126" workbookViewId="0">
+      <selection activeCell="C135" sqref="C135:C136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7000,267 +7028,267 @@
         <v>693</v>
       </c>
     </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>731</v>
+      </c>
+      <c r="B17" t="s">
+        <v>732</v>
+      </c>
+      <c r="C17" t="s">
+        <v>693</v>
+      </c>
+    </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>181</v>
+        <v>735</v>
       </c>
       <c r="B18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>79</v>
-      </c>
-      <c r="B19" t="s">
-        <v>75</v>
+        <v>734</v>
+      </c>
+      <c r="C18" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>559</v>
+        <v>181</v>
       </c>
       <c r="B20" t="s">
-        <v>560</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B21" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>559</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>560</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
       <c r="B23" t="s">
-        <v>197</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>198</v>
+        <v>82</v>
       </c>
       <c r="B24" t="s">
-        <v>199</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>196</v>
       </c>
       <c r="B25" t="s">
-        <v>85</v>
+        <v>197</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>86</v>
+        <v>198</v>
       </c>
       <c r="B26" t="s">
-        <v>87</v>
+        <v>199</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B27" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B28" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>632</v>
+        <v>81</v>
       </c>
       <c r="B29" t="s">
-        <v>633</v>
+        <v>88</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>656</v>
+        <v>89</v>
       </c>
       <c r="B30" t="s">
-        <v>657</v>
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>546</v>
+        <v>632</v>
       </c>
       <c r="B31" t="s">
-        <v>669</v>
+        <v>633</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>718</v>
+        <v>656</v>
       </c>
       <c r="B32" t="s">
-        <v>719</v>
-      </c>
-      <c r="C32" t="s">
-        <v>693</v>
+        <v>657</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>546</v>
+      </c>
+      <c r="B33" t="s">
+        <v>669</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>183</v>
+        <v>718</v>
       </c>
       <c r="B34" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>91</v>
-      </c>
-      <c r="B35" t="s">
-        <v>92</v>
+        <v>719</v>
+      </c>
+      <c r="C34" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>93</v>
+        <v>183</v>
       </c>
       <c r="B36" t="s">
-        <v>94</v>
+        <v>185</v>
       </c>
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B38" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B39" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B40" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B41" t="s">
-        <v>99</v>
-      </c>
-      <c r="C41" t="s">
-        <v>589</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B42" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>634</v>
+        <v>105</v>
       </c>
       <c r="B43" t="s">
-        <v>635</v>
+        <v>99</v>
+      </c>
+      <c r="C43" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>545</v>
+        <v>106</v>
       </c>
       <c r="B44" t="s">
-        <v>670</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>694</v>
+        <v>634</v>
       </c>
       <c r="B45" t="s">
-        <v>695</v>
-      </c>
-      <c r="C45" t="s">
-        <v>693</v>
+        <v>635</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>545</v>
+      </c>
+      <c r="B46" t="s">
+        <v>670</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>184</v>
+        <v>694</v>
       </c>
       <c r="B47" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" t="s">
-        <v>107</v>
-      </c>
-      <c r="B48" t="s">
-        <v>108</v>
-      </c>
-      <c r="C48" t="s">
-        <v>589</v>
+        <v>695</v>
+      </c>
+      <c r="C47" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" t="s">
-        <v>117</v>
+        <v>184</v>
       </c>
       <c r="B49" t="s">
-        <v>118</v>
-      </c>
-      <c r="C49" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
     </row>
     <row r="50" spans="1:3">
       <c r="A50" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="B50" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C50" t="s">
         <v>589</v>
@@ -7268,10 +7296,10 @@
     </row>
     <row r="51" spans="1:3">
       <c r="A51" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B51" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="C51" t="s">
         <v>589</v>
@@ -7279,10 +7307,10 @@
     </row>
     <row r="52" spans="1:3">
       <c r="A52" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="B52" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="C52" t="s">
         <v>589</v>
@@ -7290,10 +7318,10 @@
     </row>
     <row r="53" spans="1:3">
       <c r="A53" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B53" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C53" t="s">
         <v>589</v>
@@ -7301,553 +7329,553 @@
     </row>
     <row r="54" spans="1:3">
       <c r="A54" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B54" t="s">
-        <v>112</v>
+        <v>110</v>
+      </c>
+      <c r="C54" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="A55" t="s">
-        <v>204</v>
+        <v>115</v>
       </c>
       <c r="B55" t="s">
-        <v>494</v>
+        <v>111</v>
+      </c>
+      <c r="C55" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" t="s">
-        <v>205</v>
+        <v>116</v>
       </c>
       <c r="B56" t="s">
-        <v>593</v>
-      </c>
-      <c r="C56" t="s">
-        <v>589</v>
+        <v>112</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" t="s">
-        <v>580</v>
+        <v>204</v>
       </c>
       <c r="B57" t="s">
-        <v>594</v>
+        <v>494</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" t="s">
-        <v>547</v>
+        <v>205</v>
       </c>
       <c r="B58" t="s">
-        <v>548</v>
+        <v>593</v>
+      </c>
+      <c r="C58" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" t="s">
-        <v>555</v>
+        <v>580</v>
       </c>
       <c r="B59" t="s">
-        <v>631</v>
+        <v>594</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="B60" t="s">
-        <v>671</v>
+        <v>548</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>555</v>
+      </c>
+      <c r="B61" t="s">
+        <v>631</v>
       </c>
     </row>
     <row r="62" spans="1:3">
       <c r="A62" t="s">
-        <v>158</v>
+        <v>544</v>
       </c>
       <c r="B62" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" t="s">
-        <v>122</v>
-      </c>
-      <c r="B63" t="s">
-        <v>595</v>
+        <v>671</v>
       </c>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" t="s">
-        <v>124</v>
+        <v>158</v>
       </c>
       <c r="B64" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>636</v>
+        <v>122</v>
       </c>
       <c r="B65" t="s">
-        <v>637</v>
+        <v>595</v>
       </c>
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>543</v>
+        <v>124</v>
       </c>
       <c r="B66" t="s">
-        <v>672</v>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>636</v>
+      </c>
+      <c r="B67" t="s">
+        <v>637</v>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>186</v>
+        <v>543</v>
       </c>
       <c r="B68" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" t="s">
-        <v>125</v>
-      </c>
-      <c r="B69" t="s">
-        <v>127</v>
+        <v>672</v>
       </c>
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>126</v>
+        <v>186</v>
       </c>
       <c r="B70" t="s">
-        <v>128</v>
+        <v>187</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="B71" t="s">
-        <v>596</v>
+        <v>127</v>
       </c>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="B72" t="s">
-        <v>597</v>
+        <v>128</v>
       </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B73" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B74" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B75" t="s">
-        <v>495</v>
-      </c>
-      <c r="C75" t="s">
-        <v>687</v>
+        <v>598</v>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B76" t="s">
-        <v>497</v>
-      </c>
-      <c r="C76" t="s">
-        <v>556</v>
+        <v>599</v>
       </c>
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B77" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C77" t="s">
-        <v>556</v>
+        <v>687</v>
       </c>
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>638</v>
+        <v>143</v>
       </c>
       <c r="B78" t="s">
-        <v>639</v>
+        <v>497</v>
+      </c>
+      <c r="C78" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>542</v>
+        <v>144</v>
       </c>
       <c r="B79" t="s">
-        <v>673</v>
+        <v>498</v>
+      </c>
+      <c r="C79" t="s">
+        <v>556</v>
       </c>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>720</v>
+        <v>638</v>
       </c>
       <c r="B80" t="s">
-        <v>721</v>
-      </c>
-      <c r="C80" t="s">
-        <v>693</v>
+        <v>639</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>542</v>
+      </c>
+      <c r="B81" t="s">
+        <v>673</v>
       </c>
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>147</v>
+        <v>720</v>
       </c>
       <c r="B82" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" t="s">
-        <v>148</v>
-      </c>
-      <c r="B83" t="s">
-        <v>151</v>
+        <v>721</v>
+      </c>
+      <c r="C82" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B84" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B85" t="s">
-        <v>581</v>
-      </c>
-      <c r="C85" t="s">
-        <v>692</v>
+        <v>151</v>
       </c>
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>691</v>
+        <v>149</v>
       </c>
       <c r="B86" t="s">
-        <v>581</v>
+        <v>152</v>
       </c>
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B87" t="s">
-        <v>129</v>
+        <v>581</v>
+      </c>
+      <c r="C87" t="s">
+        <v>692</v>
       </c>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>131</v>
+        <v>691</v>
       </c>
       <c r="B88" t="s">
-        <v>600</v>
+        <v>581</v>
       </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>132</v>
+        <v>146</v>
       </c>
       <c r="B89" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>640</v>
+        <v>131</v>
       </c>
       <c r="B90" t="s">
-        <v>641</v>
+        <v>600</v>
       </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>541</v>
+        <v>132</v>
       </c>
       <c r="B91" t="s">
-        <v>674</v>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>640</v>
+      </c>
+      <c r="B92" t="s">
+        <v>641</v>
       </c>
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>188</v>
+        <v>541</v>
       </c>
       <c r="B93" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3">
-      <c r="A94" t="s">
-        <v>133</v>
-      </c>
-      <c r="B94" t="s">
-        <v>153</v>
+        <v>674</v>
       </c>
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>135</v>
+        <v>188</v>
       </c>
       <c r="B95" t="s">
-        <v>154</v>
+        <v>189</v>
       </c>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B96" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B97" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B98" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>630</v>
+        <v>136</v>
       </c>
       <c r="B99" t="s">
-        <v>696</v>
-      </c>
-      <c r="C99" t="s">
-        <v>700</v>
+        <v>156</v>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>642</v>
+        <v>137</v>
       </c>
       <c r="B100" t="s">
-        <v>643</v>
+        <v>157</v>
       </c>
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>540</v>
+        <v>630</v>
       </c>
       <c r="B101" t="s">
-        <v>675</v>
+        <v>696</v>
+      </c>
+      <c r="C101" t="s">
+        <v>700</v>
       </c>
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>722</v>
+        <v>642</v>
       </c>
       <c r="B102" t="s">
-        <v>723</v>
-      </c>
-      <c r="C102" t="s">
-        <v>693</v>
+        <v>643</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" t="s">
+        <v>540</v>
+      </c>
+      <c r="B103" t="s">
+        <v>675</v>
       </c>
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
+        <v>722</v>
+      </c>
+      <c r="B104" t="s">
+        <v>723</v>
+      </c>
+      <c r="C104" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" t="s">
         <v>711</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B106" t="s">
         <v>712</v>
       </c>
-      <c r="C104" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3">
-      <c r="A105" t="s">
-        <v>714</v>
-      </c>
-      <c r="B105" t="s">
-        <v>715</v>
-      </c>
-      <c r="C105" t="s">
+      <c r="C106" t="s">
         <v>713</v>
       </c>
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>159</v>
+        <v>714</v>
       </c>
       <c r="B107" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
-      <c r="A108" t="s">
-        <v>160</v>
-      </c>
-      <c r="B108" t="s">
-        <v>164</v>
+        <v>715</v>
+      </c>
+      <c r="C107" t="s">
+        <v>713</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B109" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B110" t="s">
-        <v>601</v>
+        <v>164</v>
       </c>
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>557</v>
+        <v>161</v>
       </c>
       <c r="B111" t="s">
-        <v>558</v>
+        <v>165</v>
       </c>
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>648</v>
+        <v>162</v>
       </c>
       <c r="B112" t="s">
-        <v>649</v>
+        <v>601</v>
       </c>
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>539</v>
+        <v>557</v>
       </c>
       <c r="B113" t="s">
-        <v>676</v>
+        <v>558</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" t="s">
+        <v>648</v>
+      </c>
+      <c r="B114" t="s">
+        <v>649</v>
       </c>
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>192</v>
+        <v>539</v>
       </c>
       <c r="B115" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3">
-      <c r="A116" t="s">
-        <v>166</v>
-      </c>
-      <c r="B116" t="s">
-        <v>168</v>
+        <v>676</v>
       </c>
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>167</v>
+        <v>192</v>
       </c>
       <c r="B117" t="s">
-        <v>169</v>
+        <v>193</v>
       </c>
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>644</v>
+        <v>166</v>
       </c>
       <c r="B118" t="s">
-        <v>645</v>
+        <v>168</v>
       </c>
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>538</v>
+        <v>167</v>
       </c>
       <c r="B119" t="s">
-        <v>677</v>
+        <v>169</v>
       </c>
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>724</v>
+        <v>644</v>
       </c>
       <c r="B120" t="s">
-        <v>725</v>
-      </c>
-      <c r="C120" t="s">
-        <v>693</v>
+        <v>645</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" t="s">
+        <v>538</v>
+      </c>
+      <c r="B121" t="s">
+        <v>677</v>
       </c>
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>190</v>
+        <v>724</v>
       </c>
       <c r="B122" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3">
-      <c r="A123" t="s">
-        <v>175</v>
-      </c>
-      <c r="B123" t="s">
-        <v>172</v>
-      </c>
-      <c r="C123" t="s">
-        <v>589</v>
+        <v>725</v>
+      </c>
+      <c r="C122" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="B124" t="s">
-        <v>173</v>
-      </c>
-      <c r="C124" t="s">
-        <v>589</v>
+        <v>191</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="B125" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C125" t="s">
         <v>589</v>
@@ -7855,1108 +7883,1111 @@
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>203</v>
+        <v>170</v>
       </c>
       <c r="B126" t="s">
-        <v>202</v>
+        <v>173</v>
+      </c>
+      <c r="C126" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>200</v>
+        <v>171</v>
       </c>
       <c r="B127" t="s">
-        <v>201</v>
+        <v>174</v>
+      </c>
+      <c r="C127" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>176</v>
+        <v>203</v>
       </c>
       <c r="B128" t="s">
-        <v>177</v>
-      </c>
-      <c r="C128" t="s">
-        <v>589</v>
+        <v>202</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>646</v>
+        <v>200</v>
       </c>
       <c r="B129" t="s">
-        <v>647</v>
+        <v>201</v>
       </c>
     </row>
     <row r="130" spans="1:3">
       <c r="A130" t="s">
-        <v>527</v>
+        <v>176</v>
       </c>
       <c r="B130" t="s">
-        <v>678</v>
+        <v>177</v>
+      </c>
+      <c r="C130" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" t="s">
+        <v>646</v>
+      </c>
+      <c r="B131" t="s">
+        <v>647</v>
       </c>
     </row>
     <row r="132" spans="1:3">
       <c r="A132" t="s">
+        <v>527</v>
+      </c>
+      <c r="B132" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" t="s">
         <v>653</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B134" t="s">
         <v>654</v>
       </c>
-      <c r="C132" t="s">
+      <c r="C134" t="s">
         <v>655</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3">
-      <c r="A133" t="s">
-        <v>729</v>
-      </c>
-      <c r="B133" t="s">
-        <v>730</v>
-      </c>
-      <c r="C133" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
-        <v>513</v>
+        <v>729</v>
       </c>
       <c r="B135" t="s">
-        <v>514</v>
+        <v>730</v>
+      </c>
+      <c r="C135" t="s">
+        <v>693</v>
       </c>
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
-        <v>662</v>
+        <v>736</v>
       </c>
       <c r="B136" t="s">
-        <v>666</v>
+        <v>737</v>
       </c>
       <c r="C136" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3">
-      <c r="A137" t="s">
-        <v>663</v>
-      </c>
-      <c r="B137" t="s">
-        <v>665</v>
-      </c>
-      <c r="C137" t="s">
-        <v>664</v>
+        <v>693</v>
       </c>
     </row>
     <row r="138" spans="1:3">
       <c r="A138" t="s">
-        <v>242</v>
+        <v>513</v>
       </c>
       <c r="B138" t="s">
-        <v>243</v>
-      </c>
-      <c r="C138" t="s">
-        <v>589</v>
+        <v>514</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>244</v>
+        <v>662</v>
       </c>
       <c r="B139" t="s">
-        <v>245</v>
+        <v>666</v>
+      </c>
+      <c r="C139" t="s">
+        <v>664</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>258</v>
+        <v>663</v>
       </c>
       <c r="B140" t="s">
-        <v>561</v>
+        <v>665</v>
       </c>
       <c r="C140" t="s">
-        <v>651</v>
+        <v>664</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B141" t="s">
-        <v>246</v>
+        <v>243</v>
+      </c>
+      <c r="C141" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>503</v>
+        <v>244</v>
       </c>
       <c r="B142" t="s">
-        <v>512</v>
+        <v>245</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c r="B143" t="s">
-        <v>248</v>
+        <v>561</v>
+      </c>
+      <c r="C143" t="s">
+        <v>651</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B144" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>251</v>
+        <v>503</v>
       </c>
       <c r="B145" t="s">
-        <v>253</v>
+        <v>512</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="B146" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="B147" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>302</v>
+        <v>251</v>
       </c>
       <c r="B148" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>349</v>
+        <v>255</v>
       </c>
       <c r="B149" t="s">
-        <v>350</v>
+        <v>254</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>658</v>
+        <v>257</v>
       </c>
       <c r="B150" t="s">
-        <v>659</v>
+        <v>256</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>703</v>
+        <v>302</v>
       </c>
       <c r="B151" t="s">
-        <v>704</v>
+        <v>248</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>526</v>
+        <v>349</v>
       </c>
       <c r="B152" t="s">
-        <v>679</v>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" t="s">
+        <v>658</v>
+      </c>
+      <c r="B153" t="s">
+        <v>659</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>515</v>
+        <v>703</v>
       </c>
       <c r="B154" t="s">
-        <v>516</v>
+        <v>704</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>259</v>
+        <v>526</v>
       </c>
       <c r="B155" t="s">
-        <v>262</v>
-      </c>
-      <c r="C155" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A156" t="s">
-        <v>261</v>
-      </c>
-      <c r="B156" t="s">
-        <v>562</v>
-      </c>
-      <c r="C156" t="s">
-        <v>697</v>
+        <v>679</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>260</v>
+        <v>515</v>
       </c>
       <c r="B157" t="s">
-        <v>263</v>
+        <v>516</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="B158" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3">
+        <v>262</v>
+      </c>
+      <c r="C158" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" ht="13.5" customHeight="1">
       <c r="A159" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B159" t="s">
-        <v>267</v>
+        <v>562</v>
+      </c>
+      <c r="C159" t="s">
+        <v>697</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="B160" t="s">
-        <v>268</v>
-      </c>
-      <c r="C160" t="s">
-        <v>661</v>
+        <v>263</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>504</v>
+        <v>265</v>
       </c>
       <c r="B161" t="s">
-        <v>571</v>
+        <v>264</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B162" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B163" t="s">
-        <v>273</v>
+        <v>268</v>
+      </c>
+      <c r="C163" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>277</v>
+        <v>504</v>
       </c>
       <c r="B164" t="s">
-        <v>287</v>
+        <v>571</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="B165" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="B166" t="s">
-        <v>285</v>
-      </c>
-      <c r="C166" t="s">
-        <v>661</v>
+        <v>273</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B167" t="s">
-        <v>606</v>
+        <v>287</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B168" t="s">
-        <v>284</v>
-      </c>
-      <c r="C168" t="s">
-        <v>661</v>
+        <v>286</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B169" t="s">
-        <v>283</v>
+        <v>285</v>
+      </c>
+      <c r="C169" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>299</v>
+        <v>280</v>
       </c>
       <c r="B170" t="s">
-        <v>300</v>
+        <v>606</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="B171" t="s">
-        <v>248</v>
+        <v>284</v>
+      </c>
+      <c r="C171" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
-        <v>304</v>
+        <v>282</v>
       </c>
       <c r="B172" t="s">
-        <v>305</v>
+        <v>283</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
-        <v>705</v>
+        <v>299</v>
       </c>
       <c r="B173" t="s">
-        <v>704</v>
+        <v>300</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>537</v>
+        <v>301</v>
       </c>
       <c r="B174" t="s">
-        <v>680</v>
+        <v>248</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>698</v>
+        <v>304</v>
       </c>
       <c r="B175" t="s">
-        <v>699</v>
-      </c>
-      <c r="C175" t="s">
-        <v>693</v>
+        <v>305</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
+      <c r="A176" t="s">
+        <v>705</v>
+      </c>
+      <c r="B176" t="s">
+        <v>704</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>517</v>
+        <v>537</v>
       </c>
       <c r="B177" t="s">
-        <v>518</v>
+        <v>680</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
-        <v>292</v>
+        <v>698</v>
       </c>
       <c r="B178" t="s">
-        <v>296</v>
+        <v>699</v>
       </c>
       <c r="C178" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3">
-      <c r="A179" t="s">
-        <v>505</v>
-      </c>
-      <c r="B179" t="s">
-        <v>572</v>
+        <v>693</v>
       </c>
     </row>
     <row r="180" spans="1:3">
       <c r="A180" t="s">
-        <v>293</v>
+        <v>517</v>
       </c>
       <c r="B180" t="s">
-        <v>297</v>
-      </c>
-      <c r="C180" t="s">
-        <v>589</v>
+        <v>518</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B181" t="s">
-        <v>298</v>
+        <v>296</v>
+      </c>
+      <c r="C181" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" t="s">
-        <v>295</v>
+        <v>505</v>
       </c>
       <c r="B182" t="s">
-        <v>563</v>
+        <v>572</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="B183" t="s">
-        <v>248</v>
+        <v>297</v>
+      </c>
+      <c r="C183" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="B184" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="B185" t="s">
-        <v>308</v>
+        <v>563</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B186" t="s">
-        <v>308</v>
+        <v>248</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B187" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" t="s">
-        <v>706</v>
+        <v>306</v>
       </c>
       <c r="B188" t="s">
-        <v>704</v>
+        <v>308</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" t="s">
-        <v>536</v>
+        <v>307</v>
       </c>
       <c r="B189" t="s">
-        <v>681</v>
+        <v>308</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3">
+      <c r="A190" t="s">
+        <v>311</v>
+      </c>
+      <c r="B190" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" t="s">
-        <v>519</v>
+        <v>706</v>
       </c>
       <c r="B191" t="s">
-        <v>520</v>
+        <v>704</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" t="s">
-        <v>499</v>
+        <v>536</v>
       </c>
       <c r="B192" t="s">
-        <v>320</v>
-      </c>
-      <c r="C192" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="193" spans="1:3">
-      <c r="A193" t="s">
-        <v>506</v>
-      </c>
-      <c r="B193" t="s">
-        <v>573</v>
+        <v>681</v>
       </c>
     </row>
     <row r="194" spans="1:3">
       <c r="A194" t="s">
-        <v>315</v>
+        <v>519</v>
       </c>
       <c r="B194" t="s">
-        <v>321</v>
-      </c>
-      <c r="C194" t="s">
-        <v>589</v>
+        <v>520</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>316</v>
+        <v>499</v>
       </c>
       <c r="B195" t="s">
-        <v>322</v>
+        <v>320</v>
+      </c>
+      <c r="C195" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>317</v>
+        <v>506</v>
       </c>
       <c r="B196" t="s">
-        <v>323</v>
+        <v>573</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B197" t="s">
-        <v>564</v>
+        <v>321</v>
+      </c>
+      <c r="C197" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B198" t="s">
-        <v>248</v>
+        <v>322</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="B199" t="s">
-        <v>325</v>
-      </c>
-      <c r="C199" t="s">
-        <v>589</v>
+        <v>323</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="B200" t="s">
-        <v>327</v>
+        <v>564</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="B201" t="s">
-        <v>328</v>
+        <v>248</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="B202" t="s">
-        <v>331</v>
+        <v>325</v>
+      </c>
+      <c r="C202" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="B203" t="s">
-        <v>256</v>
+        <v>327</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
-        <v>707</v>
+        <v>329</v>
       </c>
       <c r="B204" t="s">
-        <v>704</v>
+        <v>328</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
-        <v>535</v>
+        <v>330</v>
       </c>
       <c r="B205" t="s">
-        <v>682</v>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3">
+      <c r="A206" t="s">
+        <v>332</v>
+      </c>
+      <c r="B206" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" t="s">
-        <v>521</v>
+        <v>707</v>
       </c>
       <c r="B207" t="s">
-        <v>522</v>
+        <v>704</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
-        <v>501</v>
+        <v>535</v>
       </c>
       <c r="B208" t="s">
-        <v>338</v>
-      </c>
-      <c r="C208" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="209" spans="1:3">
-      <c r="A209" t="s">
-        <v>507</v>
-      </c>
-      <c r="B209" t="s">
-        <v>574</v>
+        <v>682</v>
       </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" t="s">
-        <v>336</v>
+        <v>521</v>
       </c>
       <c r="B210" t="s">
-        <v>339</v>
-      </c>
-      <c r="C210" t="s">
-        <v>589</v>
+        <v>522</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
-        <v>337</v>
+        <v>501</v>
       </c>
       <c r="B211" t="s">
-        <v>340</v>
+        <v>338</v>
+      </c>
+      <c r="C211" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="B212" t="s">
-        <v>565</v>
+        <v>574</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="B213" t="s">
-        <v>248</v>
+        <v>339</v>
+      </c>
+      <c r="C213" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="B214" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" t="s">
-        <v>346</v>
+        <v>500</v>
       </c>
       <c r="B215" t="s">
-        <v>342</v>
+        <v>565</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B216" t="s">
-        <v>343</v>
+        <v>248</v>
       </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="B217" t="s">
-        <v>256</v>
+        <v>341</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" t="s">
-        <v>708</v>
+        <v>346</v>
       </c>
       <c r="B218" t="s">
-        <v>704</v>
+        <v>342</v>
       </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219" t="s">
-        <v>534</v>
+        <v>347</v>
       </c>
       <c r="B219" t="s">
-        <v>683</v>
+        <v>343</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3">
+      <c r="A220" t="s">
+        <v>348</v>
+      </c>
+      <c r="B220" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" t="s">
-        <v>551</v>
+        <v>708</v>
       </c>
       <c r="B221" t="s">
-        <v>554</v>
-      </c>
-      <c r="C221" t="s">
-        <v>587</v>
+        <v>704</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" t="s">
-        <v>552</v>
+        <v>534</v>
       </c>
       <c r="B222" t="s">
-        <v>553</v>
-      </c>
-      <c r="C222" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="223" spans="1:3">
-      <c r="A223" t="s">
-        <v>586</v>
-      </c>
-      <c r="B223" t="s">
-        <v>602</v>
+        <v>683</v>
       </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" t="s">
-        <v>365</v>
+        <v>551</v>
       </c>
       <c r="B224" t="s">
-        <v>351</v>
+        <v>554</v>
+      </c>
+      <c r="C224" t="s">
+        <v>587</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" t="s">
-        <v>366</v>
+        <v>552</v>
       </c>
       <c r="B225" t="s">
-        <v>352</v>
+        <v>553</v>
       </c>
       <c r="C225" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" t="s">
-        <v>508</v>
+        <v>586</v>
       </c>
       <c r="B226" t="s">
-        <v>575</v>
+        <v>602</v>
       </c>
     </row>
     <row r="227" spans="1:3">
       <c r="A227" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B227" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B228" t="s">
-        <v>354</v>
+        <v>352</v>
+      </c>
+      <c r="C228" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" t="s">
-        <v>369</v>
+        <v>508</v>
       </c>
       <c r="B229" t="s">
-        <v>355</v>
+        <v>575</v>
       </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="B230" t="s">
-        <v>356</v>
-      </c>
-      <c r="C230" t="s">
-        <v>589</v>
+        <v>353</v>
       </c>
     </row>
     <row r="231" spans="1:3">
       <c r="A231" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B231" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B232" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="233" spans="1:3">
       <c r="A233" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B233" t="s">
-        <v>359</v>
+        <v>356</v>
+      </c>
+      <c r="C233" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B234" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="235" spans="1:3">
       <c r="A235" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B235" t="s">
-        <v>361</v>
-      </c>
-      <c r="C235" t="s">
-        <v>589</v>
+        <v>358</v>
       </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="B236" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B237" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="B238" t="s">
-        <v>364</v>
+        <v>361</v>
+      </c>
+      <c r="C238" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239" t="s">
-        <v>533</v>
+        <v>376</v>
       </c>
       <c r="B239" t="s">
-        <v>667</v>
+        <v>362</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3">
+      <c r="A240" t="s">
+        <v>377</v>
+      </c>
+      <c r="B240" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="241" spans="1:3">
       <c r="A241" t="s">
-        <v>607</v>
+        <v>378</v>
       </c>
       <c r="B241" t="s">
-        <v>608</v>
+        <v>364</v>
       </c>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" t="s">
-        <v>385</v>
+        <v>533</v>
       </c>
       <c r="B242" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="243" spans="1:3">
-      <c r="A243" t="s">
-        <v>386</v>
-      </c>
-      <c r="B243" t="s">
-        <v>400</v>
+        <v>667</v>
       </c>
     </row>
     <row r="244" spans="1:3">
       <c r="A244" t="s">
-        <v>387</v>
+        <v>607</v>
       </c>
       <c r="B244" t="s">
-        <v>401</v>
-      </c>
-      <c r="C244" t="s">
-        <v>589</v>
+        <v>608</v>
       </c>
     </row>
     <row r="245" spans="1:3">
       <c r="A245" t="s">
-        <v>509</v>
+        <v>385</v>
       </c>
       <c r="B245" t="s">
-        <v>576</v>
+        <v>403</v>
       </c>
     </row>
     <row r="246" spans="1:3">
       <c r="A246" t="s">
-        <v>404</v>
+        <v>386</v>
       </c>
       <c r="B246" t="s">
-        <v>402</v>
-      </c>
-      <c r="C246" t="s">
-        <v>589</v>
+        <v>400</v>
       </c>
     </row>
     <row r="247" spans="1:3">
       <c r="A247" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B247" t="s">
-        <v>394</v>
+        <v>401</v>
+      </c>
+      <c r="C247" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="248" spans="1:3">
       <c r="A248" t="s">
-        <v>405</v>
+        <v>509</v>
       </c>
       <c r="B248" t="s">
-        <v>395</v>
-      </c>
-      <c r="C248" t="s">
-        <v>566</v>
+        <v>576</v>
       </c>
     </row>
     <row r="249" spans="1:3">
       <c r="A249" t="s">
-        <v>389</v>
+        <v>404</v>
       </c>
       <c r="B249" t="s">
-        <v>396</v>
+        <v>402</v>
+      </c>
+      <c r="C249" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="250" spans="1:3">
       <c r="A250" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B250" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="251" spans="1:3">
       <c r="A251" t="s">
-        <v>390</v>
+        <v>405</v>
       </c>
       <c r="B251" t="s">
-        <v>398</v>
+        <v>395</v>
+      </c>
+      <c r="C251" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="252" spans="1:3">
       <c r="A252" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B252" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="253" spans="1:3">
       <c r="A253" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B253" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="254" spans="1:3">
       <c r="A254" t="s">
-        <v>532</v>
+        <v>390</v>
       </c>
       <c r="B254" t="s">
-        <v>684</v>
+        <v>398</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3">
+      <c r="A255" t="s">
+        <v>392</v>
+      </c>
+      <c r="B255" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="256" spans="1:3">
       <c r="A256" t="s">
-        <v>523</v>
+        <v>393</v>
       </c>
       <c r="B256" t="s">
-        <v>524</v>
+        <v>396</v>
       </c>
     </row>
     <row r="257" spans="1:3">
       <c r="A257" t="s">
-        <v>411</v>
+        <v>532</v>
       </c>
       <c r="B257" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="258" spans="1:3">
-      <c r="A258" t="s">
-        <v>412</v>
-      </c>
-      <c r="B258" t="s">
-        <v>423</v>
-      </c>
-      <c r="C258" t="s">
-        <v>589</v>
+        <v>684</v>
       </c>
     </row>
     <row r="259" spans="1:3">
       <c r="A259" t="s">
-        <v>577</v>
+        <v>523</v>
       </c>
       <c r="B259" t="s">
-        <v>578</v>
+        <v>524</v>
       </c>
     </row>
     <row r="260" spans="1:3">
       <c r="A260" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B260" t="s">
-        <v>424</v>
-      </c>
-      <c r="C260" t="s">
-        <v>589</v>
+        <v>422</v>
       </c>
     </row>
     <row r="261" spans="1:3">
       <c r="A261" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B261" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C261" t="s">
         <v>589</v>
@@ -8964,128 +8995,128 @@
     </row>
     <row r="262" spans="1:3">
       <c r="A262" t="s">
-        <v>415</v>
+        <v>577</v>
       </c>
       <c r="B262" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
     </row>
     <row r="263" spans="1:3">
       <c r="A263" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B263" t="s">
-        <v>426</v>
+        <v>424</v>
+      </c>
+      <c r="C263" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="264" spans="1:3">
       <c r="A264" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B264" t="s">
-        <v>427</v>
+        <v>425</v>
+      </c>
+      <c r="C264" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="265" spans="1:3">
       <c r="A265" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="B265" t="s">
-        <v>428</v>
+        <v>590</v>
       </c>
     </row>
     <row r="266" spans="1:3">
       <c r="A266" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B266" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="267" spans="1:3">
       <c r="A267" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B267" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="268" spans="1:3">
       <c r="A268" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B268" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="269" spans="1:3">
       <c r="A269" t="s">
-        <v>530</v>
+        <v>419</v>
       </c>
       <c r="B269" t="s">
-        <v>685</v>
+        <v>429</v>
       </c>
     </row>
     <row r="270" spans="1:3">
       <c r="A270" t="s">
-        <v>616</v>
+        <v>420</v>
       </c>
       <c r="B270" t="s">
-        <v>617</v>
+        <v>430</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3">
+      <c r="A271" t="s">
+        <v>421</v>
+      </c>
+      <c r="B271" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="272" spans="1:3">
       <c r="A272" t="s">
-        <v>525</v>
+        <v>530</v>
       </c>
       <c r="B272" t="s">
-        <v>524</v>
+        <v>685</v>
       </c>
     </row>
     <row r="273" spans="1:3">
       <c r="A273" t="s">
-        <v>438</v>
+        <v>616</v>
       </c>
       <c r="B273" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="274" spans="1:3">
-      <c r="A274" t="s">
-        <v>439</v>
-      </c>
-      <c r="B274" t="s">
-        <v>450</v>
-      </c>
-      <c r="C274" t="s">
-        <v>589</v>
+        <v>617</v>
       </c>
     </row>
     <row r="275" spans="1:3">
       <c r="A275" t="s">
-        <v>510</v>
+        <v>525</v>
       </c>
       <c r="B275" t="s">
-        <v>579</v>
+        <v>524</v>
       </c>
     </row>
     <row r="276" spans="1:3">
       <c r="A276" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B276" t="s">
-        <v>451</v>
-      </c>
-      <c r="C276" t="s">
-        <v>589</v>
+        <v>449</v>
       </c>
     </row>
     <row r="277" spans="1:3">
       <c r="A277" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B277" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C277" t="s">
         <v>589</v>
@@ -9093,132 +9124,162 @@
     </row>
     <row r="278" spans="1:3">
       <c r="A278" t="s">
-        <v>442</v>
+        <v>510</v>
       </c>
       <c r="B278" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
     </row>
     <row r="279" spans="1:3">
       <c r="A279" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B279" t="s">
-        <v>426</v>
+        <v>451</v>
+      </c>
+      <c r="C279" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="280" spans="1:3">
       <c r="A280" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B280" t="s">
-        <v>427</v>
+        <v>452</v>
+      </c>
+      <c r="C280" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="281" spans="1:3">
       <c r="A281" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B281" t="s">
-        <v>453</v>
+        <v>591</v>
       </c>
     </row>
     <row r="282" spans="1:3">
       <c r="A282" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B282" t="s">
-        <v>454</v>
+        <v>426</v>
       </c>
     </row>
     <row r="283" spans="1:3">
       <c r="A283" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B283" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="284" spans="1:3">
       <c r="A284" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="B284" t="s">
-        <v>431</v>
+        <v>453</v>
       </c>
     </row>
     <row r="285" spans="1:3">
       <c r="A285" t="s">
-        <v>529</v>
+        <v>446</v>
       </c>
       <c r="B285" t="s">
-        <v>685</v>
+        <v>454</v>
       </c>
     </row>
     <row r="286" spans="1:3">
       <c r="A286" t="s">
-        <v>623</v>
+        <v>447</v>
       </c>
       <c r="B286" t="s">
-        <v>617</v>
+        <v>430</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3">
+      <c r="A287" t="s">
+        <v>448</v>
+      </c>
+      <c r="B287" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="288" spans="1:3">
       <c r="A288" t="s">
-        <v>432</v>
+        <v>529</v>
       </c>
       <c r="B288" t="s">
-        <v>624</v>
+        <v>685</v>
       </c>
     </row>
     <row r="289" spans="1:3">
       <c r="A289" t="s">
-        <v>433</v>
+        <v>623</v>
       </c>
       <c r="B289" t="s">
-        <v>625</v>
-      </c>
-      <c r="C289" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="290" spans="1:3">
-      <c r="A290" t="s">
-        <v>511</v>
-      </c>
-      <c r="B290" t="s">
-        <v>626</v>
+        <v>617</v>
       </c>
     </row>
     <row r="291" spans="1:3">
       <c r="A291" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B291" t="s">
-        <v>652</v>
+        <v>624</v>
       </c>
     </row>
     <row r="292" spans="1:3">
       <c r="A292" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B292" t="s">
-        <v>627</v>
+        <v>625</v>
+      </c>
+      <c r="C292" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="293" spans="1:3">
       <c r="A293" t="s">
-        <v>436</v>
+        <v>511</v>
       </c>
       <c r="B293" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="294" spans="1:3">
       <c r="A294" t="s">
+        <v>434</v>
+      </c>
+      <c r="B294" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3">
+      <c r="A295" t="s">
+        <v>435</v>
+      </c>
+      <c r="B295" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3">
+      <c r="A296" t="s">
+        <v>436</v>
+      </c>
+      <c r="B296" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3">
+      <c r="A297" t="s">
         <v>528</v>
       </c>
-      <c r="B294" t="s">
+      <c r="B297" t="s">
         <v>686</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changes for CZI - User Story 57194
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.malyala\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raluca.ilinca.AzureAI-Jump2\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84F1CA9-3724-477F-911B-7A3B8E1139BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1216931-A0D9-4A06-8B56-85E9DBABFBB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="22440" windowHeight="11715" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="740">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="740">
   <si>
     <t>Name</t>
   </si>
@@ -2244,9 +2244,6 @@
     <t>SupportedIncomeTypes</t>
   </si>
   <si>
-    <t>Not supported Income Type. Needs manual review.</t>
-  </si>
-  <si>
     <t>ICW_NotSupportedIncomeTypes</t>
   </si>
   <si>
@@ -2260,6 +2257,9 @@
   </si>
   <si>
     <t>FailureEmailBodyActionReq</t>
+  </si>
+  <si>
+    <t>Income type included that cannot be validated with automation. Manual review required.</t>
   </si>
 </sst>
 </file>
@@ -2637,8 +2637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3986,10 +3986,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80DB68E2-2057-45AB-A45E-3EB9CF844C19}">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4316,6 +4316,14 @@
       </c>
       <c r="B40" t="s">
         <v>480</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>485</v>
+      </c>
+      <c r="B41" t="s">
+        <v>482</v>
       </c>
     </row>
   </sheetData>
@@ -4528,10 +4536,10 @@
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B21" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
@@ -6915,8 +6923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
   <dimension ref="A1:C297"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A153" workbookViewId="0">
-      <selection activeCell="A136" sqref="A136"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7055,10 +7063,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B18" t="s">
-        <v>734</v>
+        <v>739</v>
       </c>
       <c r="C18" t="s">
         <v>693</v>
@@ -7984,10 +7992,10 @@
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
+        <v>735</v>
+      </c>
+      <c r="B136" t="s">
         <v>736</v>
-      </c>
-      <c r="B136" t="s">
-        <v>737</v>
       </c>
       <c r="C136" t="s">
         <v>693</v>

</xml_diff>

<commit_message>
published new version to the Orchestrator
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raluca.ilinca.AzureAI-Jump2\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1216931-A0D9-4A06-8B56-85E9DBABFBB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0AC798-84DA-45D1-9EE4-07D545A7A6EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="22440" windowHeight="11715" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="22440" windowHeight="11715" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -3988,8 +3988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80DB68E2-2057-45AB-A45E-3EB9CF844C19}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6923,7 +6923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
   <dimension ref="A1:C297"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Upadted the defects for 012826
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raluca.ilinca.AzureAI-Jump2\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.malyala\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0AC798-84DA-45D1-9EE4-07D545A7A6EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE69021D-51FA-41D0-AC1B-91B5C7B53558}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="22440" windowHeight="11715" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="740">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="741">
   <si>
     <t>Name</t>
   </si>
@@ -2220,9 +2220,6 @@
     <t>Not all adults in the household have signed the VAWA.</t>
   </si>
   <si>
-    <t>C:\Users\raluca.ilinca.AzureAI-Jump2\Documents\AZApplicationReview\Prompts\</t>
-  </si>
-  <si>
     <t>The Housing History Disclosure form is a required document but missing from the application.</t>
   </si>
   <si>
@@ -2260,6 +2257,12 @@
   </si>
   <si>
     <t>Income type included that cannot be validated with automation. Manual review required.</t>
+  </si>
+  <si>
+    <t>C:\Users\Harika.Malyala\Documents\AZApplicationReview\Prompts\</t>
+  </si>
+  <si>
+    <t>SD_LLMExtractionJSONsFolder</t>
   </si>
 </sst>
 </file>
@@ -2637,8 +2640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2722,7 +2725,7 @@
         <v>209</v>
       </c>
       <c r="B7" t="s">
-        <v>726</v>
+        <v>739</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -3988,8 +3991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80DB68E2-2057-45AB-A45E-3EB9CF844C19}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4536,10 +4539,10 @@
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B21" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
@@ -5589,8 +5592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1011"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5935,13 +5938,20 @@
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B39" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
+        <v>732</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A40" t="s">
+        <v>740</v>
+      </c>
+      <c r="B40" t="s">
+        <v>740</v>
+      </c>
+    </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="42" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="43" spans="1:2" ht="14.25" customHeight="1"/>
@@ -6923,8 +6933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
   <dimension ref="A1:C297"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6952,10 +6962,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B5" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="C5" t="s">
         <v>693</v>
@@ -7052,10 +7062,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
+        <v>730</v>
+      </c>
+      <c r="B17" t="s">
         <v>731</v>
-      </c>
-      <c r="B17" t="s">
-        <v>732</v>
       </c>
       <c r="C17" t="s">
         <v>693</v>
@@ -7063,10 +7073,10 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B18" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C18" t="s">
         <v>693</v>
@@ -7981,10 +7991,10 @@
     </row>
     <row r="135" spans="1:3">
       <c r="A135" t="s">
+        <v>728</v>
+      </c>
+      <c r="B135" t="s">
         <v>729</v>
-      </c>
-      <c r="B135" t="s">
-        <v>730</v>
       </c>
       <c r="C135" t="s">
         <v>693</v>
@@ -7992,10 +8002,10 @@
     </row>
     <row r="136" spans="1:3">
       <c r="A136" t="s">
+        <v>734</v>
+      </c>
+      <c r="B136" t="s">
         <v>735</v>
-      </c>
-      <c r="B136" t="s">
-        <v>736</v>
       </c>
       <c r="C136" t="s">
         <v>693</v>

</xml_diff>

<commit_message>
Changes for 57817 – implementing Dominium employee logic in the EDC, consistent with the logic previously implemented in ICW.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harika.malyala\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raluca.ilinca.AzureAI-Jump2\Documents\Git\AZ-Application-Review-Process_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20BAD6E-2F96-4047-89B0-0D705F4F830B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606F359C-1347-44CC-AE74-0BE416A3A6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="13950" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28200" windowHeight="13530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="742">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="743">
   <si>
     <t>Name</t>
   </si>
@@ -2256,9 +2256,6 @@
     <t>Income type included that cannot be validated with automation. Manual review required.</t>
   </si>
   <si>
-    <t>C:\Users\Harika.Malyala\Documents\AZApplicationReview\Prompts\</t>
-  </si>
-  <si>
     <t>SD_LLMExtractionJSONsFolder</t>
   </si>
   <si>
@@ -2266,6 +2263,12 @@
   </si>
   <si>
     <t>updated by Harika</t>
+  </si>
+  <si>
+    <t>EDC_DominiumEmployee</t>
+  </si>
+  <si>
+    <t>C:\Users\raluca.ilinca.AzureAI-Jump2\Documents\AZApplicationReview\Prompts\</t>
   </si>
 </sst>
 </file>
@@ -2643,8 +2646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2728,7 +2731,7 @@
         <v>209</v>
       </c>
       <c r="B7" t="s">
-        <v>738</v>
+        <v>742</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -5949,10 +5952,10 @@
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B40" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="14.25" customHeight="1"/>
@@ -6934,10 +6937,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB30D651-CF18-42CB-8A58-9F597F965D74}">
-  <dimension ref="A1:C297"/>
+  <dimension ref="A1:C298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="B118" sqref="B118"/>
+    <sheetView topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="D137" sqref="D137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7827,10 +7830,10 @@
         <v>557</v>
       </c>
       <c r="B113" t="s">
+        <v>739</v>
+      </c>
+      <c r="C113" t="s">
         <v>740</v>
-      </c>
-      <c r="C113" t="s">
-        <v>741</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -8017,31 +8020,31 @@
         <v>692</v>
       </c>
     </row>
-    <row r="138" spans="1:3">
-      <c r="A138" t="s">
-        <v>513</v>
-      </c>
-      <c r="B138" t="s">
-        <v>514</v>
+    <row r="137" spans="1:3">
+      <c r="A137" t="s">
+        <v>741</v>
+      </c>
+      <c r="B137" t="s">
+        <v>730</v>
+      </c>
+      <c r="C137" t="s">
+        <v>692</v>
       </c>
     </row>
     <row r="139" spans="1:3">
       <c r="A139" t="s">
-        <v>661</v>
+        <v>513</v>
       </c>
       <c r="B139" t="s">
-        <v>665</v>
-      </c>
-      <c r="C139" t="s">
-        <v>663</v>
+        <v>514</v>
       </c>
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B140" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="C140" t="s">
         <v>663</v>
@@ -8049,405 +8052,408 @@
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>242</v>
+        <v>662</v>
       </c>
       <c r="B141" t="s">
-        <v>243</v>
+        <v>664</v>
       </c>
       <c r="C141" t="s">
-        <v>588</v>
+        <v>663</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B142" t="s">
-        <v>245</v>
+        <v>243</v>
+      </c>
+      <c r="C142" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="B143" t="s">
-        <v>560</v>
-      </c>
-      <c r="C143" t="s">
-        <v>650</v>
+        <v>245</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="B144" t="s">
-        <v>246</v>
+        <v>560</v>
+      </c>
+      <c r="C144" t="s">
+        <v>650</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>503</v>
+        <v>247</v>
       </c>
       <c r="B145" t="s">
-        <v>512</v>
+        <v>246</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>249</v>
+        <v>503</v>
       </c>
       <c r="B146" t="s">
-        <v>248</v>
+        <v>512</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B147" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B148" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B149" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B150" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>302</v>
+        <v>257</v>
       </c>
       <c r="B151" t="s">
-        <v>248</v>
+        <v>256</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>349</v>
+        <v>302</v>
       </c>
       <c r="B152" t="s">
-        <v>350</v>
+        <v>248</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>657</v>
+        <v>349</v>
       </c>
       <c r="B153" t="s">
-        <v>658</v>
+        <v>350</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>702</v>
+        <v>657</v>
       </c>
       <c r="B154" t="s">
-        <v>703</v>
+        <v>658</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
+        <v>702</v>
+      </c>
+      <c r="B155" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" t="s">
         <v>526</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B156" t="s">
         <v>678</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3">
-      <c r="A157" t="s">
-        <v>515</v>
-      </c>
-      <c r="B157" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
+        <v>515</v>
+      </c>
+      <c r="B158" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159" t="s">
         <v>259</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B159" t="s">
         <v>262</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C159" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="159" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A159" t="s">
+    <row r="160" spans="1:3" ht="13.5" customHeight="1">
+      <c r="A160" t="s">
         <v>261</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B160" t="s">
         <v>561</v>
       </c>
-      <c r="C159" t="s">
+      <c r="C160" t="s">
         <v>696</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3">
-      <c r="A160" t="s">
-        <v>260</v>
-      </c>
-      <c r="B160" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B161" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B162" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B163" t="s">
-        <v>268</v>
-      </c>
-      <c r="C163" t="s">
-        <v>660</v>
+        <v>267</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>504</v>
+        <v>269</v>
       </c>
       <c r="B164" t="s">
-        <v>570</v>
+        <v>268</v>
+      </c>
+      <c r="C164" t="s">
+        <v>660</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
-        <v>270</v>
+        <v>504</v>
       </c>
       <c r="B165" t="s">
-        <v>271</v>
+        <v>570</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B166" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B167" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B168" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B169" t="s">
-        <v>285</v>
-      </c>
-      <c r="C169" t="s">
-        <v>660</v>
+        <v>286</v>
       </c>
     </row>
     <row r="170" spans="1:3">
       <c r="A170" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B170" t="s">
-        <v>605</v>
+        <v>285</v>
+      </c>
+      <c r="C170" t="s">
+        <v>660</v>
       </c>
     </row>
     <row r="171" spans="1:3">
       <c r="A171" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B171" t="s">
-        <v>284</v>
-      </c>
-      <c r="C171" t="s">
-        <v>660</v>
+        <v>605</v>
       </c>
     </row>
     <row r="172" spans="1:3">
       <c r="A172" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B172" t="s">
-        <v>283</v>
+        <v>284</v>
+      </c>
+      <c r="C172" t="s">
+        <v>660</v>
       </c>
     </row>
     <row r="173" spans="1:3">
       <c r="A173" t="s">
-        <v>299</v>
+        <v>282</v>
       </c>
       <c r="B173" t="s">
-        <v>300</v>
+        <v>283</v>
       </c>
     </row>
     <row r="174" spans="1:3">
       <c r="A174" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B174" t="s">
-        <v>248</v>
+        <v>300</v>
       </c>
     </row>
     <row r="175" spans="1:3">
       <c r="A175" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B175" t="s">
-        <v>305</v>
+        <v>248</v>
       </c>
     </row>
     <row r="176" spans="1:3">
       <c r="A176" t="s">
-        <v>704</v>
+        <v>304</v>
       </c>
       <c r="B176" t="s">
-        <v>703</v>
+        <v>305</v>
       </c>
     </row>
     <row r="177" spans="1:3">
       <c r="A177" t="s">
-        <v>537</v>
+        <v>704</v>
       </c>
       <c r="B177" t="s">
-        <v>679</v>
+        <v>703</v>
       </c>
     </row>
     <row r="178" spans="1:3">
       <c r="A178" t="s">
+        <v>537</v>
+      </c>
+      <c r="B178" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3">
+      <c r="A179" t="s">
         <v>697</v>
       </c>
-      <c r="B178" t="s">
+      <c r="B179" t="s">
         <v>698</v>
       </c>
-      <c r="C178" t="s">
+      <c r="C179" t="s">
         <v>692</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3">
-      <c r="A180" t="s">
-        <v>517</v>
-      </c>
-      <c r="B180" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="181" spans="1:3">
       <c r="A181" t="s">
-        <v>292</v>
+        <v>517</v>
       </c>
       <c r="B181" t="s">
-        <v>296</v>
-      </c>
-      <c r="C181" t="s">
-        <v>588</v>
+        <v>518</v>
       </c>
     </row>
     <row r="182" spans="1:3">
       <c r="A182" t="s">
-        <v>505</v>
+        <v>292</v>
       </c>
       <c r="B182" t="s">
-        <v>571</v>
+        <v>296</v>
+      </c>
+      <c r="C182" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="183" spans="1:3">
       <c r="A183" t="s">
-        <v>293</v>
+        <v>505</v>
       </c>
       <c r="B183" t="s">
-        <v>297</v>
-      </c>
-      <c r="C183" t="s">
-        <v>588</v>
+        <v>571</v>
       </c>
     </row>
     <row r="184" spans="1:3">
       <c r="A184" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B184" t="s">
-        <v>298</v>
+        <v>297</v>
+      </c>
+      <c r="C184" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="185" spans="1:3">
       <c r="A185" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B185" t="s">
-        <v>562</v>
+        <v>298</v>
       </c>
     </row>
     <row r="186" spans="1:3">
       <c r="A186" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
       <c r="B186" t="s">
-        <v>248</v>
+        <v>562</v>
       </c>
     </row>
     <row r="187" spans="1:3">
       <c r="A187" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="B187" t="s">
-        <v>310</v>
+        <v>248</v>
       </c>
     </row>
     <row r="188" spans="1:3">
       <c r="A188" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="B188" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="189" spans="1:3">
       <c r="A189" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B189" t="s">
         <v>308</v>
@@ -8455,607 +8461,604 @@
     </row>
     <row r="190" spans="1:3">
       <c r="A190" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B190" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="191" spans="1:3">
       <c r="A191" t="s">
-        <v>705</v>
+        <v>311</v>
       </c>
       <c r="B191" t="s">
-        <v>703</v>
+        <v>312</v>
       </c>
     </row>
     <row r="192" spans="1:3">
       <c r="A192" t="s">
+        <v>705</v>
+      </c>
+      <c r="B192" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3">
+      <c r="A193" t="s">
         <v>536</v>
       </c>
-      <c r="B192" t="s">
+      <c r="B193" t="s">
         <v>680</v>
-      </c>
-    </row>
-    <row r="194" spans="1:3">
-      <c r="A194" t="s">
-        <v>519</v>
-      </c>
-      <c r="B194" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="195" spans="1:3">
       <c r="A195" t="s">
-        <v>499</v>
+        <v>519</v>
       </c>
       <c r="B195" t="s">
-        <v>320</v>
-      </c>
-      <c r="C195" t="s">
-        <v>588</v>
+        <v>520</v>
       </c>
     </row>
     <row r="196" spans="1:3">
       <c r="A196" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="B196" t="s">
-        <v>572</v>
+        <v>320</v>
+      </c>
+      <c r="C196" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="197" spans="1:3">
       <c r="A197" t="s">
-        <v>315</v>
+        <v>506</v>
       </c>
       <c r="B197" t="s">
-        <v>321</v>
-      </c>
-      <c r="C197" t="s">
-        <v>588</v>
+        <v>572</v>
       </c>
     </row>
     <row r="198" spans="1:3">
       <c r="A198" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B198" t="s">
-        <v>322</v>
+        <v>321</v>
+      </c>
+      <c r="C198" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="199" spans="1:3">
       <c r="A199" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B199" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="200" spans="1:3">
       <c r="A200" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B200" t="s">
-        <v>563</v>
+        <v>323</v>
       </c>
     </row>
     <row r="201" spans="1:3">
       <c r="A201" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B201" t="s">
-        <v>248</v>
+        <v>563</v>
       </c>
     </row>
     <row r="202" spans="1:3">
       <c r="A202" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B202" t="s">
-        <v>325</v>
-      </c>
-      <c r="C202" t="s">
-        <v>588</v>
+        <v>248</v>
       </c>
     </row>
     <row r="203" spans="1:3">
       <c r="A203" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B203" t="s">
-        <v>327</v>
+        <v>325</v>
+      </c>
+      <c r="C203" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B204" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B205" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B206" t="s">
-        <v>256</v>
+        <v>331</v>
       </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" t="s">
-        <v>706</v>
+        <v>332</v>
       </c>
       <c r="B207" t="s">
-        <v>703</v>
+        <v>256</v>
       </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" t="s">
+        <v>706</v>
+      </c>
+      <c r="B208" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
+      <c r="A209" t="s">
         <v>535</v>
       </c>
-      <c r="B208" t="s">
+      <c r="B209" t="s">
         <v>681</v>
-      </c>
-    </row>
-    <row r="210" spans="1:3">
-      <c r="A210" t="s">
-        <v>521</v>
-      </c>
-      <c r="B210" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" t="s">
-        <v>501</v>
+        <v>521</v>
       </c>
       <c r="B211" t="s">
-        <v>338</v>
-      </c>
-      <c r="C211" t="s">
-        <v>588</v>
+        <v>522</v>
       </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" t="s">
-        <v>507</v>
+        <v>501</v>
       </c>
       <c r="B212" t="s">
-        <v>573</v>
+        <v>338</v>
+      </c>
+      <c r="C212" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" t="s">
-        <v>336</v>
+        <v>507</v>
       </c>
       <c r="B213" t="s">
-        <v>339</v>
-      </c>
-      <c r="C213" t="s">
-        <v>588</v>
+        <v>573</v>
       </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B214" t="s">
-        <v>340</v>
+        <v>339</v>
+      </c>
+      <c r="C214" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" t="s">
-        <v>500</v>
+        <v>337</v>
       </c>
       <c r="B215" t="s">
-        <v>564</v>
+        <v>340</v>
       </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" t="s">
-        <v>344</v>
+        <v>500</v>
       </c>
       <c r="B216" t="s">
-        <v>248</v>
+        <v>564</v>
       </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B217" t="s">
-        <v>341</v>
+        <v>248</v>
       </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B218" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B219" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B220" t="s">
-        <v>256</v>
+        <v>343</v>
       </c>
     </row>
     <row r="221" spans="1:3">
       <c r="A221" t="s">
-        <v>707</v>
+        <v>348</v>
       </c>
       <c r="B221" t="s">
-        <v>703</v>
+        <v>256</v>
       </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" t="s">
+        <v>707</v>
+      </c>
+      <c r="B222" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3">
+      <c r="A223" t="s">
         <v>534</v>
       </c>
-      <c r="B222" t="s">
+      <c r="B223" t="s">
         <v>682</v>
-      </c>
-    </row>
-    <row r="224" spans="1:3">
-      <c r="A224" t="s">
-        <v>551</v>
-      </c>
-      <c r="B224" t="s">
-        <v>554</v>
-      </c>
-      <c r="C224" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="225" spans="1:3">
       <c r="A225" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B225" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="C225" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" t="s">
-        <v>585</v>
+        <v>552</v>
       </c>
       <c r="B226" t="s">
-        <v>601</v>
+        <v>553</v>
+      </c>
+      <c r="C226" t="s">
+        <v>587</v>
       </c>
     </row>
     <row r="227" spans="1:3">
       <c r="A227" t="s">
-        <v>365</v>
+        <v>585</v>
       </c>
       <c r="B227" t="s">
-        <v>351</v>
+        <v>601</v>
       </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B228" t="s">
-        <v>352</v>
-      </c>
-      <c r="C228" t="s">
-        <v>588</v>
+        <v>351</v>
       </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" t="s">
-        <v>508</v>
+        <v>366</v>
       </c>
       <c r="B229" t="s">
-        <v>574</v>
+        <v>352</v>
+      </c>
+      <c r="C229" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" t="s">
-        <v>367</v>
+        <v>508</v>
       </c>
       <c r="B230" t="s">
-        <v>353</v>
+        <v>574</v>
       </c>
     </row>
     <row r="231" spans="1:3">
       <c r="A231" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B231" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B232" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="233" spans="1:3">
       <c r="A233" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B233" t="s">
-        <v>356</v>
-      </c>
-      <c r="C233" t="s">
-        <v>588</v>
+        <v>355</v>
       </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B234" t="s">
-        <v>357</v>
+        <v>356</v>
+      </c>
+      <c r="C234" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="235" spans="1:3">
       <c r="A235" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B235" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B236" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B237" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B238" t="s">
-        <v>361</v>
-      </c>
-      <c r="C238" t="s">
-        <v>588</v>
+        <v>360</v>
       </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B239" t="s">
-        <v>362</v>
+        <v>361</v>
+      </c>
+      <c r="C239" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="240" spans="1:3">
       <c r="A240" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B240" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="241" spans="1:3">
       <c r="A241" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B241" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" t="s">
+        <v>378</v>
+      </c>
+      <c r="B242" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3">
+      <c r="A243" t="s">
         <v>533</v>
       </c>
-      <c r="B242" t="s">
+      <c r="B243" t="s">
         <v>666</v>
-      </c>
-    </row>
-    <row r="244" spans="1:3">
-      <c r="A244" t="s">
-        <v>606</v>
-      </c>
-      <c r="B244" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="245" spans="1:3">
       <c r="A245" t="s">
-        <v>385</v>
+        <v>606</v>
       </c>
       <c r="B245" t="s">
-        <v>403</v>
+        <v>607</v>
       </c>
     </row>
     <row r="246" spans="1:3">
       <c r="A246" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B246" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
     </row>
     <row r="247" spans="1:3">
       <c r="A247" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B247" t="s">
-        <v>401</v>
-      </c>
-      <c r="C247" t="s">
-        <v>588</v>
+        <v>400</v>
       </c>
     </row>
     <row r="248" spans="1:3">
       <c r="A248" t="s">
-        <v>509</v>
+        <v>387</v>
       </c>
       <c r="B248" t="s">
-        <v>575</v>
+        <v>401</v>
+      </c>
+      <c r="C248" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="249" spans="1:3">
       <c r="A249" t="s">
-        <v>404</v>
+        <v>509</v>
       </c>
       <c r="B249" t="s">
-        <v>402</v>
-      </c>
-      <c r="C249" t="s">
-        <v>588</v>
+        <v>575</v>
       </c>
     </row>
     <row r="250" spans="1:3">
       <c r="A250" t="s">
-        <v>388</v>
+        <v>404</v>
       </c>
       <c r="B250" t="s">
-        <v>394</v>
+        <v>402</v>
+      </c>
+      <c r="C250" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="251" spans="1:3">
       <c r="A251" t="s">
-        <v>405</v>
+        <v>388</v>
       </c>
       <c r="B251" t="s">
-        <v>395</v>
-      </c>
-      <c r="C251" t="s">
-        <v>565</v>
+        <v>394</v>
       </c>
     </row>
     <row r="252" spans="1:3">
       <c r="A252" t="s">
-        <v>389</v>
+        <v>405</v>
       </c>
       <c r="B252" t="s">
-        <v>396</v>
+        <v>395</v>
+      </c>
+      <c r="C252" t="s">
+        <v>565</v>
       </c>
     </row>
     <row r="253" spans="1:3">
       <c r="A253" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B253" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="254" spans="1:3">
       <c r="A254" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="B254" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="255" spans="1:3">
       <c r="A255" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B255" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="256" spans="1:3">
       <c r="A256" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B256" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
     </row>
     <row r="257" spans="1:3">
       <c r="A257" t="s">
+        <v>393</v>
+      </c>
+      <c r="B257" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3">
+      <c r="A258" t="s">
         <v>532</v>
       </c>
-      <c r="B257" t="s">
+      <c r="B258" t="s">
         <v>683</v>
-      </c>
-    </row>
-    <row r="259" spans="1:3">
-      <c r="A259" t="s">
-        <v>523</v>
-      </c>
-      <c r="B259" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="260" spans="1:3">
       <c r="A260" t="s">
-        <v>411</v>
+        <v>523</v>
       </c>
       <c r="B260" t="s">
-        <v>422</v>
+        <v>524</v>
       </c>
     </row>
     <row r="261" spans="1:3">
       <c r="A261" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B261" t="s">
-        <v>423</v>
-      </c>
-      <c r="C261" t="s">
-        <v>588</v>
+        <v>422</v>
       </c>
     </row>
     <row r="262" spans="1:3">
       <c r="A262" t="s">
-        <v>576</v>
+        <v>412</v>
       </c>
       <c r="B262" t="s">
-        <v>577</v>
+        <v>423</v>
+      </c>
+      <c r="C262" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="263" spans="1:3">
       <c r="A263" t="s">
-        <v>413</v>
+        <v>576</v>
       </c>
       <c r="B263" t="s">
-        <v>424</v>
-      </c>
-      <c r="C263" t="s">
-        <v>588</v>
+        <v>577</v>
       </c>
     </row>
     <row r="264" spans="1:3">
       <c r="A264" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B264" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C264" t="s">
         <v>588</v>
@@ -9063,128 +9066,128 @@
     </row>
     <row r="265" spans="1:3">
       <c r="A265" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B265" t="s">
-        <v>589</v>
+        <v>425</v>
+      </c>
+      <c r="C265" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="266" spans="1:3">
       <c r="A266" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B266" t="s">
-        <v>426</v>
+        <v>589</v>
       </c>
     </row>
     <row r="267" spans="1:3">
       <c r="A267" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B267" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="268" spans="1:3">
       <c r="A268" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B268" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="269" spans="1:3">
       <c r="A269" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B269" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="270" spans="1:3">
       <c r="A270" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B270" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="271" spans="1:3">
       <c r="A271" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B271" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="272" spans="1:3">
       <c r="A272" t="s">
-        <v>530</v>
+        <v>421</v>
       </c>
       <c r="B272" t="s">
-        <v>684</v>
+        <v>431</v>
       </c>
     </row>
     <row r="273" spans="1:3">
       <c r="A273" t="s">
+        <v>530</v>
+      </c>
+      <c r="B273" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3">
+      <c r="A274" t="s">
         <v>615</v>
       </c>
-      <c r="B273" t="s">
+      <c r="B274" t="s">
         <v>616</v>
-      </c>
-    </row>
-    <row r="275" spans="1:3">
-      <c r="A275" t="s">
-        <v>525</v>
-      </c>
-      <c r="B275" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="276" spans="1:3">
       <c r="A276" t="s">
-        <v>438</v>
+        <v>525</v>
       </c>
       <c r="B276" t="s">
-        <v>449</v>
+        <v>524</v>
       </c>
     </row>
     <row r="277" spans="1:3">
       <c r="A277" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B277" t="s">
-        <v>450</v>
-      </c>
-      <c r="C277" t="s">
-        <v>588</v>
+        <v>449</v>
       </c>
     </row>
     <row r="278" spans="1:3">
       <c r="A278" t="s">
-        <v>510</v>
+        <v>439</v>
       </c>
       <c r="B278" t="s">
-        <v>578</v>
+        <v>450</v>
+      </c>
+      <c r="C278" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="279" spans="1:3">
       <c r="A279" t="s">
-        <v>440</v>
+        <v>510</v>
       </c>
       <c r="B279" t="s">
-        <v>451</v>
-      </c>
-      <c r="C279" t="s">
-        <v>588</v>
+        <v>578</v>
       </c>
     </row>
     <row r="280" spans="1:3">
       <c r="A280" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B280" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C280" t="s">
         <v>588</v>
@@ -9192,132 +9195,143 @@
     </row>
     <row r="281" spans="1:3">
       <c r="A281" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B281" t="s">
-        <v>590</v>
+        <v>452</v>
+      </c>
+      <c r="C281" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="282" spans="1:3">
       <c r="A282" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B282" t="s">
-        <v>426</v>
+        <v>590</v>
       </c>
     </row>
     <row r="283" spans="1:3">
       <c r="A283" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B283" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="284" spans="1:3">
       <c r="A284" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B284" t="s">
-        <v>453</v>
+        <v>427</v>
       </c>
     </row>
     <row r="285" spans="1:3">
       <c r="A285" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B285" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="286" spans="1:3">
       <c r="A286" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B286" t="s">
-        <v>430</v>
+        <v>454</v>
       </c>
     </row>
     <row r="287" spans="1:3">
       <c r="A287" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B287" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="288" spans="1:3">
       <c r="A288" t="s">
-        <v>529</v>
+        <v>448</v>
       </c>
       <c r="B288" t="s">
-        <v>684</v>
+        <v>431</v>
       </c>
     </row>
     <row r="289" spans="1:3">
       <c r="A289" t="s">
+        <v>529</v>
+      </c>
+      <c r="B289" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3">
+      <c r="A290" t="s">
         <v>622</v>
       </c>
-      <c r="B289" t="s">
+      <c r="B290" t="s">
         <v>616</v>
-      </c>
-    </row>
-    <row r="291" spans="1:3">
-      <c r="A291" t="s">
-        <v>432</v>
-      </c>
-      <c r="B291" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="292" spans="1:3">
       <c r="A292" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B292" t="s">
-        <v>624</v>
-      </c>
-      <c r="C292" t="s">
-        <v>588</v>
+        <v>623</v>
       </c>
     </row>
     <row r="293" spans="1:3">
       <c r="A293" t="s">
-        <v>511</v>
+        <v>433</v>
       </c>
       <c r="B293" t="s">
-        <v>625</v>
+        <v>624</v>
+      </c>
+      <c r="C293" t="s">
+        <v>588</v>
       </c>
     </row>
     <row r="294" spans="1:3">
       <c r="A294" t="s">
-        <v>434</v>
+        <v>511</v>
       </c>
       <c r="B294" t="s">
-        <v>651</v>
+        <v>625</v>
       </c>
     </row>
     <row r="295" spans="1:3">
       <c r="A295" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B295" t="s">
-        <v>626</v>
+        <v>651</v>
       </c>
     </row>
     <row r="296" spans="1:3">
       <c r="A296" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B296" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="297" spans="1:3">
       <c r="A297" t="s">
+        <v>436</v>
+      </c>
+      <c r="B297" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3">
+      <c r="A298" t="s">
         <v>528</v>
       </c>
-      <c r="B297" t="s">
+      <c r="B298" t="s">
         <v>685</v>
       </c>
     </row>

</xml_diff>